<commit_message>
Solo falta columnas de controladores de usuarios
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C3D336-AABB-4202-AA2F-311620B6B0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5758970A-4968-433E-BD10-BB70BDBDC2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
+    <workbookView xWindow="10050" yWindow="2490" windowWidth="10395" windowHeight="7875" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
-  <si>
-    <t>Vista</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="305">
+  <si>
+    <t>Controlador</t>
   </si>
   <si>
     <t>MVC</t>
@@ -147,6 +147,9 @@
     <t>Recopilacion_inf</t>
   </si>
   <si>
+    <t>Vista:</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">                                                                                                                                                                 </t>
     </r>
@@ -346,14 +349,683 @@
     <t>/secretariahome</t>
   </si>
   <si>
-    <t>FALTAN LAS VISTAS DE CARPETA TESIS</t>
+    <t>/tesus/acta_examen</t>
+  </si>
+  <si>
+    <t>/tesis/archivosubido</t>
+  </si>
+  <si>
+    <t>/tesis/create</t>
+  </si>
+  <si>
+    <t>/tesis/create_fecha_descargar</t>
+  </si>
+  <si>
+    <t>/tesis/create_num_memo</t>
+  </si>
+  <si>
+    <t>/tesis/createnummemotitulados</t>
+  </si>
+  <si>
+    <t>/tesis/edit</t>
+  </si>
+  <si>
+    <t>/tesis/edit2</t>
+  </si>
+  <si>
+    <t>/tesis/edit3</t>
+  </si>
+  <si>
+    <t>/tesis/error_campos</t>
+  </si>
+  <si>
+    <t>/tesis/error_generar_pdf</t>
+  </si>
+  <si>
+    <t>/tesis/error_rut</t>
+  </si>
+  <si>
+    <t>/tesis/evaluar</t>
+  </si>
+  <si>
+    <t>/tesis/evaluar_director</t>
+  </si>
+  <si>
+    <t>/tesis/fecha_presentacion</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_pend_pro</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_pendiente</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_pendiente_prorroga_vencida</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_pendiente_vencida</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_prorroga</t>
+  </si>
+  <si>
+    <t>/tesis/filtro_prorroga_vencida</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_notas_pend_pro_venc</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_notas_pend_venc</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_notas_pro_venc</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_sol</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_tesis_inscritas</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_todas_tesis_ins</t>
+  </si>
+  <si>
+    <t>/tesis/imprimir_todas_tesis_sol</t>
+  </si>
+  <si>
+    <t>/tesis/index</t>
+  </si>
+  <si>
+    <t>/tesis/index1</t>
+  </si>
+  <si>
+    <t>/tesis/index2</t>
+  </si>
+  <si>
+    <t>/tesis/index2_ins_pro</t>
+  </si>
+  <si>
+    <t>/tesis/index2_ins</t>
+  </si>
+  <si>
+    <t>/tesis/index3_ins</t>
+  </si>
+  <si>
+    <t>/tesis/index3_sol</t>
+  </si>
+  <si>
+    <t>/tesis/index_al_sec</t>
+  </si>
+  <si>
+    <t>/tesis/index_solicitud_nota_pendiente</t>
+  </si>
+  <si>
+    <t>/tesis/index_solicitud_nota_pendiente_director</t>
+  </si>
+  <si>
+    <t>/tesis/index_solicitud_nota_prorroga</t>
+  </si>
+  <si>
+    <t>/tesis/index_solicitud_nota_prorroga_director</t>
+  </si>
+  <si>
+    <t>/tesis/index_titulados_sec</t>
+  </si>
+  <si>
+    <t>/tesis/informes_generar_pdf</t>
+  </si>
+  <si>
+    <t>/tesis/ingresar_nota_tesis</t>
+  </si>
+  <si>
+    <t>/tesis/lista_profes_comision_revisión</t>
+  </si>
+  <si>
+    <t>/tesis/mostrar_tesis</t>
+  </si>
+  <si>
+    <t>/tesis/noeditartesis</t>
+  </si>
+  <si>
+    <t>/tesis/nota_pendiente</t>
+  </si>
+  <si>
+    <t>/tesis/pedir_nota_prorroga</t>
+  </si>
+  <si>
+    <t>/tesis/pedir_nota_pendiente</t>
+  </si>
+  <si>
+    <t>/tesis/pend_pro_vencidas</t>
+  </si>
+  <si>
+    <t>/tesis/pendientes_vencidas</t>
+  </si>
+  <si>
+    <t>/tesis/print</t>
+  </si>
+  <si>
+    <t>/tesis/prinTesisc</t>
+  </si>
+  <si>
+    <t>/tesis/printTesisfc</t>
+  </si>
+  <si>
+    <t>/tesis/prinTesisp</t>
+  </si>
+  <si>
+    <t>/tesis/profesor_repetido_comision</t>
+  </si>
+  <si>
+    <t>/tesis/prorrogas_vencidas</t>
+  </si>
+  <si>
+    <t>/tesis/rango_fechas</t>
+  </si>
+  <si>
+    <t>/tesis/recopilacion_inf</t>
+  </si>
+  <si>
+    <t>/tesis/recopilacion_inf2</t>
+  </si>
+  <si>
+    <t>/tesis/recopilacion_inf_alumno2</t>
+  </si>
+  <si>
+    <t>/tesis/repositorio_tesis</t>
+  </si>
+  <si>
+    <t>/tesis/show</t>
+  </si>
+  <si>
+    <t>/tesis/sinpermiso</t>
+  </si>
+  <si>
+    <t>/tesis/tesis_aprobada</t>
+  </si>
+  <si>
+    <t>/tesis/tesis_comunidad</t>
+  </si>
+  <si>
+    <t>/tesis/tesis_empresa</t>
+  </si>
+  <si>
+    <t>/tesis/tesis_filtro_fecha_profesor</t>
+  </si>
+  <si>
+    <t>/tesis_fondoconcursable</t>
+  </si>
+  <si>
+    <t>/tesis/tesis_profesor_comision</t>
+  </si>
+  <si>
+    <t>/tesis/proyecto</t>
+  </si>
+  <si>
+    <t>/tesis/tesisregistrada</t>
+  </si>
+  <si>
+    <t>/tesis/usuario_no_existe</t>
+  </si>
+  <si>
+    <t>/tesis/vista_subir_acta</t>
+  </si>
+  <si>
+    <t>tesis/vista_subir_archivo</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @index</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @create</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @edit</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @update</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @destroy</t>
+  </si>
+  <si>
+    <t>Area_tesisController.php @store</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @index</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @lista_acuerdos_tesis</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @create</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @store</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @edit</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @update</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @destroy</t>
+  </si>
+  <si>
+    <t>BitacoraController.php @no_hay_acuerdo</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @create</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @store</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @lista_capitulos_tesis</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @edit_nombres</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @edit_avances</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @update_nombres</t>
+  </si>
+  <si>
+    <t>ComunidadController @index</t>
+  </si>
+  <si>
+    <t>ComunidadController @create</t>
+  </si>
+  <si>
+    <t>ComunidadController @store</t>
+  </si>
+  <si>
+    <t>ComunidadController @show</t>
+  </si>
+  <si>
+    <t>ComunidadController @edit</t>
+  </si>
+  <si>
+    <t>ComunidadController @update</t>
+  </si>
+  <si>
+    <t>ComunidadController @destroy</t>
+  </si>
+  <si>
+    <t>DocumentController @create</t>
+  </si>
+  <si>
+    <t>DocumentController @store</t>
+  </si>
+  <si>
+    <t>DocumentController @create_formulario_inscripcion</t>
+  </si>
+  <si>
+    <t>EmpresasController @index</t>
+  </si>
+  <si>
+    <t>EmpresasController @create</t>
+  </si>
+  <si>
+    <t>EmpresasController @store</t>
+  </si>
+  <si>
+    <t>EmpresasController @show</t>
+  </si>
+  <si>
+    <t>EmpresasController @edit</t>
+  </si>
+  <si>
+    <t>EmpresasController @update</t>
+  </si>
+  <si>
+    <t>EmpresasController @destroy</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @index</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @create</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @store</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @show</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @edit</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @update</t>
+  </si>
+  <si>
+    <t>FondoConcursableController @destroy</t>
+  </si>
+  <si>
+    <t>HomeController @index</t>
+  </si>
+  <si>
+    <t>MemorandumController @index</t>
+  </si>
+  <si>
+    <t>MemorandumController @create</t>
+  </si>
+  <si>
+    <t>MemorandumController @store</t>
+  </si>
+  <si>
+    <t>MemorandumController @ya_existe_memorandum</t>
+  </si>
+  <si>
+    <t>MemorandumController @edit</t>
+  </si>
+  <si>
+    <t>MemorandumController @update</t>
+  </si>
+  <si>
+    <t>ProyectosController @index</t>
+  </si>
+  <si>
+    <t>ProyectosController @create</t>
+  </si>
+  <si>
+    <t>ProyectosController @store</t>
+  </si>
+  <si>
+    <t>ProyectosController @show</t>
+  </si>
+  <si>
+    <t>ProyectosController @edit</t>
+  </si>
+  <si>
+    <t>ProyectosController @update</t>
+  </si>
+  <si>
+    <t>ProyectosController @destroy</t>
+  </si>
+  <si>
+    <t>Recopilacion_infController @create</t>
+  </si>
+  <si>
+    <t>Recopilacion_infController @store</t>
+  </si>
+  <si>
+    <t>Recopilacion_infController @edit</t>
+  </si>
+  <si>
+    <t>Recopilacion_infController @update</t>
+  </si>
+  <si>
+    <t>TesisController @repositorio_tesis</t>
+  </si>
+  <si>
+    <t>TesisController @mostrar_tesis</t>
+  </si>
+  <si>
+    <t>TesisController @index2</t>
+  </si>
+  <si>
+    <t>TesisController @index2_ins_pro</t>
+  </si>
+  <si>
+    <t>TesisController  @index3_solicitudes</t>
+  </si>
+  <si>
+    <t>TesisController  @index3_inscritas</t>
+  </si>
+  <si>
+    <t>TesisController   @imprimir_tesis_inscritas</t>
+  </si>
+  <si>
+    <t>TesisController @imprimir_todas_tesis_ins</t>
+  </si>
+  <si>
+    <t>TesisController @index1</t>
+  </si>
+  <si>
+    <t>TesisController @index</t>
+  </si>
+  <si>
+    <t>TesisController @create</t>
+  </si>
+  <si>
+    <t>TesisController @tesis_aprobada</t>
+  </si>
+  <si>
+    <t>TesisController @error_rut</t>
+  </si>
+  <si>
+    <t>TesisController @usuario_no_existe</t>
+  </si>
+  <si>
+    <t>TesisController @store</t>
+  </si>
+  <si>
+    <t>TesisController @show</t>
+  </si>
+  <si>
+    <t>TesisController @edit</t>
+  </si>
+  <si>
+    <t>TesisController @pedir_nota-pendiente</t>
+  </si>
+  <si>
+    <t>TesisController @save_nota_pendiente</t>
+  </si>
+  <si>
+    <t>TesisController  @pedir_nota_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController @save_nota_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController @noeditartesis</t>
+  </si>
+  <si>
+    <t>TesisController.php @edit2</t>
+  </si>
+  <si>
+    <t>TesisController.php @edit3</t>
+  </si>
+  <si>
+    <t>TesisController.php @sinpermiso</t>
+  </si>
+  <si>
+    <t>TesisController.php @evaluar_director</t>
+  </si>
+  <si>
+    <t>TesisController.php @evaluar</t>
+  </si>
+  <si>
+    <t>TesisController.php @llamar_filtro_pendient_vencida</t>
+  </si>
+  <si>
+    <t>TesisController.php @llamar_filtro_prorroga_vencida</t>
+  </si>
+  <si>
+    <t>TesisController.php @llamar_filtro_pendiente_prorroga_vencida</t>
+  </si>
+  <si>
+    <t>TesisController.php  @filtro_nota_pendiente_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController.php @imprimir_nota_pendpro_venc</t>
+  </si>
+  <si>
+    <t>TesisController.php @filtro_nota_pendiente</t>
+  </si>
+  <si>
+    <t>TesisController.php @imprimir_nota_pend_venc</t>
+  </si>
+  <si>
+    <t>TesisController.php @filtro_nota_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController.php @imprimir_nota_pro_venc</t>
+  </si>
+  <si>
+    <t>TesisController.php @update</t>
+  </si>
+  <si>
+    <t>TesisController.php @update2</t>
+  </si>
+  <si>
+    <t>TesisController.php @update5</t>
+  </si>
+  <si>
+    <t>TesisController.php @vista_subir_archivo</t>
+  </si>
+  <si>
+    <t>TesisController.php @update_archivo_ex</t>
+  </si>
+  <si>
+    <t>TesisController.php @update3</t>
+  </si>
+  <si>
+    <t>TesisController.php @update4</t>
+  </si>
+  <si>
+    <t>TesisController.php  @destroy</t>
+  </si>
+  <si>
+    <t>TesisController.php @printTesis</t>
+  </si>
+  <si>
+    <t>TesisController.php  @printTesisp</t>
+  </si>
+  <si>
+    <t>TesisController.php @printTesisc</t>
+  </si>
+  <si>
+    <t>TesisController.php  @printTesisfc</t>
+  </si>
+  <si>
+    <t>TesisController.php  @acta_examen</t>
+  </si>
+  <si>
+    <t>TesisController.php @index_titulados_sec</t>
+  </si>
+  <si>
+    <t>TesisController.php  @recopilacion_inf</t>
+  </si>
+  <si>
+    <t>TesisController.php  @recopilacion_inf2</t>
+  </si>
+  <si>
+    <t>TesisController.php  @ingresar_nota_tesis</t>
+  </si>
+  <si>
+    <t>TesisController.php @update_nota_tesis</t>
+  </si>
+  <si>
+    <t>TesisController.php  @fecha_presentacion</t>
+  </si>
+  <si>
+    <t>TesisController.php @update_fecha_presentacion</t>
+  </si>
+  <si>
+    <t>TesisController.php  vista_subir_acta</t>
+  </si>
+  <si>
+    <t>TesisController.php @update_acta_ex</t>
+  </si>
+  <si>
+    <t>TesisController.php @verPDF</t>
+  </si>
+  <si>
+    <t>TesisController.php  @verPDF_acta</t>
+  </si>
+  <si>
+    <t>TesisController.php  @rango_fechas</t>
+  </si>
+  <si>
+    <t>TesisController.php  @error_generar_pdf</t>
+  </si>
+  <si>
+    <t>TesisController.php  @informes_rangos_fechas</t>
+  </si>
+  <si>
+    <t>TesisController.php @imprimir_pend_venc</t>
+  </si>
+  <si>
+    <t>TesisController.php @imprimir_pro_venc</t>
+  </si>
+  <si>
+    <t>TesisController.php @profe_comision</t>
+  </si>
+  <si>
+    <t>TesisController.php @index_solicitud_nota_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController.php @aceptar_nota_pendiente</t>
+  </si>
+  <si>
+    <t>TesisController.php @aceptar_nota_prorroga</t>
+  </si>
+  <si>
+    <t>TesisController.php @pendiente_update</t>
+  </si>
+  <si>
+    <t>TesisController.php @prorroga_update</t>
+  </si>
+  <si>
+    <t>TesisController.php @create_num_memo</t>
+  </si>
+  <si>
+    <t>TesisController.php @lista_profe_comision_revision</t>
+  </si>
+  <si>
+    <t>TesisController.php @memo_revision1</t>
+  </si>
+  <si>
+    <t>TesisController.php @memo_revision2</t>
+  </si>
+  <si>
+    <t>TesisController.php @memo_revision3</t>
+  </si>
+  <si>
+    <t>TesisController.php @memo_revision4</t>
+  </si>
+  <si>
+    <t>TesisController.php @memo_revision5</t>
+  </si>
+  <si>
+    <t>TesisController.php @create_num_memo_titulados</t>
+  </si>
+  <si>
+    <t>TesisController.php @memorandum_titulados</t>
+  </si>
+  <si>
+    <t>TesisController.php @descargar_actas</t>
+  </si>
+  <si>
+    <t>TesisController.php @index_solicitud_nota_pendiente_director</t>
+  </si>
+  <si>
+    <t>TesisController.php @index_solicitud_nota_prorroga_director</t>
+  </si>
+  <si>
+    <t>TesisController.php @aceptar_nota_pendiente_director</t>
+  </si>
+  <si>
+    <t>TesisController.php @aceptar_nota_prorroga_director</t>
+  </si>
+  <si>
+    <t>TesisController.php @pendiente_director_update</t>
+  </si>
+  <si>
+    <t>TesisController.php @prorroga_director_update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +1037,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,14 +1073,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:BZ51"/>
+  <dimension ref="A1:KR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BT4" sqref="BT4"/>
+    <sheetView tabSelected="1" topLeftCell="KQ1" workbookViewId="0">
+      <selection activeCell="KR4" sqref="KR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,9 +1478,233 @@
     <col min="75" max="75" width="25.42578125" customWidth="1"/>
     <col min="76" max="76" width="18" customWidth="1"/>
     <col min="77" max="77" width="17.42578125" customWidth="1"/>
+    <col min="78" max="78" width="19" customWidth="1"/>
+    <col min="79" max="79" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="12.42578125" customWidth="1"/>
+    <col min="81" max="81" width="35.28515625" customWidth="1"/>
+    <col min="82" max="82" width="23.5703125" customWidth="1"/>
+    <col min="83" max="83" width="34.5703125" customWidth="1"/>
+    <col min="84" max="84" width="11.85546875" customWidth="1"/>
+    <col min="85" max="85" width="12.28515625" customWidth="1"/>
+    <col min="86" max="86" width="12.140625" customWidth="1"/>
+    <col min="87" max="87" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="20.85546875" customWidth="1"/>
+    <col min="89" max="89" width="24.42578125" customWidth="1"/>
+    <col min="90" max="90" width="15.7109375" customWidth="1"/>
+    <col min="91" max="91" width="14.85546875" customWidth="1"/>
+    <col min="92" max="92" width="13.42578125" customWidth="1"/>
+    <col min="93" max="93" width="22.7109375" customWidth="1"/>
+    <col min="94" max="94" width="25" customWidth="1"/>
+    <col min="95" max="95" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="30.5703125" customWidth="1"/>
+    <col min="97" max="97" width="23.42578125" customWidth="1"/>
+    <col min="98" max="98" width="39" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="37.5703125" customWidth="1"/>
+    <col min="100" max="100" width="25" customWidth="1"/>
+    <col min="101" max="101" width="30.85546875" customWidth="1"/>
+    <col min="102" max="102" width="36" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="38" customWidth="1"/>
+    <col min="104" max="104" width="30" customWidth="1"/>
+    <col min="105" max="105" width="23.28515625" customWidth="1"/>
+    <col min="106" max="106" width="29.42578125" customWidth="1"/>
+    <col min="107" max="107" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="38.28515625" customWidth="1"/>
+    <col min="109" max="109" width="16.85546875" customWidth="1"/>
+    <col min="110" max="110" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="20.85546875" customWidth="1"/>
+    <col min="112" max="112" width="20.140625" customWidth="1"/>
+    <col min="113" max="113" width="17.28515625" customWidth="1"/>
+    <col min="114" max="114" width="19.140625" customWidth="1"/>
+    <col min="115" max="115" width="20.140625" customWidth="1"/>
+    <col min="116" max="116" width="19.42578125" customWidth="1"/>
+    <col min="117" max="117" width="38.140625" customWidth="1"/>
+    <col min="118" max="118" width="43.85546875" customWidth="1"/>
+    <col min="119" max="119" width="36.85546875" customWidth="1"/>
+    <col min="120" max="120" width="43.85546875" customWidth="1"/>
+    <col min="121" max="121" width="25" customWidth="1"/>
+    <col min="122" max="122" width="28.28515625" customWidth="1"/>
+    <col min="123" max="123" width="24.85546875" customWidth="1"/>
+    <col min="124" max="124" width="35.85546875" customWidth="1"/>
+    <col min="125" max="125" width="19.5703125" customWidth="1"/>
+    <col min="126" max="126" width="20.5703125" customWidth="1"/>
+    <col min="127" max="127" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="29" customWidth="1"/>
+    <col min="129" max="129" width="26.28515625" customWidth="1"/>
+    <col min="130" max="130" width="25.140625" customWidth="1"/>
+    <col min="131" max="131" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="12.28515625" customWidth="1"/>
+    <col min="133" max="133" width="16.85546875" customWidth="1"/>
+    <col min="134" max="134" width="18" customWidth="1"/>
+    <col min="135" max="135" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="35" customWidth="1"/>
+    <col min="137" max="137" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="19.7109375" customWidth="1"/>
+    <col min="139" max="139" width="22" customWidth="1"/>
+    <col min="140" max="140" width="25.7109375" customWidth="1"/>
+    <col min="141" max="141" width="31.85546875" customWidth="1"/>
+    <col min="142" max="142" width="25.42578125" customWidth="1"/>
+    <col min="143" max="143" width="15.85546875" customWidth="1"/>
+    <col min="144" max="144" width="21.42578125" customWidth="1"/>
+    <col min="145" max="145" width="24" customWidth="1"/>
+    <col min="146" max="146" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="20.7109375" customWidth="1"/>
+    <col min="148" max="148" width="34.5703125" customWidth="1"/>
+    <col min="149" max="149" width="28.5703125" customWidth="1"/>
+    <col min="150" max="150" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="16.140625" customWidth="1"/>
+    <col min="152" max="152" width="20.42578125" customWidth="1"/>
+    <col min="153" max="154" width="24.85546875" customWidth="1"/>
+    <col min="155" max="155" width="28.140625" customWidth="1"/>
+    <col min="156" max="156" width="32.7109375" customWidth="1"/>
+    <col min="157" max="157" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="32.7109375" customWidth="1"/>
+    <col min="159" max="159" width="34.42578125" customWidth="1"/>
+    <col min="160" max="160" width="33.85546875" customWidth="1"/>
+    <col min="161" max="161" width="31.140625" customWidth="1"/>
+    <col min="162" max="162" width="40.7109375" customWidth="1"/>
+    <col min="163" max="163" width="46" customWidth="1"/>
+    <col min="164" max="164" width="30" customWidth="1"/>
+    <col min="165" max="165" width="29.140625" customWidth="1"/>
+    <col min="166" max="166" width="28.42578125" customWidth="1"/>
+    <col min="167" max="167" width="31.140625" customWidth="1"/>
+    <col min="168" max="168" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="39.28515625" customWidth="1"/>
+    <col min="170" max="170" width="36.42578125" customWidth="1"/>
+    <col min="171" max="171" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="44" customWidth="1"/>
+    <col min="173" max="173" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="37.5703125" customWidth="1"/>
+    <col min="175" max="175" width="42.140625" customWidth="1"/>
+    <col min="176" max="176" width="28.28515625" customWidth="1"/>
+    <col min="177" max="177" width="29.28515625" customWidth="1"/>
+    <col min="178" max="178" width="26.42578125" customWidth="1"/>
+    <col min="179" max="179" width="30" customWidth="1"/>
+    <col min="180" max="180" width="29.85546875" customWidth="1"/>
+    <col min="181" max="181" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="29.85546875" customWidth="1"/>
+    <col min="183" max="184" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="28.7109375" customWidth="1"/>
+    <col min="187" max="187" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="27.42578125" customWidth="1"/>
+    <col min="189" max="189" width="26.85546875" customWidth="1"/>
+    <col min="190" max="190" width="25.28515625" customWidth="1"/>
+    <col min="191" max="191" width="27.7109375" customWidth="1"/>
+    <col min="192" max="192" width="29.140625" customWidth="1"/>
+    <col min="193" max="193" width="35.42578125" customWidth="1"/>
+    <col min="194" max="194" width="35.7109375" customWidth="1"/>
+    <col min="195" max="196" width="35" customWidth="1"/>
+    <col min="197" max="197" width="34.85546875" customWidth="1"/>
+    <col min="198" max="198" width="35.42578125" customWidth="1"/>
+    <col min="199" max="199" width="38.42578125" customWidth="1"/>
+    <col min="200" max="200" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="29.7109375" customWidth="1"/>
+    <col min="204" max="204" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="30.140625" customWidth="1"/>
+    <col min="206" max="206" width="32.5703125" customWidth="1"/>
+    <col min="207" max="207" width="28.28515625" customWidth="1"/>
+    <col min="208" max="208" width="31" customWidth="1"/>
+    <col min="209" max="209" width="29.85546875" customWidth="1"/>
+    <col min="210" max="210" width="27.7109375" customWidth="1"/>
+    <col min="211" max="211" width="26.140625" customWidth="1"/>
+    <col min="212" max="212" width="28" customWidth="1"/>
+    <col min="213" max="213" width="28.28515625" customWidth="1"/>
+    <col min="214" max="214" width="34.42578125" customWidth="1"/>
+    <col min="215" max="215" width="34.85546875" customWidth="1"/>
+    <col min="216" max="216" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="35.42578125" customWidth="1"/>
+    <col min="218" max="218" width="34.7109375" customWidth="1"/>
+    <col min="219" max="219" width="31" customWidth="1"/>
+    <col min="220" max="220" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="30.28515625" customWidth="1"/>
+    <col min="222" max="222" width="38.42578125" customWidth="1"/>
+    <col min="223" max="223" width="32" customWidth="1"/>
+    <col min="224" max="224" width="39.85546875" customWidth="1"/>
+    <col min="225" max="225" width="40" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="24.85546875" customWidth="1"/>
+    <col min="227" max="227" width="23.85546875" customWidth="1"/>
+    <col min="228" max="228" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="29.85546875" customWidth="1"/>
+    <col min="230" max="230" width="26.85546875" customWidth="1"/>
+    <col min="231" max="231" width="33.42578125" customWidth="1"/>
+    <col min="232" max="232" width="22.140625" customWidth="1"/>
+    <col min="233" max="233" width="22.42578125" customWidth="1"/>
+    <col min="234" max="234" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="37.28515625" customWidth="1"/>
+    <col min="236" max="236" width="36" customWidth="1"/>
+    <col min="237" max="237" width="38.140625" customWidth="1"/>
+    <col min="238" max="238" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="30.42578125" customWidth="1"/>
+    <col min="240" max="240" width="26.28515625" customWidth="1"/>
+    <col min="241" max="241" width="27.5703125" customWidth="1"/>
+    <col min="242" max="242" width="30.42578125" customWidth="1"/>
+    <col min="243" max="243" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="32.7109375" customWidth="1"/>
+    <col min="245" max="245" width="56.42578125" customWidth="1"/>
+    <col min="246" max="246" width="54.28515625" customWidth="1"/>
+    <col min="247" max="247" width="58.85546875" customWidth="1"/>
+    <col min="248" max="248" width="50.7109375" customWidth="1"/>
+    <col min="249" max="249" width="49" customWidth="1"/>
+    <col min="250" max="250" width="42.140625" customWidth="1"/>
+    <col min="251" max="251" width="45.42578125" customWidth="1"/>
+    <col min="252" max="252" width="39.42578125" customWidth="1"/>
+    <col min="253" max="253" width="46.5703125" customWidth="1"/>
+    <col min="254" max="254" width="27.85546875" customWidth="1"/>
+    <col min="255" max="255" width="28.140625" customWidth="1"/>
+    <col min="256" max="256" width="33.7109375" customWidth="1"/>
+    <col min="257" max="257" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="38.28515625" customWidth="1"/>
+    <col min="259" max="259" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="29.28515625" customWidth="1"/>
+    <col min="261" max="261" width="30" customWidth="1"/>
+    <col min="262" max="262" width="32.140625" customWidth="1"/>
+    <col min="263" max="263" width="31.28515625" customWidth="1"/>
+    <col min="264" max="264" width="34.85546875" customWidth="1"/>
+    <col min="265" max="265" width="32.5703125" customWidth="1"/>
+    <col min="266" max="266" width="32.7109375" customWidth="1"/>
+    <col min="267" max="267" width="43.42578125" customWidth="1"/>
+    <col min="268" max="268" width="47.28515625" customWidth="1"/>
+    <col min="269" max="269" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="42.140625" customWidth="1"/>
+    <col min="271" max="271" width="37.28515625" customWidth="1"/>
+    <col min="272" max="272" width="39.42578125" customWidth="1"/>
+    <col min="273" max="273" width="49" customWidth="1"/>
+    <col min="274" max="274" width="37" customWidth="1"/>
+    <col min="275" max="275" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="28.28515625" customWidth="1"/>
+    <col min="277" max="277" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="36.140625" customWidth="1"/>
+    <col min="279" max="279" width="39.42578125" customWidth="1"/>
+    <col min="280" max="280" width="43.7109375" customWidth="1"/>
+    <col min="281" max="281" width="44.140625" customWidth="1"/>
+    <col min="282" max="282" width="40.85546875" customWidth="1"/>
+    <col min="283" max="283" width="35.42578125" customWidth="1"/>
+    <col min="284" max="284" width="50.140625" customWidth="1"/>
+    <col min="285" max="285" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="41.140625" customWidth="1"/>
+    <col min="287" max="287" width="38.140625" customWidth="1"/>
+    <col min="288" max="288" width="40.140625" customWidth="1"/>
+    <col min="289" max="289" width="37.7109375" customWidth="1"/>
+    <col min="290" max="290" width="54.140625" customWidth="1"/>
+    <col min="291" max="291" width="37.42578125" customWidth="1"/>
+    <col min="292" max="292" width="36.140625" customWidth="1"/>
+    <col min="293" max="293" width="36" customWidth="1"/>
+    <col min="294" max="294" width="41.42578125" customWidth="1"/>
+    <col min="295" max="295" width="36.42578125" customWidth="1"/>
+    <col min="296" max="296" width="50.5703125" customWidth="1"/>
+    <col min="297" max="297" width="44.42578125" customWidth="1"/>
+    <col min="298" max="298" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="299" max="299" width="58.7109375" customWidth="1"/>
+    <col min="300" max="300" width="60.42578125" customWidth="1"/>
+    <col min="301" max="301" width="50.42578125" customWidth="1"/>
+    <col min="302" max="302" width="52.28515625" customWidth="1"/>
+    <col min="303" max="303" width="47.28515625" customWidth="1"/>
+    <col min="304" max="304" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:304" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -795,12 +1715,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:304" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -814,16 +1734,298 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="4"/>
+      <c r="BG2" s="4"/>
+      <c r="BH2" s="4"/>
+      <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
+      <c r="BK2" s="4"/>
+      <c r="BL2" s="4"/>
+      <c r="BM2" s="4"/>
+      <c r="BN2" s="4"/>
+      <c r="BO2" s="4"/>
+      <c r="BP2" s="4"/>
+      <c r="BQ2" s="4"/>
+      <c r="BR2" s="4"/>
+      <c r="BS2" s="4"/>
+      <c r="BT2" s="4"/>
+      <c r="BU2" s="4"/>
+      <c r="BV2" s="4"/>
+      <c r="BW2" s="4"/>
+      <c r="BX2" s="4"/>
+      <c r="BY2" s="4"/>
+      <c r="BZ2" s="4"/>
+      <c r="CA2" s="4"/>
+      <c r="CB2" s="4"/>
+      <c r="CC2" s="4"/>
+      <c r="CD2" s="4"/>
+      <c r="CE2" s="4"/>
+      <c r="CF2" s="4"/>
+      <c r="CG2" s="4"/>
+      <c r="CH2" s="4"/>
+      <c r="CI2" s="4"/>
+      <c r="CJ2" s="4"/>
+      <c r="CK2" s="4"/>
+      <c r="CL2" s="4"/>
+      <c r="CM2" s="4"/>
+      <c r="CN2" s="4"/>
+      <c r="CO2" s="4"/>
+      <c r="CP2" s="4"/>
+      <c r="CQ2" s="4"/>
+      <c r="CR2" s="4"/>
+      <c r="CS2" s="4"/>
+      <c r="CT2" s="4"/>
+      <c r="CU2" s="4"/>
+      <c r="CV2" s="4"/>
+      <c r="CW2" s="4"/>
+      <c r="CX2" s="4"/>
+      <c r="CY2" s="4"/>
+      <c r="CZ2" s="4"/>
+      <c r="DA2" s="4"/>
+      <c r="DB2" s="4"/>
+      <c r="DC2" s="4"/>
+      <c r="DD2" s="4"/>
+      <c r="DE2" s="4"/>
+      <c r="DF2" s="4"/>
+      <c r="DG2" s="4"/>
+      <c r="DH2" s="4"/>
+      <c r="DI2" s="4"/>
+      <c r="DJ2" s="4"/>
+      <c r="DK2" s="4"/>
+      <c r="DL2" s="4"/>
+      <c r="DM2" s="4"/>
+      <c r="DN2" s="4"/>
+      <c r="DO2" s="4"/>
+      <c r="DP2" s="4"/>
+      <c r="DQ2" s="4"/>
+      <c r="DR2" s="4"/>
+      <c r="DS2" s="4"/>
+      <c r="DT2" s="4"/>
+      <c r="DU2" s="4"/>
+      <c r="DV2" s="4"/>
+      <c r="DW2" s="4"/>
+      <c r="DX2" s="4"/>
+      <c r="DY2" s="4"/>
+      <c r="DZ2" s="4"/>
+      <c r="EA2" s="4"/>
+      <c r="EB2" s="4"/>
+      <c r="EC2" s="4"/>
+      <c r="ED2" s="4"/>
+      <c r="EE2" s="4"/>
+      <c r="EF2" s="4"/>
+      <c r="EG2" s="4"/>
+      <c r="EH2" s="4"/>
+      <c r="EI2" s="4"/>
+      <c r="EJ2" s="4"/>
+      <c r="EK2" s="4"/>
+      <c r="EL2" s="4"/>
+      <c r="EM2" s="4"/>
+      <c r="EN2" s="4"/>
+      <c r="EO2" s="4"/>
+      <c r="EP2" s="4"/>
+      <c r="EQ2" s="4"/>
+      <c r="ER2" s="4"/>
+      <c r="ES2" s="4"/>
+      <c r="ET2" s="4"/>
+      <c r="EU2" s="4"/>
+      <c r="EV2" s="4"/>
+      <c r="EW2" s="4"/>
+      <c r="EX2" s="4"/>
+      <c r="EY2" s="4"/>
+      <c r="EZ2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:304" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
+      <c r="BN3" s="2"/>
+      <c r="BO3" s="2"/>
+      <c r="BP3" s="2"/>
+      <c r="BQ3" s="2"/>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="2"/>
+      <c r="BT3" s="2"/>
+      <c r="BU3" s="2"/>
+      <c r="BV3" s="2"/>
+      <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
+      <c r="BY3" s="2"/>
+      <c r="BZ3" s="2"/>
+      <c r="CA3" s="2"/>
+      <c r="CB3" s="2"/>
+      <c r="CC3" s="2"/>
+      <c r="CD3" s="2"/>
+      <c r="CE3" s="2"/>
+      <c r="CF3" s="2"/>
+      <c r="CG3" s="2"/>
+      <c r="CH3" s="2"/>
+      <c r="CI3" s="2"/>
+      <c r="CJ3" s="2"/>
+      <c r="CK3" s="2"/>
+      <c r="CL3" s="2"/>
+      <c r="CM3" s="2"/>
+      <c r="CN3" s="2"/>
+      <c r="CO3" s="2"/>
+      <c r="CP3" s="2"/>
+      <c r="CQ3" s="2"/>
+      <c r="CR3" s="2"/>
+      <c r="CS3" s="2"/>
+      <c r="CT3" s="2"/>
+      <c r="CU3" s="2"/>
+      <c r="CV3" s="2"/>
+      <c r="CW3" s="2"/>
+      <c r="CX3" s="2"/>
+      <c r="CY3" s="2"/>
+      <c r="CZ3" s="2"/>
+      <c r="DA3" s="2"/>
+      <c r="DB3" s="2"/>
+      <c r="DC3" s="2"/>
+      <c r="DD3" s="2"/>
+      <c r="DE3" s="2"/>
+      <c r="DF3" s="2"/>
+      <c r="DG3" s="2"/>
+      <c r="DH3" s="2"/>
+      <c r="DI3" s="2"/>
+      <c r="DJ3" s="2"/>
+      <c r="DK3" s="2"/>
+      <c r="DL3" s="2"/>
+      <c r="DM3" s="2"/>
+      <c r="DN3" s="2"/>
+      <c r="DO3" s="2"/>
+      <c r="DP3" s="2"/>
+      <c r="DQ3" s="2"/>
+      <c r="DR3" s="2"/>
+      <c r="DS3" s="2"/>
+      <c r="DT3" s="2"/>
+      <c r="DU3" s="2"/>
+      <c r="DV3" s="2"/>
+      <c r="DW3" s="2"/>
+      <c r="DX3" s="2"/>
+      <c r="DY3" s="2"/>
+      <c r="DZ3" s="2"/>
+      <c r="EA3" s="2"/>
+      <c r="EB3" s="2"/>
+      <c r="EC3" s="2"/>
+      <c r="ED3" s="2"/>
+      <c r="EE3" s="2"/>
+      <c r="EF3" s="2"/>
+      <c r="EG3" s="2"/>
+      <c r="EH3" s="2"/>
+      <c r="EI3" s="2"/>
+      <c r="EJ3" s="2"/>
+      <c r="EK3" s="2"/>
+      <c r="EL3" s="2"/>
+      <c r="EM3" s="2"/>
+      <c r="EN3" s="2"/>
+      <c r="EO3" s="2"/>
+      <c r="EP3" s="2"/>
+      <c r="EQ3" s="2"/>
+      <c r="ER3" s="2"/>
+      <c r="ES3" s="2"/>
+      <c r="ET3" s="2"/>
+      <c r="EU3" s="2"/>
+      <c r="EV3" s="2"/>
+      <c r="EW3" s="2"/>
+      <c r="EX3" s="2"/>
+      <c r="EY3" s="2"/>
+    </row>
+    <row r="4" spans="1:304" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -864,251 +2066,929 @@
         <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Y4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Z4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AA4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AC4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AE4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AF4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AH4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AI4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AJ4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AK4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AL4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AM4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AN4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AO4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AP4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AQ4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AR4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AS4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AT4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV4" t="s">
         <v>51</v>
       </c>
-      <c r="AU4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>50</v>
-      </c>
       <c r="AW4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX4" t="s">
         <v>53</v>
       </c>
-      <c r="AX4" t="s">
-        <v>52</v>
-      </c>
       <c r="AY4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AZ4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BA4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BB4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BC4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BD4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BE4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BG4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BH4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BI4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BJ4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BK4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BL4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BM4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BN4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BO4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BP4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BQ4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BR4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BS4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BT4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BU4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BV4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BW4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="BX4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BY4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="BZ4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>83</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>84</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>85</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>86</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>88</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>89</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CJ4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>91</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>92</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>94</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CR4" t="s">
+        <v>97</v>
+      </c>
+      <c r="CS4" t="s">
+        <v>97</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CU4" t="s">
+        <v>99</v>
+      </c>
+      <c r="CV4" t="s">
+        <v>100</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>101</v>
+      </c>
+      <c r="CX4" t="s">
+        <v>102</v>
+      </c>
+      <c r="CY4" t="s">
+        <v>103</v>
+      </c>
+      <c r="CZ4" t="s">
+        <v>104</v>
+      </c>
+      <c r="DA4" t="s">
+        <v>105</v>
+      </c>
+      <c r="DB4" t="s">
+        <v>106</v>
+      </c>
+      <c r="DC4" t="s">
+        <v>107</v>
+      </c>
+      <c r="DD4" t="s">
+        <v>108</v>
+      </c>
+      <c r="DE4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DF4" t="s">
+        <v>110</v>
+      </c>
+      <c r="DG4" t="s">
+        <v>111</v>
+      </c>
+      <c r="DH4" t="s">
+        <v>112</v>
+      </c>
+      <c r="DI4" t="s">
+        <v>113</v>
+      </c>
+      <c r="DJ4" t="s">
+        <v>114</v>
+      </c>
+      <c r="DK4" t="s">
+        <v>115</v>
+      </c>
+      <c r="DL4" t="s">
+        <v>116</v>
+      </c>
+      <c r="DM4" t="s">
+        <v>117</v>
+      </c>
+      <c r="DN4" t="s">
+        <v>118</v>
+      </c>
+      <c r="DO4" t="s">
+        <v>119</v>
+      </c>
+      <c r="DP4" t="s">
+        <v>120</v>
+      </c>
+      <c r="DQ4" t="s">
+        <v>121</v>
+      </c>
+      <c r="DR4" t="s">
+        <v>122</v>
+      </c>
+      <c r="DS4" t="s">
+        <v>123</v>
+      </c>
+      <c r="DT4" t="s">
+        <v>124</v>
+      </c>
+      <c r="DU4" t="s">
+        <v>125</v>
+      </c>
+      <c r="DV4" t="s">
+        <v>126</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DX4" t="s">
+        <v>129</v>
+      </c>
+      <c r="DY4" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ4" t="s">
+        <v>130</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>131</v>
+      </c>
+      <c r="EB4" t="s">
+        <v>132</v>
+      </c>
+      <c r="EC4" t="s">
+        <v>133</v>
+      </c>
+      <c r="ED4" t="s">
+        <v>134</v>
+      </c>
+      <c r="EE4" t="s">
+        <v>135</v>
+      </c>
+      <c r="EF4" t="s">
+        <v>136</v>
+      </c>
+      <c r="EG4" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH4" t="s">
+        <v>138</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>139</v>
+      </c>
+      <c r="EJ4" t="s">
+        <v>140</v>
+      </c>
+      <c r="EK4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EL4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EM4" t="s">
+        <v>143</v>
+      </c>
+      <c r="EN4" t="s">
+        <v>144</v>
+      </c>
+      <c r="EO4" t="s">
+        <v>145</v>
+      </c>
+      <c r="EP4" t="s">
+        <v>146</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>147</v>
+      </c>
+      <c r="ER4" t="s">
+        <v>148</v>
+      </c>
+      <c r="ES4" t="s">
+        <v>149</v>
+      </c>
+      <c r="ET4" t="s">
+        <v>150</v>
+      </c>
+      <c r="EU4" t="s">
+        <v>151</v>
+      </c>
+      <c r="EV4" t="s">
+        <v>152</v>
+      </c>
+      <c r="EW4" t="s">
+        <v>153</v>
+      </c>
+      <c r="EX4" t="s">
+        <v>154</v>
+      </c>
+      <c r="EY4" t="s">
+        <v>155</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>156</v>
+      </c>
+      <c r="FA4" t="s">
+        <v>157</v>
+      </c>
+      <c r="FB4" t="s">
+        <v>158</v>
+      </c>
+      <c r="FC4" t="s">
+        <v>159</v>
+      </c>
+      <c r="FD4" t="s">
+        <v>160</v>
+      </c>
+      <c r="FE4" t="s">
+        <v>161</v>
+      </c>
+      <c r="FF4" t="s">
+        <v>162</v>
+      </c>
+      <c r="FG4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FH4" t="s">
+        <v>164</v>
+      </c>
+      <c r="FI4" t="s">
+        <v>165</v>
+      </c>
+      <c r="FJ4" t="s">
+        <v>166</v>
+      </c>
+      <c r="FK4" t="s">
+        <v>167</v>
+      </c>
+      <c r="FL4" t="s">
+        <v>168</v>
+      </c>
+      <c r="FM4" t="s">
+        <v>169</v>
+      </c>
+      <c r="FN4" t="s">
+        <v>170</v>
+      </c>
+      <c r="FO4" t="s">
+        <v>171</v>
+      </c>
+      <c r="FP4" t="s">
+        <v>172</v>
+      </c>
+      <c r="FQ4" t="s">
+        <v>173</v>
+      </c>
+      <c r="FR4" t="s">
+        <v>174</v>
+      </c>
+      <c r="FS4" t="s">
+        <v>175</v>
+      </c>
+      <c r="FT4" t="s">
+        <v>176</v>
+      </c>
+      <c r="FU4" t="s">
+        <v>177</v>
+      </c>
+      <c r="FV4" t="s">
+        <v>178</v>
+      </c>
+      <c r="FW4" t="s">
+        <v>179</v>
+      </c>
+      <c r="FX4" t="s">
+        <v>180</v>
+      </c>
+      <c r="FY4" t="s">
+        <v>181</v>
+      </c>
+      <c r="FZ4" t="s">
+        <v>182</v>
+      </c>
+      <c r="GA4" t="s">
+        <v>183</v>
+      </c>
+      <c r="GB4" t="s">
+        <v>184</v>
+      </c>
+      <c r="GC4" t="s">
+        <v>185</v>
+      </c>
+      <c r="GD4" t="s">
+        <v>186</v>
+      </c>
+      <c r="GE4" t="s">
+        <v>187</v>
+      </c>
+      <c r="GF4" t="s">
+        <v>188</v>
+      </c>
+      <c r="GG4" t="s">
+        <v>189</v>
+      </c>
+      <c r="GH4" t="s">
+        <v>190</v>
+      </c>
+      <c r="GI4" t="s">
+        <v>191</v>
+      </c>
+      <c r="GJ4" t="s">
+        <v>192</v>
+      </c>
+      <c r="GK4" t="s">
+        <v>193</v>
+      </c>
+      <c r="GL4" t="s">
+        <v>194</v>
+      </c>
+      <c r="GM4" t="s">
+        <v>195</v>
+      </c>
+      <c r="GN4" t="s">
+        <v>196</v>
+      </c>
+      <c r="GO4" t="s">
+        <v>197</v>
+      </c>
+      <c r="GP4" t="s">
+        <v>198</v>
+      </c>
+      <c r="GQ4" t="s">
+        <v>199</v>
+      </c>
+      <c r="GR4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="GS4" t="s">
+        <v>201</v>
+      </c>
+      <c r="GT4" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="GU4" t="s">
+        <v>203</v>
+      </c>
+      <c r="GV4" t="s">
+        <v>204</v>
+      </c>
+      <c r="GW4" t="s">
+        <v>205</v>
+      </c>
+      <c r="GX4" t="s">
+        <v>206</v>
+      </c>
+      <c r="GY4" t="s">
+        <v>207</v>
+      </c>
+      <c r="GZ4" t="s">
+        <v>208</v>
+      </c>
+      <c r="HA4" t="s">
+        <v>209</v>
+      </c>
+      <c r="HB4" t="s">
+        <v>210</v>
+      </c>
+      <c r="HC4" t="s">
+        <v>211</v>
+      </c>
+      <c r="HD4" t="s">
+        <v>212</v>
+      </c>
+      <c r="HE4" t="s">
+        <v>213</v>
+      </c>
+      <c r="HF4" t="s">
+        <v>214</v>
+      </c>
+      <c r="HG4" t="s">
+        <v>215</v>
+      </c>
+      <c r="HH4" t="s">
+        <v>216</v>
+      </c>
+      <c r="HI4" t="s">
+        <v>217</v>
+      </c>
+      <c r="HJ4" t="s">
+        <v>218</v>
+      </c>
+      <c r="HK4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="HL4" t="s">
+        <v>220</v>
+      </c>
+      <c r="HM4" t="s">
+        <v>221</v>
+      </c>
+      <c r="HN4" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="HO4" t="s">
+        <v>223</v>
+      </c>
+      <c r="HP4" t="s">
+        <v>224</v>
+      </c>
+      <c r="HQ4" t="s">
+        <v>225</v>
+      </c>
+      <c r="HR4" t="s">
+        <v>226</v>
+      </c>
+      <c r="HS4" t="s">
+        <v>227</v>
+      </c>
+      <c r="HT4" t="s">
+        <v>228</v>
+      </c>
+      <c r="HU4" t="s">
+        <v>229</v>
+      </c>
+      <c r="HV4" t="s">
+        <v>230</v>
+      </c>
+      <c r="HW4" t="s">
+        <v>231</v>
+      </c>
+      <c r="HX4" t="s">
+        <v>232</v>
+      </c>
+      <c r="HY4" t="s">
+        <v>233</v>
+      </c>
+      <c r="HZ4" t="s">
+        <v>234</v>
+      </c>
+      <c r="IA4" t="s">
+        <v>235</v>
+      </c>
+      <c r="IB4" t="s">
+        <v>236</v>
+      </c>
+      <c r="IC4" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="ID4" t="s">
+        <v>238</v>
+      </c>
+      <c r="IE4" t="s">
+        <v>239</v>
+      </c>
+      <c r="IF4" t="s">
+        <v>240</v>
+      </c>
+      <c r="IG4" t="s">
+        <v>241</v>
+      </c>
+      <c r="IH4" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="II4" t="s">
+        <v>243</v>
+      </c>
+      <c r="IJ4" t="s">
+        <v>244</v>
+      </c>
+      <c r="IK4" t="s">
+        <v>245</v>
+      </c>
+      <c r="IL4" t="s">
+        <v>246</v>
+      </c>
+      <c r="IM4" t="s">
+        <v>247</v>
+      </c>
+      <c r="IN4" t="s">
+        <v>248</v>
+      </c>
+      <c r="IO4" t="s">
+        <v>249</v>
+      </c>
+      <c r="IP4" t="s">
+        <v>250</v>
+      </c>
+      <c r="IQ4" t="s">
+        <v>251</v>
+      </c>
+      <c r="IR4" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="IS4" t="s">
+        <v>253</v>
+      </c>
+      <c r="IT4" t="s">
+        <v>254</v>
+      </c>
+      <c r="IU4" t="s">
+        <v>255</v>
+      </c>
+      <c r="IV4" t="s">
+        <v>256</v>
+      </c>
+      <c r="IW4" t="s">
+        <v>257</v>
+      </c>
+      <c r="IX4" t="s">
+        <v>258</v>
+      </c>
+      <c r="IY4" t="s">
+        <v>259</v>
+      </c>
+      <c r="IZ4" t="s">
+        <v>260</v>
+      </c>
+      <c r="JA4" t="s">
+        <v>261</v>
+      </c>
+      <c r="JB4" t="s">
+        <v>262</v>
+      </c>
+      <c r="JC4" t="s">
+        <v>263</v>
+      </c>
+      <c r="JD4" t="s">
+        <v>264</v>
+      </c>
+      <c r="JE4" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="JF4" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="JG4" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="JH4" t="s">
+        <v>268</v>
+      </c>
+      <c r="JI4" t="s">
+        <v>269</v>
+      </c>
+      <c r="JJ4" t="s">
+        <v>270</v>
+      </c>
+      <c r="JK4" t="s">
+        <v>271</v>
+      </c>
+      <c r="JL4" t="s">
+        <v>272</v>
+      </c>
+      <c r="JM4" t="s">
+        <v>273</v>
+      </c>
+      <c r="JN4" t="s">
+        <v>274</v>
+      </c>
+      <c r="JO4" t="s">
+        <v>275</v>
+      </c>
+      <c r="JP4" t="s">
+        <v>276</v>
+      </c>
+      <c r="JQ4" t="s">
+        <v>277</v>
+      </c>
+      <c r="JR4" t="s">
+        <v>278</v>
+      </c>
+      <c r="JS4" t="s">
+        <v>279</v>
+      </c>
+      <c r="JT4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="JU4" t="s">
+        <v>281</v>
+      </c>
+      <c r="JV4" t="s">
+        <v>282</v>
+      </c>
+      <c r="JW4" t="s">
+        <v>283</v>
+      </c>
+      <c r="JX4" t="s">
+        <v>284</v>
+      </c>
+      <c r="JY4" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="JZ4" t="s">
+        <v>286</v>
+      </c>
+      <c r="KA4" t="s">
+        <v>287</v>
+      </c>
+      <c r="KB4" t="s">
+        <v>288</v>
+      </c>
+      <c r="KC4" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="KD4" t="s">
+        <v>290</v>
+      </c>
+      <c r="KE4" t="s">
+        <v>291</v>
+      </c>
+      <c r="KF4" t="s">
+        <v>292</v>
+      </c>
+      <c r="KG4" t="s">
+        <v>293</v>
+      </c>
+      <c r="KH4" t="s">
+        <v>294</v>
+      </c>
+      <c r="KI4" t="s">
+        <v>295</v>
+      </c>
+      <c r="KJ4" t="s">
+        <v>296</v>
+      </c>
+      <c r="KK4" t="s">
+        <v>297</v>
+      </c>
+      <c r="KL4" t="s">
+        <v>298</v>
+      </c>
+      <c r="KM4" t="s">
+        <v>299</v>
+      </c>
+      <c r="KN4" t="s">
+        <v>300</v>
+      </c>
+      <c r="KO4" t="s">
+        <v>301</v>
+      </c>
+      <c r="KP4" t="s">
+        <v>302</v>
+      </c>
+      <c r="KQ4" t="s">
+        <v>303</v>
+      </c>
+      <c r="KR4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:304" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1289,10 +3169,25 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:O2"/>
+    <mergeCell ref="P2:EY2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="GT4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
+    <hyperlink ref="HK4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
+    <hyperlink ref="HN4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
+    <hyperlink ref="IC4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
+    <hyperlink ref="IH4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
+    <hyperlink ref="IR4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
+    <hyperlink ref="JE4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
+    <hyperlink ref="JF4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
+    <hyperlink ref="JG4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JT4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="JY4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KC4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabla matriz de trazabilidad filas y columnas completadas, falta marcar con x segun requerimientos
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5758970A-4968-433E-BD10-BB70BDBDC2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3115F3B-9E20-4B41-AC42-1BA46818CAD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10050" yWindow="2490" windowWidth="10395" windowHeight="7875" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="305">
-  <si>
-    <t>Controlador</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="326">
   <si>
     <t>MVC</t>
   </si>
@@ -1019,6 +1016,72 @@
   </si>
   <si>
     <t>TesisController.php @prorroga_director_update</t>
+  </si>
+  <si>
+    <t>UsersController.php @index</t>
+  </si>
+  <si>
+    <t>UsersController.php @create</t>
+  </si>
+  <si>
+    <t>UsersController.php  @store</t>
+  </si>
+  <si>
+    <t>UsersController.php @create_grado_academico_profesor</t>
+  </si>
+  <si>
+    <t>UsersController.php  @show</t>
+  </si>
+  <si>
+    <t>UsersController.php @edit</t>
+  </si>
+  <si>
+    <t>UsersController.php  @update</t>
+  </si>
+  <si>
+    <t>UsersController.php @destroy</t>
+  </si>
+  <si>
+    <t>UsersController.php  @save_profe_grado_academico</t>
+  </si>
+  <si>
+    <t>UsersController.php @editar_informacion_profesor</t>
+  </si>
+  <si>
+    <t>UsersController.php @update_profesor</t>
+  </si>
+  <si>
+    <t>UsersController.php @store_grado_academico</t>
+  </si>
+  <si>
+    <t>UsersController.php  @definir_director_escuela</t>
+  </si>
+  <si>
+    <t>UsersController.php  @guardar_director_escuela</t>
+  </si>
+  <si>
+    <t>UsersController.php @showLinkRequestForm</t>
+  </si>
+  <si>
+    <t>UsersController.php @sendResetLinkEmail</t>
+  </si>
+  <si>
+    <t>UsersController.php @validateEmail</t>
+  </si>
+  <si>
+    <t>UsersController.php @credentials</t>
+  </si>
+  <si>
+    <t>UsersController.php @broker</t>
+  </si>
+  <si>
+    <t>UsersController.php @sendResetLinkFailedResponse</t>
+  </si>
+  <si>
+    <t>UsersController.php @sendResetLinkResponse</t>
+  </si>
+  <si>
+    <t>Controlador:</t>
   </si>
 </sst>
 </file>
@@ -1056,12 +1119,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1077,17 +1158,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1403,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:KR51"/>
+  <dimension ref="A1:LM51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="KQ1" workbookViewId="0">
-      <selection activeCell="KR4" sqref="KR4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,1293 +1789,1545 @@
     <col min="302" max="302" width="52.28515625" customWidth="1"/>
     <col min="303" max="303" width="47.28515625" customWidth="1"/>
     <col min="304" max="304" width="43.28515625" customWidth="1"/>
+    <col min="305" max="305" width="26.7109375" customWidth="1"/>
+    <col min="306" max="306" width="27" customWidth="1"/>
+    <col min="307" max="307" width="29.85546875" customWidth="1"/>
+    <col min="308" max="308" width="52.5703125" customWidth="1"/>
+    <col min="309" max="309" width="27" customWidth="1"/>
+    <col min="310" max="310" width="24.42578125" customWidth="1"/>
+    <col min="311" max="311" width="33.140625" customWidth="1"/>
+    <col min="312" max="312" width="32.85546875" customWidth="1"/>
+    <col min="313" max="313" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="314" max="314" width="48" customWidth="1"/>
+    <col min="315" max="315" width="35.85546875" customWidth="1"/>
+    <col min="316" max="317" width="43" customWidth="1"/>
+    <col min="318" max="318" width="45.5703125" customWidth="1"/>
+    <col min="319" max="319" width="42.5703125" customWidth="1"/>
+    <col min="320" max="320" width="40.85546875" customWidth="1"/>
+    <col min="321" max="321" width="34" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="31.5703125" customWidth="1"/>
+    <col min="323" max="323" width="43.5703125" customWidth="1"/>
+    <col min="324" max="324" width="30.7109375" customWidth="1"/>
+    <col min="325" max="325" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:325" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:325" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="7"/>
+      <c r="AZ2" s="7"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="7"/>
+      <c r="BK2" s="7"/>
+      <c r="BL2" s="7"/>
+      <c r="BM2" s="7"/>
+      <c r="BN2" s="7"/>
+      <c r="BO2" s="7"/>
+      <c r="BP2" s="7"/>
+      <c r="BQ2" s="7"/>
+      <c r="BR2" s="7"/>
+      <c r="BS2" s="7"/>
+      <c r="BT2" s="7"/>
+      <c r="BU2" s="7"/>
+      <c r="BV2" s="7"/>
+      <c r="BW2" s="7"/>
+      <c r="BX2" s="7"/>
+      <c r="BY2" s="7"/>
+      <c r="BZ2" s="7"/>
+      <c r="CA2" s="7"/>
+      <c r="CB2" s="7"/>
+      <c r="CC2" s="7"/>
+      <c r="CD2" s="7"/>
+      <c r="CE2" s="7"/>
+      <c r="CF2" s="7"/>
+      <c r="CG2" s="7"/>
+      <c r="CH2" s="7"/>
+      <c r="CI2" s="7"/>
+      <c r="CJ2" s="7"/>
+      <c r="CK2" s="7"/>
+      <c r="CL2" s="7"/>
+      <c r="CM2" s="7"/>
+      <c r="CN2" s="7"/>
+      <c r="CO2" s="7"/>
+      <c r="CP2" s="7"/>
+      <c r="CQ2" s="7"/>
+      <c r="CR2" s="7"/>
+      <c r="CS2" s="7"/>
+      <c r="CT2" s="7"/>
+      <c r="CU2" s="7"/>
+      <c r="CV2" s="7"/>
+      <c r="CW2" s="7"/>
+      <c r="CX2" s="7"/>
+      <c r="CY2" s="7"/>
+      <c r="CZ2" s="7"/>
+      <c r="DA2" s="7"/>
+      <c r="DB2" s="7"/>
+      <c r="DC2" s="7"/>
+      <c r="DD2" s="7"/>
+      <c r="DE2" s="7"/>
+      <c r="DF2" s="7"/>
+      <c r="DG2" s="7"/>
+      <c r="DH2" s="7"/>
+      <c r="DI2" s="7"/>
+      <c r="DJ2" s="7"/>
+      <c r="DK2" s="7"/>
+      <c r="DL2" s="7"/>
+      <c r="DM2" s="7"/>
+      <c r="DN2" s="7"/>
+      <c r="DO2" s="7"/>
+      <c r="DP2" s="7"/>
+      <c r="DQ2" s="7"/>
+      <c r="DR2" s="7"/>
+      <c r="DS2" s="7"/>
+      <c r="DT2" s="7"/>
+      <c r="DU2" s="7"/>
+      <c r="DV2" s="7"/>
+      <c r="DW2" s="7"/>
+      <c r="DX2" s="7"/>
+      <c r="DY2" s="7"/>
+      <c r="DZ2" s="7"/>
+      <c r="EA2" s="7"/>
+      <c r="EB2" s="7"/>
+      <c r="EC2" s="7"/>
+      <c r="ED2" s="7"/>
+      <c r="EE2" s="7"/>
+      <c r="EF2" s="7"/>
+      <c r="EG2" s="7"/>
+      <c r="EH2" s="7"/>
+      <c r="EI2" s="7"/>
+      <c r="EJ2" s="7"/>
+      <c r="EK2" s="7"/>
+      <c r="EL2" s="7"/>
+      <c r="EM2" s="7"/>
+      <c r="EN2" s="7"/>
+      <c r="EO2" s="7"/>
+      <c r="EP2" s="7"/>
+      <c r="EQ2" s="7"/>
+      <c r="ER2" s="7"/>
+      <c r="ES2" s="7"/>
+      <c r="ET2" s="7"/>
+      <c r="EU2" s="7"/>
+      <c r="EV2" s="7"/>
+      <c r="EW2" s="7"/>
+      <c r="EX2" s="7"/>
+      <c r="EY2" s="7"/>
+      <c r="EZ2" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="FA2" s="4"/>
+      <c r="FB2" s="4"/>
+      <c r="FC2" s="4"/>
+      <c r="FD2" s="4"/>
+      <c r="FE2" s="4"/>
+      <c r="FF2" s="4"/>
+      <c r="FG2" s="4"/>
+      <c r="FH2" s="4"/>
+      <c r="FI2" s="4"/>
+      <c r="FJ2" s="4"/>
+      <c r="FK2" s="4"/>
+      <c r="FL2" s="4"/>
+      <c r="FM2" s="4"/>
+      <c r="FN2" s="4"/>
+      <c r="FO2" s="4"/>
+      <c r="FP2" s="4"/>
+      <c r="FQ2" s="4"/>
+      <c r="FR2" s="4"/>
+      <c r="FS2" s="4"/>
+      <c r="FT2" s="4"/>
+      <c r="FU2" s="4"/>
+      <c r="FV2" s="4"/>
+      <c r="FW2" s="4"/>
+      <c r="FX2" s="4"/>
+      <c r="FY2" s="4"/>
+      <c r="FZ2" s="4"/>
+      <c r="GA2" s="4"/>
+      <c r="GB2" s="4"/>
+      <c r="GC2" s="4"/>
+      <c r="GD2" s="4"/>
+      <c r="GE2" s="4"/>
+      <c r="GF2" s="4"/>
+      <c r="GG2" s="4"/>
+      <c r="GH2" s="4"/>
+      <c r="GI2" s="4"/>
+      <c r="GJ2" s="4"/>
+      <c r="GK2" s="4"/>
+      <c r="GL2" s="4"/>
+      <c r="GM2" s="4"/>
+      <c r="GN2" s="4"/>
+      <c r="GO2" s="4"/>
+      <c r="GP2" s="4"/>
+      <c r="GQ2" s="4"/>
+      <c r="GR2" s="4"/>
+      <c r="GS2" s="4"/>
+      <c r="GT2" s="4"/>
+      <c r="GU2" s="4"/>
+      <c r="GV2" s="4"/>
+      <c r="GW2" s="4"/>
+      <c r="GX2" s="4"/>
+      <c r="GY2" s="4"/>
+      <c r="GZ2" s="4"/>
+      <c r="HA2" s="4"/>
+      <c r="HB2" s="4"/>
+      <c r="HC2" s="4"/>
+      <c r="HD2" s="4"/>
+      <c r="HE2" s="4"/>
+      <c r="HF2" s="4"/>
+      <c r="HG2" s="4"/>
+      <c r="HH2" s="4"/>
+      <c r="HI2" s="4"/>
+      <c r="HJ2" s="4"/>
+      <c r="HK2" s="4"/>
+      <c r="HL2" s="4"/>
+      <c r="HM2" s="4"/>
+      <c r="HN2" s="4"/>
+      <c r="HO2" s="4"/>
+      <c r="HP2" s="4"/>
+      <c r="HQ2" s="4"/>
+      <c r="HR2" s="4"/>
+      <c r="HS2" s="4"/>
+      <c r="HT2" s="4"/>
+      <c r="HU2" s="4"/>
+      <c r="HV2" s="4"/>
+      <c r="HW2" s="4"/>
+      <c r="HX2" s="4"/>
+      <c r="HY2" s="4"/>
+      <c r="HZ2" s="4"/>
+      <c r="IA2" s="4"/>
+      <c r="IB2" s="4"/>
+      <c r="IC2" s="4"/>
+      <c r="ID2" s="4"/>
+      <c r="IE2" s="4"/>
+      <c r="IF2" s="4"/>
+      <c r="IG2" s="4"/>
+      <c r="IH2" s="4"/>
+      <c r="II2" s="4"/>
+      <c r="IJ2" s="4"/>
+      <c r="IK2" s="4"/>
+      <c r="IL2" s="4"/>
+      <c r="IM2" s="4"/>
+      <c r="IN2" s="4"/>
+      <c r="IO2" s="4"/>
+      <c r="IP2" s="4"/>
+      <c r="IQ2" s="4"/>
+      <c r="IR2" s="4"/>
+      <c r="IS2" s="4"/>
+      <c r="IT2" s="4"/>
+      <c r="IU2" s="4"/>
+      <c r="IV2" s="4"/>
+      <c r="IW2" s="4"/>
+      <c r="IX2" s="4"/>
+      <c r="IY2" s="4"/>
+      <c r="IZ2" s="4"/>
+      <c r="JA2" s="4"/>
+      <c r="JB2" s="4"/>
+      <c r="JC2" s="4"/>
+      <c r="JD2" s="4"/>
+      <c r="JE2" s="4"/>
+      <c r="JF2" s="4"/>
+      <c r="JG2" s="4"/>
+      <c r="JH2" s="4"/>
+      <c r="JI2" s="4"/>
+      <c r="JJ2" s="4"/>
+      <c r="JK2" s="4"/>
+      <c r="JL2" s="4"/>
+      <c r="JM2" s="4"/>
+      <c r="JN2" s="4"/>
+      <c r="JO2" s="4"/>
+      <c r="JP2" s="4"/>
+      <c r="JQ2" s="4"/>
+      <c r="JR2" s="4"/>
+      <c r="JS2" s="4"/>
+      <c r="JT2" s="4"/>
+      <c r="JU2" s="4"/>
+      <c r="JV2" s="4"/>
+      <c r="JW2" s="4"/>
+      <c r="JX2" s="4"/>
+      <c r="JY2" s="4"/>
+      <c r="JZ2" s="4"/>
+      <c r="KA2" s="4"/>
+      <c r="KB2" s="4"/>
+      <c r="KC2" s="4"/>
+      <c r="KD2" s="4"/>
+      <c r="KE2" s="4"/>
+      <c r="KF2" s="4"/>
+      <c r="KG2" s="4"/>
+      <c r="KH2" s="4"/>
+      <c r="KI2" s="4"/>
+      <c r="KJ2" s="4"/>
+      <c r="KK2" s="4"/>
+      <c r="KL2" s="4"/>
+      <c r="KM2" s="4"/>
+      <c r="KN2" s="4"/>
+      <c r="KO2" s="4"/>
+      <c r="KP2" s="4"/>
+      <c r="KQ2" s="4"/>
+      <c r="KR2" s="4"/>
+      <c r="KS2" s="4"/>
+      <c r="KT2" s="4"/>
+      <c r="KU2" s="4"/>
+      <c r="KV2" s="4"/>
+      <c r="KW2" s="4"/>
+      <c r="KX2" s="4"/>
+      <c r="KY2" s="4"/>
+      <c r="KZ2" s="4"/>
+      <c r="LA2" s="4"/>
+      <c r="LB2" s="4"/>
+      <c r="LC2" s="4"/>
+      <c r="LD2" s="4"/>
+      <c r="LE2" s="4"/>
+      <c r="LF2" s="4"/>
+      <c r="LG2" s="4"/>
+      <c r="LH2" s="4"/>
+      <c r="LI2" s="4"/>
+      <c r="LJ2" s="4"/>
+      <c r="LK2" s="4"/>
+      <c r="LL2" s="4"/>
+      <c r="LM2" s="4"/>
+    </row>
+    <row r="3" spans="1:325" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BO3" s="1"/>
+      <c r="BP3" s="1"/>
+      <c r="BQ3" s="1"/>
+      <c r="BR3" s="1"/>
+      <c r="BS3" s="1"/>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+      <c r="BV3" s="1"/>
+      <c r="BW3" s="1"/>
+      <c r="BX3" s="1"/>
+      <c r="BY3" s="1"/>
+      <c r="BZ3" s="1"/>
+      <c r="CA3" s="1"/>
+      <c r="CB3" s="1"/>
+      <c r="CC3" s="1"/>
+      <c r="CD3" s="1"/>
+      <c r="CE3" s="1"/>
+      <c r="CF3" s="1"/>
+      <c r="CG3" s="1"/>
+      <c r="CH3" s="1"/>
+      <c r="CI3" s="1"/>
+      <c r="CJ3" s="1"/>
+      <c r="CK3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CM3" s="1"/>
+      <c r="CN3" s="1"/>
+      <c r="CO3" s="1"/>
+      <c r="CP3" s="1"/>
+      <c r="CQ3" s="1"/>
+      <c r="CR3" s="1"/>
+      <c r="CS3" s="1"/>
+      <c r="CT3" s="1"/>
+      <c r="CU3" s="1"/>
+      <c r="CV3" s="1"/>
+      <c r="CW3" s="1"/>
+      <c r="CX3" s="1"/>
+      <c r="CY3" s="1"/>
+      <c r="CZ3" s="1"/>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1"/>
+      <c r="DC3" s="1"/>
+      <c r="DD3" s="1"/>
+      <c r="DE3" s="1"/>
+      <c r="DF3" s="1"/>
+      <c r="DG3" s="1"/>
+      <c r="DH3" s="1"/>
+      <c r="DI3" s="1"/>
+      <c r="DJ3" s="1"/>
+      <c r="DK3" s="1"/>
+      <c r="DL3" s="1"/>
+      <c r="DM3" s="1"/>
+      <c r="DN3" s="1"/>
+      <c r="DO3" s="1"/>
+      <c r="DP3" s="1"/>
+      <c r="DQ3" s="1"/>
+      <c r="DR3" s="1"/>
+      <c r="DS3" s="1"/>
+      <c r="DT3" s="1"/>
+      <c r="DU3" s="1"/>
+      <c r="DV3" s="1"/>
+      <c r="DW3" s="1"/>
+      <c r="DX3" s="1"/>
+      <c r="DY3" s="1"/>
+      <c r="DZ3" s="1"/>
+      <c r="EA3" s="1"/>
+      <c r="EB3" s="1"/>
+      <c r="EC3" s="1"/>
+      <c r="ED3" s="1"/>
+      <c r="EE3" s="1"/>
+      <c r="EF3" s="1"/>
+      <c r="EG3" s="1"/>
+      <c r="EH3" s="1"/>
+      <c r="EI3" s="1"/>
+      <c r="EJ3" s="1"/>
+      <c r="EK3" s="1"/>
+      <c r="EL3" s="1"/>
+      <c r="EM3" s="1"/>
+      <c r="EN3" s="1"/>
+      <c r="EO3" s="1"/>
+      <c r="EP3" s="1"/>
+      <c r="EQ3" s="1"/>
+      <c r="ER3" s="1"/>
+      <c r="ES3" s="1"/>
+      <c r="ET3" s="1"/>
+      <c r="EU3" s="1"/>
+      <c r="EV3" s="1"/>
+      <c r="EW3" s="1"/>
+      <c r="EX3" s="1"/>
+      <c r="EY3" s="1"/>
+    </row>
+    <row r="4" spans="1:325" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:304" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="P4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="4"/>
-      <c r="BB2" s="4"/>
-      <c r="BC2" s="4"/>
-      <c r="BD2" s="4"/>
-      <c r="BE2" s="4"/>
-      <c r="BF2" s="4"/>
-      <c r="BG2" s="4"/>
-      <c r="BH2" s="4"/>
-      <c r="BI2" s="4"/>
-      <c r="BJ2" s="4"/>
-      <c r="BK2" s="4"/>
-      <c r="BL2" s="4"/>
-      <c r="BM2" s="4"/>
-      <c r="BN2" s="4"/>
-      <c r="BO2" s="4"/>
-      <c r="BP2" s="4"/>
-      <c r="BQ2" s="4"/>
-      <c r="BR2" s="4"/>
-      <c r="BS2" s="4"/>
-      <c r="BT2" s="4"/>
-      <c r="BU2" s="4"/>
-      <c r="BV2" s="4"/>
-      <c r="BW2" s="4"/>
-      <c r="BX2" s="4"/>
-      <c r="BY2" s="4"/>
-      <c r="BZ2" s="4"/>
-      <c r="CA2" s="4"/>
-      <c r="CB2" s="4"/>
-      <c r="CC2" s="4"/>
-      <c r="CD2" s="4"/>
-      <c r="CE2" s="4"/>
-      <c r="CF2" s="4"/>
-      <c r="CG2" s="4"/>
-      <c r="CH2" s="4"/>
-      <c r="CI2" s="4"/>
-      <c r="CJ2" s="4"/>
-      <c r="CK2" s="4"/>
-      <c r="CL2" s="4"/>
-      <c r="CM2" s="4"/>
-      <c r="CN2" s="4"/>
-      <c r="CO2" s="4"/>
-      <c r="CP2" s="4"/>
-      <c r="CQ2" s="4"/>
-      <c r="CR2" s="4"/>
-      <c r="CS2" s="4"/>
-      <c r="CT2" s="4"/>
-      <c r="CU2" s="4"/>
-      <c r="CV2" s="4"/>
-      <c r="CW2" s="4"/>
-      <c r="CX2" s="4"/>
-      <c r="CY2" s="4"/>
-      <c r="CZ2" s="4"/>
-      <c r="DA2" s="4"/>
-      <c r="DB2" s="4"/>
-      <c r="DC2" s="4"/>
-      <c r="DD2" s="4"/>
-      <c r="DE2" s="4"/>
-      <c r="DF2" s="4"/>
-      <c r="DG2" s="4"/>
-      <c r="DH2" s="4"/>
-      <c r="DI2" s="4"/>
-      <c r="DJ2" s="4"/>
-      <c r="DK2" s="4"/>
-      <c r="DL2" s="4"/>
-      <c r="DM2" s="4"/>
-      <c r="DN2" s="4"/>
-      <c r="DO2" s="4"/>
-      <c r="DP2" s="4"/>
-      <c r="DQ2" s="4"/>
-      <c r="DR2" s="4"/>
-      <c r="DS2" s="4"/>
-      <c r="DT2" s="4"/>
-      <c r="DU2" s="4"/>
-      <c r="DV2" s="4"/>
-      <c r="DW2" s="4"/>
-      <c r="DX2" s="4"/>
-      <c r="DY2" s="4"/>
-      <c r="DZ2" s="4"/>
-      <c r="EA2" s="4"/>
-      <c r="EB2" s="4"/>
-      <c r="EC2" s="4"/>
-      <c r="ED2" s="4"/>
-      <c r="EE2" s="4"/>
-      <c r="EF2" s="4"/>
-      <c r="EG2" s="4"/>
-      <c r="EH2" s="4"/>
-      <c r="EI2" s="4"/>
-      <c r="EJ2" s="4"/>
-      <c r="EK2" s="4"/>
-      <c r="EL2" s="4"/>
-      <c r="EM2" s="4"/>
-      <c r="EN2" s="4"/>
-      <c r="EO2" s="4"/>
-      <c r="EP2" s="4"/>
-      <c r="EQ2" s="4"/>
-      <c r="ER2" s="4"/>
-      <c r="ES2" s="4"/>
-      <c r="ET2" s="4"/>
-      <c r="EU2" s="4"/>
-      <c r="EV2" s="4"/>
-      <c r="EW2" s="4"/>
-      <c r="EX2" s="4"/>
-      <c r="EY2" s="4"/>
-      <c r="EZ2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:304" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-      <c r="BK3" s="2"/>
-      <c r="BL3" s="2"/>
-      <c r="BM3" s="2"/>
-      <c r="BN3" s="2"/>
-      <c r="BO3" s="2"/>
-      <c r="BP3" s="2"/>
-      <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
-      <c r="BS3" s="2"/>
-      <c r="BT3" s="2"/>
-      <c r="BU3" s="2"/>
-      <c r="BV3" s="2"/>
-      <c r="BW3" s="2"/>
-      <c r="BX3" s="2"/>
-      <c r="BY3" s="2"/>
-      <c r="BZ3" s="2"/>
-      <c r="CA3" s="2"/>
-      <c r="CB3" s="2"/>
-      <c r="CC3" s="2"/>
-      <c r="CD3" s="2"/>
-      <c r="CE3" s="2"/>
-      <c r="CF3" s="2"/>
-      <c r="CG3" s="2"/>
-      <c r="CH3" s="2"/>
-      <c r="CI3" s="2"/>
-      <c r="CJ3" s="2"/>
-      <c r="CK3" s="2"/>
-      <c r="CL3" s="2"/>
-      <c r="CM3" s="2"/>
-      <c r="CN3" s="2"/>
-      <c r="CO3" s="2"/>
-      <c r="CP3" s="2"/>
-      <c r="CQ3" s="2"/>
-      <c r="CR3" s="2"/>
-      <c r="CS3" s="2"/>
-      <c r="CT3" s="2"/>
-      <c r="CU3" s="2"/>
-      <c r="CV3" s="2"/>
-      <c r="CW3" s="2"/>
-      <c r="CX3" s="2"/>
-      <c r="CY3" s="2"/>
-      <c r="CZ3" s="2"/>
-      <c r="DA3" s="2"/>
-      <c r="DB3" s="2"/>
-      <c r="DC3" s="2"/>
-      <c r="DD3" s="2"/>
-      <c r="DE3" s="2"/>
-      <c r="DF3" s="2"/>
-      <c r="DG3" s="2"/>
-      <c r="DH3" s="2"/>
-      <c r="DI3" s="2"/>
-      <c r="DJ3" s="2"/>
-      <c r="DK3" s="2"/>
-      <c r="DL3" s="2"/>
-      <c r="DM3" s="2"/>
-      <c r="DN3" s="2"/>
-      <c r="DO3" s="2"/>
-      <c r="DP3" s="2"/>
-      <c r="DQ3" s="2"/>
-      <c r="DR3" s="2"/>
-      <c r="DS3" s="2"/>
-      <c r="DT3" s="2"/>
-      <c r="DU3" s="2"/>
-      <c r="DV3" s="2"/>
-      <c r="DW3" s="2"/>
-      <c r="DX3" s="2"/>
-      <c r="DY3" s="2"/>
-      <c r="DZ3" s="2"/>
-      <c r="EA3" s="2"/>
-      <c r="EB3" s="2"/>
-      <c r="EC3" s="2"/>
-      <c r="ED3" s="2"/>
-      <c r="EE3" s="2"/>
-      <c r="EF3" s="2"/>
-      <c r="EG3" s="2"/>
-      <c r="EH3" s="2"/>
-      <c r="EI3" s="2"/>
-      <c r="EJ3" s="2"/>
-      <c r="EK3" s="2"/>
-      <c r="EL3" s="2"/>
-      <c r="EM3" s="2"/>
-      <c r="EN3" s="2"/>
-      <c r="EO3" s="2"/>
-      <c r="EP3" s="2"/>
-      <c r="EQ3" s="2"/>
-      <c r="ER3" s="2"/>
-      <c r="ES3" s="2"/>
-      <c r="ET3" s="2"/>
-      <c r="EU3" s="2"/>
-      <c r="EV3" s="2"/>
-      <c r="EW3" s="2"/>
-      <c r="EX3" s="2"/>
-      <c r="EY3" s="2"/>
-    </row>
-    <row r="4" spans="1:304" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>21</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>22</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>23</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>25</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>26</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>27</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>28</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>30</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>31</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>32</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>33</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>34</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>35</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>37</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>38</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>40</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>41</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>42</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>43</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>44</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>45</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>46</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>47</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>48</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU4" t="s">
         <v>49</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AV4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX4" t="s">
         <v>52</v>
       </c>
-      <c r="AU4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW4" t="s">
+      <c r="AY4" t="s">
         <v>54</v>
       </c>
-      <c r="AX4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY4" t="s">
+      <c r="AZ4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA4" t="s">
         <v>55</v>
       </c>
-      <c r="AZ4" t="s">
-        <v>55</v>
-      </c>
-      <c r="BA4" t="s">
+      <c r="BB4" t="s">
         <v>56</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BC4" t="s">
         <v>57</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BD4" t="s">
         <v>58</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BE4" t="s">
         <v>59</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BF4" t="s">
         <v>60</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>61</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>62</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BI4" t="s">
         <v>63</v>
       </c>
-      <c r="BI4" t="s">
+      <c r="BJ4" t="s">
         <v>64</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="BK4" t="s">
         <v>65</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>66</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>67</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
         <v>68</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BO4" t="s">
         <v>69</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
         <v>70</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BQ4" t="s">
         <v>71</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" t="s">
         <v>72</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BS4" t="s">
         <v>73</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BT4" t="s">
         <v>74</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BU4" t="s">
         <v>75</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BV4" t="s">
         <v>76</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BW4" t="s">
         <v>77</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BX4" t="s">
         <v>78</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="BY4" t="s">
         <v>79</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" t="s">
         <v>80</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CA4" t="s">
         <v>81</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" t="s">
         <v>82</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CC4" t="s">
         <v>83</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>84</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>85</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>86</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>87</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>88</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>89</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CJ4" t="s">
+        <v>89</v>
+      </c>
+      <c r="CK4" t="s">
         <v>90</v>
       </c>
-      <c r="CJ4" t="s">
-        <v>90</v>
-      </c>
-      <c r="CK4" t="s">
+      <c r="CL4" t="s">
         <v>91</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>92</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
+        <v>92</v>
+      </c>
+      <c r="CO4" t="s">
         <v>93</v>
       </c>
-      <c r="CN4" t="s">
-        <v>93</v>
-      </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>94</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>95</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CR4" t="s">
         <v>96</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CS4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT4" t="s">
         <v>97</v>
       </c>
-      <c r="CS4" t="s">
-        <v>97</v>
-      </c>
-      <c r="CT4" t="s">
+      <c r="CU4" t="s">
         <v>98</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="CV4" t="s">
         <v>99</v>
       </c>
-      <c r="CV4" t="s">
+      <c r="CW4" t="s">
         <v>100</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="CX4" t="s">
         <v>101</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="CY4" t="s">
         <v>102</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="CZ4" t="s">
         <v>103</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DA4" t="s">
         <v>104</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DB4" t="s">
         <v>105</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DC4" t="s">
         <v>106</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DD4" t="s">
         <v>107</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DE4" t="s">
         <v>108</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DF4" t="s">
         <v>109</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DG4" t="s">
         <v>110</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DH4" t="s">
         <v>111</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DI4" t="s">
         <v>112</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DJ4" t="s">
         <v>113</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DK4" t="s">
         <v>114</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DL4" t="s">
         <v>115</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DM4" t="s">
         <v>116</v>
       </c>
-      <c r="DM4" t="s">
+      <c r="DN4" t="s">
         <v>117</v>
       </c>
-      <c r="DN4" t="s">
+      <c r="DO4" t="s">
         <v>118</v>
       </c>
-      <c r="DO4" t="s">
+      <c r="DP4" t="s">
         <v>119</v>
       </c>
-      <c r="DP4" t="s">
+      <c r="DQ4" t="s">
         <v>120</v>
       </c>
-      <c r="DQ4" t="s">
+      <c r="DR4" t="s">
         <v>121</v>
       </c>
-      <c r="DR4" t="s">
+      <c r="DS4" t="s">
         <v>122</v>
       </c>
-      <c r="DS4" t="s">
+      <c r="DT4" t="s">
         <v>123</v>
       </c>
-      <c r="DT4" t="s">
+      <c r="DU4" t="s">
         <v>124</v>
       </c>
-      <c r="DU4" t="s">
+      <c r="DV4" t="s">
         <v>125</v>
       </c>
-      <c r="DV4" t="s">
+      <c r="DW4" t="s">
         <v>126</v>
       </c>
-      <c r="DW4" t="s">
+      <c r="DX4" t="s">
+        <v>128</v>
+      </c>
+      <c r="DY4" t="s">
         <v>127</v>
       </c>
-      <c r="DX4" t="s">
+      <c r="DZ4" t="s">
         <v>129</v>
       </c>
-      <c r="DY4" t="s">
-        <v>128</v>
-      </c>
-      <c r="DZ4" t="s">
+      <c r="EA4" t="s">
         <v>130</v>
       </c>
-      <c r="EA4" t="s">
+      <c r="EB4" t="s">
         <v>131</v>
       </c>
-      <c r="EB4" t="s">
+      <c r="EC4" t="s">
         <v>132</v>
       </c>
-      <c r="EC4" t="s">
+      <c r="ED4" t="s">
         <v>133</v>
       </c>
-      <c r="ED4" t="s">
+      <c r="EE4" t="s">
         <v>134</v>
       </c>
-      <c r="EE4" t="s">
+      <c r="EF4" t="s">
         <v>135</v>
       </c>
-      <c r="EF4" t="s">
+      <c r="EG4" t="s">
         <v>136</v>
       </c>
-      <c r="EG4" t="s">
+      <c r="EH4" t="s">
         <v>137</v>
       </c>
-      <c r="EH4" t="s">
+      <c r="EI4" t="s">
         <v>138</v>
       </c>
-      <c r="EI4" t="s">
+      <c r="EJ4" t="s">
         <v>139</v>
       </c>
-      <c r="EJ4" t="s">
+      <c r="EK4" t="s">
         <v>140</v>
       </c>
-      <c r="EK4" t="s">
+      <c r="EL4" t="s">
         <v>141</v>
       </c>
-      <c r="EL4" t="s">
+      <c r="EM4" t="s">
         <v>142</v>
       </c>
-      <c r="EM4" t="s">
+      <c r="EN4" t="s">
         <v>143</v>
       </c>
-      <c r="EN4" t="s">
+      <c r="EO4" t="s">
         <v>144</v>
       </c>
-      <c r="EO4" t="s">
+      <c r="EP4" t="s">
         <v>145</v>
       </c>
-      <c r="EP4" t="s">
+      <c r="EQ4" t="s">
         <v>146</v>
       </c>
-      <c r="EQ4" t="s">
+      <c r="ER4" t="s">
         <v>147</v>
       </c>
-      <c r="ER4" t="s">
+      <c r="ES4" t="s">
         <v>148</v>
       </c>
-      <c r="ES4" t="s">
+      <c r="ET4" t="s">
         <v>149</v>
       </c>
-      <c r="ET4" t="s">
+      <c r="EU4" t="s">
         <v>150</v>
       </c>
-      <c r="EU4" t="s">
+      <c r="EV4" t="s">
         <v>151</v>
       </c>
-      <c r="EV4" t="s">
+      <c r="EW4" t="s">
         <v>152</v>
       </c>
-      <c r="EW4" t="s">
+      <c r="EX4" t="s">
         <v>153</v>
       </c>
-      <c r="EX4" t="s">
+      <c r="EY4" t="s">
         <v>154</v>
       </c>
-      <c r="EY4" t="s">
+      <c r="EZ4" t="s">
         <v>155</v>
       </c>
-      <c r="EZ4" t="s">
+      <c r="FA4" t="s">
         <v>156</v>
       </c>
-      <c r="FA4" t="s">
+      <c r="FB4" t="s">
         <v>157</v>
       </c>
-      <c r="FB4" t="s">
+      <c r="FC4" t="s">
         <v>158</v>
       </c>
-      <c r="FC4" t="s">
+      <c r="FD4" t="s">
         <v>159</v>
       </c>
-      <c r="FD4" t="s">
+      <c r="FE4" t="s">
         <v>160</v>
       </c>
-      <c r="FE4" t="s">
+      <c r="FF4" t="s">
         <v>161</v>
       </c>
-      <c r="FF4" t="s">
+      <c r="FG4" t="s">
         <v>162</v>
       </c>
-      <c r="FG4" t="s">
+      <c r="FH4" t="s">
         <v>163</v>
       </c>
-      <c r="FH4" t="s">
+      <c r="FI4" t="s">
         <v>164</v>
       </c>
-      <c r="FI4" t="s">
+      <c r="FJ4" t="s">
         <v>165</v>
       </c>
-      <c r="FJ4" t="s">
+      <c r="FK4" t="s">
         <v>166</v>
       </c>
-      <c r="FK4" t="s">
+      <c r="FL4" t="s">
         <v>167</v>
       </c>
-      <c r="FL4" t="s">
+      <c r="FM4" t="s">
         <v>168</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FN4" t="s">
         <v>169</v>
       </c>
-      <c r="FN4" t="s">
+      <c r="FO4" t="s">
         <v>170</v>
       </c>
-      <c r="FO4" t="s">
+      <c r="FP4" t="s">
         <v>171</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FQ4" t="s">
         <v>172</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FR4" t="s">
         <v>173</v>
       </c>
-      <c r="FR4" t="s">
+      <c r="FS4" t="s">
         <v>174</v>
       </c>
-      <c r="FS4" t="s">
+      <c r="FT4" t="s">
         <v>175</v>
       </c>
-      <c r="FT4" t="s">
+      <c r="FU4" t="s">
         <v>176</v>
       </c>
-      <c r="FU4" t="s">
+      <c r="FV4" t="s">
         <v>177</v>
       </c>
-      <c r="FV4" t="s">
+      <c r="FW4" t="s">
         <v>178</v>
       </c>
-      <c r="FW4" t="s">
+      <c r="FX4" t="s">
         <v>179</v>
       </c>
-      <c r="FX4" t="s">
+      <c r="FY4" t="s">
         <v>180</v>
       </c>
-      <c r="FY4" t="s">
+      <c r="FZ4" t="s">
         <v>181</v>
       </c>
-      <c r="FZ4" t="s">
+      <c r="GA4" t="s">
         <v>182</v>
       </c>
-      <c r="GA4" t="s">
+      <c r="GB4" t="s">
         <v>183</v>
       </c>
-      <c r="GB4" t="s">
+      <c r="GC4" t="s">
         <v>184</v>
       </c>
-      <c r="GC4" t="s">
+      <c r="GD4" t="s">
         <v>185</v>
       </c>
-      <c r="GD4" t="s">
+      <c r="GE4" t="s">
         <v>186</v>
       </c>
-      <c r="GE4" t="s">
+      <c r="GF4" t="s">
         <v>187</v>
       </c>
-      <c r="GF4" t="s">
+      <c r="GG4" t="s">
         <v>188</v>
       </c>
-      <c r="GG4" t="s">
+      <c r="GH4" t="s">
         <v>189</v>
       </c>
-      <c r="GH4" t="s">
+      <c r="GI4" t="s">
         <v>190</v>
       </c>
-      <c r="GI4" t="s">
+      <c r="GJ4" t="s">
         <v>191</v>
       </c>
-      <c r="GJ4" t="s">
+      <c r="GK4" t="s">
         <v>192</v>
       </c>
-      <c r="GK4" t="s">
+      <c r="GL4" t="s">
         <v>193</v>
       </c>
-      <c r="GL4" t="s">
+      <c r="GM4" t="s">
         <v>194</v>
       </c>
-      <c r="GM4" t="s">
+      <c r="GN4" t="s">
         <v>195</v>
       </c>
-      <c r="GN4" t="s">
+      <c r="GO4" t="s">
         <v>196</v>
       </c>
-      <c r="GO4" t="s">
+      <c r="GP4" t="s">
         <v>197</v>
       </c>
-      <c r="GP4" t="s">
+      <c r="GQ4" t="s">
         <v>198</v>
       </c>
-      <c r="GQ4" t="s">
+      <c r="GR4" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="GR4" s="5" t="s">
+      <c r="GS4" t="s">
         <v>200</v>
       </c>
-      <c r="GS4" t="s">
+      <c r="GT4" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="GT4" s="5" t="s">
+      <c r="GU4" t="s">
         <v>202</v>
       </c>
-      <c r="GU4" t="s">
+      <c r="GV4" t="s">
         <v>203</v>
       </c>
-      <c r="GV4" t="s">
+      <c r="GW4" t="s">
         <v>204</v>
       </c>
-      <c r="GW4" t="s">
+      <c r="GX4" t="s">
         <v>205</v>
       </c>
-      <c r="GX4" t="s">
+      <c r="GY4" t="s">
         <v>206</v>
       </c>
-      <c r="GY4" t="s">
+      <c r="GZ4" t="s">
         <v>207</v>
       </c>
-      <c r="GZ4" t="s">
+      <c r="HA4" t="s">
         <v>208</v>
       </c>
-      <c r="HA4" t="s">
+      <c r="HB4" t="s">
         <v>209</v>
       </c>
-      <c r="HB4" t="s">
+      <c r="HC4" t="s">
         <v>210</v>
       </c>
-      <c r="HC4" t="s">
+      <c r="HD4" t="s">
         <v>211</v>
       </c>
-      <c r="HD4" t="s">
+      <c r="HE4" t="s">
         <v>212</v>
       </c>
-      <c r="HE4" t="s">
+      <c r="HF4" t="s">
         <v>213</v>
       </c>
-      <c r="HF4" t="s">
+      <c r="HG4" t="s">
         <v>214</v>
       </c>
-      <c r="HG4" t="s">
+      <c r="HH4" t="s">
         <v>215</v>
       </c>
-      <c r="HH4" t="s">
+      <c r="HI4" t="s">
         <v>216</v>
       </c>
-      <c r="HI4" t="s">
+      <c r="HJ4" t="s">
         <v>217</v>
       </c>
-      <c r="HJ4" t="s">
+      <c r="HK4" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="HK4" s="5" t="s">
+      <c r="HL4" t="s">
         <v>219</v>
       </c>
-      <c r="HL4" t="s">
+      <c r="HM4" t="s">
         <v>220</v>
       </c>
-      <c r="HM4" t="s">
+      <c r="HN4" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="HN4" s="5" t="s">
+      <c r="HO4" t="s">
         <v>222</v>
       </c>
-      <c r="HO4" t="s">
+      <c r="HP4" t="s">
         <v>223</v>
       </c>
-      <c r="HP4" t="s">
+      <c r="HQ4" t="s">
         <v>224</v>
       </c>
-      <c r="HQ4" t="s">
+      <c r="HR4" t="s">
         <v>225</v>
       </c>
-      <c r="HR4" t="s">
+      <c r="HS4" t="s">
         <v>226</v>
       </c>
-      <c r="HS4" t="s">
+      <c r="HT4" t="s">
         <v>227</v>
       </c>
-      <c r="HT4" t="s">
+      <c r="HU4" t="s">
         <v>228</v>
       </c>
-      <c r="HU4" t="s">
+      <c r="HV4" t="s">
         <v>229</v>
       </c>
-      <c r="HV4" t="s">
+      <c r="HW4" t="s">
         <v>230</v>
       </c>
-      <c r="HW4" t="s">
+      <c r="HX4" t="s">
         <v>231</v>
       </c>
-      <c r="HX4" t="s">
+      <c r="HY4" t="s">
         <v>232</v>
       </c>
-      <c r="HY4" t="s">
+      <c r="HZ4" t="s">
         <v>233</v>
       </c>
-      <c r="HZ4" t="s">
+      <c r="IA4" t="s">
         <v>234</v>
       </c>
-      <c r="IA4" t="s">
+      <c r="IB4" t="s">
         <v>235</v>
       </c>
-      <c r="IB4" t="s">
+      <c r="IC4" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="IC4" s="5" t="s">
+      <c r="ID4" t="s">
         <v>237</v>
       </c>
-      <c r="ID4" t="s">
+      <c r="IE4" t="s">
         <v>238</v>
       </c>
-      <c r="IE4" t="s">
+      <c r="IF4" t="s">
         <v>239</v>
       </c>
-      <c r="IF4" t="s">
+      <c r="IG4" t="s">
         <v>240</v>
       </c>
-      <c r="IG4" t="s">
+      <c r="IH4" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="IH4" s="5" t="s">
+      <c r="II4" t="s">
         <v>242</v>
       </c>
-      <c r="II4" t="s">
+      <c r="IJ4" t="s">
         <v>243</v>
       </c>
-      <c r="IJ4" t="s">
+      <c r="IK4" t="s">
         <v>244</v>
       </c>
-      <c r="IK4" t="s">
+      <c r="IL4" t="s">
         <v>245</v>
       </c>
-      <c r="IL4" t="s">
+      <c r="IM4" t="s">
         <v>246</v>
       </c>
-      <c r="IM4" t="s">
+      <c r="IN4" t="s">
         <v>247</v>
       </c>
-      <c r="IN4" t="s">
+      <c r="IO4" t="s">
         <v>248</v>
       </c>
-      <c r="IO4" t="s">
+      <c r="IP4" t="s">
         <v>249</v>
       </c>
-      <c r="IP4" t="s">
+      <c r="IQ4" t="s">
         <v>250</v>
       </c>
-      <c r="IQ4" t="s">
+      <c r="IR4" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="IR4" s="5" t="s">
+      <c r="IS4" t="s">
         <v>252</v>
       </c>
-      <c r="IS4" t="s">
+      <c r="IT4" t="s">
         <v>253</v>
       </c>
-      <c r="IT4" t="s">
+      <c r="IU4" t="s">
         <v>254</v>
       </c>
-      <c r="IU4" t="s">
+      <c r="IV4" t="s">
         <v>255</v>
       </c>
-      <c r="IV4" t="s">
+      <c r="IW4" t="s">
         <v>256</v>
       </c>
-      <c r="IW4" t="s">
+      <c r="IX4" t="s">
         <v>257</v>
       </c>
-      <c r="IX4" t="s">
+      <c r="IY4" t="s">
         <v>258</v>
       </c>
-      <c r="IY4" t="s">
+      <c r="IZ4" t="s">
         <v>259</v>
       </c>
-      <c r="IZ4" t="s">
+      <c r="JA4" t="s">
         <v>260</v>
       </c>
-      <c r="JA4" t="s">
+      <c r="JB4" t="s">
         <v>261</v>
       </c>
-      <c r="JB4" t="s">
+      <c r="JC4" t="s">
         <v>262</v>
       </c>
-      <c r="JC4" t="s">
+      <c r="JD4" t="s">
         <v>263</v>
       </c>
-      <c r="JD4" t="s">
+      <c r="JE4" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="JE4" s="5" t="s">
+      <c r="JF4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="JF4" s="5" t="s">
+      <c r="JG4" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="JG4" s="5" t="s">
+      <c r="JH4" t="s">
         <v>267</v>
       </c>
-      <c r="JH4" t="s">
+      <c r="JI4" t="s">
         <v>268</v>
       </c>
-      <c r="JI4" t="s">
+      <c r="JJ4" t="s">
         <v>269</v>
       </c>
-      <c r="JJ4" t="s">
+      <c r="JK4" t="s">
         <v>270</v>
       </c>
-      <c r="JK4" t="s">
+      <c r="JL4" t="s">
         <v>271</v>
       </c>
-      <c r="JL4" t="s">
+      <c r="JM4" t="s">
         <v>272</v>
       </c>
-      <c r="JM4" t="s">
+      <c r="JN4" t="s">
         <v>273</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JO4" t="s">
         <v>274</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JP4" t="s">
         <v>275</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JQ4" t="s">
         <v>276</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JR4" t="s">
         <v>277</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JS4" t="s">
         <v>278</v>
       </c>
-      <c r="JS4" t="s">
+      <c r="JT4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="JT4" s="5" t="s">
+      <c r="JU4" t="s">
         <v>280</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JV4" t="s">
         <v>281</v>
       </c>
-      <c r="JV4" t="s">
+      <c r="JW4" t="s">
         <v>282</v>
       </c>
-      <c r="JW4" t="s">
+      <c r="JX4" t="s">
         <v>283</v>
       </c>
-      <c r="JX4" t="s">
+      <c r="JY4" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="JY4" s="5" t="s">
+      <c r="JZ4" t="s">
         <v>285</v>
       </c>
-      <c r="JZ4" t="s">
+      <c r="KA4" t="s">
         <v>286</v>
       </c>
-      <c r="KA4" t="s">
+      <c r="KB4" t="s">
         <v>287</v>
       </c>
-      <c r="KB4" t="s">
+      <c r="KC4" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="KC4" s="5" t="s">
+      <c r="KD4" t="s">
         <v>289</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KE4" t="s">
         <v>290</v>
       </c>
-      <c r="KE4" t="s">
+      <c r="KF4" t="s">
         <v>291</v>
       </c>
-      <c r="KF4" t="s">
+      <c r="KG4" t="s">
         <v>292</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KH4" t="s">
         <v>293</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KI4" t="s">
         <v>294</v>
       </c>
-      <c r="KI4" t="s">
+      <c r="KJ4" t="s">
         <v>295</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KK4" t="s">
         <v>296</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KL4" t="s">
         <v>297</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KM4" t="s">
         <v>298</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KN4" t="s">
         <v>299</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KO4" t="s">
         <v>300</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KP4" t="s">
         <v>301</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KQ4" t="s">
         <v>302</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KR4" t="s">
         <v>303</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KS4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:304" x14ac:dyDescent="0.25">
+      <c r="KT4" t="s">
+        <v>305</v>
+      </c>
+      <c r="KU4" t="s">
+        <v>306</v>
+      </c>
+      <c r="KV4" t="s">
+        <v>307</v>
+      </c>
+      <c r="KW4" t="s">
+        <v>308</v>
+      </c>
+      <c r="KX4" t="s">
+        <v>309</v>
+      </c>
+      <c r="KY4" t="s">
+        <v>310</v>
+      </c>
+      <c r="KZ4" t="s">
+        <v>311</v>
+      </c>
+      <c r="LA4" t="s">
+        <v>312</v>
+      </c>
+      <c r="LB4" t="s">
+        <v>313</v>
+      </c>
+      <c r="LC4" t="s">
+        <v>314</v>
+      </c>
+      <c r="LD4" t="s">
+        <v>315</v>
+      </c>
+      <c r="LE4" t="s">
+        <v>316</v>
+      </c>
+      <c r="LF4" t="s">
+        <v>317</v>
+      </c>
+      <c r="LG4" t="s">
+        <v>318</v>
+      </c>
+      <c r="LH4" t="s">
+        <v>319</v>
+      </c>
+      <c r="LI4" t="s">
+        <v>320</v>
+      </c>
+      <c r="LJ4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="LK4" t="s">
+        <v>324</v>
+      </c>
+      <c r="LL4" t="s">
+        <v>323</v>
+      </c>
+      <c r="LM4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:304" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:325" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3169,9 +3508,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C2:O2"/>
     <mergeCell ref="P2:EY2"/>
+    <mergeCell ref="EZ2:LM2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="GT4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
@@ -3186,8 +3526,9 @@
     <hyperlink ref="JT4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
     <hyperlink ref="JY4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
     <hyperlink ref="KC4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LJ4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustando detalles de informes director tesis, 20/47 requerimientos en tabla excel
Ajustando detalles de informes director tesis, 20/47 requerimientos en matriz trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1414D1F-679F-4577-9233-0566BC1DD3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71EC372-EB46-4604-91F4-7E65CABCFCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="354">
   <si>
     <t>MVC</t>
   </si>
@@ -433,9 +433,6 @@
     <t>/tesis/index2_ins_pro</t>
   </si>
   <si>
-    <t>/tesis/index2_ins</t>
-  </si>
-  <si>
     <t>/tesis/index3_ins</t>
   </si>
   <si>
@@ -799,9 +796,6 @@
     <t>TesisController @edit</t>
   </si>
   <si>
-    <t>TesisController @pedir_nota-pendiente</t>
-  </si>
-  <si>
     <t>TesisController @save_nota_pendiente</t>
   </si>
   <si>
@@ -1108,12 +1102,6 @@
     <t>RegisterController.php   @validator</t>
   </si>
   <si>
-    <t>RegisterController.php   @create</t>
-  </si>
-  <si>
-    <t>LoginController.php</t>
-  </si>
-  <si>
     <t>/tesis/acta_examen</t>
   </si>
   <si>
@@ -1121,13 +1109,90 @@
   </si>
   <si>
     <t>Alumno</t>
+  </si>
+  <si>
+    <t>Profesor Guia</t>
+  </si>
+  <si>
+    <t>Profesor  Guia</t>
+  </si>
+  <si>
+    <t>Director Escuela</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Director Tesis</t>
+  </si>
+  <si>
+    <t>TesisController @pedir_nota_pendiente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Controlad</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or:</t>
+    </r>
+  </si>
+  <si>
+    <t>/tesis/aceptar_nota_pendiente</t>
+  </si>
+  <si>
+    <t>/tesis/aceptar_nota_prorroga</t>
+  </si>
+  <si>
+    <t>/tesis/aceptar_nota_pendiente_director</t>
+  </si>
+  <si>
+    <t>/tesis_aceptar_nota_prorroga_director</t>
+  </si>
+  <si>
+    <t>21a</t>
+  </si>
+  <si>
+    <t>21b</t>
+  </si>
+  <si>
+    <t>21c</t>
+  </si>
+  <si>
+    <t>21d</t>
+  </si>
+  <si>
+    <t>21e</t>
+  </si>
+  <si>
+    <t>21f</t>
+  </si>
+  <si>
+    <t>21g</t>
+  </si>
+  <si>
+    <t>21h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1152,6 +1217,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1197,16 +1284,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1215,9 +1299,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1534,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LO78"/>
+  <dimension ref="A1:LP78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ID1" workbookViewId="0">
-      <selection activeCell="II14" sqref="II14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,9 +1701,9 @@
     <col min="75" max="75" width="25.42578125" customWidth="1"/>
     <col min="76" max="76" width="18" customWidth="1"/>
     <col min="77" max="77" width="17.42578125" customWidth="1"/>
-    <col min="78" max="78" width="19" customWidth="1"/>
-    <col min="79" max="79" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="12.42578125" customWidth="1"/>
+    <col min="78" max="78" width="31.5703125" customWidth="1"/>
+    <col min="79" max="79" width="28.7109375" customWidth="1"/>
+    <col min="80" max="80" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="35.28515625" customWidth="1"/>
     <col min="82" max="82" width="23.5703125" customWidth="1"/>
     <col min="83" max="83" width="34.5703125" customWidth="1"/>
@@ -1658,13 +1749,13 @@
     <col min="123" max="123" width="24.85546875" customWidth="1"/>
     <col min="124" max="124" width="35.85546875" customWidth="1"/>
     <col min="125" max="125" width="19.5703125" customWidth="1"/>
-    <col min="126" max="126" width="20.5703125" customWidth="1"/>
-    <col min="127" max="127" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="32.140625" customWidth="1"/>
     <col min="128" max="128" width="29" customWidth="1"/>
     <col min="129" max="129" width="26.28515625" customWidth="1"/>
     <col min="130" max="130" width="25.140625" customWidth="1"/>
     <col min="131" max="131" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="12.28515625" customWidth="1"/>
+    <col min="132" max="132" width="21.28515625" customWidth="1"/>
     <col min="133" max="133" width="16.85546875" customWidth="1"/>
     <col min="134" max="134" width="18" customWidth="1"/>
     <col min="135" max="135" width="16.140625" bestFit="1" customWidth="1"/>
@@ -1749,7 +1840,7 @@
     <col min="217" max="217" width="35.42578125" customWidth="1"/>
     <col min="218" max="218" width="34.7109375" customWidth="1"/>
     <col min="219" max="219" width="31" customWidth="1"/>
-    <col min="220" max="220" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="38.5703125" customWidth="1"/>
     <col min="221" max="221" width="30.28515625" customWidth="1"/>
     <col min="222" max="222" width="38.42578125" customWidth="1"/>
     <col min="223" max="223" width="45.5703125" customWidth="1"/>
@@ -1762,16 +1853,16 @@
     <col min="230" max="230" width="26.85546875" customWidth="1"/>
     <col min="231" max="231" width="33.42578125" customWidth="1"/>
     <col min="232" max="232" width="22.140625" customWidth="1"/>
-    <col min="233" max="233" width="22.42578125" customWidth="1"/>
-    <col min="234" max="234" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="43.5703125" customWidth="1"/>
+    <col min="234" max="234" width="39.85546875" customWidth="1"/>
     <col min="235" max="235" width="37.28515625" customWidth="1"/>
     <col min="236" max="236" width="36" customWidth="1"/>
     <col min="237" max="237" width="38.140625" customWidth="1"/>
     <col min="238" max="238" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="239" max="239" width="30.42578125" customWidth="1"/>
     <col min="240" max="240" width="26.28515625" customWidth="1"/>
-    <col min="241" max="241" width="27.5703125" customWidth="1"/>
-    <col min="242" max="242" width="30.42578125" customWidth="1"/>
+    <col min="241" max="241" width="39" customWidth="1"/>
+    <col min="242" max="242" width="38.28515625" customWidth="1"/>
     <col min="243" max="243" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="244" max="244" width="32.7109375" customWidth="1"/>
     <col min="245" max="245" width="56.42578125" customWidth="1"/>
@@ -1812,7 +1903,7 @@
     <col min="280" max="280" width="43.7109375" customWidth="1"/>
     <col min="281" max="281" width="44.140625" customWidth="1"/>
     <col min="282" max="282" width="40.85546875" customWidth="1"/>
-    <col min="283" max="283" width="35.42578125" customWidth="1"/>
+    <col min="283" max="283" width="46.7109375" customWidth="1"/>
     <col min="284" max="284" width="50.140625" customWidth="1"/>
     <col min="285" max="285" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="286" max="286" width="41.140625" customWidth="1"/>
@@ -1834,8 +1925,8 @@
     <col min="302" max="302" width="52.28515625" customWidth="1"/>
     <col min="303" max="303" width="47.28515625" customWidth="1"/>
     <col min="304" max="304" width="43.28515625" customWidth="1"/>
-    <col min="305" max="305" width="26.7109375" customWidth="1"/>
-    <col min="306" max="306" width="27" customWidth="1"/>
+    <col min="305" max="305" width="50.85546875" customWidth="1"/>
+    <col min="306" max="306" width="50.7109375" customWidth="1"/>
     <col min="307" max="307" width="29.85546875" customWidth="1"/>
     <col min="308" max="308" width="52.5703125" customWidth="1"/>
     <col min="309" max="309" width="27" customWidth="1"/>
@@ -1853,13 +1944,13 @@
     <col min="322" max="322" width="31.5703125" customWidth="1"/>
     <col min="323" max="323" width="43.5703125" customWidth="1"/>
     <col min="324" max="324" width="59.7109375" customWidth="1"/>
-    <col min="325" max="325" width="28.42578125" customWidth="1"/>
+    <col min="325" max="325" width="38.28515625" customWidth="1"/>
     <col min="326" max="326" width="35.42578125" customWidth="1"/>
     <col min="327" max="327" width="34.7109375" customWidth="1"/>
     <col min="328" max="328" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:327" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:328" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1870,500 +1961,533 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:327" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:328" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-      <c r="AZ2" s="8"/>
-      <c r="BA2" s="8"/>
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="8"/>
-      <c r="BI2" s="8"/>
-      <c r="BJ2" s="8"/>
-      <c r="BK2" s="8"/>
-      <c r="BL2" s="8"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="8"/>
-      <c r="BO2" s="8"/>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="8"/>
-      <c r="BR2" s="8"/>
-      <c r="BS2" s="8"/>
-      <c r="BT2" s="8"/>
-      <c r="BU2" s="8"/>
-      <c r="BV2" s="8"/>
-      <c r="BW2" s="8"/>
-      <c r="BX2" s="8"/>
-      <c r="BY2" s="8"/>
-      <c r="BZ2" s="8"/>
-      <c r="CA2" s="8"/>
-      <c r="CB2" s="8"/>
-      <c r="CC2" s="8"/>
-      <c r="CD2" s="8"/>
-      <c r="CE2" s="8"/>
-      <c r="CF2" s="8"/>
-      <c r="CG2" s="8"/>
-      <c r="CH2" s="8"/>
-      <c r="CI2" s="8"/>
-      <c r="CJ2" s="8"/>
-      <c r="CK2" s="8"/>
-      <c r="CL2" s="8"/>
-      <c r="CM2" s="8"/>
-      <c r="CN2" s="8"/>
-      <c r="CO2" s="8"/>
-      <c r="CP2" s="8"/>
-      <c r="CQ2" s="8"/>
-      <c r="CR2" s="8"/>
-      <c r="CS2" s="8"/>
-      <c r="CT2" s="8"/>
-      <c r="CU2" s="8"/>
-      <c r="CV2" s="8"/>
-      <c r="CW2" s="8"/>
-      <c r="CX2" s="8"/>
-      <c r="CY2" s="8"/>
-      <c r="CZ2" s="8"/>
-      <c r="DA2" s="8"/>
-      <c r="DB2" s="8"/>
-      <c r="DC2" s="8"/>
-      <c r="DD2" s="8"/>
-      <c r="DE2" s="8"/>
-      <c r="DF2" s="8"/>
-      <c r="DG2" s="8"/>
-      <c r="DH2" s="8"/>
-      <c r="DI2" s="8"/>
-      <c r="DJ2" s="8"/>
-      <c r="DK2" s="8"/>
-      <c r="DL2" s="8"/>
-      <c r="DM2" s="8"/>
-      <c r="DN2" s="8"/>
-      <c r="DO2" s="8"/>
-      <c r="DP2" s="8"/>
-      <c r="DQ2" s="8"/>
-      <c r="DR2" s="8"/>
-      <c r="DS2" s="8"/>
-      <c r="DT2" s="8"/>
-      <c r="DU2" s="8"/>
-      <c r="DV2" s="8"/>
-      <c r="DW2" s="8"/>
-      <c r="DX2" s="8"/>
-      <c r="DY2" s="8"/>
-      <c r="DZ2" s="8"/>
-      <c r="EA2" s="8"/>
-      <c r="EB2" s="8"/>
-      <c r="EC2" s="8"/>
-      <c r="ED2" s="8"/>
-      <c r="EE2" s="8"/>
-      <c r="EF2" s="8"/>
-      <c r="EG2" s="8"/>
-      <c r="EH2" s="8"/>
-      <c r="EI2" s="8"/>
-      <c r="EJ2" s="8"/>
-      <c r="EK2" s="8"/>
-      <c r="EL2" s="8"/>
-      <c r="EM2" s="8"/>
-      <c r="EN2" s="8"/>
-      <c r="EO2" s="8"/>
-      <c r="EP2" s="8"/>
-      <c r="EQ2" s="8"/>
-      <c r="ER2" s="8"/>
-      <c r="ES2" s="8"/>
-      <c r="ET2" s="8"/>
-      <c r="EU2" s="8"/>
-      <c r="EV2" s="8"/>
-      <c r="EW2" s="8"/>
-      <c r="EX2" s="8"/>
-      <c r="EY2" s="8"/>
-      <c r="EZ2" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="FA2" s="5"/>
-      <c r="FB2" s="5"/>
-      <c r="FC2" s="5"/>
-      <c r="FD2" s="5"/>
-      <c r="FE2" s="5"/>
-      <c r="FF2" s="5"/>
-      <c r="FG2" s="5"/>
-      <c r="FH2" s="5"/>
-      <c r="FI2" s="5"/>
-      <c r="FJ2" s="5"/>
-      <c r="FK2" s="5"/>
-      <c r="FL2" s="5"/>
-      <c r="FM2" s="5"/>
-      <c r="FN2" s="5"/>
-      <c r="FO2" s="5"/>
-      <c r="FP2" s="5"/>
-      <c r="FQ2" s="5"/>
-      <c r="FR2" s="5"/>
-      <c r="FS2" s="5"/>
-      <c r="FT2" s="5"/>
-      <c r="FU2" s="5"/>
-      <c r="FV2" s="5"/>
-      <c r="FW2" s="5"/>
-      <c r="FX2" s="5"/>
-      <c r="FY2" s="5"/>
-      <c r="FZ2" s="5"/>
-      <c r="GA2" s="5"/>
-      <c r="GB2" s="5"/>
-      <c r="GC2" s="5"/>
-      <c r="GD2" s="5"/>
-      <c r="GE2" s="5"/>
-      <c r="GF2" s="5"/>
-      <c r="GG2" s="5"/>
-      <c r="GH2" s="5"/>
-      <c r="GI2" s="5"/>
-      <c r="GJ2" s="5"/>
-      <c r="GK2" s="5"/>
-      <c r="GL2" s="5"/>
-      <c r="GM2" s="5"/>
-      <c r="GN2" s="5"/>
-      <c r="GO2" s="5"/>
-      <c r="GP2" s="5"/>
-      <c r="GQ2" s="5"/>
-      <c r="GR2" s="5"/>
-      <c r="GS2" s="5"/>
-      <c r="GT2" s="5"/>
-      <c r="GU2" s="5"/>
-      <c r="GV2" s="5"/>
-      <c r="GW2" s="5"/>
-      <c r="GX2" s="5"/>
-      <c r="GY2" s="5"/>
-      <c r="GZ2" s="5"/>
-      <c r="HA2" s="5"/>
-      <c r="HB2" s="5"/>
-      <c r="HC2" s="5"/>
-      <c r="HD2" s="5"/>
-      <c r="HE2" s="5"/>
-      <c r="HF2" s="5"/>
-      <c r="HG2" s="5"/>
-      <c r="HH2" s="5"/>
-      <c r="HI2" s="5"/>
-      <c r="HJ2" s="5"/>
-      <c r="HK2" s="5"/>
-      <c r="HL2" s="5"/>
-      <c r="HM2" s="5"/>
-      <c r="HN2" s="5"/>
-      <c r="HO2" s="5"/>
-      <c r="HP2" s="5"/>
-      <c r="HQ2" s="5"/>
-      <c r="HR2" s="5"/>
-      <c r="HS2" s="5"/>
-      <c r="HT2" s="5"/>
-      <c r="HU2" s="5"/>
-      <c r="HV2" s="5"/>
-      <c r="HW2" s="5"/>
-      <c r="HX2" s="5"/>
-      <c r="HY2" s="5"/>
-      <c r="HZ2" s="5"/>
-      <c r="IA2" s="5"/>
-      <c r="IB2" s="5"/>
-      <c r="IC2" s="5"/>
-      <c r="ID2" s="5"/>
-      <c r="IE2" s="5"/>
-      <c r="IF2" s="5"/>
-      <c r="IG2" s="5"/>
-      <c r="IH2" s="5"/>
-      <c r="II2" s="5"/>
-      <c r="IJ2" s="5"/>
-      <c r="IK2" s="5"/>
-      <c r="IL2" s="5"/>
-      <c r="IM2" s="5"/>
-      <c r="IN2" s="5"/>
-      <c r="IO2" s="5"/>
-      <c r="IP2" s="5"/>
-      <c r="IQ2" s="5"/>
-      <c r="IR2" s="5"/>
-      <c r="IS2" s="5"/>
-      <c r="IT2" s="5"/>
-      <c r="IU2" s="5"/>
-      <c r="IV2" s="5"/>
-      <c r="IW2" s="5"/>
-      <c r="IX2" s="5"/>
-      <c r="IY2" s="5"/>
-      <c r="IZ2" s="5"/>
-      <c r="JA2" s="5"/>
-      <c r="JB2" s="5"/>
-      <c r="JC2" s="5"/>
-      <c r="JD2" s="5"/>
-      <c r="JE2" s="5"/>
-      <c r="JF2" s="5"/>
-      <c r="JG2" s="5"/>
-      <c r="JH2" s="5"/>
-      <c r="JI2" s="5"/>
-      <c r="JJ2" s="5"/>
-      <c r="JK2" s="5"/>
-      <c r="JL2" s="5"/>
-      <c r="JM2" s="5"/>
-      <c r="JN2" s="5"/>
-      <c r="JO2" s="5"/>
-      <c r="JP2" s="5"/>
-      <c r="JQ2" s="5"/>
-      <c r="JR2" s="5"/>
-      <c r="JS2" s="5"/>
-      <c r="JT2" s="5"/>
-      <c r="JU2" s="5"/>
-      <c r="JV2" s="5"/>
-      <c r="JW2" s="5"/>
-      <c r="JX2" s="5"/>
-      <c r="JY2" s="5"/>
-      <c r="JZ2" s="5"/>
-      <c r="KA2" s="5"/>
-      <c r="KB2" s="5"/>
-      <c r="KC2" s="5"/>
-      <c r="KD2" s="5"/>
-      <c r="KE2" s="5"/>
-      <c r="KF2" s="5"/>
-      <c r="KG2" s="5"/>
-      <c r="KH2" s="5"/>
-      <c r="KI2" s="5"/>
-      <c r="KJ2" s="5"/>
-      <c r="KK2" s="5"/>
-      <c r="KL2" s="5"/>
-      <c r="KM2" s="5"/>
-      <c r="KN2" s="5"/>
-      <c r="KO2" s="5"/>
-      <c r="KP2" s="5"/>
-      <c r="KQ2" s="5"/>
-      <c r="KR2" s="5"/>
-      <c r="KS2" s="5"/>
-      <c r="KT2" s="5"/>
-      <c r="KU2" s="5"/>
-      <c r="KV2" s="5"/>
-      <c r="KW2" s="5"/>
-      <c r="KX2" s="5"/>
-      <c r="KY2" s="5"/>
-      <c r="KZ2" s="5"/>
-      <c r="LA2" s="5"/>
-      <c r="LB2" s="5"/>
-      <c r="LC2" s="5"/>
-      <c r="LD2" s="5"/>
-      <c r="LE2" s="5"/>
-      <c r="LF2" s="5"/>
-      <c r="LG2" s="5"/>
-      <c r="LH2" s="5"/>
-      <c r="LI2" s="5"/>
-      <c r="LJ2" s="5"/>
-      <c r="LK2" s="5"/>
-      <c r="LL2" s="5"/>
-      <c r="LM2" s="5"/>
-    </row>
-    <row r="3" spans="1:327" x14ac:dyDescent="0.25">
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="7"/>
+      <c r="AZ2" s="7"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="7"/>
+      <c r="BK2" s="7"/>
+      <c r="BL2" s="7"/>
+      <c r="BM2" s="7"/>
+      <c r="BN2" s="7"/>
+      <c r="BO2" s="7"/>
+      <c r="BP2" s="7"/>
+      <c r="BQ2" s="7"/>
+      <c r="BR2" s="7"/>
+      <c r="BS2" s="7"/>
+      <c r="BT2" s="7"/>
+      <c r="BU2" s="7"/>
+      <c r="BV2" s="7"/>
+      <c r="BW2" s="7"/>
+      <c r="BX2" s="7"/>
+      <c r="BY2" s="7"/>
+      <c r="BZ2" s="7"/>
+      <c r="CA2" s="7"/>
+      <c r="CB2" s="7"/>
+      <c r="CC2" s="7"/>
+      <c r="CD2" s="7"/>
+      <c r="CE2" s="7"/>
+      <c r="CF2" s="7"/>
+      <c r="CG2" s="7"/>
+      <c r="CH2" s="7"/>
+      <c r="CI2" s="7"/>
+      <c r="CJ2" s="7"/>
+      <c r="CK2" s="7"/>
+      <c r="CL2" s="7"/>
+      <c r="CM2" s="7"/>
+      <c r="CN2" s="7"/>
+      <c r="CO2" s="7"/>
+      <c r="CP2" s="7"/>
+      <c r="CQ2" s="7"/>
+      <c r="CR2" s="7"/>
+      <c r="CS2" s="7"/>
+      <c r="CT2" s="7"/>
+      <c r="CU2" s="7"/>
+      <c r="CV2" s="7"/>
+      <c r="CW2" s="7"/>
+      <c r="CX2" s="7"/>
+      <c r="CY2" s="7"/>
+      <c r="CZ2" s="7"/>
+      <c r="DA2" s="7"/>
+      <c r="DB2" s="7"/>
+      <c r="DC2" s="7"/>
+      <c r="DD2" s="7"/>
+      <c r="DE2" s="7"/>
+      <c r="DF2" s="7"/>
+      <c r="DG2" s="7"/>
+      <c r="DH2" s="7"/>
+      <c r="DI2" s="7"/>
+      <c r="DJ2" s="7"/>
+      <c r="DK2" s="7"/>
+      <c r="DL2" s="7"/>
+      <c r="DM2" s="7"/>
+      <c r="DN2" s="7"/>
+      <c r="DO2" s="7"/>
+      <c r="DP2" s="7"/>
+      <c r="DQ2" s="7"/>
+      <c r="DR2" s="7"/>
+      <c r="DS2" s="7"/>
+      <c r="DT2" s="7"/>
+      <c r="DU2" s="7"/>
+      <c r="DV2" s="7"/>
+      <c r="DW2" s="7"/>
+      <c r="DX2" s="7"/>
+      <c r="DY2" s="7"/>
+      <c r="DZ2" s="7"/>
+      <c r="EA2" s="7"/>
+      <c r="EB2" s="7"/>
+      <c r="EC2" s="7"/>
+      <c r="ED2" s="7"/>
+      <c r="EE2" s="7"/>
+      <c r="EF2" s="7"/>
+      <c r="EG2" s="7"/>
+      <c r="EH2" s="7"/>
+      <c r="EI2" s="7"/>
+      <c r="EJ2" s="7"/>
+      <c r="EK2" s="7"/>
+      <c r="EL2" s="7"/>
+      <c r="EM2" s="7"/>
+      <c r="EN2" s="7"/>
+      <c r="EO2" s="7"/>
+      <c r="EP2" s="7"/>
+      <c r="EQ2" s="7"/>
+      <c r="ER2" s="7"/>
+      <c r="ES2" s="7"/>
+      <c r="ET2" s="7"/>
+      <c r="EU2" s="7"/>
+      <c r="EV2" s="7"/>
+      <c r="EW2" s="7"/>
+      <c r="EX2" s="7"/>
+      <c r="EY2" s="7"/>
+      <c r="EZ2" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="FA2" s="10"/>
+      <c r="FB2" s="10"/>
+      <c r="FC2" s="10"/>
+      <c r="FD2" s="10"/>
+      <c r="FE2" s="10"/>
+      <c r="FF2" s="10"/>
+      <c r="FG2" s="10"/>
+      <c r="FH2" s="10"/>
+      <c r="FI2" s="10"/>
+      <c r="FJ2" s="10"/>
+      <c r="FK2" s="10"/>
+      <c r="FL2" s="10"/>
+      <c r="FM2" s="10"/>
+      <c r="FN2" s="10"/>
+      <c r="FO2" s="10"/>
+      <c r="FP2" s="10"/>
+      <c r="FQ2" s="10"/>
+      <c r="FR2" s="10"/>
+      <c r="FS2" s="10"/>
+      <c r="FT2" s="10"/>
+      <c r="FU2" s="10"/>
+      <c r="FV2" s="10"/>
+      <c r="FW2" s="10"/>
+      <c r="FX2" s="10"/>
+      <c r="FY2" s="10"/>
+      <c r="FZ2" s="10"/>
+      <c r="GA2" s="10"/>
+      <c r="GB2" s="10"/>
+      <c r="GC2" s="10"/>
+      <c r="GD2" s="10"/>
+      <c r="GE2" s="10"/>
+      <c r="GF2" s="10"/>
+      <c r="GG2" s="10"/>
+      <c r="GH2" s="10"/>
+      <c r="GI2" s="10"/>
+      <c r="GJ2" s="10"/>
+      <c r="GK2" s="10"/>
+      <c r="GL2" s="10"/>
+      <c r="GM2" s="10"/>
+      <c r="GN2" s="10"/>
+      <c r="GO2" s="10"/>
+      <c r="GP2" s="10"/>
+      <c r="GQ2" s="10"/>
+      <c r="GR2" s="10"/>
+      <c r="GS2" s="10"/>
+      <c r="GT2" s="10"/>
+      <c r="GU2" s="10"/>
+      <c r="GV2" s="10"/>
+      <c r="GW2" s="10"/>
+      <c r="GX2" s="10"/>
+      <c r="GY2" s="10"/>
+      <c r="GZ2" s="10"/>
+      <c r="HA2" s="10"/>
+      <c r="HB2" s="10"/>
+      <c r="HC2" s="10"/>
+      <c r="HD2" s="10"/>
+      <c r="HE2" s="10"/>
+      <c r="HF2" s="10"/>
+      <c r="HG2" s="10"/>
+      <c r="HH2" s="10"/>
+      <c r="HI2" s="10"/>
+      <c r="HJ2" s="10"/>
+      <c r="HK2" s="10"/>
+      <c r="HL2" s="10"/>
+      <c r="HM2" s="10"/>
+      <c r="HN2" s="10"/>
+      <c r="HO2" s="10"/>
+      <c r="HP2" s="10"/>
+      <c r="HQ2" s="10"/>
+      <c r="HR2" s="10"/>
+      <c r="HS2" s="10"/>
+      <c r="HT2" s="10"/>
+      <c r="HU2" s="10"/>
+      <c r="HV2" s="10"/>
+      <c r="HW2" s="10"/>
+      <c r="HX2" s="10"/>
+      <c r="HY2" s="10"/>
+      <c r="HZ2" s="10"/>
+      <c r="IA2" s="10"/>
+      <c r="IB2" s="10"/>
+      <c r="IC2" s="10"/>
+      <c r="ID2" s="10"/>
+      <c r="IE2" s="10"/>
+      <c r="IF2" s="10"/>
+      <c r="IG2" s="10"/>
+      <c r="IH2" s="10"/>
+      <c r="II2" s="10"/>
+      <c r="IJ2" s="10"/>
+      <c r="IK2" s="10"/>
+      <c r="IL2" s="10"/>
+      <c r="IM2" s="10"/>
+      <c r="IN2" s="10"/>
+      <c r="IO2" s="10"/>
+      <c r="IP2" s="10"/>
+      <c r="IQ2" s="10"/>
+      <c r="IR2" s="10"/>
+      <c r="IS2" s="10"/>
+      <c r="IT2" s="10"/>
+      <c r="IU2" s="10"/>
+      <c r="IV2" s="10"/>
+      <c r="IW2" s="10"/>
+      <c r="IX2" s="10"/>
+      <c r="IY2" s="10"/>
+      <c r="IZ2" s="10"/>
+      <c r="JA2" s="10"/>
+      <c r="JB2" s="10"/>
+      <c r="JC2" s="10"/>
+      <c r="JD2" s="10"/>
+      <c r="JE2" s="10"/>
+      <c r="JF2" s="10"/>
+      <c r="JG2" s="10"/>
+      <c r="JH2" s="10"/>
+      <c r="JI2" s="10"/>
+      <c r="JJ2" s="10"/>
+      <c r="JK2" s="10"/>
+      <c r="JL2" s="10"/>
+      <c r="JM2" s="10"/>
+      <c r="JN2" s="10"/>
+      <c r="JO2" s="10"/>
+      <c r="JP2" s="10"/>
+      <c r="JQ2" s="10"/>
+      <c r="JR2" s="10"/>
+      <c r="JS2" s="10"/>
+      <c r="JT2" s="10"/>
+      <c r="JU2" s="10"/>
+      <c r="JV2" s="10"/>
+      <c r="JW2" s="10"/>
+      <c r="JX2" s="10"/>
+      <c r="JY2" s="10"/>
+      <c r="JZ2" s="10"/>
+      <c r="KA2" s="10"/>
+      <c r="KB2" s="10"/>
+      <c r="KC2" s="10"/>
+      <c r="KD2" s="10"/>
+      <c r="KE2" s="10"/>
+      <c r="KF2" s="10"/>
+      <c r="KG2" s="10"/>
+      <c r="KH2" s="10"/>
+      <c r="KI2" s="10"/>
+      <c r="KJ2" s="10"/>
+      <c r="KK2" s="10"/>
+      <c r="KL2" s="10"/>
+      <c r="KM2" s="10"/>
+      <c r="KN2" s="10"/>
+      <c r="KO2" s="10"/>
+      <c r="KP2" s="10"/>
+      <c r="KQ2" s="10"/>
+      <c r="KR2" s="10"/>
+      <c r="KS2" s="10"/>
+      <c r="KT2" s="10"/>
+      <c r="KU2" s="10"/>
+      <c r="KV2" s="10"/>
+      <c r="KW2" s="10"/>
+      <c r="KX2" s="10"/>
+      <c r="KY2" s="10"/>
+      <c r="KZ2" s="10"/>
+      <c r="LA2" s="10"/>
+      <c r="LB2" s="10"/>
+      <c r="LC2" s="10"/>
+      <c r="LD2" s="10"/>
+      <c r="LE2" s="10"/>
+      <c r="LF2" s="10"/>
+      <c r="LG2" s="10"/>
+      <c r="LH2" s="10"/>
+      <c r="LI2" s="10"/>
+      <c r="LJ2" s="10"/>
+      <c r="LK2" s="10"/>
+      <c r="LL2" s="10"/>
+      <c r="LM2" s="10"/>
+      <c r="LN2" s="11"/>
+      <c r="LO2" s="11"/>
+      <c r="LP2" s="11"/>
+    </row>
+    <row r="3" spans="1:328" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-      <c r="BK3" s="2"/>
-      <c r="BL3" s="2"/>
-      <c r="BM3" s="2"/>
-      <c r="BN3" s="2"/>
-      <c r="BO3" s="2"/>
-      <c r="BP3" s="2"/>
-      <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
-      <c r="BS3" s="2"/>
-      <c r="BT3" s="2"/>
-      <c r="BU3" s="2"/>
-      <c r="BV3" s="2"/>
-      <c r="BW3" s="2"/>
-      <c r="BX3" s="2"/>
-      <c r="BY3" s="2"/>
-      <c r="BZ3" s="2"/>
-      <c r="CA3" s="2"/>
-      <c r="CB3" s="2"/>
-      <c r="CC3" s="2"/>
-      <c r="CD3" s="2"/>
-      <c r="CE3" s="2"/>
-      <c r="CF3" s="2"/>
-      <c r="CG3" s="2"/>
-      <c r="CH3" s="2"/>
-      <c r="CI3" s="2"/>
-      <c r="CJ3" s="2"/>
-      <c r="CK3" s="2"/>
-      <c r="CL3" s="2"/>
-      <c r="CM3" s="2"/>
-      <c r="CN3" s="2"/>
-      <c r="CO3" s="2"/>
-      <c r="CP3" s="2"/>
-      <c r="CQ3" s="2"/>
-      <c r="CR3" s="2"/>
-      <c r="CS3" s="2"/>
-      <c r="CT3" s="2"/>
-      <c r="CU3" s="2"/>
-      <c r="CV3" s="2"/>
-      <c r="CW3" s="2"/>
-      <c r="CX3" s="2"/>
-      <c r="CY3" s="2"/>
-      <c r="CZ3" s="2"/>
-      <c r="DA3" s="2"/>
-      <c r="DB3" s="2"/>
-      <c r="DC3" s="2"/>
-      <c r="DD3" s="2"/>
-      <c r="DE3" s="2"/>
-      <c r="DF3" s="2"/>
-      <c r="DG3" s="2"/>
-      <c r="DH3" s="2"/>
-      <c r="DI3" s="2"/>
-      <c r="DJ3" s="2"/>
-      <c r="DK3" s="2"/>
-      <c r="DL3" s="2"/>
-      <c r="DM3" s="2"/>
-      <c r="DN3" s="2"/>
-      <c r="DO3" s="2"/>
-      <c r="DP3" s="2"/>
-      <c r="DQ3" s="2"/>
-      <c r="DR3" s="2"/>
-      <c r="DS3" s="2"/>
-      <c r="DT3" s="2"/>
-      <c r="DU3" s="2"/>
-      <c r="DV3" s="2"/>
-      <c r="DW3" s="2"/>
-      <c r="DX3" s="2"/>
-      <c r="DY3" s="2"/>
-      <c r="DZ3" s="2"/>
-      <c r="EA3" s="2"/>
-      <c r="EB3" s="2"/>
-      <c r="EC3" s="2"/>
-      <c r="ED3" s="2"/>
-      <c r="EE3" s="2"/>
-      <c r="EF3" s="2"/>
-      <c r="EG3" s="2"/>
-      <c r="EH3" s="2"/>
-      <c r="EI3" s="2"/>
-      <c r="EJ3" s="2"/>
-      <c r="EK3" s="2"/>
-      <c r="EL3" s="2"/>
-      <c r="EM3" s="2"/>
-      <c r="EN3" s="2"/>
-      <c r="EO3" s="2"/>
-      <c r="EP3" s="2"/>
-      <c r="EQ3" s="2"/>
-      <c r="ER3" s="2"/>
-      <c r="ES3" s="2"/>
-      <c r="ET3" s="2"/>
-      <c r="EU3" s="2"/>
-      <c r="EV3" s="2"/>
-      <c r="EW3" s="2"/>
-      <c r="EX3" s="2"/>
-      <c r="EY3" s="2"/>
-      <c r="HZ3" t="s">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BO3" s="1"/>
+      <c r="BP3" s="1"/>
+      <c r="BQ3" s="1"/>
+      <c r="BR3" s="1"/>
+      <c r="BS3" s="1"/>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+      <c r="BV3" s="1"/>
+      <c r="BW3" s="1"/>
+      <c r="BX3" s="1"/>
+      <c r="BY3" s="1"/>
+      <c r="CD3" s="1"/>
+      <c r="CE3" s="1"/>
+      <c r="CF3" s="1"/>
+      <c r="CG3" s="1"/>
+      <c r="CH3" s="1"/>
+      <c r="CI3" s="1"/>
+      <c r="CJ3" s="1"/>
+      <c r="CK3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CM3" s="1"/>
+      <c r="CN3" s="1"/>
+      <c r="CO3" s="1"/>
+      <c r="CP3" s="1"/>
+      <c r="CQ3" s="1"/>
+      <c r="CR3" s="1"/>
+      <c r="CS3" s="1"/>
+      <c r="CT3" s="1"/>
+      <c r="CU3" s="1"/>
+      <c r="CV3" s="1"/>
+      <c r="CW3" s="1"/>
+      <c r="CX3" s="1"/>
+      <c r="CY3" s="1"/>
+      <c r="CZ3" s="1"/>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1"/>
+      <c r="DC3" s="1"/>
+      <c r="DD3" s="1"/>
+      <c r="DE3" s="1"/>
+      <c r="DF3" s="1"/>
+      <c r="DG3" s="1"/>
+      <c r="DH3" s="1"/>
+      <c r="DI3" s="1"/>
+      <c r="DJ3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="DL3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="DM3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="DN3" s="1"/>
+      <c r="DO3" s="1"/>
+      <c r="DP3" s="1"/>
+      <c r="DQ3" s="1"/>
+      <c r="DR3" s="1"/>
+      <c r="DS3" s="1"/>
+      <c r="DT3" s="1"/>
+      <c r="DU3" s="1"/>
+      <c r="DV3" s="1"/>
+      <c r="DW3" s="1"/>
+      <c r="DX3" s="1"/>
+      <c r="DY3" s="1"/>
+      <c r="DZ3" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="EA3" s="1"/>
+      <c r="EB3" s="1"/>
+      <c r="EC3" s="1"/>
+      <c r="ED3" s="1"/>
+      <c r="EE3" s="1"/>
+      <c r="EF3" s="1"/>
+      <c r="EG3" s="1"/>
+      <c r="EH3" s="1"/>
+      <c r="EI3" s="1"/>
+      <c r="EJ3" s="1"/>
+      <c r="EK3" s="1"/>
+      <c r="EL3" s="1"/>
+      <c r="EM3" s="1"/>
+      <c r="EN3" s="1"/>
+      <c r="EO3" s="1"/>
+      <c r="EP3" s="1"/>
+      <c r="EQ3" s="1"/>
+      <c r="ER3" s="1"/>
+      <c r="ES3" s="1"/>
+      <c r="ET3" s="1"/>
+      <c r="EU3" s="1"/>
+      <c r="EV3" s="1"/>
+      <c r="EW3" s="1"/>
+      <c r="EX3" s="1"/>
+      <c r="EY3" s="1"/>
+      <c r="EZ3" s="1"/>
+      <c r="FA3" s="1"/>
+      <c r="FB3" s="1"/>
+      <c r="HN3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>339</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>339</v>
+      </c>
+      <c r="IC3" t="s">
+        <v>334</v>
+      </c>
+      <c r="II3" t="s">
+        <v>336</v>
+      </c>
+      <c r="IJ3" t="s">
         <v>338</v>
       </c>
-      <c r="IF3" t="s">
+      <c r="IK3" t="s">
         <v>337</v>
       </c>
-      <c r="IT3" t="s">
-        <v>338</v>
-      </c>
-      <c r="IU3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:327" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>325</v>
+      <c r="IL3" t="s">
+        <v>335</v>
+      </c>
+      <c r="IW3" t="s">
+        <v>334</v>
+      </c>
+      <c r="IX3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:328" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2423,13 +2547,13 @@
         <v>25</v>
       </c>
       <c r="V4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="W4" t="s">
+        <v>328</v>
+      </c>
+      <c r="X4" t="s">
         <v>330</v>
-      </c>
-      <c r="X4" t="s">
-        <v>332</v>
       </c>
       <c r="Y4" t="s">
         <v>26</v>
@@ -2591,1023 +2715,1119 @@
         <v>77</v>
       </c>
       <c r="BZ4" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="CA4" t="s">
+        <v>343</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>344</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>345</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>332</v>
+      </c>
+      <c r="CE4" t="s">
         <v>78</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CF4" t="s">
         <v>79</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CG4" t="s">
         <v>80</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CH4" t="s">
         <v>81</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CI4" t="s">
         <v>82</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CJ4" t="s">
         <v>83</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CK4" t="s">
         <v>84</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CL4" t="s">
         <v>85</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CM4" t="s">
         <v>86</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CN4" t="s">
         <v>86</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CO4" t="s">
         <v>87</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CP4" t="s">
         <v>88</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CQ4" t="s">
         <v>89</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CR4" t="s">
         <v>90</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CS4" t="s">
         <v>91</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CT4" t="s">
         <v>92</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CU4" t="s">
         <v>93</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CV4" t="s">
         <v>93</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CW4" t="s">
         <v>94</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CX4" t="s">
         <v>95</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="CY4" t="s">
         <v>96</v>
       </c>
-      <c r="CV4" t="s">
+      <c r="CZ4" t="s">
         <v>97</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="DA4" t="s">
         <v>98</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="DB4" t="s">
         <v>99</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="DC4" t="s">
         <v>100</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DD4" t="s">
         <v>101</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DE4" t="s">
         <v>102</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DF4" t="s">
         <v>103</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DG4" t="s">
         <v>104</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DH4" t="s">
         <v>105</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DI4" t="s">
         <v>106</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DJ4" t="s">
         <v>107</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DK4" t="s">
         <v>108</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DL4" t="s">
         <v>109</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DM4" t="s">
         <v>110</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DN4" t="s">
         <v>111</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DO4" t="s">
         <v>112</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DP4" t="s">
         <v>113</v>
       </c>
-      <c r="DM4" t="s">
+      <c r="DQ4" t="s">
         <v>114</v>
       </c>
-      <c r="DN4" t="s">
+      <c r="DR4" t="s">
         <v>115</v>
       </c>
-      <c r="DO4" t="s">
+      <c r="DS4" t="s">
         <v>116</v>
       </c>
-      <c r="DP4" t="s">
+      <c r="DT4" t="s">
         <v>117</v>
       </c>
-      <c r="DQ4" t="s">
+      <c r="DU4" t="s">
         <v>118</v>
       </c>
-      <c r="DR4" t="s">
+      <c r="DV4" t="s">
         <v>119</v>
       </c>
-      <c r="DS4" t="s">
+      <c r="DW4" t="s">
         <v>120</v>
       </c>
-      <c r="DT4" t="s">
+      <c r="DX4" t="s">
         <v>121</v>
       </c>
-      <c r="DU4" t="s">
+      <c r="DY4" t="s">
         <v>122</v>
       </c>
-      <c r="DV4" t="s">
+      <c r="DZ4" t="s">
+        <v>124</v>
+      </c>
+      <c r="EA4" t="s">
         <v>123</v>
       </c>
-      <c r="DW4" t="s">
+      <c r="EB4" t="s">
         <v>125</v>
       </c>
-      <c r="DX4" t="s">
-        <v>124</v>
-      </c>
-      <c r="DY4" t="s">
+      <c r="EC4" t="s">
         <v>126</v>
       </c>
-      <c r="DZ4" t="s">
+      <c r="ED4" t="s">
         <v>127</v>
       </c>
-      <c r="EA4" t="s">
+      <c r="EE4" t="s">
         <v>128</v>
       </c>
-      <c r="EB4" t="s">
+      <c r="EF4" t="s">
         <v>129</v>
       </c>
-      <c r="EC4" t="s">
+      <c r="EG4" t="s">
         <v>130</v>
       </c>
-      <c r="ED4" t="s">
+      <c r="EH4" t="s">
         <v>131</v>
       </c>
-      <c r="EE4" t="s">
+      <c r="EI4" t="s">
         <v>132</v>
       </c>
-      <c r="EF4" t="s">
+      <c r="EJ4" t="s">
         <v>133</v>
       </c>
-      <c r="EG4" t="s">
+      <c r="EK4" t="s">
         <v>134</v>
       </c>
-      <c r="EH4" t="s">
+      <c r="EL4" t="s">
         <v>135</v>
       </c>
-      <c r="EI4" t="s">
+      <c r="EM4" t="s">
         <v>136</v>
       </c>
-      <c r="EJ4" t="s">
+      <c r="EN4" t="s">
         <v>137</v>
       </c>
-      <c r="EK4" t="s">
+      <c r="EO4" t="s">
         <v>138</v>
       </c>
-      <c r="EL4" t="s">
+      <c r="EP4" t="s">
         <v>139</v>
       </c>
-      <c r="EM4" t="s">
+      <c r="EQ4" t="s">
         <v>140</v>
       </c>
-      <c r="EN4" t="s">
+      <c r="ER4" t="s">
         <v>141</v>
       </c>
-      <c r="EO4" t="s">
+      <c r="ES4" t="s">
         <v>142</v>
       </c>
-      <c r="EP4" t="s">
+      <c r="ET4" t="s">
         <v>143</v>
       </c>
-      <c r="EQ4" t="s">
+      <c r="EU4" t="s">
         <v>144</v>
       </c>
-      <c r="ER4" t="s">
+      <c r="EV4" t="s">
         <v>145</v>
       </c>
-      <c r="ES4" t="s">
+      <c r="EW4" t="s">
         <v>146</v>
       </c>
-      <c r="ET4" t="s">
+      <c r="EX4" t="s">
         <v>147</v>
       </c>
-      <c r="EU4" t="s">
+      <c r="EY4" t="s">
         <v>148</v>
       </c>
-      <c r="EV4" t="s">
+      <c r="EZ4" t="s">
         <v>149</v>
       </c>
-      <c r="EW4" t="s">
+      <c r="FA4" t="s">
         <v>150</v>
       </c>
-      <c r="EX4" t="s">
+      <c r="FB4" t="s">
         <v>151</v>
       </c>
-      <c r="EY4" t="s">
+      <c r="FC4" t="s">
         <v>152</v>
       </c>
-      <c r="EZ4" t="s">
+      <c r="FD4" t="s">
         <v>153</v>
       </c>
-      <c r="FA4" t="s">
+      <c r="FE4" t="s">
         <v>154</v>
       </c>
-      <c r="FB4" t="s">
+      <c r="FF4" t="s">
         <v>155</v>
       </c>
-      <c r="FC4" t="s">
+      <c r="FG4" t="s">
         <v>156</v>
       </c>
-      <c r="FD4" t="s">
+      <c r="FH4" t="s">
         <v>157</v>
       </c>
-      <c r="FE4" t="s">
+      <c r="FI4" t="s">
         <v>158</v>
       </c>
-      <c r="FF4" t="s">
+      <c r="FJ4" t="s">
         <v>159</v>
       </c>
-      <c r="FG4" t="s">
+      <c r="FK4" t="s">
         <v>160</v>
       </c>
-      <c r="FH4" t="s">
+      <c r="FL4" t="s">
         <v>161</v>
       </c>
-      <c r="FI4" t="s">
+      <c r="FM4" t="s">
         <v>162</v>
       </c>
-      <c r="FJ4" t="s">
+      <c r="FN4" t="s">
         <v>163</v>
       </c>
-      <c r="FK4" t="s">
+      <c r="FO4" t="s">
         <v>164</v>
       </c>
-      <c r="FL4" t="s">
+      <c r="FP4" t="s">
         <v>165</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FQ4" t="s">
         <v>166</v>
       </c>
-      <c r="FN4" t="s">
+      <c r="FR4" t="s">
         <v>167</v>
       </c>
-      <c r="FO4" t="s">
+      <c r="FS4" t="s">
         <v>168</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FT4" t="s">
         <v>169</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FU4" t="s">
         <v>170</v>
       </c>
-      <c r="FR4" t="s">
+      <c r="FV4" t="s">
         <v>171</v>
       </c>
-      <c r="FS4" t="s">
+      <c r="FW4" t="s">
         <v>172</v>
       </c>
-      <c r="FT4" t="s">
+      <c r="FX4" t="s">
         <v>173</v>
       </c>
-      <c r="FU4" t="s">
+      <c r="FY4" t="s">
         <v>174</v>
       </c>
-      <c r="FV4" t="s">
+      <c r="FZ4" t="s">
         <v>175</v>
       </c>
-      <c r="FW4" t="s">
+      <c r="GA4" t="s">
         <v>176</v>
       </c>
-      <c r="FX4" t="s">
+      <c r="GB4" t="s">
         <v>177</v>
       </c>
-      <c r="FY4" t="s">
+      <c r="GC4" t="s">
         <v>178</v>
       </c>
-      <c r="FZ4" t="s">
+      <c r="GD4" t="s">
         <v>179</v>
       </c>
-      <c r="GA4" t="s">
+      <c r="GE4" t="s">
         <v>180</v>
       </c>
-      <c r="GB4" t="s">
+      <c r="GF4" t="s">
         <v>181</v>
       </c>
-      <c r="GC4" t="s">
+      <c r="GG4" t="s">
         <v>182</v>
       </c>
-      <c r="GD4" t="s">
+      <c r="GH4" t="s">
         <v>183</v>
       </c>
-      <c r="GE4" t="s">
+      <c r="GI4" t="s">
         <v>184</v>
       </c>
-      <c r="GF4" t="s">
+      <c r="GJ4" t="s">
         <v>185</v>
       </c>
-      <c r="GG4" t="s">
+      <c r="GK4" t="s">
         <v>186</v>
       </c>
-      <c r="GH4" t="s">
+      <c r="GL4" t="s">
         <v>187</v>
       </c>
-      <c r="GI4" t="s">
+      <c r="GM4" t="s">
         <v>188</v>
       </c>
-      <c r="GJ4" t="s">
+      <c r="GN4" t="s">
         <v>189</v>
       </c>
-      <c r="GK4" t="s">
+      <c r="GO4" t="s">
         <v>190</v>
       </c>
-      <c r="GL4" t="s">
+      <c r="GP4" t="s">
         <v>191</v>
       </c>
-      <c r="GM4" t="s">
+      <c r="GQ4" t="s">
         <v>192</v>
       </c>
-      <c r="GN4" t="s">
+      <c r="GR4" t="s">
         <v>193</v>
       </c>
-      <c r="GO4" t="s">
+      <c r="GS4" t="s">
         <v>194</v>
       </c>
-      <c r="GP4" t="s">
+      <c r="GT4" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="GQ4" s="3" t="s">
+      <c r="GU4" t="s">
         <v>196</v>
       </c>
-      <c r="GR4" t="s">
+      <c r="GV4" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="GS4" s="3" t="s">
+      <c r="GW4" t="s">
         <v>198</v>
       </c>
-      <c r="GT4" t="s">
+      <c r="GX4" t="s">
         <v>199</v>
       </c>
-      <c r="GU4" t="s">
+      <c r="GY4" t="s">
         <v>200</v>
       </c>
-      <c r="GV4" t="s">
+      <c r="GZ4" t="s">
         <v>201</v>
       </c>
-      <c r="GW4" t="s">
+      <c r="HA4" t="s">
         <v>202</v>
       </c>
-      <c r="GX4" t="s">
+      <c r="HB4" t="s">
         <v>203</v>
       </c>
-      <c r="GY4" t="s">
+      <c r="HC4" t="s">
         <v>204</v>
       </c>
-      <c r="GZ4" t="s">
+      <c r="HD4" t="s">
         <v>205</v>
       </c>
-      <c r="HA4" t="s">
+      <c r="HE4" t="s">
         <v>206</v>
       </c>
-      <c r="HB4" t="s">
+      <c r="HF4" t="s">
         <v>207</v>
       </c>
-      <c r="HC4" t="s">
+      <c r="HG4" t="s">
         <v>208</v>
       </c>
-      <c r="HD4" t="s">
+      <c r="HH4" t="s">
         <v>209</v>
       </c>
-      <c r="HE4" t="s">
+      <c r="HI4" t="s">
         <v>210</v>
       </c>
-      <c r="HF4" t="s">
+      <c r="HJ4" t="s">
         <v>211</v>
       </c>
-      <c r="HG4" t="s">
+      <c r="HK4" t="s">
         <v>212</v>
       </c>
-      <c r="HH4" t="s">
+      <c r="HL4" t="s">
         <v>213</v>
       </c>
-      <c r="HI4" t="s">
+      <c r="HM4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="HJ4" s="3" t="s">
+      <c r="HN4" t="s">
         <v>215</v>
       </c>
-      <c r="HK4" t="s">
+      <c r="HO4" t="s">
         <v>216</v>
       </c>
-      <c r="HL4" t="s">
+      <c r="HP4" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="HM4" s="3" t="s">
+      <c r="HQ4" t="s">
         <v>218</v>
       </c>
-      <c r="HN4" t="s">
+      <c r="HR4" t="s">
         <v>219</v>
       </c>
-      <c r="HO4" t="s">
+      <c r="HS4" t="s">
         <v>220</v>
       </c>
-      <c r="HP4" t="s">
+      <c r="HT4" t="s">
         <v>221</v>
       </c>
-      <c r="HQ4" t="s">
+      <c r="HU4" t="s">
         <v>222</v>
       </c>
-      <c r="HR4" t="s">
+      <c r="HV4" t="s">
         <v>223</v>
       </c>
-      <c r="HS4" t="s">
+      <c r="HW4" t="s">
         <v>224</v>
       </c>
-      <c r="HT4" t="s">
+      <c r="HX4" t="s">
         <v>225</v>
       </c>
-      <c r="HU4" t="s">
+      <c r="HY4" t="s">
         <v>226</v>
       </c>
-      <c r="HV4" t="s">
+      <c r="HZ4" t="s">
         <v>227</v>
       </c>
-      <c r="HW4" t="s">
+      <c r="IA4" t="s">
         <v>228</v>
       </c>
-      <c r="HX4" t="s">
+      <c r="IB4" t="s">
         <v>229</v>
       </c>
-      <c r="HY4" t="s">
+      <c r="IC4" t="s">
+        <v>340</v>
+      </c>
+      <c r="ID4" t="s">
         <v>230</v>
       </c>
-      <c r="HZ4" t="s">
+      <c r="IE4" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="IA4" t="s">
+      <c r="IF4" t="s">
         <v>232</v>
       </c>
-      <c r="IB4" s="3" t="s">
+      <c r="IG4" t="s">
         <v>233</v>
       </c>
-      <c r="IC4" t="s">
+      <c r="IH4" t="s">
         <v>234</v>
       </c>
-      <c r="ID4" t="s">
+      <c r="II4" t="s">
         <v>235</v>
       </c>
-      <c r="IE4" t="s">
+      <c r="IJ4" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="IF4" t="s">
+      <c r="IK4" t="s">
         <v>237</v>
       </c>
-      <c r="IG4" s="3" t="s">
+      <c r="IL4" t="s">
         <v>238</v>
       </c>
-      <c r="IH4" t="s">
+      <c r="IM4" t="s">
         <v>239</v>
       </c>
-      <c r="II4" t="s">
+      <c r="IN4" t="s">
         <v>240</v>
       </c>
-      <c r="IJ4" t="s">
+      <c r="IO4" t="s">
         <v>241</v>
       </c>
-      <c r="IK4" t="s">
+      <c r="IP4" t="s">
         <v>242</v>
       </c>
-      <c r="IL4" t="s">
+      <c r="IQ4" t="s">
         <v>243</v>
       </c>
-      <c r="IM4" t="s">
+      <c r="IR4" t="s">
         <v>244</v>
       </c>
-      <c r="IN4" t="s">
+      <c r="IS4" t="s">
         <v>245</v>
       </c>
-      <c r="IO4" t="s">
+      <c r="IT4" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="IP4" t="s">
+      <c r="IU4" t="s">
         <v>247</v>
       </c>
-      <c r="IQ4" s="3" t="s">
+      <c r="IV4" t="s">
         <v>248</v>
       </c>
-      <c r="IR4" t="s">
+      <c r="IW4" t="s">
         <v>249</v>
       </c>
-      <c r="IS4" t="s">
+      <c r="IX4" t="s">
         <v>250</v>
       </c>
-      <c r="IT4" t="s">
+      <c r="IY4" t="s">
         <v>251</v>
       </c>
-      <c r="IU4" t="s">
+      <c r="IZ4" t="s">
         <v>252</v>
       </c>
-      <c r="IV4" t="s">
+      <c r="JA4" t="s">
         <v>253</v>
       </c>
-      <c r="IW4" t="s">
+      <c r="JB4" t="s">
         <v>254</v>
       </c>
-      <c r="IX4" t="s">
+      <c r="JC4" t="s">
         <v>255</v>
       </c>
-      <c r="IY4" t="s">
+      <c r="JD4" t="s">
         <v>256</v>
       </c>
-      <c r="IZ4" t="s">
+      <c r="JE4" t="s">
         <v>257</v>
       </c>
-      <c r="JA4" t="s">
+      <c r="JF4" t="s">
         <v>258</v>
       </c>
-      <c r="JB4" t="s">
+      <c r="JG4" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="JC4" t="s">
+      <c r="JH4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="JD4" s="3" t="s">
+      <c r="JI4" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="JE4" s="3" t="s">
+      <c r="JJ4" t="s">
         <v>262</v>
       </c>
-      <c r="JF4" s="3" t="s">
+      <c r="JK4" t="s">
         <v>263</v>
       </c>
-      <c r="JG4" t="s">
+      <c r="JL4" t="s">
         <v>264</v>
       </c>
-      <c r="JH4" t="s">
+      <c r="JM4" t="s">
         <v>265</v>
       </c>
-      <c r="JI4" t="s">
+      <c r="JN4" t="s">
         <v>266</v>
       </c>
-      <c r="JJ4" t="s">
+      <c r="JO4" t="s">
         <v>267</v>
       </c>
-      <c r="JK4" t="s">
+      <c r="JP4" t="s">
         <v>268</v>
       </c>
-      <c r="JL4" t="s">
+      <c r="JQ4" t="s">
         <v>269</v>
       </c>
-      <c r="JM4" t="s">
+      <c r="JR4" t="s">
         <v>270</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JS4" t="s">
         <v>271</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JT4" t="s">
         <v>272</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JU4" t="s">
         <v>273</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JV4" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JW4" t="s">
         <v>275</v>
       </c>
-      <c r="JS4" s="3" t="s">
+      <c r="JX4" t="s">
         <v>276</v>
       </c>
-      <c r="JT4" t="s">
+      <c r="JY4" t="s">
         <v>277</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JZ4" t="s">
         <v>278</v>
       </c>
-      <c r="JV4" t="s">
+      <c r="KA4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="JW4" t="s">
+      <c r="KB4" t="s">
         <v>280</v>
       </c>
-      <c r="JX4" s="3" t="s">
+      <c r="KC4" t="s">
         <v>281</v>
       </c>
-      <c r="JY4" t="s">
+      <c r="KD4" t="s">
         <v>282</v>
       </c>
-      <c r="JZ4" t="s">
+      <c r="KE4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="KA4" t="s">
+      <c r="KF4" t="s">
         <v>284</v>
       </c>
-      <c r="KB4" s="3" t="s">
+      <c r="KG4" t="s">
         <v>285</v>
       </c>
-      <c r="KC4" t="s">
+      <c r="KH4" t="s">
         <v>286</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KI4" t="s">
         <v>287</v>
       </c>
-      <c r="KE4" t="s">
+      <c r="KJ4" t="s">
         <v>288</v>
       </c>
-      <c r="KF4" t="s">
+      <c r="KK4" t="s">
         <v>289</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KL4" t="s">
         <v>290</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KM4" t="s">
         <v>291</v>
       </c>
-      <c r="KI4" t="s">
+      <c r="KN4" t="s">
         <v>292</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KO4" t="s">
         <v>293</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KP4" t="s">
         <v>294</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KQ4" t="s">
         <v>295</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KR4" t="s">
         <v>296</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KS4" t="s">
         <v>297</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KT4" t="s">
         <v>298</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KU4" t="s">
         <v>299</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KV4" t="s">
         <v>300</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KW4" t="s">
         <v>301</v>
       </c>
-      <c r="KS4" t="s">
+      <c r="KX4" t="s">
         <v>302</v>
       </c>
-      <c r="KT4" t="s">
+      <c r="KY4" t="s">
         <v>303</v>
       </c>
-      <c r="KU4" t="s">
+      <c r="KZ4" t="s">
         <v>304</v>
       </c>
-      <c r="KV4" t="s">
+      <c r="LA4" t="s">
         <v>305</v>
       </c>
-      <c r="KW4" t="s">
+      <c r="LB4" t="s">
         <v>306</v>
       </c>
-      <c r="KX4" t="s">
+      <c r="LC4" t="s">
         <v>307</v>
       </c>
-      <c r="KY4" t="s">
+      <c r="LD4" t="s">
         <v>308</v>
       </c>
-      <c r="KZ4" t="s">
+      <c r="LE4" t="s">
         <v>309</v>
       </c>
-      <c r="LA4" t="s">
+      <c r="LF4" t="s">
         <v>310</v>
       </c>
-      <c r="LB4" t="s">
+      <c r="LG4" t="s">
         <v>311</v>
       </c>
-      <c r="LC4" t="s">
+      <c r="LH4" t="s">
         <v>312</v>
       </c>
-      <c r="LD4" t="s">
+      <c r="LI4" t="s">
         <v>313</v>
       </c>
-      <c r="LE4" t="s">
+      <c r="LJ4" t="s">
         <v>314</v>
       </c>
-      <c r="LF4" t="s">
+      <c r="LK4" t="s">
         <v>315</v>
       </c>
-      <c r="LG4" t="s">
+      <c r="LL4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="LH4" t="s">
+      <c r="LM4" t="s">
+        <v>319</v>
+      </c>
+      <c r="LN4" t="s">
+        <v>318</v>
+      </c>
+      <c r="LO4" t="s">
         <v>317</v>
       </c>
-      <c r="LI4" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="LJ4" t="s">
-        <v>321</v>
-      </c>
-      <c r="LK4" t="s">
-        <v>320</v>
-      </c>
-      <c r="LL4" t="s">
-        <v>319</v>
-      </c>
-      <c r="LM4" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="LN4" t="s">
-        <v>334</v>
-      </c>
-      <c r="LO4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:327" x14ac:dyDescent="0.25">
+      <c r="LP4" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BL5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BM5" t="s">
-        <v>323</v>
-      </c>
-      <c r="KS5" t="s">
-        <v>323</v>
-      </c>
-      <c r="KT5" t="s">
-        <v>323</v>
-      </c>
-      <c r="KU5" t="s">
-        <v>323</v>
-      </c>
-      <c r="KZ5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="KV5" t="s">
+        <v>321</v>
+      </c>
+      <c r="KW5" t="s">
+        <v>321</v>
+      </c>
+      <c r="KX5" t="s">
+        <v>321</v>
+      </c>
+      <c r="LC5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="W6" t="s">
-        <v>323</v>
-      </c>
-      <c r="LM6" t="s">
-        <v>323</v>
-      </c>
-      <c r="LN6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="LP6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>323</v>
-      </c>
-      <c r="LO7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="8" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="V8" t="s">
-        <v>323</v>
-      </c>
-      <c r="CB8" t="s">
-        <v>323</v>
-      </c>
-      <c r="HS8" t="s">
-        <v>323</v>
-      </c>
-      <c r="HW8" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>321</v>
+      </c>
+      <c r="HV8" t="s">
+        <v>321</v>
+      </c>
+      <c r="HZ8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>323</v>
-      </c>
-      <c r="CG9" t="s">
-        <v>323</v>
-      </c>
-      <c r="IE9" t="s">
-        <v>323</v>
-      </c>
-      <c r="IT9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="CK9" t="s">
+        <v>321</v>
+      </c>
+      <c r="IH9" t="s">
+        <v>321</v>
+      </c>
+      <c r="IW9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="N10" t="s">
-        <v>323</v>
-      </c>
-      <c r="CG10" t="s">
-        <v>323</v>
-      </c>
-      <c r="IE10" t="s">
-        <v>323</v>
-      </c>
-      <c r="IT10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="CK10" t="s">
+        <v>321</v>
+      </c>
+      <c r="IH10" t="s">
+        <v>321</v>
+      </c>
+      <c r="IW10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="N11" t="s">
-        <v>323</v>
-      </c>
-      <c r="CF11" t="s">
-        <v>323</v>
-      </c>
-      <c r="HY11" t="s">
-        <v>323</v>
-      </c>
-      <c r="IS11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="CJ11" t="s">
+        <v>321</v>
+      </c>
+      <c r="IB11" t="s">
+        <v>321</v>
+      </c>
+      <c r="IV11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="N12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="13" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="N13" t="s">
-        <v>323</v>
-      </c>
-      <c r="CF13" t="s">
-        <v>323</v>
-      </c>
-      <c r="CG13" t="s">
-        <v>323</v>
-      </c>
-      <c r="CN13" t="s">
-        <v>323</v>
-      </c>
-      <c r="HY13" t="s">
-        <v>323</v>
-      </c>
-      <c r="IE13" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="CJ13" t="s">
+        <v>321</v>
+      </c>
+      <c r="CK13" t="s">
+        <v>321</v>
+      </c>
+      <c r="CR13" t="s">
+        <v>321</v>
+      </c>
+      <c r="IB13" t="s">
+        <v>321</v>
       </c>
       <c r="IH13" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="14" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="IK13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>323</v>
-      </c>
-      <c r="CF14" t="s">
-        <v>323</v>
-      </c>
-      <c r="CM14" t="s">
-        <v>323</v>
-      </c>
-      <c r="HY14" t="s">
-        <v>323</v>
-      </c>
-      <c r="II14" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="15" spans="1:327" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="CJ14" t="s">
+        <v>321</v>
+      </c>
+      <c r="CQ14" t="s">
+        <v>321</v>
+      </c>
+      <c r="IB14" t="s">
+        <v>321</v>
+      </c>
+      <c r="IL14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:327" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:328" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>321</v>
+      </c>
+      <c r="DJ17" t="s">
+        <v>321</v>
+      </c>
+      <c r="HN17" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>321</v>
+      </c>
+      <c r="DK18" t="s">
+        <v>321</v>
+      </c>
+      <c r="HO18" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>321</v>
+      </c>
+      <c r="DM19" t="s">
+        <v>321</v>
+      </c>
+      <c r="HP19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>321</v>
+      </c>
+      <c r="DL20" t="s">
+        <v>321</v>
+      </c>
+      <c r="HQ20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>321</v>
+      </c>
+      <c r="DZ21" t="s">
+        <v>321</v>
+      </c>
+      <c r="IC21" t="s">
+        <v>321</v>
+      </c>
+      <c r="ID21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>321</v>
+      </c>
+      <c r="EA22" t="s">
+        <v>321</v>
+      </c>
+      <c r="IE22" t="s">
+        <v>321</v>
+      </c>
+      <c r="IF22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>321</v>
+      </c>
+      <c r="BZ23" t="s">
+        <v>321</v>
+      </c>
+      <c r="CA23" t="s">
+        <v>321</v>
+      </c>
+      <c r="KA23" t="s">
+        <v>321</v>
+      </c>
+      <c r="KB23" t="s">
+        <v>321</v>
+      </c>
+      <c r="KC23" t="s">
+        <v>321</v>
+      </c>
+      <c r="KD23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>28</v>
+      <c r="CB24" t="s">
+        <v>321</v>
+      </c>
+      <c r="CC24" t="s">
+        <v>321</v>
+      </c>
+      <c r="KQ24" t="s">
+        <v>321</v>
+      </c>
+      <c r="KR24" t="s">
+        <v>321</v>
+      </c>
+      <c r="KS24" t="s">
+        <v>321</v>
+      </c>
+      <c r="KT24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -3707,20 +3927,20 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>322</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="9" t="s">
-        <v>322</v>
+      <c r="H70" s="3" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="10">
+      <c r="A71" s="4">
         <v>1</v>
       </c>
       <c r="B71" t="s">
@@ -3730,17 +3950,17 @@
         <v>64</v>
       </c>
       <c r="H71" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
+      <c r="A72" s="4"/>
       <c r="H72" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
+      <c r="A73" s="4"/>
       <c r="B73" t="s">
         <v>5</v>
       </c>
@@ -3748,17 +3968,17 @@
         <v>65</v>
       </c>
       <c r="H73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="H74" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="H74" t="s">
-        <v>329</v>
-      </c>
-    </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="10">
+      <c r="A75" s="4">
         <v>2</v>
       </c>
       <c r="B75" t="s">
@@ -3766,13 +3986,13 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
+      <c r="A76" s="4"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
+      <c r="A77" s="4"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
+      <c r="A78" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3783,20 +4003,20 @@
     <mergeCell ref="A71:A74"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="GS4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
-    <hyperlink ref="HJ4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
-    <hyperlink ref="HM4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
-    <hyperlink ref="IB4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
-    <hyperlink ref="IG4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
-    <hyperlink ref="IQ4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
-    <hyperlink ref="JD4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
-    <hyperlink ref="JE4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
-    <hyperlink ref="JF4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
-    <hyperlink ref="JS4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
-    <hyperlink ref="JX4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
-    <hyperlink ref="KB4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
-    <hyperlink ref="LI4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
-    <hyperlink ref="LM4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
+    <hyperlink ref="GV4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
+    <hyperlink ref="HM4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
+    <hyperlink ref="HP4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
+    <hyperlink ref="IE4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
+    <hyperlink ref="IJ4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
+    <hyperlink ref="IT4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
+    <hyperlink ref="JG4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
+    <hyperlink ref="JH4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
+    <hyperlink ref="JI4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JV4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="KA4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KE4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LL4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
+    <hyperlink ref="LP4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
ajustando detalles de informes listos, añadidos a matriz de trazabilidad
ajustando detalles de informes listos, añadidos a matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71EC372-EB46-4604-91F4-7E65CABCFCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C440D7B8-4BFE-45B2-ACDF-F8C8B9D529D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="357">
   <si>
     <t>MVC</t>
   </si>
@@ -1186,6 +1186,15 @@
   </si>
   <si>
     <t>21h</t>
+  </si>
+  <si>
+    <t>Director de Tesis</t>
+  </si>
+  <si>
+    <t>21i</t>
+  </si>
+  <si>
+    <t>21j</t>
   </si>
 </sst>
 </file>
@@ -1627,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
   <dimension ref="A1:LP78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="EG14" workbookViewId="0">
+      <selection activeCell="EI34" sqref="EI34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,11 +1737,11 @@
     <col min="102" max="102" width="36" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="38" customWidth="1"/>
     <col min="104" max="104" width="30" customWidth="1"/>
-    <col min="105" max="105" width="23.28515625" customWidth="1"/>
-    <col min="106" max="106" width="29.42578125" customWidth="1"/>
+    <col min="105" max="105" width="37.42578125" customWidth="1"/>
+    <col min="106" max="106" width="32.7109375" customWidth="1"/>
     <col min="107" max="107" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="38.28515625" customWidth="1"/>
-    <col min="109" max="109" width="16.85546875" customWidth="1"/>
+    <col min="109" max="109" width="49.28515625" customWidth="1"/>
     <col min="110" max="110" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="20.85546875" customWidth="1"/>
     <col min="112" max="112" width="20.140625" customWidth="1"/>
@@ -1756,13 +1765,13 @@
     <col min="130" max="130" width="25.140625" customWidth="1"/>
     <col min="131" max="131" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="132" max="132" width="21.28515625" customWidth="1"/>
-    <col min="133" max="133" width="16.85546875" customWidth="1"/>
+    <col min="133" max="133" width="26.7109375" customWidth="1"/>
     <col min="134" max="134" width="18" customWidth="1"/>
-    <col min="135" max="135" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="19.42578125" customWidth="1"/>
     <col min="136" max="136" width="35" customWidth="1"/>
     <col min="137" max="137" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="19.7109375" customWidth="1"/>
-    <col min="139" max="139" width="22" customWidth="1"/>
+    <col min="138" max="138" width="43.85546875" customWidth="1"/>
+    <col min="139" max="139" width="33.28515625" customWidth="1"/>
     <col min="140" max="140" width="25.7109375" customWidth="1"/>
     <col min="141" max="141" width="31.85546875" customWidth="1"/>
     <col min="142" max="142" width="25.42578125" customWidth="1"/>
@@ -1846,7 +1855,7 @@
     <col min="223" max="223" width="45.5703125" customWidth="1"/>
     <col min="224" max="224" width="39.85546875" customWidth="1"/>
     <col min="225" max="225" width="40" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="24.85546875" customWidth="1"/>
+    <col min="226" max="226" width="54.140625" customWidth="1"/>
     <col min="227" max="227" width="23.85546875" customWidth="1"/>
     <col min="228" max="228" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="29.85546875" customWidth="1"/>
@@ -1870,12 +1879,12 @@
     <col min="247" max="247" width="58.85546875" customWidth="1"/>
     <col min="248" max="248" width="50.7109375" customWidth="1"/>
     <col min="249" max="249" width="49" customWidth="1"/>
-    <col min="250" max="250" width="42.140625" customWidth="1"/>
-    <col min="251" max="251" width="45.42578125" customWidth="1"/>
+    <col min="250" max="250" width="51.42578125" customWidth="1"/>
+    <col min="251" max="251" width="53.5703125" customWidth="1"/>
     <col min="252" max="252" width="39.42578125" customWidth="1"/>
-    <col min="253" max="253" width="46.5703125" customWidth="1"/>
+    <col min="253" max="253" width="51.42578125" customWidth="1"/>
     <col min="254" max="254" width="27.85546875" customWidth="1"/>
-    <col min="255" max="255" width="28.140625" customWidth="1"/>
+    <col min="255" max="255" width="47.7109375" customWidth="1"/>
     <col min="256" max="256" width="33.7109375" customWidth="1"/>
     <col min="257" max="257" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="258" max="258" width="38.28515625" customWidth="1"/>
@@ -2388,8 +2397,12 @@
       <c r="CY3" s="1"/>
       <c r="CZ3" s="1"/>
       <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
-      <c r="DC3" s="1"/>
+      <c r="DB3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="DC3" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="DD3" s="1"/>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
@@ -2426,9 +2439,15 @@
       <c r="EA3" s="1"/>
       <c r="EB3" s="1"/>
       <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
-      <c r="EE3" s="1"/>
-      <c r="EF3" s="1"/>
+      <c r="ED3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="EE3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="EF3" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="EG3" s="1"/>
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
@@ -2478,6 +2497,12 @@
       <c r="IL3" t="s">
         <v>335</v>
       </c>
+      <c r="IS3" t="s">
+        <v>354</v>
+      </c>
+      <c r="IU3" t="s">
+        <v>354</v>
+      </c>
       <c r="IW3" t="s">
         <v>334</v>
       </c>
@@ -3771,6 +3796,9 @@
       <c r="A24">
         <v>20</v>
       </c>
+      <c r="N24" t="s">
+        <v>321</v>
+      </c>
       <c r="CB24" t="s">
         <v>321</v>
       </c>
@@ -3794,134 +3822,258 @@
       <c r="A25" s="12" t="s">
         <v>346</v>
       </c>
+      <c r="N25" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT25" t="s">
+        <v>321</v>
+      </c>
+      <c r="ED25" t="s">
+        <v>321</v>
+      </c>
+      <c r="JD25" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="26" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>347</v>
       </c>
+      <c r="N26" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT26" t="s">
+        <v>321</v>
+      </c>
+      <c r="EG26" t="s">
+        <v>321</v>
+      </c>
+      <c r="JE26" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="27" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>348</v>
       </c>
+      <c r="N27" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT27" t="s">
+        <v>321</v>
+      </c>
+      <c r="EF27" t="s">
+        <v>321</v>
+      </c>
+      <c r="JG27" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="28" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>349</v>
       </c>
+      <c r="N28" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT28" t="s">
+        <v>321</v>
+      </c>
+      <c r="EE28" t="s">
+        <v>321</v>
+      </c>
+      <c r="JF28" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="29" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>350</v>
       </c>
+      <c r="N29" t="s">
+        <v>321</v>
+      </c>
+      <c r="DB29" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT29" t="s">
+        <v>321</v>
+      </c>
+      <c r="IS29" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="30" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>351</v>
       </c>
+      <c r="N30" t="s">
+        <v>321</v>
+      </c>
+      <c r="DC30" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT30" t="s">
+        <v>321</v>
+      </c>
+      <c r="IU30" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="31" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>352</v>
       </c>
+      <c r="N31" t="s">
+        <v>321</v>
+      </c>
+      <c r="DA31" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT31" t="s">
+        <v>321</v>
+      </c>
+      <c r="IQ31" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="32" spans="1:306" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="N32" t="s">
+        <v>321</v>
+      </c>
+      <c r="DE32" t="s">
+        <v>321</v>
+      </c>
+      <c r="DT32" t="s">
+        <v>321</v>
+      </c>
+      <c r="HR32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="33" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>355</v>
+      </c>
+      <c r="N33" t="s">
+        <v>321</v>
+      </c>
+      <c r="EC33" t="s">
+        <v>321</v>
+      </c>
+      <c r="JW33" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>356</v>
+      </c>
+      <c r="N34" t="s">
+        <v>321</v>
+      </c>
+      <c r="EI34" t="s">
+        <v>321</v>
+      </c>
+      <c r="JX34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="36" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="37" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="38" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="39" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="40" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="41" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="42" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="43" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="44" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="45" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="46" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="47" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="48" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
25 de 47 requerimientos en matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C440D7B8-4BFE-45B2-ACDF-F8C8B9D529D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369D6CE2-86ED-4B03-B70C-3827B062343F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="359">
   <si>
     <t>MVC</t>
   </si>
@@ -1195,6 +1195,12 @@
   </si>
   <si>
     <t>21j</t>
+  </si>
+  <si>
+    <t>TesisController.php @index_al_sec</t>
+  </si>
+  <si>
+    <t>Secretaria</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LP78"/>
+  <dimension ref="A1:LQ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EG14" workbookViewId="0">
-      <selection activeCell="EI34" sqref="EI34"/>
+    <sheetView tabSelected="1" topLeftCell="HJ18" workbookViewId="0">
+      <selection activeCell="HL39" sqref="HL39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1735,7 @@
     <col min="94" max="94" width="25" customWidth="1"/>
     <col min="95" max="95" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="30.5703125" customWidth="1"/>
-    <col min="97" max="97" width="23.42578125" customWidth="1"/>
+    <col min="97" max="97" width="28.5703125" customWidth="1"/>
     <col min="98" max="98" width="39" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="37.5703125" customWidth="1"/>
     <col min="100" max="100" width="25" customWidth="1"/>
@@ -1888,8 +1894,8 @@
     <col min="256" max="256" width="33.7109375" customWidth="1"/>
     <col min="257" max="257" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="258" max="258" width="38.28515625" customWidth="1"/>
-    <col min="259" max="259" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="29.28515625" customWidth="1"/>
+    <col min="259" max="259" width="45.85546875" customWidth="1"/>
+    <col min="260" max="260" width="39" customWidth="1"/>
     <col min="261" max="261" width="30" customWidth="1"/>
     <col min="262" max="262" width="32.140625" customWidth="1"/>
     <col min="263" max="263" width="31.28515625" customWidth="1"/>
@@ -1904,8 +1910,8 @@
     <col min="272" max="272" width="39.42578125" customWidth="1"/>
     <col min="273" max="273" width="49" customWidth="1"/>
     <col min="274" max="274" width="37" customWidth="1"/>
-    <col min="275" max="275" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="28.28515625" customWidth="1"/>
+    <col min="275" max="275" width="45.42578125" customWidth="1"/>
+    <col min="276" max="276" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="277" max="277" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="278" max="278" width="36.140625" customWidth="1"/>
     <col min="279" max="279" width="39.42578125" customWidth="1"/>
@@ -1956,10 +1962,10 @@
     <col min="325" max="325" width="38.28515625" customWidth="1"/>
     <col min="326" max="326" width="35.42578125" customWidth="1"/>
     <col min="327" max="327" width="34.7109375" customWidth="1"/>
-    <col min="328" max="328" width="27.85546875" customWidth="1"/>
+    <col min="328" max="328" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:329" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:329" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2313,7 @@
       <c r="LO2" s="11"/>
       <c r="LP2" s="11"/>
     </row>
-    <row r="3" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:329" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2509,8 +2515,11 @@
       <c r="IX3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="4" spans="1:328" x14ac:dyDescent="0.25">
+      <c r="JI3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>323</v>
       </c>
@@ -3312,188 +3321,191 @@
       <c r="JH4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="JI4" s="2" t="s">
+      <c r="JI4" t="s">
+        <v>357</v>
+      </c>
+      <c r="JJ4" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="JJ4" t="s">
+      <c r="JK4" t="s">
         <v>262</v>
       </c>
-      <c r="JK4" t="s">
+      <c r="JL4" t="s">
         <v>263</v>
       </c>
-      <c r="JL4" t="s">
+      <c r="JM4" t="s">
         <v>264</v>
       </c>
-      <c r="JM4" t="s">
+      <c r="JN4" t="s">
         <v>265</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JO4" t="s">
         <v>266</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JP4" t="s">
         <v>267</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JQ4" t="s">
         <v>268</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JR4" t="s">
         <v>269</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JS4" t="s">
         <v>270</v>
       </c>
-      <c r="JS4" t="s">
+      <c r="JT4" t="s">
         <v>271</v>
       </c>
-      <c r="JT4" t="s">
+      <c r="JU4" t="s">
         <v>272</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JV4" t="s">
         <v>273</v>
       </c>
-      <c r="JV4" s="2" t="s">
+      <c r="JW4" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="JW4" t="s">
+      <c r="JX4" t="s">
         <v>275</v>
       </c>
-      <c r="JX4" t="s">
+      <c r="JY4" t="s">
         <v>276</v>
       </c>
-      <c r="JY4" t="s">
+      <c r="JZ4" t="s">
         <v>277</v>
       </c>
-      <c r="JZ4" t="s">
+      <c r="KA4" t="s">
         <v>278</v>
       </c>
-      <c r="KA4" s="2" t="s">
+      <c r="KB4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="KB4" t="s">
+      <c r="KC4" t="s">
         <v>280</v>
       </c>
-      <c r="KC4" t="s">
+      <c r="KD4" t="s">
         <v>281</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KE4" t="s">
         <v>282</v>
       </c>
-      <c r="KE4" s="2" t="s">
+      <c r="KF4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="KF4" t="s">
+      <c r="KG4" t="s">
         <v>284</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KH4" t="s">
         <v>285</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KI4" t="s">
         <v>286</v>
       </c>
-      <c r="KI4" t="s">
+      <c r="KJ4" t="s">
         <v>287</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KK4" t="s">
         <v>288</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KL4" t="s">
         <v>289</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KM4" t="s">
         <v>290</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KN4" t="s">
         <v>291</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KO4" t="s">
         <v>292</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KP4" t="s">
         <v>293</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KQ4" t="s">
         <v>294</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KR4" t="s">
         <v>295</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KS4" t="s">
         <v>296</v>
       </c>
-      <c r="KS4" t="s">
+      <c r="KT4" t="s">
         <v>297</v>
       </c>
-      <c r="KT4" t="s">
+      <c r="KU4" t="s">
         <v>298</v>
       </c>
-      <c r="KU4" t="s">
+      <c r="KV4" t="s">
         <v>299</v>
       </c>
-      <c r="KV4" t="s">
+      <c r="KW4" t="s">
         <v>300</v>
       </c>
-      <c r="KW4" t="s">
+      <c r="KX4" t="s">
         <v>301</v>
       </c>
-      <c r="KX4" t="s">
+      <c r="KY4" t="s">
         <v>302</v>
       </c>
-      <c r="KY4" t="s">
+      <c r="KZ4" t="s">
         <v>303</v>
       </c>
-      <c r="KZ4" t="s">
+      <c r="LA4" t="s">
         <v>304</v>
       </c>
-      <c r="LA4" t="s">
+      <c r="LB4" t="s">
         <v>305</v>
       </c>
-      <c r="LB4" t="s">
+      <c r="LC4" t="s">
         <v>306</v>
       </c>
-      <c r="LC4" t="s">
+      <c r="LD4" t="s">
         <v>307</v>
       </c>
-      <c r="LD4" t="s">
+      <c r="LE4" t="s">
         <v>308</v>
       </c>
-      <c r="LE4" t="s">
+      <c r="LF4" t="s">
         <v>309</v>
       </c>
-      <c r="LF4" t="s">
+      <c r="LG4" t="s">
         <v>310</v>
       </c>
-      <c r="LG4" t="s">
+      <c r="LH4" t="s">
         <v>311</v>
       </c>
-      <c r="LH4" t="s">
+      <c r="LI4" t="s">
         <v>312</v>
       </c>
-      <c r="LI4" t="s">
+      <c r="LJ4" t="s">
         <v>313</v>
       </c>
-      <c r="LJ4" t="s">
+      <c r="LK4" t="s">
         <v>314</v>
       </c>
-      <c r="LK4" t="s">
+      <c r="LL4" t="s">
         <v>315</v>
       </c>
-      <c r="LL4" s="2" t="s">
+      <c r="LM4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="LM4" t="s">
+      <c r="LN4" t="s">
         <v>319</v>
       </c>
-      <c r="LN4" t="s">
+      <c r="LO4" t="s">
         <v>318</v>
       </c>
-      <c r="LO4" t="s">
+      <c r="LP4" t="s">
         <v>317</v>
       </c>
-      <c r="LP4" s="2" t="s">
+      <c r="LQ4" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3506,20 +3518,20 @@
       <c r="BM5" t="s">
         <v>321</v>
       </c>
-      <c r="KV5" t="s">
-        <v>321</v>
-      </c>
       <c r="KW5" t="s">
         <v>321</v>
       </c>
       <c r="KX5" t="s">
         <v>321</v>
       </c>
-      <c r="LC5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:328" x14ac:dyDescent="0.25">
+      <c r="KY5" t="s">
+        <v>321</v>
+      </c>
+      <c r="LD5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3529,11 +3541,11 @@
       <c r="W6" t="s">
         <v>321</v>
       </c>
-      <c r="LP6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:328" x14ac:dyDescent="0.25">
+      <c r="LQ6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3541,7 +3553,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3561,7 +3573,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3578,7 +3590,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3595,7 +3607,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3612,7 +3624,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3620,7 +3632,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3646,7 +3658,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3666,17 +3678,17 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:328" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3690,7 +3702,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3704,7 +3716,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3718,7 +3730,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3732,7 +3744,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="21" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3749,7 +3761,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="22" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3766,7 +3778,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="23" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3779,9 +3791,6 @@
       <c r="CA23" t="s">
         <v>321</v>
       </c>
-      <c r="KA23" t="s">
-        <v>321</v>
-      </c>
       <c r="KB23" t="s">
         <v>321</v>
       </c>
@@ -3791,8 +3800,11 @@
       <c r="KD23" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="24" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="KE23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3805,7 +3817,7 @@
       <c r="CC24" t="s">
         <v>321</v>
       </c>
-      <c r="KQ24" t="s">
+      <c r="CS24" t="s">
         <v>321</v>
       </c>
       <c r="KR24" t="s">
@@ -3817,8 +3829,11 @@
       <c r="KT24" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="25" spans="1:306" x14ac:dyDescent="0.25">
+      <c r="KU24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>346</v>
       </c>
@@ -3835,7 +3850,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>347</v>
       </c>
@@ -3852,7 +3867,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>348</v>
       </c>
@@ -3869,7 +3884,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="28" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>349</v>
       </c>
@@ -3886,7 +3901,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="29" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>350</v>
       </c>
@@ -3903,7 +3918,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="30" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>351</v>
       </c>
@@ -3920,7 +3935,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="31" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>352</v>
       </c>
@@ -3937,7 +3952,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="32" spans="1:306" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:307" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>353</v>
       </c>
@@ -3954,7 +3969,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="33" spans="1:284" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:285" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>355</v>
       </c>
@@ -3964,11 +3979,11 @@
       <c r="EC33" t="s">
         <v>321</v>
       </c>
-      <c r="JW33" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="34" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="JX33" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:285" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>356</v>
       </c>
@@ -3978,102 +3993,188 @@
       <c r="EI34" t="s">
         <v>321</v>
       </c>
-      <c r="JX34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="35" spans="1:284" x14ac:dyDescent="0.25">
+      <c r="JY34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:285" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>22</v>
+      </c>
+      <c r="N35" t="s">
+        <v>321</v>
+      </c>
+      <c r="DN35" t="s">
+        <v>321</v>
+      </c>
+      <c r="JI35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="N36" t="s">
+        <v>321</v>
+      </c>
+      <c r="FA36" t="s">
+        <v>321</v>
+      </c>
+      <c r="IY36" t="s">
+        <v>321</v>
+      </c>
+      <c r="IZ36" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="37" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>24</v>
+      </c>
+      <c r="N37" t="s">
+        <v>321</v>
+      </c>
+      <c r="JO37" t="s">
+        <v>321</v>
+      </c>
+      <c r="JP37" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="N38" t="s">
+        <v>321</v>
+      </c>
+      <c r="CS38" t="s">
+        <v>321</v>
+      </c>
+      <c r="JO38" t="s">
+        <v>321</v>
+      </c>
+      <c r="JP38" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>26</v>
+      </c>
+      <c r="N39" t="s">
+        <v>321</v>
+      </c>
+      <c r="EN39" t="s">
+        <v>321</v>
+      </c>
+      <c r="HL39" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="40" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="43" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="44" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="45" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="46" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="47" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="48" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:284" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>47</v>
       </c>
     </row>
@@ -4163,12 +4264,12 @@
     <hyperlink ref="IT4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
     <hyperlink ref="JG4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
     <hyperlink ref="JH4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
-    <hyperlink ref="JI4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
-    <hyperlink ref="JV4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
-    <hyperlink ref="KA4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
-    <hyperlink ref="KE4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
-    <hyperlink ref="LL4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
-    <hyperlink ref="LP4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
+    <hyperlink ref="JJ4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JW4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="KB4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KF4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LM4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
+    <hyperlink ref="LQ4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
Cambiando nombre de titulo a vista tesis_profes_comision requerimientos, requerimientos en la matriz de trazabilidad casi listos, solo faltan homes de tipos de usuarios
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369D6CE2-86ED-4B03-B70C-3827B062343F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3F5175-09C3-4815-96A6-A23EE2485401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="367">
   <si>
     <t>MVC</t>
   </si>
@@ -295,9 +295,6 @@
     <t>/recopilacion/recopilacion_edit</t>
   </si>
   <si>
-    <t>/recopilacion/recopilacion_informacion</t>
-  </si>
-  <si>
     <t>/users/create</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
     <t>/tesis/create</t>
   </si>
   <si>
-    <t>/tesis/create_fecha_descargar</t>
-  </si>
-  <si>
     <t>/tesis/create_num_memo</t>
   </si>
   <si>
@@ -461,9 +455,6 @@
   </si>
   <si>
     <t>/tesis/ingresar_nota_tesis</t>
-  </si>
-  <si>
-    <t>/tesis/lista_profes_comision_revisión</t>
   </si>
   <si>
     <t>/tesis/mostrar_tesis</t>
@@ -1201,6 +1192,39 @@
   </si>
   <si>
     <t>Secretaria</t>
+  </si>
+  <si>
+    <t>Profesor_Guia</t>
+  </si>
+  <si>
+    <t>/recopilacion/recopilacion_informacion_titulados</t>
+  </si>
+  <si>
+    <t>secretaria</t>
+  </si>
+  <si>
+    <t>/memorandum/index</t>
+  </si>
+  <si>
+    <t>/tesis/lista_profes_comision_revision</t>
+  </si>
+  <si>
+    <t>/tesis/create_fecha_descargar_actas</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Capitulos_TesisController @update_avances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t>Director de Tesis/Profesor</t>
+  </si>
+  <si>
+    <t>Profesor Guia /Director Tesis</t>
   </si>
 </sst>
 </file>
@@ -1640,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LQ78"/>
+  <dimension ref="A1:LR99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HJ18" workbookViewId="0">
-      <selection activeCell="HL39" sqref="HL39"/>
+    <sheetView tabSelected="1" topLeftCell="FI54" workbookViewId="0">
+      <selection activeCell="FK70" sqref="FK70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,8 +1679,8 @@
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" customWidth="1"/>
     <col min="17" max="17" width="15.5703125" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
@@ -1666,14 +1690,15 @@
     <col min="22" max="22" width="21.5703125" customWidth="1"/>
     <col min="23" max="23" width="23.5703125" customWidth="1"/>
     <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" customWidth="1"/>
+    <col min="25" max="25" width="25.42578125" customWidth="1"/>
     <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="28.42578125" customWidth="1"/>
     <col min="28" max="28" width="29" customWidth="1"/>
     <col min="29" max="29" width="36.5703125" customWidth="1"/>
     <col min="30" max="30" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="30.85546875" customWidth="1"/>
-    <col min="32" max="33" width="15.5703125" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" customWidth="1"/>
+    <col min="33" max="33" width="18.28515625" customWidth="1"/>
     <col min="34" max="34" width="23.7109375" customWidth="1"/>
     <col min="35" max="35" width="25.140625" customWidth="1"/>
     <col min="36" max="36" width="28.7109375" customWidth="1"/>
@@ -1691,7 +1716,7 @@
     <col min="48" max="48" width="15.85546875" customWidth="1"/>
     <col min="49" max="49" width="21.7109375" customWidth="1"/>
     <col min="50" max="50" width="21.42578125" customWidth="1"/>
-    <col min="51" max="51" width="37.42578125" customWidth="1"/>
+    <col min="51" max="51" width="25.42578125" customWidth="1"/>
     <col min="52" max="52" width="37.7109375" customWidth="1"/>
     <col min="53" max="53" width="38.85546875" customWidth="1"/>
     <col min="54" max="55" width="38" bestFit="1" customWidth="1"/>
@@ -1702,7 +1727,7 @@
     <col min="60" max="60" width="16.42578125" customWidth="1"/>
     <col min="61" max="61" width="17.42578125" customWidth="1"/>
     <col min="62" max="62" width="33" customWidth="1"/>
-    <col min="63" max="63" width="37.28515625" customWidth="1"/>
+    <col min="63" max="63" width="54" customWidth="1"/>
     <col min="64" max="64" width="14.7109375" customWidth="1"/>
     <col min="65" max="65" width="30.28515625" customWidth="1"/>
     <col min="66" max="66" width="29.85546875" customWidth="1"/>
@@ -1711,7 +1736,7 @@
     <col min="69" max="69" width="16.7109375" customWidth="1"/>
     <col min="70" max="71" width="15.5703125" customWidth="1"/>
     <col min="72" max="72" width="14.42578125" customWidth="1"/>
-    <col min="73" max="73" width="18" customWidth="1"/>
+    <col min="73" max="73" width="24" customWidth="1"/>
     <col min="74" max="74" width="16.42578125" customWidth="1"/>
     <col min="75" max="75" width="25.42578125" customWidth="1"/>
     <col min="76" max="76" width="18" customWidth="1"/>
@@ -1722,10 +1747,10 @@
     <col min="81" max="81" width="35.28515625" customWidth="1"/>
     <col min="82" max="82" width="23.5703125" customWidth="1"/>
     <col min="83" max="83" width="34.5703125" customWidth="1"/>
-    <col min="84" max="84" width="11.85546875" customWidth="1"/>
-    <col min="85" max="85" width="12.28515625" customWidth="1"/>
+    <col min="84" max="84" width="16.7109375" customWidth="1"/>
+    <col min="85" max="85" width="34.5703125" customWidth="1"/>
     <col min="86" max="86" width="12.140625" customWidth="1"/>
-    <col min="87" max="87" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="34.85546875" customWidth="1"/>
     <col min="88" max="88" width="20.85546875" customWidth="1"/>
     <col min="89" max="89" width="24.42578125" customWidth="1"/>
     <col min="90" max="90" width="15.7109375" customWidth="1"/>
@@ -1761,10 +1786,10 @@
     <col min="120" max="120" width="43.85546875" customWidth="1"/>
     <col min="121" max="121" width="25" customWidth="1"/>
     <col min="122" max="122" width="28.28515625" customWidth="1"/>
-    <col min="123" max="123" width="24.85546875" customWidth="1"/>
+    <col min="123" max="123" width="37.42578125" customWidth="1"/>
     <col min="124" max="124" width="35.85546875" customWidth="1"/>
     <col min="125" max="125" width="19.5703125" customWidth="1"/>
-    <col min="126" max="126" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="38.5703125" customWidth="1"/>
     <col min="127" max="127" width="32.140625" customWidth="1"/>
     <col min="128" max="128" width="29" customWidth="1"/>
     <col min="129" max="129" width="26.28515625" customWidth="1"/>
@@ -1781,7 +1806,7 @@
     <col min="140" max="140" width="25.7109375" customWidth="1"/>
     <col min="141" max="141" width="31.85546875" customWidth="1"/>
     <col min="142" max="142" width="25.42578125" customWidth="1"/>
-    <col min="143" max="143" width="15.85546875" customWidth="1"/>
+    <col min="143" max="143" width="31" customWidth="1"/>
     <col min="144" max="144" width="21.42578125" customWidth="1"/>
     <col min="145" max="145" width="24" customWidth="1"/>
     <col min="146" max="146" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -1790,7 +1815,7 @@
     <col min="149" max="149" width="28.5703125" customWidth="1"/>
     <col min="150" max="150" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="151" max="151" width="16.140625" customWidth="1"/>
-    <col min="152" max="152" width="20.42578125" customWidth="1"/>
+    <col min="152" max="152" width="32.5703125" customWidth="1"/>
     <col min="153" max="154" width="24.85546875" customWidth="1"/>
     <col min="155" max="155" width="28.140625" customWidth="1"/>
     <col min="156" max="156" width="32.7109375" customWidth="1"/>
@@ -1802,7 +1827,7 @@
     <col min="162" max="162" width="40.7109375" customWidth="1"/>
     <col min="163" max="163" width="46" customWidth="1"/>
     <col min="164" max="164" width="30" customWidth="1"/>
-    <col min="165" max="165" width="29.140625" customWidth="1"/>
+    <col min="165" max="165" width="47" customWidth="1"/>
     <col min="166" max="166" width="28.42578125" customWidth="1"/>
     <col min="167" max="167" width="31.140625" customWidth="1"/>
     <col min="168" max="168" width="39.42578125" customWidth="1"/>
@@ -1813,17 +1838,18 @@
     <col min="173" max="173" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="174" max="174" width="50.7109375" customWidth="1"/>
     <col min="175" max="175" width="42.140625" customWidth="1"/>
-    <col min="176" max="176" width="28.28515625" customWidth="1"/>
-    <col min="177" max="177" width="29.28515625" customWidth="1"/>
-    <col min="178" max="178" width="26.42578125" customWidth="1"/>
+    <col min="176" max="176" width="38.7109375" customWidth="1"/>
+    <col min="177" max="177" width="45.5703125" customWidth="1"/>
+    <col min="178" max="178" width="57.28515625" customWidth="1"/>
     <col min="179" max="179" width="30" customWidth="1"/>
     <col min="180" max="180" width="29.85546875" customWidth="1"/>
     <col min="181" max="181" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="182" max="182" width="29.85546875" customWidth="1"/>
-    <col min="183" max="184" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="45.42578125" customWidth="1"/>
+    <col min="184" max="184" width="35" customWidth="1"/>
     <col min="185" max="185" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="186" max="186" width="28.7109375" customWidth="1"/>
-    <col min="187" max="187" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="53.7109375" customWidth="1"/>
     <col min="188" max="188" width="27.42578125" customWidth="1"/>
     <col min="189" max="189" width="26.85546875" customWidth="1"/>
     <col min="190" max="190" width="25.28515625" customWidth="1"/>
@@ -1838,7 +1864,7 @@
     <col min="200" max="200" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="201" max="201" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="29.7109375" customWidth="1"/>
+    <col min="203" max="203" width="31.42578125" customWidth="1"/>
     <col min="204" max="204" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="205" max="205" width="30.140625" customWidth="1"/>
     <col min="206" max="206" width="32.5703125" customWidth="1"/>
@@ -1851,10 +1877,10 @@
     <col min="213" max="213" width="28.28515625" customWidth="1"/>
     <col min="214" max="214" width="34.42578125" customWidth="1"/>
     <col min="215" max="215" width="34.85546875" customWidth="1"/>
-    <col min="216" max="216" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="38.140625" customWidth="1"/>
     <col min="217" max="217" width="35.42578125" customWidth="1"/>
     <col min="218" max="218" width="34.7109375" customWidth="1"/>
-    <col min="219" max="219" width="31" customWidth="1"/>
+    <col min="219" max="219" width="37.140625" customWidth="1"/>
     <col min="220" max="220" width="38.5703125" customWidth="1"/>
     <col min="221" max="221" width="30.28515625" customWidth="1"/>
     <col min="222" max="222" width="38.42578125" customWidth="1"/>
@@ -1945,7 +1971,7 @@
     <col min="307" max="307" width="29.85546875" customWidth="1"/>
     <col min="308" max="308" width="52.5703125" customWidth="1"/>
     <col min="309" max="309" width="27" customWidth="1"/>
-    <col min="310" max="310" width="24.42578125" customWidth="1"/>
+    <col min="310" max="310" width="28.85546875" customWidth="1"/>
     <col min="311" max="311" width="33.140625" customWidth="1"/>
     <col min="312" max="312" width="32.85546875" customWidth="1"/>
     <col min="313" max="313" width="49.140625" bestFit="1" customWidth="1"/>
@@ -1956,16 +1982,18 @@
     <col min="319" max="319" width="42.5703125" customWidth="1"/>
     <col min="320" max="320" width="40.85546875" customWidth="1"/>
     <col min="321" max="321" width="34" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="31.5703125" customWidth="1"/>
+    <col min="322" max="322" width="45.85546875" customWidth="1"/>
     <col min="323" max="323" width="43.5703125" customWidth="1"/>
     <col min="324" max="324" width="59.7109375" customWidth="1"/>
     <col min="325" max="325" width="38.28515625" customWidth="1"/>
-    <col min="326" max="326" width="35.42578125" customWidth="1"/>
-    <col min="327" max="327" width="34.7109375" customWidth="1"/>
+    <col min="326" max="326" width="50.140625" customWidth="1"/>
+    <col min="327" max="327" width="50.7109375" customWidth="1"/>
     <col min="328" max="328" width="36.85546875" customWidth="1"/>
+    <col min="329" max="329" width="37.5703125" customWidth="1"/>
+    <col min="330" max="330" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:329" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:330" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1976,7 +2004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:329" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:330" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2166,7 @@
       <c r="EX2" s="7"/>
       <c r="EY2" s="7"/>
       <c r="EZ2" s="9" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="FA2" s="10"/>
       <c r="FB2" s="10"/>
@@ -2313,31 +2341,61 @@
       <c r="LO2" s="11"/>
       <c r="LP2" s="11"/>
     </row>
-    <row r="3" spans="1:329" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:330" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
+      <c r="AI3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
@@ -2350,15 +2408,23 @@
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
+      <c r="AW3" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
+      <c r="BE3" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
       <c r="BH3" s="1"/>
@@ -2374,7 +2440,9 @@
       <c r="BR3" s="1"/>
       <c r="BS3" s="1"/>
       <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
+      <c r="BU3" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="BV3" s="1"/>
       <c r="BW3" s="1"/>
       <c r="BX3" s="1"/>
@@ -2404,30 +2472,34 @@
       <c r="CZ3" s="1"/>
       <c r="DA3" s="1"/>
       <c r="DB3" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="DC3" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="DD3" s="1"/>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
       <c r="DG3" s="1"/>
       <c r="DH3" s="1"/>
-      <c r="DI3" s="1"/>
+      <c r="DI3" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="DJ3" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="DK3" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="DL3" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="DM3" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="DN3" s="1"/>
+        <v>336</v>
+      </c>
+      <c r="DN3" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="DO3" s="1"/>
       <c r="DP3" s="1"/>
       <c r="DQ3" s="1"/>
@@ -2440,19 +2512,19 @@
       <c r="DX3" s="1"/>
       <c r="DY3" s="1"/>
       <c r="DZ3" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="EA3" s="1"/>
       <c r="EB3" s="1"/>
       <c r="EC3" s="1"/>
       <c r="ED3" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="EE3" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="EF3" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="EG3" s="1"/>
       <c r="EH3" s="1"/>
@@ -2469,59 +2541,100 @@
       <c r="ES3" s="1"/>
       <c r="ET3" s="1"/>
       <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
+      <c r="EV3" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="EW3" s="1"/>
       <c r="EX3" s="1"/>
       <c r="EY3" s="1"/>
       <c r="EZ3" s="1"/>
       <c r="FA3" s="1"/>
       <c r="FB3" s="1"/>
-      <c r="HN3" t="s">
+      <c r="FH3" t="s">
+        <v>351</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>365</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>332</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>332</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>351</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HJ3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>332</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>332</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>336</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>336</v>
+      </c>
+      <c r="ID3" t="s">
+        <v>331</v>
+      </c>
+      <c r="IJ3" t="s">
+        <v>333</v>
+      </c>
+      <c r="IK3" t="s">
         <v>335</v>
       </c>
-      <c r="HO3" t="s">
-        <v>335</v>
-      </c>
-      <c r="HP3" t="s">
-        <v>339</v>
-      </c>
-      <c r="HQ3" t="s">
-        <v>339</v>
-      </c>
-      <c r="IC3" t="s">
+      <c r="IL3" t="s">
         <v>334</v>
       </c>
-      <c r="II3" t="s">
-        <v>336</v>
-      </c>
-      <c r="IJ3" t="s">
-        <v>338</v>
-      </c>
-      <c r="IK3" t="s">
-        <v>337</v>
-      </c>
-      <c r="IL3" t="s">
-        <v>335</v>
-      </c>
-      <c r="IS3" t="s">
-        <v>354</v>
-      </c>
-      <c r="IU3" t="s">
-        <v>354</v>
-      </c>
-      <c r="IW3" t="s">
-        <v>334</v>
+      <c r="IM3" t="s">
+        <v>332</v>
+      </c>
+      <c r="IT3" t="s">
+        <v>351</v>
+      </c>
+      <c r="IV3" t="s">
+        <v>351</v>
       </c>
       <c r="IX3" t="s">
-        <v>333</v>
-      </c>
-      <c r="JI3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:329" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="IY3" t="s">
+        <v>330</v>
+      </c>
+      <c r="JJ3" t="s">
+        <v>355</v>
+      </c>
+      <c r="KA3" t="s">
+        <v>356</v>
+      </c>
+      <c r="LA3" t="s">
+        <v>362</v>
+      </c>
+      <c r="LB3" t="s">
+        <v>362</v>
+      </c>
+      <c r="LC3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2581,13 +2694,13 @@
         <v>25</v>
       </c>
       <c r="V4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="W4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="X4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Y4" t="s">
         <v>26</v>
@@ -2668,7 +2781,7 @@
         <v>50</v>
       </c>
       <c r="AY4" t="s">
-        <v>52</v>
+        <v>359</v>
       </c>
       <c r="AZ4" t="s">
         <v>52</v>
@@ -2704,1572 +2817,2059 @@
         <v>62</v>
       </c>
       <c r="BK4" t="s">
+        <v>357</v>
+      </c>
+      <c r="BL4" t="s">
         <v>63</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>64</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
         <v>65</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BO4" t="s">
         <v>66</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
         <v>67</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BQ4" t="s">
         <v>68</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" t="s">
         <v>69</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BS4" t="s">
         <v>70</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BT4" t="s">
         <v>71</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BU4" t="s">
         <v>72</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BV4" t="s">
         <v>73</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BW4" t="s">
         <v>74</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BX4" t="s">
         <v>75</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="BY4" t="s">
         <v>76</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" t="s">
+        <v>339</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>340</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>341</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>342</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>329</v>
+      </c>
+      <c r="CE4" t="s">
         <v>77</v>
       </c>
-      <c r="BZ4" t="s">
-        <v>342</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>343</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>344</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>345</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>332</v>
-      </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>78</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
+        <v>361</v>
+      </c>
+      <c r="CH4" t="s">
         <v>79</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CI4" t="s">
         <v>80</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CJ4" t="s">
         <v>81</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CK4" t="s">
         <v>82</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CL4" t="s">
         <v>83</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CM4" t="s">
         <v>84</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CN4" t="s">
+        <v>84</v>
+      </c>
+      <c r="CO4" t="s">
         <v>85</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CP4" t="s">
         <v>86</v>
       </c>
-      <c r="CN4" t="s">
-        <v>86</v>
-      </c>
-      <c r="CO4" t="s">
+      <c r="CQ4" t="s">
         <v>87</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CR4" t="s">
         <v>88</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CS4" t="s">
         <v>89</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CT4" t="s">
         <v>90</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CU4" t="s">
         <v>91</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CV4" t="s">
+        <v>91</v>
+      </c>
+      <c r="CW4" t="s">
         <v>92</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="CX4" t="s">
         <v>93</v>
       </c>
-      <c r="CV4" t="s">
-        <v>93</v>
-      </c>
-      <c r="CW4" t="s">
+      <c r="CY4" t="s">
         <v>94</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="CZ4" t="s">
         <v>95</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="DA4" t="s">
         <v>96</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DB4" t="s">
         <v>97</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DC4" t="s">
         <v>98</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DD4" t="s">
         <v>99</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DE4" t="s">
         <v>100</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DF4" t="s">
         <v>101</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DG4" t="s">
         <v>102</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DH4" t="s">
         <v>103</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DI4" t="s">
         <v>104</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DJ4" t="s">
         <v>105</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DK4" t="s">
         <v>106</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DL4" t="s">
         <v>107</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DM4" t="s">
         <v>108</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DN4" t="s">
         <v>109</v>
       </c>
-      <c r="DM4" t="s">
+      <c r="DO4" t="s">
         <v>110</v>
       </c>
-      <c r="DN4" t="s">
+      <c r="DP4" t="s">
         <v>111</v>
       </c>
-      <c r="DO4" t="s">
+      <c r="DQ4" t="s">
         <v>112</v>
       </c>
-      <c r="DP4" t="s">
+      <c r="DR4" t="s">
         <v>113</v>
       </c>
-      <c r="DQ4" t="s">
+      <c r="DS4" t="s">
         <v>114</v>
       </c>
-      <c r="DR4" t="s">
+      <c r="DT4" t="s">
         <v>115</v>
       </c>
-      <c r="DS4" t="s">
+      <c r="DU4" t="s">
         <v>116</v>
       </c>
-      <c r="DT4" t="s">
+      <c r="DV4" t="s">
+        <v>360</v>
+      </c>
+      <c r="DW4" t="s">
         <v>117</v>
       </c>
-      <c r="DU4" t="s">
+      <c r="DX4" t="s">
         <v>118</v>
       </c>
-      <c r="DV4" t="s">
+      <c r="DY4" t="s">
         <v>119</v>
       </c>
-      <c r="DW4" t="s">
+      <c r="DZ4" t="s">
+        <v>121</v>
+      </c>
+      <c r="EA4" t="s">
         <v>120</v>
       </c>
-      <c r="DX4" t="s">
-        <v>121</v>
-      </c>
-      <c r="DY4" t="s">
+      <c r="EB4" t="s">
         <v>122</v>
       </c>
-      <c r="DZ4" t="s">
+      <c r="EC4" t="s">
+        <v>123</v>
+      </c>
+      <c r="ED4" t="s">
         <v>124</v>
       </c>
-      <c r="EA4" t="s">
-        <v>123</v>
-      </c>
-      <c r="EB4" t="s">
+      <c r="EE4" t="s">
         <v>125</v>
       </c>
-      <c r="EC4" t="s">
+      <c r="EF4" t="s">
         <v>126</v>
       </c>
-      <c r="ED4" t="s">
+      <c r="EG4" t="s">
         <v>127</v>
       </c>
-      <c r="EE4" t="s">
+      <c r="EH4" t="s">
         <v>128</v>
       </c>
-      <c r="EF4" t="s">
+      <c r="EI4" t="s">
         <v>129</v>
       </c>
-      <c r="EG4" t="s">
+      <c r="EJ4" t="s">
         <v>130</v>
       </c>
-      <c r="EH4" t="s">
+      <c r="EK4" t="s">
         <v>131</v>
       </c>
-      <c r="EI4" t="s">
+      <c r="EL4" t="s">
         <v>132</v>
       </c>
-      <c r="EJ4" t="s">
+      <c r="EM4" t="s">
         <v>133</v>
       </c>
-      <c r="EK4" t="s">
+      <c r="EN4" t="s">
         <v>134</v>
       </c>
-      <c r="EL4" t="s">
+      <c r="EO4" t="s">
         <v>135</v>
       </c>
-      <c r="EM4" t="s">
+      <c r="EP4" t="s">
         <v>136</v>
       </c>
-      <c r="EN4" t="s">
+      <c r="EQ4" t="s">
         <v>137</v>
       </c>
-      <c r="EO4" t="s">
+      <c r="ER4" t="s">
         <v>138</v>
       </c>
-      <c r="EP4" t="s">
+      <c r="ES4" t="s">
         <v>139</v>
       </c>
-      <c r="EQ4" t="s">
+      <c r="ET4" t="s">
         <v>140</v>
       </c>
-      <c r="ER4" t="s">
+      <c r="EU4" t="s">
         <v>141</v>
       </c>
-      <c r="ES4" t="s">
+      <c r="EV4" t="s">
         <v>142</v>
       </c>
-      <c r="ET4" t="s">
+      <c r="EW4" t="s">
         <v>143</v>
       </c>
-      <c r="EU4" t="s">
+      <c r="EX4" t="s">
         <v>144</v>
       </c>
-      <c r="EV4" t="s">
+      <c r="EY4" t="s">
         <v>145</v>
       </c>
-      <c r="EW4" t="s">
+      <c r="EZ4" t="s">
         <v>146</v>
       </c>
-      <c r="EX4" t="s">
+      <c r="FA4" t="s">
         <v>147</v>
       </c>
-      <c r="EY4" t="s">
+      <c r="FB4" t="s">
         <v>148</v>
       </c>
-      <c r="EZ4" t="s">
+      <c r="FC4" t="s">
         <v>149</v>
       </c>
-      <c r="FA4" t="s">
+      <c r="FD4" t="s">
         <v>150</v>
       </c>
-      <c r="FB4" t="s">
+      <c r="FE4" t="s">
         <v>151</v>
       </c>
-      <c r="FC4" t="s">
+      <c r="FF4" t="s">
         <v>152</v>
       </c>
-      <c r="FD4" t="s">
+      <c r="FG4" t="s">
         <v>153</v>
       </c>
-      <c r="FE4" t="s">
+      <c r="FH4" t="s">
         <v>154</v>
       </c>
-      <c r="FF4" t="s">
+      <c r="FI4" t="s">
         <v>155</v>
       </c>
-      <c r="FG4" t="s">
+      <c r="FJ4" t="s">
         <v>156</v>
       </c>
-      <c r="FH4" t="s">
+      <c r="FK4" t="s">
         <v>157</v>
       </c>
-      <c r="FI4" t="s">
+      <c r="FL4" t="s">
         <v>158</v>
       </c>
-      <c r="FJ4" t="s">
+      <c r="FM4" t="s">
         <v>159</v>
       </c>
-      <c r="FK4" t="s">
+      <c r="FN4" t="s">
         <v>160</v>
       </c>
-      <c r="FL4" t="s">
+      <c r="FO4" t="s">
         <v>161</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FP4" t="s">
         <v>162</v>
       </c>
-      <c r="FN4" t="s">
+      <c r="FQ4" t="s">
         <v>163</v>
       </c>
-      <c r="FO4" t="s">
+      <c r="FR4" t="s">
         <v>164</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FS4" t="s">
         <v>165</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FT4" t="s">
         <v>166</v>
       </c>
-      <c r="FR4" t="s">
+      <c r="FU4" t="s">
         <v>167</v>
       </c>
-      <c r="FS4" t="s">
+      <c r="FV4" t="s">
+        <v>363</v>
+      </c>
+      <c r="FW4" t="s">
         <v>168</v>
       </c>
-      <c r="FT4" t="s">
+      <c r="FX4" t="s">
         <v>169</v>
       </c>
-      <c r="FU4" t="s">
+      <c r="FY4" t="s">
         <v>170</v>
       </c>
-      <c r="FV4" t="s">
+      <c r="FZ4" t="s">
         <v>171</v>
       </c>
-      <c r="FW4" t="s">
+      <c r="GA4" t="s">
         <v>172</v>
       </c>
-      <c r="FX4" t="s">
+      <c r="GB4" t="s">
         <v>173</v>
       </c>
-      <c r="FY4" t="s">
+      <c r="GC4" t="s">
         <v>174</v>
       </c>
-      <c r="FZ4" t="s">
+      <c r="GD4" t="s">
         <v>175</v>
       </c>
-      <c r="GA4" t="s">
+      <c r="GE4" t="s">
         <v>176</v>
       </c>
-      <c r="GB4" t="s">
+      <c r="GF4" t="s">
         <v>177</v>
       </c>
-      <c r="GC4" t="s">
+      <c r="GG4" t="s">
         <v>178</v>
       </c>
-      <c r="GD4" t="s">
+      <c r="GH4" t="s">
         <v>179</v>
       </c>
-      <c r="GE4" t="s">
+      <c r="GI4" t="s">
         <v>180</v>
       </c>
-      <c r="GF4" t="s">
+      <c r="GJ4" t="s">
         <v>181</v>
       </c>
-      <c r="GG4" t="s">
+      <c r="GK4" t="s">
         <v>182</v>
       </c>
-      <c r="GH4" t="s">
+      <c r="GL4" t="s">
         <v>183</v>
       </c>
-      <c r="GI4" t="s">
+      <c r="GM4" t="s">
         <v>184</v>
       </c>
-      <c r="GJ4" t="s">
+      <c r="GN4" t="s">
         <v>185</v>
       </c>
-      <c r="GK4" t="s">
+      <c r="GO4" t="s">
         <v>186</v>
       </c>
-      <c r="GL4" t="s">
+      <c r="GP4" t="s">
         <v>187</v>
       </c>
-      <c r="GM4" t="s">
+      <c r="GQ4" t="s">
         <v>188</v>
       </c>
-      <c r="GN4" t="s">
+      <c r="GR4" t="s">
         <v>189</v>
       </c>
-      <c r="GO4" t="s">
+      <c r="GS4" t="s">
         <v>190</v>
       </c>
-      <c r="GP4" t="s">
+      <c r="GT4" t="s">
         <v>191</v>
       </c>
-      <c r="GQ4" t="s">
+      <c r="GU4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="GR4" t="s">
+      <c r="GV4" t="s">
         <v>193</v>
       </c>
-      <c r="GS4" t="s">
+      <c r="GW4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="GT4" s="2" t="s">
+      <c r="GX4" t="s">
         <v>195</v>
       </c>
-      <c r="GU4" t="s">
+      <c r="GY4" t="s">
         <v>196</v>
       </c>
-      <c r="GV4" s="2" t="s">
+      <c r="GZ4" t="s">
         <v>197</v>
       </c>
-      <c r="GW4" t="s">
+      <c r="HA4" t="s">
         <v>198</v>
       </c>
-      <c r="GX4" t="s">
+      <c r="HB4" t="s">
         <v>199</v>
       </c>
-      <c r="GY4" t="s">
+      <c r="HC4" t="s">
         <v>200</v>
       </c>
-      <c r="GZ4" t="s">
+      <c r="HD4" t="s">
         <v>201</v>
       </c>
-      <c r="HA4" t="s">
+      <c r="HE4" t="s">
         <v>202</v>
       </c>
-      <c r="HB4" t="s">
+      <c r="HF4" t="s">
         <v>203</v>
       </c>
-      <c r="HC4" t="s">
+      <c r="HG4" t="s">
         <v>204</v>
       </c>
-      <c r="HD4" t="s">
+      <c r="HH4" t="s">
         <v>205</v>
       </c>
-      <c r="HE4" t="s">
+      <c r="HI4" t="s">
         <v>206</v>
       </c>
-      <c r="HF4" t="s">
+      <c r="HJ4" t="s">
         <v>207</v>
       </c>
-      <c r="HG4" t="s">
+      <c r="HK4" t="s">
         <v>208</v>
       </c>
-      <c r="HH4" t="s">
+      <c r="HL4" t="s">
         <v>209</v>
       </c>
-      <c r="HI4" t="s">
+      <c r="HM4" t="s">
         <v>210</v>
       </c>
-      <c r="HJ4" t="s">
+      <c r="HN4" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="HK4" t="s">
+      <c r="HO4" t="s">
         <v>212</v>
       </c>
-      <c r="HL4" t="s">
+      <c r="HP4" t="s">
         <v>213</v>
       </c>
-      <c r="HM4" s="2" t="s">
+      <c r="HQ4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="HN4" t="s">
+      <c r="HR4" t="s">
         <v>215</v>
       </c>
-      <c r="HO4" t="s">
+      <c r="HS4" t="s">
         <v>216</v>
       </c>
-      <c r="HP4" s="2" t="s">
+      <c r="HT4" t="s">
         <v>217</v>
       </c>
-      <c r="HQ4" t="s">
+      <c r="HU4" t="s">
         <v>218</v>
       </c>
-      <c r="HR4" t="s">
+      <c r="HV4" t="s">
         <v>219</v>
       </c>
-      <c r="HS4" t="s">
+      <c r="HW4" t="s">
         <v>220</v>
       </c>
-      <c r="HT4" t="s">
+      <c r="HX4" t="s">
         <v>221</v>
       </c>
-      <c r="HU4" t="s">
+      <c r="HY4" t="s">
         <v>222</v>
       </c>
-      <c r="HV4" t="s">
+      <c r="HZ4" t="s">
         <v>223</v>
       </c>
-      <c r="HW4" t="s">
+      <c r="IA4" t="s">
         <v>224</v>
       </c>
-      <c r="HX4" t="s">
+      <c r="IB4" t="s">
         <v>225</v>
       </c>
-      <c r="HY4" t="s">
+      <c r="IC4" t="s">
         <v>226</v>
       </c>
-      <c r="HZ4" t="s">
+      <c r="ID4" t="s">
+        <v>337</v>
+      </c>
+      <c r="IE4" t="s">
         <v>227</v>
       </c>
-      <c r="IA4" t="s">
+      <c r="IF4" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="IB4" t="s">
+      <c r="IG4" t="s">
         <v>229</v>
       </c>
-      <c r="IC4" t="s">
-        <v>340</v>
-      </c>
-      <c r="ID4" t="s">
+      <c r="IH4" t="s">
         <v>230</v>
       </c>
-      <c r="IE4" s="2" t="s">
+      <c r="II4" t="s">
         <v>231</v>
       </c>
-      <c r="IF4" t="s">
+      <c r="IJ4" t="s">
         <v>232</v>
       </c>
-      <c r="IG4" t="s">
+      <c r="IK4" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="IH4" t="s">
+      <c r="IL4" t="s">
         <v>234</v>
       </c>
-      <c r="II4" t="s">
+      <c r="IM4" t="s">
         <v>235</v>
       </c>
-      <c r="IJ4" s="2" t="s">
+      <c r="IN4" t="s">
         <v>236</v>
       </c>
-      <c r="IK4" t="s">
+      <c r="IO4" t="s">
         <v>237</v>
       </c>
-      <c r="IL4" t="s">
+      <c r="IP4" t="s">
         <v>238</v>
       </c>
-      <c r="IM4" t="s">
+      <c r="IQ4" t="s">
         <v>239</v>
       </c>
-      <c r="IN4" t="s">
+      <c r="IR4" t="s">
         <v>240</v>
       </c>
-      <c r="IO4" t="s">
+      <c r="IS4" t="s">
         <v>241</v>
       </c>
-      <c r="IP4" t="s">
+      <c r="IT4" t="s">
         <v>242</v>
       </c>
-      <c r="IQ4" t="s">
+      <c r="IU4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="IR4" t="s">
+      <c r="IV4" t="s">
         <v>244</v>
       </c>
-      <c r="IS4" t="s">
+      <c r="IW4" t="s">
         <v>245</v>
       </c>
-      <c r="IT4" s="2" t="s">
+      <c r="IX4" t="s">
         <v>246</v>
       </c>
-      <c r="IU4" t="s">
+      <c r="IY4" t="s">
         <v>247</v>
       </c>
-      <c r="IV4" t="s">
+      <c r="IZ4" t="s">
         <v>248</v>
       </c>
-      <c r="IW4" t="s">
+      <c r="JA4" t="s">
         <v>249</v>
       </c>
-      <c r="IX4" t="s">
+      <c r="JB4" t="s">
         <v>250</v>
       </c>
-      <c r="IY4" t="s">
+      <c r="JC4" t="s">
         <v>251</v>
       </c>
-      <c r="IZ4" t="s">
+      <c r="JD4" t="s">
         <v>252</v>
       </c>
-      <c r="JA4" t="s">
+      <c r="JE4" t="s">
         <v>253</v>
       </c>
-      <c r="JB4" t="s">
+      <c r="JF4" t="s">
         <v>254</v>
       </c>
-      <c r="JC4" t="s">
+      <c r="JG4" t="s">
         <v>255</v>
       </c>
-      <c r="JD4" t="s">
+      <c r="JH4" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="JE4" t="s">
+      <c r="JI4" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="JF4" t="s">
+      <c r="JJ4" t="s">
+        <v>354</v>
+      </c>
+      <c r="JK4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="JG4" s="2" t="s">
+      <c r="JL4" t="s">
         <v>259</v>
       </c>
-      <c r="JH4" s="2" t="s">
+      <c r="JM4" t="s">
         <v>260</v>
       </c>
-      <c r="JI4" t="s">
-        <v>357</v>
-      </c>
-      <c r="JJ4" s="2" t="s">
+      <c r="JN4" t="s">
         <v>261</v>
       </c>
-      <c r="JK4" t="s">
+      <c r="JO4" t="s">
         <v>262</v>
       </c>
-      <c r="JL4" t="s">
+      <c r="JP4" t="s">
         <v>263</v>
       </c>
-      <c r="JM4" t="s">
+      <c r="JQ4" t="s">
         <v>264</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JR4" t="s">
         <v>265</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JS4" t="s">
         <v>266</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JT4" t="s">
         <v>267</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JU4" t="s">
         <v>268</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JV4" t="s">
         <v>269</v>
       </c>
-      <c r="JS4" t="s">
+      <c r="JW4" t="s">
         <v>270</v>
       </c>
-      <c r="JT4" t="s">
+      <c r="JX4" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JY4" t="s">
         <v>272</v>
       </c>
-      <c r="JV4" t="s">
+      <c r="JZ4" t="s">
         <v>273</v>
       </c>
-      <c r="JW4" s="2" t="s">
+      <c r="KA4" t="s">
         <v>274</v>
       </c>
-      <c r="JX4" t="s">
+      <c r="KB4" t="s">
         <v>275</v>
       </c>
-      <c r="JY4" t="s">
+      <c r="KC4" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="JZ4" t="s">
+      <c r="KD4" t="s">
         <v>277</v>
       </c>
-      <c r="KA4" t="s">
+      <c r="KE4" t="s">
         <v>278</v>
       </c>
-      <c r="KB4" s="2" t="s">
+      <c r="KF4" t="s">
         <v>279</v>
       </c>
-      <c r="KC4" t="s">
+      <c r="KG4" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KH4" t="s">
         <v>281</v>
       </c>
-      <c r="KE4" t="s">
+      <c r="KI4" t="s">
         <v>282</v>
       </c>
-      <c r="KF4" s="2" t="s">
+      <c r="KJ4" t="s">
         <v>283</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KK4" t="s">
         <v>284</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KL4" t="s">
         <v>285</v>
       </c>
-      <c r="KI4" t="s">
+      <c r="KM4" t="s">
         <v>286</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KN4" t="s">
         <v>287</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KO4" t="s">
         <v>288</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KP4" t="s">
         <v>289</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KQ4" t="s">
         <v>290</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KR4" t="s">
         <v>291</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KS4" t="s">
         <v>292</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KT4" t="s">
         <v>293</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KU4" t="s">
         <v>294</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KV4" t="s">
         <v>295</v>
       </c>
-      <c r="KS4" t="s">
+      <c r="KW4" t="s">
         <v>296</v>
       </c>
-      <c r="KT4" t="s">
+      <c r="KX4" t="s">
         <v>297</v>
       </c>
-      <c r="KU4" t="s">
+      <c r="KY4" t="s">
         <v>298</v>
       </c>
-      <c r="KV4" t="s">
+      <c r="KZ4" t="s">
         <v>299</v>
       </c>
-      <c r="KW4" t="s">
+      <c r="LA4" t="s">
         <v>300</v>
       </c>
-      <c r="KX4" t="s">
+      <c r="LB4" t="s">
         <v>301</v>
       </c>
-      <c r="KY4" t="s">
+      <c r="LC4" t="s">
         <v>302</v>
       </c>
-      <c r="KZ4" t="s">
+      <c r="LD4" t="s">
         <v>303</v>
       </c>
-      <c r="LA4" t="s">
+      <c r="LE4" t="s">
         <v>304</v>
       </c>
-      <c r="LB4" t="s">
+      <c r="LF4" t="s">
         <v>305</v>
       </c>
-      <c r="LC4" t="s">
+      <c r="LG4" t="s">
         <v>306</v>
       </c>
-      <c r="LD4" t="s">
+      <c r="LH4" t="s">
         <v>307</v>
       </c>
-      <c r="LE4" t="s">
+      <c r="LI4" t="s">
         <v>308</v>
       </c>
-      <c r="LF4" t="s">
+      <c r="LJ4" t="s">
         <v>309</v>
       </c>
-      <c r="LG4" t="s">
+      <c r="LK4" t="s">
         <v>310</v>
       </c>
-      <c r="LH4" t="s">
+      <c r="LL4" t="s">
         <v>311</v>
       </c>
-      <c r="LI4" t="s">
+      <c r="LM4" t="s">
         <v>312</v>
       </c>
-      <c r="LJ4" t="s">
+      <c r="LN4" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LK4" t="s">
+      <c r="LO4" t="s">
+        <v>316</v>
+      </c>
+      <c r="LP4" t="s">
+        <v>315</v>
+      </c>
+      <c r="LQ4" t="s">
         <v>314</v>
       </c>
-      <c r="LL4" t="s">
-        <v>315</v>
-      </c>
-      <c r="LM4" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="LN4" t="s">
-        <v>319</v>
-      </c>
-      <c r="LO4" t="s">
-        <v>318</v>
-      </c>
-      <c r="LP4" t="s">
-        <v>317</v>
-      </c>
-      <c r="LQ4" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="LR4" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="BL5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="BM5" t="s">
-        <v>321</v>
-      </c>
-      <c r="KW5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KX5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KY5" t="s">
-        <v>321</v>
-      </c>
-      <c r="LD5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="KZ5" t="s">
+        <v>318</v>
+      </c>
+      <c r="LE5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="W6" t="s">
-        <v>321</v>
-      </c>
-      <c r="LQ6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="LR6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CF8" t="s">
-        <v>321</v>
-      </c>
-      <c r="HV8" t="s">
-        <v>321</v>
-      </c>
-      <c r="HZ8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HW8" t="s">
+        <v>318</v>
+      </c>
+      <c r="IA8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CK9" t="s">
-        <v>321</v>
-      </c>
-      <c r="IH9" t="s">
-        <v>321</v>
-      </c>
-      <c r="IW9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="II9" t="s">
+        <v>318</v>
+      </c>
+      <c r="IX9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="N10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CK10" t="s">
-        <v>321</v>
-      </c>
-      <c r="IH10" t="s">
-        <v>321</v>
-      </c>
-      <c r="IW10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="II10" t="s">
+        <v>318</v>
+      </c>
+      <c r="IX10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="N11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CJ11" t="s">
-        <v>321</v>
-      </c>
-      <c r="IB11" t="s">
-        <v>321</v>
-      </c>
-      <c r="IV11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="12" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="IC11" t="s">
+        <v>318</v>
+      </c>
+      <c r="IW11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="N12" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="N13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CJ13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CK13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CR13" t="s">
-        <v>321</v>
-      </c>
-      <c r="IB13" t="s">
-        <v>321</v>
-      </c>
-      <c r="IH13" t="s">
-        <v>321</v>
-      </c>
-      <c r="IK13" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="IC13" t="s">
+        <v>318</v>
+      </c>
+      <c r="II13" t="s">
+        <v>318</v>
+      </c>
+      <c r="IL13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CJ14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CQ14" t="s">
-        <v>321</v>
-      </c>
-      <c r="IB14" t="s">
-        <v>321</v>
-      </c>
-      <c r="IL14" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="15" spans="1:329" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="IC14" t="s">
+        <v>318</v>
+      </c>
+      <c r="IM14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:329" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:307" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="N17" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DJ17" t="s">
-        <v>321</v>
-      </c>
-      <c r="HN17" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="18" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HO17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DK18" t="s">
-        <v>321</v>
-      </c>
-      <c r="HO18" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="19" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HP18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="N19" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DM19" t="s">
-        <v>321</v>
-      </c>
-      <c r="HP19" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="20" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HQ19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DL20" t="s">
-        <v>321</v>
-      </c>
-      <c r="HQ20" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HR20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DZ21" t="s">
-        <v>321</v>
-      </c>
-      <c r="IC21" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="ID21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="22" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="IE21" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="N22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="EA22" t="s">
-        <v>321</v>
-      </c>
-      <c r="IE22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="IF22" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="23" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="IG22" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="N23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="BZ23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CA23" t="s">
-        <v>321</v>
-      </c>
-      <c r="KB23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KC23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KD23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KE23" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="KF23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="N24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CB24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CC24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CS24" t="s">
-        <v>321</v>
-      </c>
-      <c r="KR24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KS24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KT24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="KU24" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="1:307" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="KV24" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:308" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="N25" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT25" t="s">
+        <v>318</v>
+      </c>
+      <c r="ED25" t="s">
+        <v>318</v>
+      </c>
+      <c r="JE25" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>344</v>
+      </c>
+      <c r="N26" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT26" t="s">
+        <v>318</v>
+      </c>
+      <c r="EG26" t="s">
+        <v>318</v>
+      </c>
+      <c r="JF26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>345</v>
+      </c>
+      <c r="N27" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT27" t="s">
+        <v>318</v>
+      </c>
+      <c r="EF27" t="s">
+        <v>318</v>
+      </c>
+      <c r="JH27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>346</v>
       </c>
-      <c r="N25" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT25" t="s">
-        <v>321</v>
-      </c>
-      <c r="ED25" t="s">
-        <v>321</v>
-      </c>
-      <c r="JD25" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="26" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="N28" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT28" t="s">
+        <v>318</v>
+      </c>
+      <c r="EE28" t="s">
+        <v>318</v>
+      </c>
+      <c r="JG28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>347</v>
       </c>
-      <c r="N26" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT26" t="s">
-        <v>321</v>
-      </c>
-      <c r="EG26" t="s">
-        <v>321</v>
-      </c>
-      <c r="JE26" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="27" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="N29" t="s">
+        <v>318</v>
+      </c>
+      <c r="DB29" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT29" t="s">
+        <v>318</v>
+      </c>
+      <c r="IT29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>348</v>
       </c>
-      <c r="N27" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT27" t="s">
-        <v>321</v>
-      </c>
-      <c r="EF27" t="s">
-        <v>321</v>
-      </c>
-      <c r="JG27" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="N30" t="s">
+        <v>318</v>
+      </c>
+      <c r="DC30" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT30" t="s">
+        <v>318</v>
+      </c>
+      <c r="IV30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>349</v>
       </c>
-      <c r="N28" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT28" t="s">
-        <v>321</v>
-      </c>
-      <c r="EE28" t="s">
-        <v>321</v>
-      </c>
-      <c r="JF28" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="29" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="N31" t="s">
+        <v>318</v>
+      </c>
+      <c r="DA31" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT31" t="s">
+        <v>318</v>
+      </c>
+      <c r="IR31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>350</v>
       </c>
-      <c r="N29" t="s">
-        <v>321</v>
-      </c>
-      <c r="DB29" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT29" t="s">
-        <v>321</v>
-      </c>
-      <c r="IS29" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="30" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>351</v>
-      </c>
-      <c r="N30" t="s">
-        <v>321</v>
-      </c>
-      <c r="DC30" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT30" t="s">
-        <v>321</v>
-      </c>
-      <c r="IU30" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="31" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="N32" t="s">
+        <v>318</v>
+      </c>
+      <c r="DE32" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT32" t="s">
+        <v>318</v>
+      </c>
+      <c r="HS32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>352</v>
       </c>
-      <c r="N31" t="s">
-        <v>321</v>
-      </c>
-      <c r="DA31" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT31" t="s">
-        <v>321</v>
-      </c>
-      <c r="IQ31" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="32" spans="1:307" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="N33" t="s">
+        <v>318</v>
+      </c>
+      <c r="EC33" t="s">
+        <v>318</v>
+      </c>
+      <c r="JY33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>353</v>
       </c>
-      <c r="N32" t="s">
-        <v>321</v>
-      </c>
-      <c r="DE32" t="s">
-        <v>321</v>
-      </c>
-      <c r="DT32" t="s">
-        <v>321</v>
-      </c>
-      <c r="HR32" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="33" spans="1:285" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>355</v>
-      </c>
-      <c r="N33" t="s">
-        <v>321</v>
-      </c>
-      <c r="EC33" t="s">
-        <v>321</v>
-      </c>
-      <c r="JX33" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="34" spans="1:285" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>356</v>
-      </c>
       <c r="N34" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="EI34" t="s">
-        <v>321</v>
-      </c>
-      <c r="JY34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="35" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="JZ34" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
       <c r="N35" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="DN35" t="s">
-        <v>321</v>
-      </c>
-      <c r="JI35" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="36" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="JJ35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>23</v>
       </c>
       <c r="N36" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="FA36" t="s">
-        <v>321</v>
-      </c>
-      <c r="IY36" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="IZ36" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="JA36" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="37" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>24</v>
       </c>
       <c r="N37" t="s">
-        <v>321</v>
-      </c>
-      <c r="JO37" t="s">
-        <v>321</v>
+        <v>318</v>
+      </c>
+      <c r="CS37" t="s">
+        <v>318</v>
       </c>
       <c r="JP37" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="38" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="JQ37" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="38" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="CS38" t="s">
-        <v>321</v>
-      </c>
-      <c r="JO38" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="JP38" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="39" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="JQ38" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>26</v>
       </c>
       <c r="N39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="EN39" t="s">
-        <v>321</v>
-      </c>
-      <c r="HL39" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="40" spans="1:285" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="HM39" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>318</v>
+      </c>
+      <c r="DW40" t="s">
+        <v>318</v>
+      </c>
+      <c r="HN40" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>318</v>
+      </c>
+      <c r="R41" t="s">
+        <v>318</v>
+      </c>
+      <c r="FB41" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>318</v>
+      </c>
+      <c r="P42" t="s">
+        <v>318</v>
+      </c>
+      <c r="R42" t="s">
+        <v>318</v>
+      </c>
+      <c r="FB42" t="s">
+        <v>318</v>
+      </c>
+      <c r="FC42" t="s">
+        <v>318</v>
+      </c>
+      <c r="FG42" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>318</v>
+      </c>
+      <c r="R43" t="s">
+        <v>318</v>
+      </c>
+      <c r="FB43" t="s">
+        <v>318</v>
+      </c>
+      <c r="FD43" t="s">
+        <v>318</v>
+      </c>
+      <c r="FE43" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="44" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>318</v>
+      </c>
+      <c r="R44" t="s">
+        <v>318</v>
+      </c>
+      <c r="FF44" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>318</v>
+      </c>
+      <c r="EV45" t="s">
+        <v>318</v>
+      </c>
+      <c r="KA45" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="46" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>318</v>
+      </c>
+      <c r="BU46" t="s">
+        <v>318</v>
+      </c>
+      <c r="GD46" t="s">
+        <v>318</v>
+      </c>
+      <c r="GE46" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="47" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:285" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>318</v>
+      </c>
+      <c r="S47" t="s">
+        <v>318</v>
+      </c>
+      <c r="T47" t="s">
+        <v>318</v>
+      </c>
+      <c r="U47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LK47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LL47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LM47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LN47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LO47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LP47" t="s">
+        <v>318</v>
+      </c>
+      <c r="LQ47" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:329" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>318</v>
+      </c>
+      <c r="BK48" t="s">
+        <v>318</v>
+      </c>
+      <c r="HI48" t="s">
+        <v>318</v>
+      </c>
+      <c r="HJ48" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>318</v>
+      </c>
+      <c r="BJ49" t="s">
+        <v>318</v>
+      </c>
+      <c r="HK49" t="s">
+        <v>318</v>
+      </c>
+      <c r="HL49" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>318</v>
+      </c>
+      <c r="DS50" t="s">
+        <v>318</v>
+      </c>
+      <c r="JK50" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>318</v>
+      </c>
+      <c r="N51" t="s">
+        <v>318</v>
+      </c>
+      <c r="BE51" t="s">
+        <v>318</v>
+      </c>
+      <c r="CI51" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="M52" t="s">
+        <v>318</v>
+      </c>
+      <c r="N52" t="s">
+        <v>318</v>
+      </c>
+      <c r="EK52" t="s">
+        <v>318</v>
+      </c>
+      <c r="EL52" t="s">
+        <v>318</v>
+      </c>
+      <c r="JL52" t="s">
+        <v>318</v>
+      </c>
+      <c r="JM52" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="53" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
+        <v>318</v>
+      </c>
+      <c r="AY53" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV53" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="54" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L54" t="s">
+        <v>318</v>
+      </c>
+      <c r="AW54" t="s">
+        <v>318</v>
+      </c>
+      <c r="GW54" t="s">
+        <v>318</v>
+      </c>
+      <c r="GX54" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="55" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L55" t="s">
+        <v>318</v>
+      </c>
+      <c r="AX55" t="s">
+        <v>318</v>
+      </c>
+      <c r="GY55" t="s">
+        <v>318</v>
+      </c>
+      <c r="GZ55" t="s">
+        <v>318</v>
+      </c>
+      <c r="HA55" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="56" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>318</v>
+      </c>
+      <c r="AZ56" t="s">
+        <v>318</v>
+      </c>
+      <c r="BA56" t="s">
+        <v>318</v>
+      </c>
+      <c r="BB56" t="s">
+        <v>318</v>
+      </c>
+      <c r="BC56" t="s">
+        <v>318</v>
+      </c>
+      <c r="BD56" t="s">
+        <v>318</v>
+      </c>
+      <c r="DV56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KI56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KJ56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KK56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KL56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KM56" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="57" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>318</v>
+      </c>
+      <c r="N57" t="s">
+        <v>318</v>
+      </c>
+      <c r="DI57" t="s">
+        <v>318</v>
+      </c>
+      <c r="GF57" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="58" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>318</v>
+      </c>
+      <c r="N58" t="s">
+        <v>318</v>
+      </c>
+      <c r="CG58" t="s">
+        <v>318</v>
+      </c>
+      <c r="CK58" t="s">
+        <v>318</v>
+      </c>
+      <c r="CL58" t="s">
+        <v>318</v>
+      </c>
+      <c r="KP58" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>46</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>318</v>
+      </c>
+      <c r="N59" t="s">
+        <v>318</v>
+      </c>
+      <c r="EH59" t="s">
+        <v>318</v>
+      </c>
+      <c r="II59" t="s">
+        <v>318</v>
+      </c>
+      <c r="IJ59" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="60" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>47</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="O60" t="s">
+        <v>318</v>
+      </c>
+      <c r="BO60" t="s">
+        <v>318</v>
+      </c>
+      <c r="LB60" t="s">
+        <v>318</v>
+      </c>
+      <c r="LC60" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>48</v>
+      </c>
+      <c r="E61" t="s">
+        <v>318</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>318</v>
+      </c>
+      <c r="DK61" t="s">
+        <v>318</v>
+      </c>
+      <c r="FR61" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="62" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>49</v>
+      </c>
+      <c r="E62" t="s">
+        <v>318</v>
+      </c>
+      <c r="AI62" t="s">
+        <v>318</v>
+      </c>
+      <c r="FS62" t="s">
+        <v>318</v>
+      </c>
+      <c r="FU62" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="63" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>50</v>
+      </c>
+      <c r="E63" t="s">
+        <v>318</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>318</v>
+      </c>
+      <c r="FT63" t="s">
+        <v>318</v>
+      </c>
+      <c r="FV63" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>51</v>
+      </c>
+      <c r="D64" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>318</v>
+      </c>
+      <c r="FI64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>52</v>
+      </c>
+      <c r="D65" t="s">
+        <v>318</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>318</v>
+      </c>
+      <c r="FL65" t="s">
+        <v>318</v>
+      </c>
+      <c r="FM65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>53</v>
+      </c>
+      <c r="D66" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>318</v>
+      </c>
+      <c r="FN66" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>54</v>
+      </c>
+      <c r="D67" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>318</v>
+      </c>
+      <c r="FI67" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="68" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>55</v>
+      </c>
+      <c r="C68" t="s">
+        <v>364</v>
+      </c>
+      <c r="D68" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>318</v>
+      </c>
+      <c r="FI68" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="69" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>56</v>
+      </c>
+      <c r="D69" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>318</v>
+      </c>
+      <c r="FH69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>57</v>
+      </c>
+      <c r="D70" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>318</v>
+      </c>
+      <c r="FK70" t="s">
+        <v>318</v>
+      </c>
+      <c r="FO70" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>58</v>
+      </c>
+      <c r="D71" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>318</v>
+      </c>
+      <c r="FK71" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>319</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>63</v>
+      </c>
+      <c r="H92" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="H93" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>64</v>
+      </c>
+      <c r="H94" t="s">
         <v>322</v>
       </c>
-      <c r="B70" s="3" t="s">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="8"/>
+      <c r="H95" t="s">
         <v>324</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>2</v>
+      </c>
+      <c r="B96" t="s">
         <v>5</v>
       </c>
-      <c r="D71" t="s">
-        <v>64</v>
-      </c>
-      <c r="H71" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="H72" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" t="s">
-        <v>65</v>
-      </c>
-      <c r="H73" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
-      <c r="H74" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
-        <v>2</v>
-      </c>
-      <c r="B75" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A96:A99"/>
     <mergeCell ref="C2:O2"/>
     <mergeCell ref="P2:EY2"/>
     <mergeCell ref="EZ2:LM2"/>
-    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A92:A95"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="GV4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
-    <hyperlink ref="HM4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
-    <hyperlink ref="HP4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
-    <hyperlink ref="IE4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
-    <hyperlink ref="IJ4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
-    <hyperlink ref="IT4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
-    <hyperlink ref="JG4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
-    <hyperlink ref="JH4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
-    <hyperlink ref="JJ4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
-    <hyperlink ref="JW4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
-    <hyperlink ref="KB4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
-    <hyperlink ref="KF4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
-    <hyperlink ref="LM4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
-    <hyperlink ref="LQ4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
+    <hyperlink ref="GW4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
+    <hyperlink ref="HN4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
+    <hyperlink ref="HQ4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
+    <hyperlink ref="IF4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
+    <hyperlink ref="IK4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
+    <hyperlink ref="IU4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
+    <hyperlink ref="JH4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
+    <hyperlink ref="JI4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
+    <hyperlink ref="JK4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JX4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="KC4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KG4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LN4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
+    <hyperlink ref="LR4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
homedirectordeTesis y añadiendo homes a requerimientos y matriz de trazablidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3F5175-09C3-4815-96A6-A23EE2485401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7173AC3-5511-4D76-9AA3-0A5912B17C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="367">
   <si>
     <t>MVC</t>
   </si>
@@ -1090,9 +1090,6 @@
     <t>/auth/verify</t>
   </si>
   <si>
-    <t>RegisterController.php   @validator</t>
-  </si>
-  <si>
     <t>/tesis/acta_examen</t>
   </si>
   <si>
@@ -1225,6 +1222,9 @@
   </si>
   <si>
     <t>Profesor Guia /Director Tesis</t>
+  </si>
+  <si>
+    <t>/director_escuelahome</t>
   </si>
 </sst>
 </file>
@@ -1666,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
   <dimension ref="A1:LR99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FI54" workbookViewId="0">
-      <selection activeCell="FK70" sqref="FK70"/>
+    <sheetView tabSelected="1" topLeftCell="BQ52" workbookViewId="0">
+      <selection activeCell="BT72" sqref="BT72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2166,7 @@
       <c r="EX2" s="7"/>
       <c r="EY2" s="7"/>
       <c r="EZ2" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="FA2" s="10"/>
       <c r="FB2" s="10"/>
@@ -2346,43 +2346,43 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="W3" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -2391,10 +2391,10 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -2409,13 +2409,13 @@
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
@@ -2423,7 +2423,7 @@
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
       <c r="BE3" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
@@ -2438,16 +2438,24 @@
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
+      <c r="BS3" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="BU3" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="BX3" s="1"/>
       <c r="BY3" s="1"/>
-      <c r="CD3" s="1"/>
+      <c r="BZ3" s="1"/>
       <c r="CE3" s="1"/>
       <c r="CF3" s="1"/>
       <c r="CG3" s="1"/>
@@ -2471,36 +2479,36 @@
       <c r="CY3" s="1"/>
       <c r="CZ3" s="1"/>
       <c r="DA3" s="1"/>
-      <c r="DB3" s="1" t="s">
-        <v>351</v>
-      </c>
+      <c r="DB3" s="1"/>
       <c r="DC3" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="DD3" s="1"/>
+        <v>350</v>
+      </c>
+      <c r="DD3" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
       <c r="DG3" s="1"/>
       <c r="DH3" s="1"/>
-      <c r="DI3" s="1" t="s">
+      <c r="DI3" s="1"/>
+      <c r="DJ3" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="DK3" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="DJ3" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="DK3" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="DL3" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="DM3" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="DN3" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="DO3" s="1"/>
+        <v>335</v>
+      </c>
+      <c r="DO3" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="DP3" s="1"/>
       <c r="DQ3" s="1"/>
       <c r="DR3" s="1"/>
@@ -2511,22 +2519,22 @@
       <c r="DW3" s="1"/>
       <c r="DX3" s="1"/>
       <c r="DY3" s="1"/>
-      <c r="DZ3" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="EA3" s="1"/>
+      <c r="DZ3" s="1"/>
+      <c r="EA3" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="EB3" s="1"/>
       <c r="EC3" s="1"/>
-      <c r="ED3" s="1" t="s">
-        <v>351</v>
-      </c>
+      <c r="ED3" s="1"/>
       <c r="EE3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="EF3" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="EG3" s="1"/>
+        <v>350</v>
+      </c>
+      <c r="EG3" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
       <c r="EJ3" s="1"/>
@@ -2541,95 +2549,96 @@
       <c r="ES3" s="1"/>
       <c r="ET3" s="1"/>
       <c r="EU3" s="1"/>
-      <c r="EV3" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="EW3" s="1"/>
+      <c r="EV3" s="1"/>
+      <c r="EW3" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="EX3" s="1"/>
       <c r="EY3" s="1"/>
       <c r="EZ3" s="1"/>
       <c r="FA3" s="1"/>
       <c r="FB3" s="1"/>
-      <c r="FH3" t="s">
-        <v>351</v>
-      </c>
+      <c r="FC3" s="1"/>
       <c r="FI3" t="s">
-        <v>365</v>
-      </c>
-      <c r="GD3" t="s">
+        <v>350</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>364</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>331</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>331</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>350</v>
+      </c>
+      <c r="HJ3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>331</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>335</v>
+      </c>
+      <c r="IE3" t="s">
+        <v>330</v>
+      </c>
+      <c r="IK3" t="s">
         <v>332</v>
-      </c>
-      <c r="GE3" t="s">
-        <v>332</v>
-      </c>
-      <c r="GV3" t="s">
-        <v>351</v>
-      </c>
-      <c r="HI3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HJ3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HK3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HL3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HO3" t="s">
-        <v>332</v>
-      </c>
-      <c r="HP3" t="s">
-        <v>332</v>
-      </c>
-      <c r="HQ3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HR3" t="s">
-        <v>336</v>
-      </c>
-      <c r="ID3" t="s">
-        <v>331</v>
-      </c>
-      <c r="IJ3" t="s">
-        <v>333</v>
-      </c>
-      <c r="IK3" t="s">
-        <v>335</v>
       </c>
       <c r="IL3" t="s">
         <v>334</v>
       </c>
       <c r="IM3" t="s">
-        <v>332</v>
-      </c>
-      <c r="IT3" t="s">
-        <v>351</v>
-      </c>
-      <c r="IV3" t="s">
-        <v>351</v>
-      </c>
-      <c r="IX3" t="s">
+        <v>333</v>
+      </c>
+      <c r="IN3" t="s">
         <v>331</v>
+      </c>
+      <c r="IU3" t="s">
+        <v>350</v>
+      </c>
+      <c r="IW3" t="s">
+        <v>350</v>
       </c>
       <c r="IY3" t="s">
         <v>330</v>
       </c>
-      <c r="JJ3" t="s">
+      <c r="IZ3" t="s">
+        <v>329</v>
+      </c>
+      <c r="JK3" t="s">
+        <v>354</v>
+      </c>
+      <c r="KB3" t="s">
         <v>355</v>
       </c>
-      <c r="KA3" t="s">
-        <v>356</v>
-      </c>
-      <c r="LA3" t="s">
-        <v>362</v>
-      </c>
       <c r="LB3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="LC3" t="s">
-        <v>362</v>
+        <v>361</v>
+      </c>
+      <c r="LD3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:330" x14ac:dyDescent="0.25">
@@ -2781,7 +2790,7 @@
         <v>50</v>
       </c>
       <c r="AY4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AZ4" t="s">
         <v>52</v>
@@ -2817,7 +2826,7 @@
         <v>62</v>
       </c>
       <c r="BK4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="BL4" t="s">
         <v>63</v>
@@ -2853,772 +2862,772 @@
         <v>73</v>
       </c>
       <c r="BW4" t="s">
+        <v>366</v>
+      </c>
+      <c r="BX4" t="s">
         <v>74</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="BY4" t="s">
         <v>75</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" t="s">
         <v>76</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CA4" t="s">
+        <v>338</v>
+      </c>
+      <c r="CB4" t="s">
         <v>339</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CC4" t="s">
         <v>340</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CD4" t="s">
         <v>341</v>
       </c>
-      <c r="CC4" t="s">
-        <v>342</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>329</v>
-      </c>
       <c r="CE4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CF4" t="s">
         <v>77</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>78</v>
       </c>
-      <c r="CG4" t="s">
-        <v>361</v>
-      </c>
       <c r="CH4" t="s">
+        <v>360</v>
+      </c>
+      <c r="CI4" t="s">
         <v>79</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CJ4" t="s">
         <v>80</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CK4" t="s">
         <v>81</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CL4" t="s">
         <v>82</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>83</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>84</v>
       </c>
       <c r="CN4" t="s">
         <v>84</v>
       </c>
       <c r="CO4" t="s">
+        <v>84</v>
+      </c>
+      <c r="CP4" t="s">
         <v>85</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>86</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CR4" t="s">
         <v>87</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CS4" t="s">
         <v>88</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CT4" t="s">
         <v>89</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CU4" t="s">
         <v>90</v>
-      </c>
-      <c r="CU4" t="s">
-        <v>91</v>
       </c>
       <c r="CV4" t="s">
         <v>91</v>
       </c>
       <c r="CW4" t="s">
+        <v>91</v>
+      </c>
+      <c r="CX4" t="s">
         <v>92</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="CY4" t="s">
         <v>93</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="CZ4" t="s">
         <v>94</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DA4" t="s">
         <v>95</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DB4" t="s">
         <v>96</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DC4" t="s">
         <v>97</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DD4" t="s">
         <v>98</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DE4" t="s">
         <v>99</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DF4" t="s">
         <v>100</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DG4" t="s">
         <v>101</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DH4" t="s">
         <v>102</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DI4" t="s">
         <v>103</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DJ4" t="s">
         <v>104</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DK4" t="s">
         <v>105</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DL4" t="s">
         <v>106</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DM4" t="s">
         <v>107</v>
       </c>
-      <c r="DM4" t="s">
+      <c r="DN4" t="s">
         <v>108</v>
       </c>
-      <c r="DN4" t="s">
+      <c r="DO4" t="s">
         <v>109</v>
       </c>
-      <c r="DO4" t="s">
+      <c r="DP4" t="s">
         <v>110</v>
       </c>
-      <c r="DP4" t="s">
+      <c r="DQ4" t="s">
         <v>111</v>
       </c>
-      <c r="DQ4" t="s">
+      <c r="DR4" t="s">
         <v>112</v>
       </c>
-      <c r="DR4" t="s">
+      <c r="DS4" t="s">
         <v>113</v>
       </c>
-      <c r="DS4" t="s">
+      <c r="DT4" t="s">
         <v>114</v>
       </c>
-      <c r="DT4" t="s">
+      <c r="DU4" t="s">
         <v>115</v>
       </c>
-      <c r="DU4" t="s">
+      <c r="DV4" t="s">
         <v>116</v>
       </c>
-      <c r="DV4" t="s">
-        <v>360</v>
-      </c>
       <c r="DW4" t="s">
+        <v>359</v>
+      </c>
+      <c r="DX4" t="s">
         <v>117</v>
       </c>
-      <c r="DX4" t="s">
+      <c r="DY4" t="s">
         <v>118</v>
       </c>
-      <c r="DY4" t="s">
+      <c r="DZ4" t="s">
         <v>119</v>
       </c>
-      <c r="DZ4" t="s">
+      <c r="EA4" t="s">
         <v>121</v>
       </c>
-      <c r="EA4" t="s">
+      <c r="EB4" t="s">
         <v>120</v>
       </c>
-      <c r="EB4" t="s">
+      <c r="EC4" t="s">
         <v>122</v>
       </c>
-      <c r="EC4" t="s">
+      <c r="ED4" t="s">
         <v>123</v>
       </c>
-      <c r="ED4" t="s">
+      <c r="EE4" t="s">
         <v>124</v>
       </c>
-      <c r="EE4" t="s">
+      <c r="EF4" t="s">
         <v>125</v>
       </c>
-      <c r="EF4" t="s">
+      <c r="EG4" t="s">
         <v>126</v>
       </c>
-      <c r="EG4" t="s">
+      <c r="EH4" t="s">
         <v>127</v>
       </c>
-      <c r="EH4" t="s">
+      <c r="EI4" t="s">
         <v>128</v>
       </c>
-      <c r="EI4" t="s">
+      <c r="EJ4" t="s">
         <v>129</v>
       </c>
-      <c r="EJ4" t="s">
+      <c r="EK4" t="s">
         <v>130</v>
       </c>
-      <c r="EK4" t="s">
+      <c r="EL4" t="s">
         <v>131</v>
       </c>
-      <c r="EL4" t="s">
+      <c r="EM4" t="s">
         <v>132</v>
       </c>
-      <c r="EM4" t="s">
+      <c r="EN4" t="s">
         <v>133</v>
       </c>
-      <c r="EN4" t="s">
+      <c r="EO4" t="s">
         <v>134</v>
       </c>
-      <c r="EO4" t="s">
+      <c r="EP4" t="s">
         <v>135</v>
       </c>
-      <c r="EP4" t="s">
+      <c r="EQ4" t="s">
         <v>136</v>
       </c>
-      <c r="EQ4" t="s">
+      <c r="ER4" t="s">
         <v>137</v>
       </c>
-      <c r="ER4" t="s">
+      <c r="ES4" t="s">
         <v>138</v>
       </c>
-      <c r="ES4" t="s">
+      <c r="ET4" t="s">
         <v>139</v>
       </c>
-      <c r="ET4" t="s">
+      <c r="EU4" t="s">
         <v>140</v>
       </c>
-      <c r="EU4" t="s">
+      <c r="EV4" t="s">
         <v>141</v>
       </c>
-      <c r="EV4" t="s">
+      <c r="EW4" t="s">
         <v>142</v>
       </c>
-      <c r="EW4" t="s">
+      <c r="EX4" t="s">
         <v>143</v>
       </c>
-      <c r="EX4" t="s">
+      <c r="EY4" t="s">
         <v>144</v>
       </c>
-      <c r="EY4" t="s">
+      <c r="EZ4" t="s">
         <v>145</v>
       </c>
-      <c r="EZ4" t="s">
+      <c r="FA4" t="s">
         <v>146</v>
       </c>
-      <c r="FA4" t="s">
+      <c r="FB4" t="s">
         <v>147</v>
       </c>
-      <c r="FB4" t="s">
+      <c r="FC4" t="s">
         <v>148</v>
       </c>
-      <c r="FC4" t="s">
+      <c r="FD4" t="s">
         <v>149</v>
       </c>
-      <c r="FD4" t="s">
+      <c r="FE4" t="s">
         <v>150</v>
       </c>
-      <c r="FE4" t="s">
+      <c r="FF4" t="s">
         <v>151</v>
       </c>
-      <c r="FF4" t="s">
+      <c r="FG4" t="s">
         <v>152</v>
       </c>
-      <c r="FG4" t="s">
+      <c r="FH4" t="s">
         <v>153</v>
       </c>
-      <c r="FH4" t="s">
+      <c r="FI4" t="s">
         <v>154</v>
       </c>
-      <c r="FI4" t="s">
+      <c r="FJ4" t="s">
         <v>155</v>
       </c>
-      <c r="FJ4" t="s">
+      <c r="FK4" t="s">
         <v>156</v>
       </c>
-      <c r="FK4" t="s">
+      <c r="FL4" t="s">
         <v>157</v>
       </c>
-      <c r="FL4" t="s">
+      <c r="FM4" t="s">
         <v>158</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FN4" t="s">
         <v>159</v>
       </c>
-      <c r="FN4" t="s">
+      <c r="FO4" t="s">
         <v>160</v>
       </c>
-      <c r="FO4" t="s">
+      <c r="FP4" t="s">
         <v>161</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FQ4" t="s">
         <v>162</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FR4" t="s">
         <v>163</v>
       </c>
-      <c r="FR4" t="s">
+      <c r="FS4" t="s">
         <v>164</v>
       </c>
-      <c r="FS4" t="s">
+      <c r="FT4" t="s">
         <v>165</v>
       </c>
-      <c r="FT4" t="s">
+      <c r="FU4" t="s">
         <v>166</v>
       </c>
-      <c r="FU4" t="s">
+      <c r="FV4" t="s">
         <v>167</v>
       </c>
-      <c r="FV4" t="s">
-        <v>363</v>
-      </c>
       <c r="FW4" t="s">
+        <v>362</v>
+      </c>
+      <c r="FX4" t="s">
         <v>168</v>
       </c>
-      <c r="FX4" t="s">
+      <c r="FY4" t="s">
         <v>169</v>
       </c>
-      <c r="FY4" t="s">
+      <c r="FZ4" t="s">
         <v>170</v>
       </c>
-      <c r="FZ4" t="s">
+      <c r="GA4" t="s">
         <v>171</v>
       </c>
-      <c r="GA4" t="s">
+      <c r="GB4" t="s">
         <v>172</v>
       </c>
-      <c r="GB4" t="s">
+      <c r="GC4" t="s">
         <v>173</v>
       </c>
-      <c r="GC4" t="s">
+      <c r="GD4" t="s">
         <v>174</v>
       </c>
-      <c r="GD4" t="s">
+      <c r="GE4" t="s">
         <v>175</v>
       </c>
-      <c r="GE4" t="s">
+      <c r="GF4" t="s">
         <v>176</v>
       </c>
-      <c r="GF4" t="s">
+      <c r="GG4" t="s">
         <v>177</v>
       </c>
-      <c r="GG4" t="s">
+      <c r="GH4" t="s">
         <v>178</v>
       </c>
-      <c r="GH4" t="s">
+      <c r="GI4" t="s">
         <v>179</v>
       </c>
-      <c r="GI4" t="s">
+      <c r="GJ4" t="s">
         <v>180</v>
       </c>
-      <c r="GJ4" t="s">
+      <c r="GK4" t="s">
         <v>181</v>
       </c>
-      <c r="GK4" t="s">
+      <c r="GL4" t="s">
         <v>182</v>
       </c>
-      <c r="GL4" t="s">
+      <c r="GM4" t="s">
         <v>183</v>
       </c>
-      <c r="GM4" t="s">
+      <c r="GN4" t="s">
         <v>184</v>
       </c>
-      <c r="GN4" t="s">
+      <c r="GO4" t="s">
         <v>185</v>
       </c>
-      <c r="GO4" t="s">
+      <c r="GP4" t="s">
         <v>186</v>
       </c>
-      <c r="GP4" t="s">
+      <c r="GQ4" t="s">
         <v>187</v>
       </c>
-      <c r="GQ4" t="s">
+      <c r="GR4" t="s">
         <v>188</v>
       </c>
-      <c r="GR4" t="s">
+      <c r="GS4" t="s">
         <v>189</v>
       </c>
-      <c r="GS4" t="s">
+      <c r="GT4" t="s">
         <v>190</v>
       </c>
-      <c r="GT4" t="s">
+      <c r="GU4" t="s">
         <v>191</v>
       </c>
-      <c r="GU4" s="2" t="s">
+      <c r="GV4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="GV4" t="s">
+      <c r="GW4" t="s">
         <v>193</v>
       </c>
-      <c r="GW4" s="2" t="s">
+      <c r="GX4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="GX4" t="s">
+      <c r="GY4" t="s">
         <v>195</v>
       </c>
-      <c r="GY4" t="s">
+      <c r="GZ4" t="s">
         <v>196</v>
       </c>
-      <c r="GZ4" t="s">
+      <c r="HA4" t="s">
         <v>197</v>
       </c>
-      <c r="HA4" t="s">
+      <c r="HB4" t="s">
         <v>198</v>
       </c>
-      <c r="HB4" t="s">
+      <c r="HC4" t="s">
         <v>199</v>
       </c>
-      <c r="HC4" t="s">
+      <c r="HD4" t="s">
         <v>200</v>
       </c>
-      <c r="HD4" t="s">
+      <c r="HE4" t="s">
         <v>201</v>
       </c>
-      <c r="HE4" t="s">
+      <c r="HF4" t="s">
         <v>202</v>
       </c>
-      <c r="HF4" t="s">
+      <c r="HG4" t="s">
         <v>203</v>
       </c>
-      <c r="HG4" t="s">
+      <c r="HH4" t="s">
         <v>204</v>
       </c>
-      <c r="HH4" t="s">
+      <c r="HI4" t="s">
         <v>205</v>
       </c>
-      <c r="HI4" t="s">
+      <c r="HJ4" t="s">
         <v>206</v>
       </c>
-      <c r="HJ4" t="s">
+      <c r="HK4" t="s">
         <v>207</v>
       </c>
-      <c r="HK4" t="s">
+      <c r="HL4" t="s">
         <v>208</v>
       </c>
-      <c r="HL4" t="s">
+      <c r="HM4" t="s">
         <v>209</v>
       </c>
-      <c r="HM4" t="s">
+      <c r="HN4" t="s">
         <v>210</v>
       </c>
-      <c r="HN4" s="2" t="s">
+      <c r="HO4" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="HO4" t="s">
+      <c r="HP4" t="s">
         <v>212</v>
       </c>
-      <c r="HP4" t="s">
+      <c r="HQ4" t="s">
         <v>213</v>
       </c>
-      <c r="HQ4" s="2" t="s">
+      <c r="HR4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="HR4" t="s">
+      <c r="HS4" t="s">
         <v>215</v>
       </c>
-      <c r="HS4" t="s">
+      <c r="HT4" t="s">
         <v>216</v>
       </c>
-      <c r="HT4" t="s">
+      <c r="HU4" t="s">
         <v>217</v>
       </c>
-      <c r="HU4" t="s">
+      <c r="HV4" t="s">
         <v>218</v>
       </c>
-      <c r="HV4" t="s">
+      <c r="HW4" t="s">
         <v>219</v>
       </c>
-      <c r="HW4" t="s">
+      <c r="HX4" t="s">
         <v>220</v>
       </c>
-      <c r="HX4" t="s">
+      <c r="HY4" t="s">
         <v>221</v>
       </c>
-      <c r="HY4" t="s">
+      <c r="HZ4" t="s">
         <v>222</v>
       </c>
-      <c r="HZ4" t="s">
+      <c r="IA4" t="s">
         <v>223</v>
       </c>
-      <c r="IA4" t="s">
+      <c r="IB4" t="s">
         <v>224</v>
       </c>
-      <c r="IB4" t="s">
+      <c r="IC4" t="s">
         <v>225</v>
       </c>
-      <c r="IC4" t="s">
+      <c r="ID4" t="s">
         <v>226</v>
       </c>
-      <c r="ID4" t="s">
-        <v>337</v>
-      </c>
       <c r="IE4" t="s">
+        <v>336</v>
+      </c>
+      <c r="IF4" t="s">
         <v>227</v>
       </c>
-      <c r="IF4" s="2" t="s">
+      <c r="IG4" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="IG4" t="s">
+      <c r="IH4" t="s">
         <v>229</v>
       </c>
-      <c r="IH4" t="s">
+      <c r="II4" t="s">
         <v>230</v>
       </c>
-      <c r="II4" t="s">
+      <c r="IJ4" t="s">
         <v>231</v>
       </c>
-      <c r="IJ4" t="s">
+      <c r="IK4" t="s">
         <v>232</v>
       </c>
-      <c r="IK4" s="2" t="s">
+      <c r="IL4" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="IL4" t="s">
+      <c r="IM4" t="s">
         <v>234</v>
       </c>
-      <c r="IM4" t="s">
+      <c r="IN4" t="s">
         <v>235</v>
       </c>
-      <c r="IN4" t="s">
+      <c r="IO4" t="s">
         <v>236</v>
       </c>
-      <c r="IO4" t="s">
+      <c r="IP4" t="s">
         <v>237</v>
       </c>
-      <c r="IP4" t="s">
+      <c r="IQ4" t="s">
         <v>238</v>
       </c>
-      <c r="IQ4" t="s">
+      <c r="IR4" t="s">
         <v>239</v>
       </c>
-      <c r="IR4" t="s">
+      <c r="IS4" t="s">
         <v>240</v>
       </c>
-      <c r="IS4" t="s">
+      <c r="IT4" t="s">
         <v>241</v>
       </c>
-      <c r="IT4" t="s">
+      <c r="IU4" t="s">
         <v>242</v>
       </c>
-      <c r="IU4" s="2" t="s">
+      <c r="IV4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="IV4" t="s">
+      <c r="IW4" t="s">
         <v>244</v>
       </c>
-      <c r="IW4" t="s">
+      <c r="IX4" t="s">
         <v>245</v>
       </c>
-      <c r="IX4" t="s">
+      <c r="IY4" t="s">
         <v>246</v>
       </c>
-      <c r="IY4" t="s">
+      <c r="IZ4" t="s">
         <v>247</v>
       </c>
-      <c r="IZ4" t="s">
+      <c r="JA4" t="s">
         <v>248</v>
       </c>
-      <c r="JA4" t="s">
+      <c r="JB4" t="s">
         <v>249</v>
       </c>
-      <c r="JB4" t="s">
+      <c r="JC4" t="s">
         <v>250</v>
       </c>
-      <c r="JC4" t="s">
+      <c r="JD4" t="s">
         <v>251</v>
       </c>
-      <c r="JD4" t="s">
+      <c r="JE4" t="s">
         <v>252</v>
       </c>
-      <c r="JE4" t="s">
+      <c r="JF4" t="s">
         <v>253</v>
       </c>
-      <c r="JF4" t="s">
+      <c r="JG4" t="s">
         <v>254</v>
       </c>
-      <c r="JG4" t="s">
+      <c r="JH4" t="s">
         <v>255</v>
       </c>
-      <c r="JH4" s="2" t="s">
+      <c r="JI4" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="JI4" s="2" t="s">
+      <c r="JJ4" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="JJ4" t="s">
-        <v>354</v>
-      </c>
-      <c r="JK4" s="2" t="s">
+      <c r="JK4" t="s">
+        <v>353</v>
+      </c>
+      <c r="JL4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="JL4" t="s">
+      <c r="JM4" t="s">
         <v>259</v>
       </c>
-      <c r="JM4" t="s">
+      <c r="JN4" t="s">
         <v>260</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JO4" t="s">
         <v>261</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JP4" t="s">
         <v>262</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JQ4" t="s">
         <v>263</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JR4" t="s">
         <v>264</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JS4" t="s">
         <v>265</v>
       </c>
-      <c r="JS4" t="s">
+      <c r="JT4" t="s">
         <v>266</v>
       </c>
-      <c r="JT4" t="s">
+      <c r="JU4" t="s">
         <v>267</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JV4" t="s">
         <v>268</v>
       </c>
-      <c r="JV4" t="s">
+      <c r="JW4" t="s">
         <v>269</v>
       </c>
-      <c r="JW4" t="s">
+      <c r="JX4" t="s">
         <v>270</v>
       </c>
-      <c r="JX4" s="2" t="s">
+      <c r="JY4" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="JY4" t="s">
+      <c r="JZ4" t="s">
         <v>272</v>
       </c>
-      <c r="JZ4" t="s">
+      <c r="KA4" t="s">
         <v>273</v>
       </c>
-      <c r="KA4" t="s">
+      <c r="KB4" t="s">
         <v>274</v>
       </c>
-      <c r="KB4" t="s">
+      <c r="KC4" t="s">
         <v>275</v>
       </c>
-      <c r="KC4" s="2" t="s">
+      <c r="KD4" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KE4" t="s">
         <v>277</v>
       </c>
-      <c r="KE4" t="s">
+      <c r="KF4" t="s">
         <v>278</v>
       </c>
-      <c r="KF4" t="s">
+      <c r="KG4" t="s">
         <v>279</v>
       </c>
-      <c r="KG4" s="2" t="s">
+      <c r="KH4" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KI4" t="s">
         <v>281</v>
       </c>
-      <c r="KI4" t="s">
+      <c r="KJ4" t="s">
         <v>282</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KK4" t="s">
         <v>283</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KL4" t="s">
         <v>284</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KM4" t="s">
         <v>285</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KN4" t="s">
         <v>286</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KO4" t="s">
         <v>287</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KP4" t="s">
         <v>288</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KQ4" t="s">
         <v>289</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KR4" t="s">
         <v>290</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KS4" t="s">
         <v>291</v>
       </c>
-      <c r="KS4" t="s">
+      <c r="KT4" t="s">
         <v>292</v>
       </c>
-      <c r="KT4" t="s">
+      <c r="KU4" t="s">
         <v>293</v>
       </c>
-      <c r="KU4" t="s">
+      <c r="KV4" t="s">
         <v>294</v>
       </c>
-      <c r="KV4" t="s">
+      <c r="KW4" t="s">
         <v>295</v>
       </c>
-      <c r="KW4" t="s">
+      <c r="KX4" t="s">
         <v>296</v>
       </c>
-      <c r="KX4" t="s">
+      <c r="KY4" t="s">
         <v>297</v>
       </c>
-      <c r="KY4" t="s">
+      <c r="KZ4" t="s">
         <v>298</v>
       </c>
-      <c r="KZ4" t="s">
+      <c r="LA4" t="s">
         <v>299</v>
       </c>
-      <c r="LA4" t="s">
+      <c r="LB4" t="s">
         <v>300</v>
       </c>
-      <c r="LB4" t="s">
+      <c r="LC4" t="s">
         <v>301</v>
       </c>
-      <c r="LC4" t="s">
+      <c r="LD4" t="s">
         <v>302</v>
       </c>
-      <c r="LD4" t="s">
+      <c r="LE4" t="s">
         <v>303</v>
       </c>
-      <c r="LE4" t="s">
+      <c r="LF4" t="s">
         <v>304</v>
       </c>
-      <c r="LF4" t="s">
+      <c r="LG4" t="s">
         <v>305</v>
       </c>
-      <c r="LG4" t="s">
+      <c r="LH4" t="s">
         <v>306</v>
       </c>
-      <c r="LH4" t="s">
+      <c r="LI4" t="s">
         <v>307</v>
       </c>
-      <c r="LI4" t="s">
+      <c r="LJ4" t="s">
         <v>308</v>
       </c>
-      <c r="LJ4" t="s">
+      <c r="LK4" t="s">
         <v>309</v>
       </c>
-      <c r="LK4" t="s">
+      <c r="LL4" t="s">
         <v>310</v>
       </c>
-      <c r="LL4" t="s">
+      <c r="LM4" t="s">
         <v>311</v>
       </c>
-      <c r="LM4" t="s">
+      <c r="LN4" t="s">
         <v>312</v>
       </c>
-      <c r="LN4" s="2" t="s">
+      <c r="LO4" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LO4" t="s">
+      <c r="LP4" t="s">
         <v>316</v>
       </c>
-      <c r="LP4" t="s">
+      <c r="LQ4" t="s">
         <v>315</v>
       </c>
-      <c r="LQ4" t="s">
+      <c r="LR4" t="s">
         <v>314</v>
-      </c>
-      <c r="LR4" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:330" x14ac:dyDescent="0.25">
@@ -3634,16 +3643,16 @@
       <c r="BM5" t="s">
         <v>318</v>
       </c>
-      <c r="KX5" t="s">
-        <v>318</v>
-      </c>
       <c r="KY5" t="s">
         <v>318</v>
       </c>
       <c r="KZ5" t="s">
         <v>318</v>
       </c>
-      <c r="LE5" t="s">
+      <c r="LA5" t="s">
+        <v>318</v>
+      </c>
+      <c r="LF5" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3657,9 +3666,6 @@
       <c r="W6" t="s">
         <v>318</v>
       </c>
-      <c r="LR6" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="7" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3679,13 +3685,13 @@
       <c r="V8" t="s">
         <v>318</v>
       </c>
-      <c r="CF8" t="s">
-        <v>318</v>
-      </c>
-      <c r="HW8" t="s">
-        <v>318</v>
-      </c>
-      <c r="IA8" t="s">
+      <c r="CG8" t="s">
+        <v>318</v>
+      </c>
+      <c r="HX8" t="s">
+        <v>318</v>
+      </c>
+      <c r="IB8" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3696,13 +3702,13 @@
       <c r="N9" t="s">
         <v>318</v>
       </c>
-      <c r="CK9" t="s">
-        <v>318</v>
-      </c>
-      <c r="II9" t="s">
-        <v>318</v>
-      </c>
-      <c r="IX9" t="s">
+      <c r="CL9" t="s">
+        <v>318</v>
+      </c>
+      <c r="IJ9" t="s">
+        <v>318</v>
+      </c>
+      <c r="IY9" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3713,13 +3719,13 @@
       <c r="N10" t="s">
         <v>318</v>
       </c>
-      <c r="CK10" t="s">
-        <v>318</v>
-      </c>
-      <c r="II10" t="s">
-        <v>318</v>
-      </c>
-      <c r="IX10" t="s">
+      <c r="CL10" t="s">
+        <v>318</v>
+      </c>
+      <c r="IJ10" t="s">
+        <v>318</v>
+      </c>
+      <c r="IY10" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3730,13 +3736,13 @@
       <c r="N11" t="s">
         <v>318</v>
       </c>
-      <c r="CJ11" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC11" t="s">
-        <v>318</v>
-      </c>
-      <c r="IW11" t="s">
+      <c r="CK11" t="s">
+        <v>318</v>
+      </c>
+      <c r="ID11" t="s">
+        <v>318</v>
+      </c>
+      <c r="IX11" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3755,22 +3761,22 @@
       <c r="N13" t="s">
         <v>318</v>
       </c>
-      <c r="CJ13" t="s">
-        <v>318</v>
-      </c>
       <c r="CK13" t="s">
         <v>318</v>
       </c>
-      <c r="CR13" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC13" t="s">
-        <v>318</v>
-      </c>
-      <c r="II13" t="s">
-        <v>318</v>
-      </c>
-      <c r="IL13" t="s">
+      <c r="CL13" t="s">
+        <v>318</v>
+      </c>
+      <c r="CS13" t="s">
+        <v>318</v>
+      </c>
+      <c r="ID13" t="s">
+        <v>318</v>
+      </c>
+      <c r="IJ13" t="s">
+        <v>318</v>
+      </c>
+      <c r="IM13" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3781,16 +3787,16 @@
       <c r="N14" t="s">
         <v>318</v>
       </c>
-      <c r="CJ14" t="s">
-        <v>318</v>
-      </c>
-      <c r="CQ14" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC14" t="s">
-        <v>318</v>
-      </c>
-      <c r="IM14" t="s">
+      <c r="CK14" t="s">
+        <v>318</v>
+      </c>
+      <c r="CR14" t="s">
+        <v>318</v>
+      </c>
+      <c r="ID14" t="s">
+        <v>318</v>
+      </c>
+      <c r="IN14" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3804,110 +3810,107 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:308" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="N17" t="s">
         <v>318</v>
       </c>
-      <c r="DJ17" t="s">
-        <v>318</v>
-      </c>
-      <c r="HO17" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="DK17" t="s">
+        <v>318</v>
+      </c>
+      <c r="HP17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="N18" t="s">
         <v>318</v>
       </c>
-      <c r="DK18" t="s">
-        <v>318</v>
-      </c>
-      <c r="HP18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="DL18" t="s">
+        <v>318</v>
+      </c>
+      <c r="HQ18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="N19" t="s">
         <v>318</v>
       </c>
-      <c r="DM19" t="s">
-        <v>318</v>
-      </c>
-      <c r="HQ19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="DN19" t="s">
+        <v>318</v>
+      </c>
+      <c r="HR19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="N20" t="s">
         <v>318</v>
       </c>
-      <c r="DL20" t="s">
-        <v>318</v>
-      </c>
-      <c r="HR20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="DM20" t="s">
+        <v>318</v>
+      </c>
+      <c r="HS20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="N21" t="s">
         <v>318</v>
       </c>
-      <c r="DZ21" t="s">
-        <v>318</v>
-      </c>
-      <c r="ID21" t="s">
+      <c r="EA21" t="s">
         <v>318</v>
       </c>
       <c r="IE21" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="22" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="IF21" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="N22" t="s">
         <v>318</v>
       </c>
-      <c r="EA22" t="s">
-        <v>318</v>
-      </c>
-      <c r="IF22" t="s">
+      <c r="EB22" t="s">
         <v>318</v>
       </c>
       <c r="IG22" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="23" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="IH22" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="N23" t="s">
         <v>318</v>
       </c>
-      <c r="BZ23" t="s">
-        <v>318</v>
-      </c>
       <c r="CA23" t="s">
         <v>318</v>
       </c>
-      <c r="KC23" t="s">
+      <c r="CB23" t="s">
         <v>318</v>
       </c>
       <c r="KD23" t="s">
@@ -3919,24 +3922,24 @@
       <c r="KF23" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="24" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="KG23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="N24" t="s">
         <v>318</v>
       </c>
-      <c r="CB24" t="s">
-        <v>318</v>
-      </c>
       <c r="CC24" t="s">
         <v>318</v>
       </c>
-      <c r="CS24" t="s">
-        <v>318</v>
-      </c>
-      <c r="KS24" t="s">
+      <c r="CD24" t="s">
+        <v>318</v>
+      </c>
+      <c r="CT24" t="s">
         <v>318</v>
       </c>
       <c r="KT24" t="s">
@@ -3948,265 +3951,268 @@
       <c r="KV24" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="25" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="KW24" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="N25" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>318</v>
+      </c>
+      <c r="EE25" t="s">
+        <v>318</v>
+      </c>
+      <c r="JF25" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>343</v>
       </c>
-      <c r="N25" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT25" t="s">
-        <v>318</v>
-      </c>
-      <c r="ED25" t="s">
-        <v>318</v>
-      </c>
-      <c r="JE25" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="26" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="N26" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU26" t="s">
+        <v>318</v>
+      </c>
+      <c r="EH26" t="s">
+        <v>318</v>
+      </c>
+      <c r="JG26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>344</v>
       </c>
-      <c r="N26" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT26" t="s">
-        <v>318</v>
-      </c>
-      <c r="EG26" t="s">
-        <v>318</v>
-      </c>
-      <c r="JF26" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="27" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="N27" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU27" t="s">
+        <v>318</v>
+      </c>
+      <c r="EG27" t="s">
+        <v>318</v>
+      </c>
+      <c r="JI27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>345</v>
       </c>
-      <c r="N27" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT27" t="s">
-        <v>318</v>
-      </c>
-      <c r="EF27" t="s">
-        <v>318</v>
-      </c>
-      <c r="JH27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="N28" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU28" t="s">
+        <v>318</v>
+      </c>
+      <c r="EF28" t="s">
+        <v>318</v>
+      </c>
+      <c r="JH28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>346</v>
       </c>
-      <c r="N28" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT28" t="s">
-        <v>318</v>
-      </c>
-      <c r="EE28" t="s">
-        <v>318</v>
-      </c>
-      <c r="JG28" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="N29" t="s">
+        <v>318</v>
+      </c>
+      <c r="DC29" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU29" t="s">
+        <v>318</v>
+      </c>
+      <c r="IU29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>347</v>
       </c>
-      <c r="N29" t="s">
-        <v>318</v>
-      </c>
-      <c r="DB29" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT29" t="s">
-        <v>318</v>
-      </c>
-      <c r="IT29" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="N30" t="s">
+        <v>318</v>
+      </c>
+      <c r="DD30" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU30" t="s">
+        <v>318</v>
+      </c>
+      <c r="IW30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>348</v>
       </c>
-      <c r="N30" t="s">
-        <v>318</v>
-      </c>
-      <c r="DC30" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT30" t="s">
-        <v>318</v>
-      </c>
-      <c r="IV30" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="31" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="N31" t="s">
+        <v>318</v>
+      </c>
+      <c r="DB31" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU31" t="s">
+        <v>318</v>
+      </c>
+      <c r="IS31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:309" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>349</v>
       </c>
-      <c r="N31" t="s">
-        <v>318</v>
-      </c>
-      <c r="DA31" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT31" t="s">
-        <v>318</v>
-      </c>
-      <c r="IR31" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="32" spans="1:308" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>350</v>
-      </c>
       <c r="N32" t="s">
         <v>318</v>
       </c>
-      <c r="DE32" t="s">
-        <v>318</v>
-      </c>
-      <c r="DT32" t="s">
-        <v>318</v>
-      </c>
-      <c r="HS32" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="33" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="DF32" t="s">
+        <v>318</v>
+      </c>
+      <c r="DU32" t="s">
+        <v>318</v>
+      </c>
+      <c r="HT32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>351</v>
+      </c>
+      <c r="N33" t="s">
+        <v>318</v>
+      </c>
+      <c r="ED33" t="s">
+        <v>318</v>
+      </c>
+      <c r="JZ33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:330" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>352</v>
       </c>
-      <c r="N33" t="s">
-        <v>318</v>
-      </c>
-      <c r="EC33" t="s">
-        <v>318</v>
-      </c>
-      <c r="JY33" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="34" spans="1:329" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>353</v>
-      </c>
       <c r="N34" t="s">
         <v>318</v>
       </c>
-      <c r="EI34" t="s">
-        <v>318</v>
-      </c>
-      <c r="JZ34" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="35" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="EJ34" t="s">
+        <v>318</v>
+      </c>
+      <c r="KA34" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
       <c r="N35" t="s">
         <v>318</v>
       </c>
-      <c r="DN35" t="s">
-        <v>318</v>
-      </c>
-      <c r="JJ35" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="36" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="DO35" t="s">
+        <v>318</v>
+      </c>
+      <c r="JK35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>23</v>
       </c>
       <c r="N36" t="s">
         <v>318</v>
       </c>
-      <c r="FA36" t="s">
-        <v>318</v>
-      </c>
-      <c r="IZ36" t="s">
+      <c r="FB36" t="s">
         <v>318</v>
       </c>
       <c r="JA36" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="37" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="JB36" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="37" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>24</v>
       </c>
       <c r="N37" t="s">
         <v>318</v>
       </c>
-      <c r="CS37" t="s">
-        <v>318</v>
-      </c>
-      <c r="JP37" t="s">
+      <c r="CT37" t="s">
         <v>318</v>
       </c>
       <c r="JQ37" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="38" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="JR37" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="38" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>25</v>
       </c>
       <c r="N38" t="s">
         <v>318</v>
       </c>
-      <c r="CS38" t="s">
-        <v>318</v>
-      </c>
-      <c r="JP38" t="s">
+      <c r="CT38" t="s">
         <v>318</v>
       </c>
       <c r="JQ38" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="39" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="JR38" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>26</v>
       </c>
       <c r="N39" t="s">
         <v>318</v>
       </c>
-      <c r="EN39" t="s">
-        <v>318</v>
-      </c>
-      <c r="HM39" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="40" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="EO39" t="s">
+        <v>318</v>
+      </c>
+      <c r="HN39" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>27</v>
       </c>
       <c r="N40" t="s">
         <v>318</v>
       </c>
-      <c r="DW40" t="s">
-        <v>318</v>
-      </c>
-      <c r="HN40" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="41" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="DX40" t="s">
+        <v>318</v>
+      </c>
+      <c r="HO40" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28</v>
       </c>
@@ -4216,11 +4222,11 @@
       <c r="R41" t="s">
         <v>318</v>
       </c>
-      <c r="FB41" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="42" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="FC41" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>29</v>
       </c>
@@ -4233,17 +4239,17 @@
       <c r="R42" t="s">
         <v>318</v>
       </c>
-      <c r="FB42" t="s">
-        <v>318</v>
-      </c>
       <c r="FC42" t="s">
         <v>318</v>
       </c>
-      <c r="FG42" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="43" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="FD42" t="s">
+        <v>318</v>
+      </c>
+      <c r="FH42" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>30</v>
       </c>
@@ -4256,17 +4262,17 @@
       <c r="R43" t="s">
         <v>318</v>
       </c>
-      <c r="FB43" t="s">
-        <v>318</v>
-      </c>
-      <c r="FD43" t="s">
+      <c r="FC43" t="s">
         <v>318</v>
       </c>
       <c r="FE43" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="44" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="FF43" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="44" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>31</v>
       </c>
@@ -4276,25 +4282,25 @@
       <c r="R44" t="s">
         <v>318</v>
       </c>
-      <c r="FF44" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="45" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="FG44" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>32</v>
       </c>
       <c r="N45" t="s">
         <v>318</v>
       </c>
-      <c r="EV45" t="s">
-        <v>318</v>
-      </c>
-      <c r="KA45" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="EW45" t="s">
+        <v>318</v>
+      </c>
+      <c r="KB45" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="46" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>33</v>
       </c>
@@ -4304,14 +4310,14 @@
       <c r="BU46" t="s">
         <v>318</v>
       </c>
-      <c r="GD46" t="s">
-        <v>318</v>
-      </c>
       <c r="GE46" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="47" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="GF46" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="47" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>34</v>
       </c>
@@ -4327,9 +4333,6 @@
       <c r="U47" t="s">
         <v>318</v>
       </c>
-      <c r="LK47" t="s">
-        <v>318</v>
-      </c>
       <c r="LL47" t="s">
         <v>318</v>
       </c>
@@ -4348,8 +4351,11 @@
       <c r="LQ47" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="48" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="LR47" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>35</v>
       </c>
@@ -4359,14 +4365,14 @@
       <c r="BK48" t="s">
         <v>318</v>
       </c>
-      <c r="HI48" t="s">
-        <v>318</v>
-      </c>
       <c r="HJ48" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="49" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="HK48" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>36</v>
       </c>
@@ -4376,28 +4382,28 @@
       <c r="BJ49" t="s">
         <v>318</v>
       </c>
-      <c r="HK49" t="s">
-        <v>318</v>
-      </c>
       <c r="HL49" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="50" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="HM49" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>37</v>
       </c>
       <c r="N50" t="s">
         <v>318</v>
       </c>
-      <c r="DS50" t="s">
-        <v>318</v>
-      </c>
-      <c r="JK50" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="51" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="DT50" t="s">
+        <v>318</v>
+      </c>
+      <c r="JL50" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>38</v>
       </c>
@@ -4410,11 +4416,11 @@
       <c r="BE51" t="s">
         <v>318</v>
       </c>
-      <c r="CI51" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="52" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="CJ51" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>39</v>
       </c>
@@ -4424,20 +4430,20 @@
       <c r="N52" t="s">
         <v>318</v>
       </c>
-      <c r="EK52" t="s">
-        <v>318</v>
-      </c>
       <c r="EL52" t="s">
         <v>318</v>
       </c>
-      <c r="JL52" t="s">
+      <c r="EM52" t="s">
         <v>318</v>
       </c>
       <c r="JM52" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="53" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="JN52" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="53" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>40</v>
       </c>
@@ -4447,11 +4453,11 @@
       <c r="AY53" t="s">
         <v>318</v>
       </c>
-      <c r="GV53" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="54" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="GW53" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="54" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>41</v>
       </c>
@@ -4461,14 +4467,14 @@
       <c r="AW54" t="s">
         <v>318</v>
       </c>
-      <c r="GW54" t="s">
-        <v>318</v>
-      </c>
       <c r="GX54" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="55" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="GY54" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="55" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>42</v>
       </c>
@@ -4478,17 +4484,17 @@
       <c r="AX55" t="s">
         <v>318</v>
       </c>
-      <c r="GY55" t="s">
-        <v>318</v>
-      </c>
       <c r="GZ55" t="s">
         <v>318</v>
       </c>
       <c r="HA55" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="56" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="HB55" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="56" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>43</v>
       </c>
@@ -4510,10 +4516,7 @@
       <c r="BD56" t="s">
         <v>318</v>
       </c>
-      <c r="DV56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KI56" t="s">
+      <c r="DW56" t="s">
         <v>318</v>
       </c>
       <c r="KJ56" t="s">
@@ -4528,8 +4531,11 @@
       <c r="KM56" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="57" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="KN56" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="57" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>44</v>
       </c>
@@ -4539,14 +4545,14 @@
       <c r="N57" t="s">
         <v>318</v>
       </c>
-      <c r="DI57" t="s">
-        <v>318</v>
-      </c>
-      <c r="GF57" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="58" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="DJ57" t="s">
+        <v>318</v>
+      </c>
+      <c r="GG57" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="58" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>45</v>
       </c>
@@ -4556,20 +4562,20 @@
       <c r="N58" t="s">
         <v>318</v>
       </c>
-      <c r="CG58" t="s">
-        <v>318</v>
-      </c>
-      <c r="CK58" t="s">
+      <c r="CH58" t="s">
         <v>318</v>
       </c>
       <c r="CL58" t="s">
         <v>318</v>
       </c>
-      <c r="KP58" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="59" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="CM58" t="s">
+        <v>318</v>
+      </c>
+      <c r="KQ58" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>46</v>
       </c>
@@ -4579,17 +4585,17 @@
       <c r="N59" t="s">
         <v>318</v>
       </c>
-      <c r="EH59" t="s">
-        <v>318</v>
-      </c>
-      <c r="II59" t="s">
+      <c r="EI59" t="s">
         <v>318</v>
       </c>
       <c r="IJ59" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="60" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="IK59" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="60" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>47</v>
       </c>
@@ -4599,14 +4605,14 @@
       <c r="BO60" t="s">
         <v>318</v>
       </c>
-      <c r="LB60" t="s">
-        <v>318</v>
-      </c>
       <c r="LC60" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="61" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="LD60" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>48</v>
       </c>
@@ -4616,14 +4622,14 @@
       <c r="AJ61" t="s">
         <v>318</v>
       </c>
-      <c r="DK61" t="s">
-        <v>318</v>
-      </c>
-      <c r="FR61" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="62" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="DL61" t="s">
+        <v>318</v>
+      </c>
+      <c r="FS61" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="62" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>49</v>
       </c>
@@ -4633,14 +4639,14 @@
       <c r="AI62" t="s">
         <v>318</v>
       </c>
-      <c r="FS62" t="s">
-        <v>318</v>
-      </c>
-      <c r="FU62" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="63" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="FT62" t="s">
+        <v>318</v>
+      </c>
+      <c r="FV62" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="63" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>50</v>
       </c>
@@ -4650,14 +4656,14 @@
       <c r="AH63" t="s">
         <v>318</v>
       </c>
-      <c r="FT63" t="s">
-        <v>318</v>
-      </c>
-      <c r="FV63" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="64" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="FU63" t="s">
+        <v>318</v>
+      </c>
+      <c r="FW63" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:316" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>51</v>
       </c>
@@ -4667,11 +4673,11 @@
       <c r="AB64" t="s">
         <v>318</v>
       </c>
-      <c r="FI64" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FJ64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>52</v>
       </c>
@@ -4681,14 +4687,14 @@
       <c r="Z65" t="s">
         <v>318</v>
       </c>
-      <c r="FL65" t="s">
-        <v>318</v>
-      </c>
       <c r="FM65" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="66" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FN65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>53</v>
       </c>
@@ -4698,11 +4704,11 @@
       <c r="AB66" t="s">
         <v>318</v>
       </c>
-      <c r="FN66" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FO66" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>54</v>
       </c>
@@ -4712,16 +4718,16 @@
       <c r="AB67" t="s">
         <v>318</v>
       </c>
-      <c r="FI67" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="68" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FJ67" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="68" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D68" t="s">
         <v>318</v>
@@ -4729,11 +4735,11 @@
       <c r="AB68" t="s">
         <v>318</v>
       </c>
-      <c r="FI68" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="69" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FJ68" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="69" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>56</v>
       </c>
@@ -4743,11 +4749,11 @@
       <c r="AA69" t="s">
         <v>318</v>
       </c>
-      <c r="FH69" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="70" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FI69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>57</v>
       </c>
@@ -4757,14 +4763,14 @@
       <c r="AD70" t="s">
         <v>318</v>
       </c>
-      <c r="FK70" t="s">
-        <v>318</v>
-      </c>
-      <c r="FO70" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:171" x14ac:dyDescent="0.25">
+      <c r="FL70" t="s">
+        <v>318</v>
+      </c>
+      <c r="FP70" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>58</v>
       </c>
@@ -4774,7 +4780,91 @@
       <c r="Y71" t="s">
         <v>318</v>
       </c>
-      <c r="FK71" t="s">
+      <c r="FL71" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="72" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>59</v>
+      </c>
+      <c r="O72" t="s">
+        <v>318</v>
+      </c>
+      <c r="BT72" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV72" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="73" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>60</v>
+      </c>
+      <c r="O73" t="s">
+        <v>318</v>
+      </c>
+      <c r="BY73" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV73" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="74" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>61</v>
+      </c>
+      <c r="O74" t="s">
+        <v>318</v>
+      </c>
+      <c r="BW74" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV74" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>62</v>
+      </c>
+      <c r="O75" t="s">
+        <v>318</v>
+      </c>
+      <c r="BV75" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV75" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="76" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>63</v>
+      </c>
+      <c r="O76" t="s">
+        <v>318</v>
+      </c>
+      <c r="BZ76" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV76" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>64</v>
+      </c>
+      <c r="O77" t="s">
+        <v>318</v>
+      </c>
+      <c r="BS77" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV77" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4856,22 +4946,21 @@
     <mergeCell ref="A92:A95"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="GW4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
-    <hyperlink ref="HN4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
-    <hyperlink ref="HQ4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
-    <hyperlink ref="IF4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
-    <hyperlink ref="IK4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
-    <hyperlink ref="IU4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
-    <hyperlink ref="JH4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
-    <hyperlink ref="JI4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
-    <hyperlink ref="JK4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
-    <hyperlink ref="JX4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
-    <hyperlink ref="KC4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
-    <hyperlink ref="KG4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
-    <hyperlink ref="LN4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
-    <hyperlink ref="LR4" r:id="rId14" display="Register@Controller  " xr:uid="{E0CE53F3-FAFD-4FBD-A4AF-A47BFFE0BA85}"/>
+    <hyperlink ref="GX4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
+    <hyperlink ref="HO4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
+    <hyperlink ref="HR4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
+    <hyperlink ref="IG4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
+    <hyperlink ref="IL4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
+    <hyperlink ref="IV4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
+    <hyperlink ref="JI4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
+    <hyperlink ref="JJ4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
+    <hyperlink ref="JL4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JY4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="KD4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KH4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LO4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Requerimientos de detalle de informacion para tesis(alumno, profesor guia y director tesis) y usuarios(administrador), completando matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E352C4EA-F294-4F2F-9BD2-44F2BF70BABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1DC5CF-A0FB-4F47-BED4-284F5DD9FD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="369">
   <si>
     <t>MVC</t>
   </si>
@@ -1225,6 +1226,12 @@
   </si>
   <si>
     <t>/director_escuelahome</t>
+  </si>
+  <si>
+    <t>Alumno/Profesor Guia/Director Tesis</t>
+  </si>
+  <si>
+    <t>Alumno/Profesor_Guia/DirectorTesis</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1335,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1338,17 +1346,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1664,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LR99"/>
+  <dimension ref="A1:LR81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ52" workbookViewId="0">
-      <selection activeCell="BT72" sqref="BT72"/>
+    <sheetView tabSelected="1" topLeftCell="IA60" workbookViewId="0">
+      <selection activeCell="IC80" sqref="IC80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,12 +1816,12 @@
     <col min="143" max="143" width="31" customWidth="1"/>
     <col min="144" max="144" width="21.42578125" customWidth="1"/>
     <col min="145" max="145" width="24" customWidth="1"/>
-    <col min="146" max="146" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="35.85546875" customWidth="1"/>
     <col min="147" max="147" width="20.7109375" customWidth="1"/>
     <col min="148" max="148" width="34.5703125" customWidth="1"/>
     <col min="149" max="149" width="28.5703125" customWidth="1"/>
     <col min="150" max="150" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="16.140625" customWidth="1"/>
+    <col min="151" max="151" width="32.140625" customWidth="1"/>
     <col min="152" max="152" width="32.5703125" customWidth="1"/>
     <col min="153" max="154" width="24.85546875" customWidth="1"/>
     <col min="155" max="155" width="28.140625" customWidth="1"/>
@@ -1889,7 +1896,7 @@
     <col min="225" max="225" width="40" bestFit="1" customWidth="1"/>
     <col min="226" max="226" width="54.140625" customWidth="1"/>
     <col min="227" max="227" width="23.85546875" customWidth="1"/>
-    <col min="228" max="228" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="45" customWidth="1"/>
     <col min="229" max="229" width="29.85546875" customWidth="1"/>
     <col min="230" max="230" width="26.85546875" customWidth="1"/>
     <col min="231" max="231" width="33.42578125" customWidth="1"/>
@@ -2008,163 +2015,163 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="7"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="7"/>
-      <c r="BH2" s="7"/>
-      <c r="BI2" s="7"/>
-      <c r="BJ2" s="7"/>
-      <c r="BK2" s="7"/>
-      <c r="BL2" s="7"/>
-      <c r="BM2" s="7"/>
-      <c r="BN2" s="7"/>
-      <c r="BO2" s="7"/>
-      <c r="BP2" s="7"/>
-      <c r="BQ2" s="7"/>
-      <c r="BR2" s="7"/>
-      <c r="BS2" s="7"/>
-      <c r="BT2" s="7"/>
-      <c r="BU2" s="7"/>
-      <c r="BV2" s="7"/>
-      <c r="BW2" s="7"/>
-      <c r="BX2" s="7"/>
-      <c r="BY2" s="7"/>
-      <c r="BZ2" s="7"/>
-      <c r="CA2" s="7"/>
-      <c r="CB2" s="7"/>
-      <c r="CC2" s="7"/>
-      <c r="CD2" s="7"/>
-      <c r="CE2" s="7"/>
-      <c r="CF2" s="7"/>
-      <c r="CG2" s="7"/>
-      <c r="CH2" s="7"/>
-      <c r="CI2" s="7"/>
-      <c r="CJ2" s="7"/>
-      <c r="CK2" s="7"/>
-      <c r="CL2" s="7"/>
-      <c r="CM2" s="7"/>
-      <c r="CN2" s="7"/>
-      <c r="CO2" s="7"/>
-      <c r="CP2" s="7"/>
-      <c r="CQ2" s="7"/>
-      <c r="CR2" s="7"/>
-      <c r="CS2" s="7"/>
-      <c r="CT2" s="7"/>
-      <c r="CU2" s="7"/>
-      <c r="CV2" s="7"/>
-      <c r="CW2" s="7"/>
-      <c r="CX2" s="7"/>
-      <c r="CY2" s="7"/>
-      <c r="CZ2" s="7"/>
-      <c r="DA2" s="7"/>
-      <c r="DB2" s="7"/>
-      <c r="DC2" s="7"/>
-      <c r="DD2" s="7"/>
-      <c r="DE2" s="7"/>
-      <c r="DF2" s="7"/>
-      <c r="DG2" s="7"/>
-      <c r="DH2" s="7"/>
-      <c r="DI2" s="7"/>
-      <c r="DJ2" s="7"/>
-      <c r="DK2" s="7"/>
-      <c r="DL2" s="7"/>
-      <c r="DM2" s="7"/>
-      <c r="DN2" s="7"/>
-      <c r="DO2" s="7"/>
-      <c r="DP2" s="7"/>
-      <c r="DQ2" s="7"/>
-      <c r="DR2" s="7"/>
-      <c r="DS2" s="7"/>
-      <c r="DT2" s="7"/>
-      <c r="DU2" s="7"/>
-      <c r="DV2" s="7"/>
-      <c r="DW2" s="7"/>
-      <c r="DX2" s="7"/>
-      <c r="DY2" s="7"/>
-      <c r="DZ2" s="7"/>
-      <c r="EA2" s="7"/>
-      <c r="EB2" s="7"/>
-      <c r="EC2" s="7"/>
-      <c r="ED2" s="7"/>
-      <c r="EE2" s="7"/>
-      <c r="EF2" s="7"/>
-      <c r="EG2" s="7"/>
-      <c r="EH2" s="7"/>
-      <c r="EI2" s="7"/>
-      <c r="EJ2" s="7"/>
-      <c r="EK2" s="7"/>
-      <c r="EL2" s="7"/>
-      <c r="EM2" s="7"/>
-      <c r="EN2" s="7"/>
-      <c r="EO2" s="7"/>
-      <c r="EP2" s="7"/>
-      <c r="EQ2" s="7"/>
-      <c r="ER2" s="7"/>
-      <c r="ES2" s="7"/>
-      <c r="ET2" s="7"/>
-      <c r="EU2" s="7"/>
-      <c r="EV2" s="7"/>
-      <c r="EW2" s="7"/>
-      <c r="EX2" s="7"/>
-      <c r="EY2" s="7"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
+      <c r="DA2" s="8"/>
+      <c r="DB2" s="8"/>
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8"/>
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
+      <c r="DS2" s="8"/>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8"/>
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8"/>
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
+      <c r="EP2" s="8"/>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
+      <c r="ET2" s="8"/>
+      <c r="EU2" s="8"/>
+      <c r="EV2" s="8"/>
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
       <c r="EZ2" s="9" t="s">
         <v>337</v>
       </c>
@@ -2337,9 +2344,9 @@
       <c r="LK2" s="10"/>
       <c r="LL2" s="10"/>
       <c r="LM2" s="10"/>
-      <c r="LN2" s="11"/>
-      <c r="LO2" s="11"/>
-      <c r="LP2" s="11"/>
+      <c r="LN2" s="4"/>
+      <c r="LO2" s="4"/>
+      <c r="LP2" s="4"/>
     </row>
     <row r="3" spans="1:330" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2542,8 +2549,12 @@
       <c r="EL3" s="1"/>
       <c r="EM3" s="1"/>
       <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
-      <c r="EP3" s="1"/>
+      <c r="EO3" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="EP3" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="EQ3" s="1"/>
       <c r="ER3" s="1"/>
       <c r="ES3" s="1"/>
@@ -2598,6 +2609,9 @@
       <c r="HS3" t="s">
         <v>335</v>
       </c>
+      <c r="IC3" t="s">
+        <v>367</v>
+      </c>
       <c r="IE3" t="s">
         <v>330</v>
       </c>
@@ -3956,7 +3970,7 @@
       </c>
     </row>
     <row r="25" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="5" t="s">
         <v>342</v>
       </c>
       <c r="N25" t="s">
@@ -4677,7 +4691,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="65" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>52</v>
       </c>
@@ -4694,7 +4708,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="66" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>53</v>
       </c>
@@ -4708,7 +4722,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="67" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>54</v>
       </c>
@@ -4722,7 +4736,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="68" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>55</v>
       </c>
@@ -4739,7 +4753,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="69" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>56</v>
       </c>
@@ -4753,7 +4767,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="70" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>57</v>
       </c>
@@ -4770,7 +4784,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="71" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>58</v>
       </c>
@@ -4784,7 +4798,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="72" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>59</v>
       </c>
@@ -4798,7 +4812,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="73" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>60</v>
       </c>
@@ -4812,7 +4826,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="74" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>61</v>
       </c>
@@ -4826,7 +4840,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="75" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>62</v>
       </c>
@@ -4840,7 +4854,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>63</v>
       </c>
@@ -4854,7 +4868,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="77" spans="1:204" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:237" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>64</v>
       </c>
@@ -4868,82 +4882,67 @@
         <v>318</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>319</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
-        <v>1</v>
-      </c>
-      <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" t="s">
-        <v>63</v>
-      </c>
-      <c r="H92" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="H93" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" t="s">
-        <v>64</v>
-      </c>
-      <c r="H94" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="8"/>
-      <c r="H95" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>2</v>
-      </c>
-      <c r="B96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
+    <row r="78" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>65</v>
+      </c>
+      <c r="N78" t="s">
+        <v>318</v>
+      </c>
+      <c r="EP78" t="s">
+        <v>318</v>
+      </c>
+      <c r="IC78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>66</v>
+      </c>
+      <c r="N79" t="s">
+        <v>318</v>
+      </c>
+      <c r="EP79" t="s">
+        <v>318</v>
+      </c>
+      <c r="IC79" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="80" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>67</v>
+      </c>
+      <c r="N80" t="s">
+        <v>318</v>
+      </c>
+      <c r="EP80" t="s">
+        <v>318</v>
+      </c>
+      <c r="IC80" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>68</v>
+      </c>
+      <c r="O81" t="s">
+        <v>318</v>
+      </c>
+      <c r="BR81" t="s">
+        <v>318</v>
+      </c>
+      <c r="LB81" t="s">
+        <v>318</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A96:A99"/>
+  <mergeCells count="3">
     <mergeCell ref="C2:O2"/>
     <mergeCell ref="P2:EY2"/>
     <mergeCell ref="EZ2:LM2"/>
-    <mergeCell ref="A92:A95"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="GX4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
@@ -4963,4 +4962,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191156FB-FCF6-4308-A9F0-C873C9D0C68D}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="H3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="H5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Requerimientos de CRU de vinculacion añadidas por profesor listo en requerimientos y matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1DC5CF-A0FB-4F47-BED4-284F5DD9FD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77474B95-24B6-4129-8DC0-1CB4D0CDE535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="369">
   <si>
     <t>MVC</t>
   </si>
@@ -1198,9 +1198,6 @@
     <t>/recopilacion/recopilacion_informacion_titulados</t>
   </si>
   <si>
-    <t>secretaria</t>
-  </si>
-  <si>
     <t>/memorandum/index</t>
   </si>
   <si>
@@ -1232,6 +1229,9 @@
   </si>
   <si>
     <t>Alumno/Profesor_Guia/DirectorTesis</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1339,6 +1339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1671,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LR81"/>
+  <dimension ref="A1:LR93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="IA60" workbookViewId="0">
-      <selection activeCell="IC80" sqref="IC80"/>
+    <sheetView tabSelected="1" topLeftCell="GY1" workbookViewId="0">
+      <selection activeCell="HD3" sqref="HD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,6 +1686,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.85546875" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
@@ -2015,335 +2017,335 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-      <c r="AZ2" s="8"/>
-      <c r="BA2" s="8"/>
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="8"/>
-      <c r="BI2" s="8"/>
-      <c r="BJ2" s="8"/>
-      <c r="BK2" s="8"/>
-      <c r="BL2" s="8"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="8"/>
-      <c r="BO2" s="8"/>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="8"/>
-      <c r="BR2" s="8"/>
-      <c r="BS2" s="8"/>
-      <c r="BT2" s="8"/>
-      <c r="BU2" s="8"/>
-      <c r="BV2" s="8"/>
-      <c r="BW2" s="8"/>
-      <c r="BX2" s="8"/>
-      <c r="BY2" s="8"/>
-      <c r="BZ2" s="8"/>
-      <c r="CA2" s="8"/>
-      <c r="CB2" s="8"/>
-      <c r="CC2" s="8"/>
-      <c r="CD2" s="8"/>
-      <c r="CE2" s="8"/>
-      <c r="CF2" s="8"/>
-      <c r="CG2" s="8"/>
-      <c r="CH2" s="8"/>
-      <c r="CI2" s="8"/>
-      <c r="CJ2" s="8"/>
-      <c r="CK2" s="8"/>
-      <c r="CL2" s="8"/>
-      <c r="CM2" s="8"/>
-      <c r="CN2" s="8"/>
-      <c r="CO2" s="8"/>
-      <c r="CP2" s="8"/>
-      <c r="CQ2" s="8"/>
-      <c r="CR2" s="8"/>
-      <c r="CS2" s="8"/>
-      <c r="CT2" s="8"/>
-      <c r="CU2" s="8"/>
-      <c r="CV2" s="8"/>
-      <c r="CW2" s="8"/>
-      <c r="CX2" s="8"/>
-      <c r="CY2" s="8"/>
-      <c r="CZ2" s="8"/>
-      <c r="DA2" s="8"/>
-      <c r="DB2" s="8"/>
-      <c r="DC2" s="8"/>
-      <c r="DD2" s="8"/>
-      <c r="DE2" s="8"/>
-      <c r="DF2" s="8"/>
-      <c r="DG2" s="8"/>
-      <c r="DH2" s="8"/>
-      <c r="DI2" s="8"/>
-      <c r="DJ2" s="8"/>
-      <c r="DK2" s="8"/>
-      <c r="DL2" s="8"/>
-      <c r="DM2" s="8"/>
-      <c r="DN2" s="8"/>
-      <c r="DO2" s="8"/>
-      <c r="DP2" s="8"/>
-      <c r="DQ2" s="8"/>
-      <c r="DR2" s="8"/>
-      <c r="DS2" s="8"/>
-      <c r="DT2" s="8"/>
-      <c r="DU2" s="8"/>
-      <c r="DV2" s="8"/>
-      <c r="DW2" s="8"/>
-      <c r="DX2" s="8"/>
-      <c r="DY2" s="8"/>
-      <c r="DZ2" s="8"/>
-      <c r="EA2" s="8"/>
-      <c r="EB2" s="8"/>
-      <c r="EC2" s="8"/>
-      <c r="ED2" s="8"/>
-      <c r="EE2" s="8"/>
-      <c r="EF2" s="8"/>
-      <c r="EG2" s="8"/>
-      <c r="EH2" s="8"/>
-      <c r="EI2" s="8"/>
-      <c r="EJ2" s="8"/>
-      <c r="EK2" s="8"/>
-      <c r="EL2" s="8"/>
-      <c r="EM2" s="8"/>
-      <c r="EN2" s="8"/>
-      <c r="EO2" s="8"/>
-      <c r="EP2" s="8"/>
-      <c r="EQ2" s="8"/>
-      <c r="ER2" s="8"/>
-      <c r="ES2" s="8"/>
-      <c r="ET2" s="8"/>
-      <c r="EU2" s="8"/>
-      <c r="EV2" s="8"/>
-      <c r="EW2" s="8"/>
-      <c r="EX2" s="8"/>
-      <c r="EY2" s="8"/>
-      <c r="EZ2" s="9" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9"/>
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="9"/>
+      <c r="BS2" s="9"/>
+      <c r="BT2" s="9"/>
+      <c r="BU2" s="9"/>
+      <c r="BV2" s="9"/>
+      <c r="BW2" s="9"/>
+      <c r="BX2" s="9"/>
+      <c r="BY2" s="9"/>
+      <c r="BZ2" s="9"/>
+      <c r="CA2" s="9"/>
+      <c r="CB2" s="9"/>
+      <c r="CC2" s="9"/>
+      <c r="CD2" s="9"/>
+      <c r="CE2" s="9"/>
+      <c r="CF2" s="9"/>
+      <c r="CG2" s="9"/>
+      <c r="CH2" s="9"/>
+      <c r="CI2" s="9"/>
+      <c r="CJ2" s="9"/>
+      <c r="CK2" s="9"/>
+      <c r="CL2" s="9"/>
+      <c r="CM2" s="9"/>
+      <c r="CN2" s="9"/>
+      <c r="CO2" s="9"/>
+      <c r="CP2" s="9"/>
+      <c r="CQ2" s="9"/>
+      <c r="CR2" s="9"/>
+      <c r="CS2" s="9"/>
+      <c r="CT2" s="9"/>
+      <c r="CU2" s="9"/>
+      <c r="CV2" s="9"/>
+      <c r="CW2" s="9"/>
+      <c r="CX2" s="9"/>
+      <c r="CY2" s="9"/>
+      <c r="CZ2" s="9"/>
+      <c r="DA2" s="9"/>
+      <c r="DB2" s="9"/>
+      <c r="DC2" s="9"/>
+      <c r="DD2" s="9"/>
+      <c r="DE2" s="9"/>
+      <c r="DF2" s="9"/>
+      <c r="DG2" s="9"/>
+      <c r="DH2" s="9"/>
+      <c r="DI2" s="9"/>
+      <c r="DJ2" s="9"/>
+      <c r="DK2" s="9"/>
+      <c r="DL2" s="9"/>
+      <c r="DM2" s="9"/>
+      <c r="DN2" s="9"/>
+      <c r="DO2" s="9"/>
+      <c r="DP2" s="9"/>
+      <c r="DQ2" s="9"/>
+      <c r="DR2" s="9"/>
+      <c r="DS2" s="9"/>
+      <c r="DT2" s="9"/>
+      <c r="DU2" s="9"/>
+      <c r="DV2" s="9"/>
+      <c r="DW2" s="9"/>
+      <c r="DX2" s="9"/>
+      <c r="DY2" s="9"/>
+      <c r="DZ2" s="9"/>
+      <c r="EA2" s="9"/>
+      <c r="EB2" s="9"/>
+      <c r="EC2" s="9"/>
+      <c r="ED2" s="9"/>
+      <c r="EE2" s="9"/>
+      <c r="EF2" s="9"/>
+      <c r="EG2" s="9"/>
+      <c r="EH2" s="9"/>
+      <c r="EI2" s="9"/>
+      <c r="EJ2" s="9"/>
+      <c r="EK2" s="9"/>
+      <c r="EL2" s="9"/>
+      <c r="EM2" s="9"/>
+      <c r="EN2" s="9"/>
+      <c r="EO2" s="9"/>
+      <c r="EP2" s="9"/>
+      <c r="EQ2" s="9"/>
+      <c r="ER2" s="9"/>
+      <c r="ES2" s="9"/>
+      <c r="ET2" s="9"/>
+      <c r="EU2" s="9"/>
+      <c r="EV2" s="9"/>
+      <c r="EW2" s="9"/>
+      <c r="EX2" s="9"/>
+      <c r="EY2" s="9"/>
+      <c r="EZ2" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="FA2" s="10"/>
-      <c r="FB2" s="10"/>
-      <c r="FC2" s="10"/>
-      <c r="FD2" s="10"/>
-      <c r="FE2" s="10"/>
-      <c r="FF2" s="10"/>
-      <c r="FG2" s="10"/>
-      <c r="FH2" s="10"/>
-      <c r="FI2" s="10"/>
-      <c r="FJ2" s="10"/>
-      <c r="FK2" s="10"/>
-      <c r="FL2" s="10"/>
-      <c r="FM2" s="10"/>
-      <c r="FN2" s="10"/>
-      <c r="FO2" s="10"/>
-      <c r="FP2" s="10"/>
-      <c r="FQ2" s="10"/>
-      <c r="FR2" s="10"/>
-      <c r="FS2" s="10"/>
-      <c r="FT2" s="10"/>
-      <c r="FU2" s="10"/>
-      <c r="FV2" s="10"/>
-      <c r="FW2" s="10"/>
-      <c r="FX2" s="10"/>
-      <c r="FY2" s="10"/>
-      <c r="FZ2" s="10"/>
-      <c r="GA2" s="10"/>
-      <c r="GB2" s="10"/>
-      <c r="GC2" s="10"/>
-      <c r="GD2" s="10"/>
-      <c r="GE2" s="10"/>
-      <c r="GF2" s="10"/>
-      <c r="GG2" s="10"/>
-      <c r="GH2" s="10"/>
-      <c r="GI2" s="10"/>
-      <c r="GJ2" s="10"/>
-      <c r="GK2" s="10"/>
-      <c r="GL2" s="10"/>
-      <c r="GM2" s="10"/>
-      <c r="GN2" s="10"/>
-      <c r="GO2" s="10"/>
-      <c r="GP2" s="10"/>
-      <c r="GQ2" s="10"/>
-      <c r="GR2" s="10"/>
-      <c r="GS2" s="10"/>
-      <c r="GT2" s="10"/>
-      <c r="GU2" s="10"/>
-      <c r="GV2" s="10"/>
-      <c r="GW2" s="10"/>
-      <c r="GX2" s="10"/>
-      <c r="GY2" s="10"/>
-      <c r="GZ2" s="10"/>
-      <c r="HA2" s="10"/>
-      <c r="HB2" s="10"/>
-      <c r="HC2" s="10"/>
-      <c r="HD2" s="10"/>
-      <c r="HE2" s="10"/>
-      <c r="HF2" s="10"/>
-      <c r="HG2" s="10"/>
-      <c r="HH2" s="10"/>
-      <c r="HI2" s="10"/>
-      <c r="HJ2" s="10"/>
-      <c r="HK2" s="10"/>
-      <c r="HL2" s="10"/>
-      <c r="HM2" s="10"/>
-      <c r="HN2" s="10"/>
-      <c r="HO2" s="10"/>
-      <c r="HP2" s="10"/>
-      <c r="HQ2" s="10"/>
-      <c r="HR2" s="10"/>
-      <c r="HS2" s="10"/>
-      <c r="HT2" s="10"/>
-      <c r="HU2" s="10"/>
-      <c r="HV2" s="10"/>
-      <c r="HW2" s="10"/>
-      <c r="HX2" s="10"/>
-      <c r="HY2" s="10"/>
-      <c r="HZ2" s="10"/>
-      <c r="IA2" s="10"/>
-      <c r="IB2" s="10"/>
-      <c r="IC2" s="10"/>
-      <c r="ID2" s="10"/>
-      <c r="IE2" s="10"/>
-      <c r="IF2" s="10"/>
-      <c r="IG2" s="10"/>
-      <c r="IH2" s="10"/>
-      <c r="II2" s="10"/>
-      <c r="IJ2" s="10"/>
-      <c r="IK2" s="10"/>
-      <c r="IL2" s="10"/>
-      <c r="IM2" s="10"/>
-      <c r="IN2" s="10"/>
-      <c r="IO2" s="10"/>
-      <c r="IP2" s="10"/>
-      <c r="IQ2" s="10"/>
-      <c r="IR2" s="10"/>
-      <c r="IS2" s="10"/>
-      <c r="IT2" s="10"/>
-      <c r="IU2" s="10"/>
-      <c r="IV2" s="10"/>
-      <c r="IW2" s="10"/>
-      <c r="IX2" s="10"/>
-      <c r="IY2" s="10"/>
-      <c r="IZ2" s="10"/>
-      <c r="JA2" s="10"/>
-      <c r="JB2" s="10"/>
-      <c r="JC2" s="10"/>
-      <c r="JD2" s="10"/>
-      <c r="JE2" s="10"/>
-      <c r="JF2" s="10"/>
-      <c r="JG2" s="10"/>
-      <c r="JH2" s="10"/>
-      <c r="JI2" s="10"/>
-      <c r="JJ2" s="10"/>
-      <c r="JK2" s="10"/>
-      <c r="JL2" s="10"/>
-      <c r="JM2" s="10"/>
-      <c r="JN2" s="10"/>
-      <c r="JO2" s="10"/>
-      <c r="JP2" s="10"/>
-      <c r="JQ2" s="10"/>
-      <c r="JR2" s="10"/>
-      <c r="JS2" s="10"/>
-      <c r="JT2" s="10"/>
-      <c r="JU2" s="10"/>
-      <c r="JV2" s="10"/>
-      <c r="JW2" s="10"/>
-      <c r="JX2" s="10"/>
-      <c r="JY2" s="10"/>
-      <c r="JZ2" s="10"/>
-      <c r="KA2" s="10"/>
-      <c r="KB2" s="10"/>
-      <c r="KC2" s="10"/>
-      <c r="KD2" s="10"/>
-      <c r="KE2" s="10"/>
-      <c r="KF2" s="10"/>
-      <c r="KG2" s="10"/>
-      <c r="KH2" s="10"/>
-      <c r="KI2" s="10"/>
-      <c r="KJ2" s="10"/>
-      <c r="KK2" s="10"/>
-      <c r="KL2" s="10"/>
-      <c r="KM2" s="10"/>
-      <c r="KN2" s="10"/>
-      <c r="KO2" s="10"/>
-      <c r="KP2" s="10"/>
-      <c r="KQ2" s="10"/>
-      <c r="KR2" s="10"/>
-      <c r="KS2" s="10"/>
-      <c r="KT2" s="10"/>
-      <c r="KU2" s="10"/>
-      <c r="KV2" s="10"/>
-      <c r="KW2" s="10"/>
-      <c r="KX2" s="10"/>
-      <c r="KY2" s="10"/>
-      <c r="KZ2" s="10"/>
-      <c r="LA2" s="10"/>
-      <c r="LB2" s="10"/>
-      <c r="LC2" s="10"/>
-      <c r="LD2" s="10"/>
-      <c r="LE2" s="10"/>
-      <c r="LF2" s="10"/>
-      <c r="LG2" s="10"/>
-      <c r="LH2" s="10"/>
-      <c r="LI2" s="10"/>
-      <c r="LJ2" s="10"/>
-      <c r="LK2" s="10"/>
-      <c r="LL2" s="10"/>
-      <c r="LM2" s="10"/>
+      <c r="FA2" s="11"/>
+      <c r="FB2" s="11"/>
+      <c r="FC2" s="11"/>
+      <c r="FD2" s="11"/>
+      <c r="FE2" s="11"/>
+      <c r="FF2" s="11"/>
+      <c r="FG2" s="11"/>
+      <c r="FH2" s="11"/>
+      <c r="FI2" s="11"/>
+      <c r="FJ2" s="11"/>
+      <c r="FK2" s="11"/>
+      <c r="FL2" s="11"/>
+      <c r="FM2" s="11"/>
+      <c r="FN2" s="11"/>
+      <c r="FO2" s="11"/>
+      <c r="FP2" s="11"/>
+      <c r="FQ2" s="11"/>
+      <c r="FR2" s="11"/>
+      <c r="FS2" s="11"/>
+      <c r="FT2" s="11"/>
+      <c r="FU2" s="11"/>
+      <c r="FV2" s="11"/>
+      <c r="FW2" s="11"/>
+      <c r="FX2" s="11"/>
+      <c r="FY2" s="11"/>
+      <c r="FZ2" s="11"/>
+      <c r="GA2" s="11"/>
+      <c r="GB2" s="11"/>
+      <c r="GC2" s="11"/>
+      <c r="GD2" s="11"/>
+      <c r="GE2" s="11"/>
+      <c r="GF2" s="11"/>
+      <c r="GG2" s="11"/>
+      <c r="GH2" s="11"/>
+      <c r="GI2" s="11"/>
+      <c r="GJ2" s="11"/>
+      <c r="GK2" s="11"/>
+      <c r="GL2" s="11"/>
+      <c r="GM2" s="11"/>
+      <c r="GN2" s="11"/>
+      <c r="GO2" s="11"/>
+      <c r="GP2" s="11"/>
+      <c r="GQ2" s="11"/>
+      <c r="GR2" s="11"/>
+      <c r="GS2" s="11"/>
+      <c r="GT2" s="11"/>
+      <c r="GU2" s="11"/>
+      <c r="GV2" s="11"/>
+      <c r="GW2" s="11"/>
+      <c r="GX2" s="11"/>
+      <c r="GY2" s="11"/>
+      <c r="GZ2" s="11"/>
+      <c r="HA2" s="11"/>
+      <c r="HB2" s="11"/>
+      <c r="HC2" s="11"/>
+      <c r="HD2" s="11"/>
+      <c r="HE2" s="11"/>
+      <c r="HF2" s="11"/>
+      <c r="HG2" s="11"/>
+      <c r="HH2" s="11"/>
+      <c r="HI2" s="11"/>
+      <c r="HJ2" s="11"/>
+      <c r="HK2" s="11"/>
+      <c r="HL2" s="11"/>
+      <c r="HM2" s="11"/>
+      <c r="HN2" s="11"/>
+      <c r="HO2" s="11"/>
+      <c r="HP2" s="11"/>
+      <c r="HQ2" s="11"/>
+      <c r="HR2" s="11"/>
+      <c r="HS2" s="11"/>
+      <c r="HT2" s="11"/>
+      <c r="HU2" s="11"/>
+      <c r="HV2" s="11"/>
+      <c r="HW2" s="11"/>
+      <c r="HX2" s="11"/>
+      <c r="HY2" s="11"/>
+      <c r="HZ2" s="11"/>
+      <c r="IA2" s="11"/>
+      <c r="IB2" s="11"/>
+      <c r="IC2" s="11"/>
+      <c r="ID2" s="11"/>
+      <c r="IE2" s="11"/>
+      <c r="IF2" s="11"/>
+      <c r="IG2" s="11"/>
+      <c r="IH2" s="11"/>
+      <c r="II2" s="11"/>
+      <c r="IJ2" s="11"/>
+      <c r="IK2" s="11"/>
+      <c r="IL2" s="11"/>
+      <c r="IM2" s="11"/>
+      <c r="IN2" s="11"/>
+      <c r="IO2" s="11"/>
+      <c r="IP2" s="11"/>
+      <c r="IQ2" s="11"/>
+      <c r="IR2" s="11"/>
+      <c r="IS2" s="11"/>
+      <c r="IT2" s="11"/>
+      <c r="IU2" s="11"/>
+      <c r="IV2" s="11"/>
+      <c r="IW2" s="11"/>
+      <c r="IX2" s="11"/>
+      <c r="IY2" s="11"/>
+      <c r="IZ2" s="11"/>
+      <c r="JA2" s="11"/>
+      <c r="JB2" s="11"/>
+      <c r="JC2" s="11"/>
+      <c r="JD2" s="11"/>
+      <c r="JE2" s="11"/>
+      <c r="JF2" s="11"/>
+      <c r="JG2" s="11"/>
+      <c r="JH2" s="11"/>
+      <c r="JI2" s="11"/>
+      <c r="JJ2" s="11"/>
+      <c r="JK2" s="11"/>
+      <c r="JL2" s="11"/>
+      <c r="JM2" s="11"/>
+      <c r="JN2" s="11"/>
+      <c r="JO2" s="11"/>
+      <c r="JP2" s="11"/>
+      <c r="JQ2" s="11"/>
+      <c r="JR2" s="11"/>
+      <c r="JS2" s="11"/>
+      <c r="JT2" s="11"/>
+      <c r="JU2" s="11"/>
+      <c r="JV2" s="11"/>
+      <c r="JW2" s="11"/>
+      <c r="JX2" s="11"/>
+      <c r="JY2" s="11"/>
+      <c r="JZ2" s="11"/>
+      <c r="KA2" s="11"/>
+      <c r="KB2" s="11"/>
+      <c r="KC2" s="11"/>
+      <c r="KD2" s="11"/>
+      <c r="KE2" s="11"/>
+      <c r="KF2" s="11"/>
+      <c r="KG2" s="11"/>
+      <c r="KH2" s="11"/>
+      <c r="KI2" s="11"/>
+      <c r="KJ2" s="11"/>
+      <c r="KK2" s="11"/>
+      <c r="KL2" s="11"/>
+      <c r="KM2" s="11"/>
+      <c r="KN2" s="11"/>
+      <c r="KO2" s="11"/>
+      <c r="KP2" s="11"/>
+      <c r="KQ2" s="11"/>
+      <c r="KR2" s="11"/>
+      <c r="KS2" s="11"/>
+      <c r="KT2" s="11"/>
+      <c r="KU2" s="11"/>
+      <c r="KV2" s="11"/>
+      <c r="KW2" s="11"/>
+      <c r="KX2" s="11"/>
+      <c r="KY2" s="11"/>
+      <c r="KZ2" s="11"/>
+      <c r="LA2" s="11"/>
+      <c r="LB2" s="11"/>
+      <c r="LC2" s="11"/>
+      <c r="LD2" s="11"/>
+      <c r="LE2" s="11"/>
+      <c r="LF2" s="11"/>
+      <c r="LG2" s="11"/>
+      <c r="LH2" s="11"/>
+      <c r="LI2" s="11"/>
+      <c r="LJ2" s="11"/>
+      <c r="LK2" s="11"/>
+      <c r="LL2" s="11"/>
+      <c r="LM2" s="11"/>
       <c r="LN2" s="4"/>
       <c r="LO2" s="4"/>
       <c r="LP2" s="4"/>
@@ -2353,13 +2355,13 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>334</v>
@@ -2389,7 +2391,7 @@
         <v>350</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -2424,13 +2426,23 @@
       <c r="AY3" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
+      <c r="AZ3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="BC3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="BD3" s="6" t="s">
+        <v>354</v>
+      </c>
       <c r="BE3" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
@@ -2446,7 +2458,7 @@
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
       <c r="BS3" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="BT3" s="1" t="s">
         <v>330</v>
@@ -2553,7 +2565,7 @@
         <v>334</v>
       </c>
       <c r="EP3" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="EQ3" s="1"/>
       <c r="ER3" s="1"/>
@@ -2574,7 +2586,7 @@
         <v>350</v>
       </c>
       <c r="FJ3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="GE3" t="s">
         <v>331</v>
@@ -2585,6 +2597,18 @@
       <c r="GW3" t="s">
         <v>350</v>
       </c>
+      <c r="HD3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HH3" t="s">
+        <v>329</v>
+      </c>
       <c r="HJ3" t="s">
         <v>330</v>
       </c>
@@ -2610,7 +2634,7 @@
         <v>335</v>
       </c>
       <c r="IC3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="IE3" t="s">
         <v>330</v>
@@ -2646,13 +2670,13 @@
         <v>355</v>
       </c>
       <c r="LB3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="LC3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="LD3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:330" x14ac:dyDescent="0.25">
@@ -2681,7 +2705,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>368</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -2804,7 +2828,7 @@
         <v>50</v>
       </c>
       <c r="AY4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AZ4" t="s">
         <v>52</v>
@@ -2876,7 +2900,7 @@
         <v>73</v>
       </c>
       <c r="BW4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BX4" t="s">
         <v>74</v>
@@ -2909,7 +2933,7 @@
         <v>78</v>
       </c>
       <c r="CH4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CI4" t="s">
         <v>79</v>
@@ -3032,7 +3056,7 @@
         <v>116</v>
       </c>
       <c r="DW4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="DX4" t="s">
         <v>117</v>
@@ -3188,7 +3212,7 @@
         <v>167</v>
       </c>
       <c r="FW4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="FX4" t="s">
         <v>168</v>
@@ -4741,7 +4765,7 @@
         <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D68" t="s">
         <v>318</v>
@@ -4935,6 +4959,198 @@
         <v>318</v>
       </c>
       <c r="LB81" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="82" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>69</v>
+      </c>
+      <c r="H82" t="s">
+        <v>318</v>
+      </c>
+      <c r="AR82" t="s">
+        <v>318</v>
+      </c>
+      <c r="GH82" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="83" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>70</v>
+      </c>
+      <c r="H83" t="s">
+        <v>318</v>
+      </c>
+      <c r="AP83" t="s">
+        <v>318</v>
+      </c>
+      <c r="GI83" t="s">
+        <v>318</v>
+      </c>
+      <c r="GJ83" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="84" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>71</v>
+      </c>
+      <c r="H84" t="s">
+        <v>318</v>
+      </c>
+      <c r="AQ84" t="s">
+        <v>318</v>
+      </c>
+      <c r="GK84" t="s">
+        <v>318</v>
+      </c>
+      <c r="GL84" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="85" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>72</v>
+      </c>
+      <c r="G85" t="s">
+        <v>318</v>
+      </c>
+      <c r="AN85" t="s">
+        <v>318</v>
+      </c>
+      <c r="FX85" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="86" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>73</v>
+      </c>
+      <c r="G86" t="s">
+        <v>318</v>
+      </c>
+      <c r="AL86" t="s">
+        <v>318</v>
+      </c>
+      <c r="FY86" t="s">
+        <v>318</v>
+      </c>
+      <c r="FZ86" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="87" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>74</v>
+      </c>
+      <c r="G87" t="s">
+        <v>318</v>
+      </c>
+      <c r="GB87" t="s">
+        <v>318</v>
+      </c>
+      <c r="GC87" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>75</v>
+      </c>
+      <c r="I88" t="s">
+        <v>318</v>
+      </c>
+      <c r="AM88" t="s">
+        <v>318</v>
+      </c>
+      <c r="AS88" t="s">
+        <v>318</v>
+      </c>
+      <c r="AU88" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="89" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>76</v>
+      </c>
+      <c r="I89" t="s">
+        <v>318</v>
+      </c>
+      <c r="AT89" t="s">
+        <v>318</v>
+      </c>
+      <c r="GO89" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>77</v>
+      </c>
+      <c r="I90" t="s">
+        <v>318</v>
+      </c>
+      <c r="GP90" t="s">
+        <v>318</v>
+      </c>
+      <c r="GQ90" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="91" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>78</v>
+      </c>
+      <c r="J91" t="s">
+        <v>318</v>
+      </c>
+      <c r="BI91" t="s">
+        <v>318</v>
+      </c>
+      <c r="GS91" t="s">
+        <v>318</v>
+      </c>
+      <c r="GT91" t="s">
+        <v>318</v>
+      </c>
+      <c r="HC91" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="92" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>79</v>
+      </c>
+      <c r="J92" t="s">
+        <v>318</v>
+      </c>
+      <c r="BG92" t="s">
+        <v>318</v>
+      </c>
+      <c r="HD92" t="s">
+        <v>318</v>
+      </c>
+      <c r="HE92" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="93" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>80</v>
+      </c>
+      <c r="J93" t="s">
+        <v>318</v>
+      </c>
+      <c r="BH93" t="s">
+        <v>318</v>
+      </c>
+      <c r="HG93" t="s">
+        <v>318</v>
+      </c>
+      <c r="HH93" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4989,7 +5205,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -5003,13 +5219,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="H3" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -5021,13 +5237,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="H5" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -5035,13 +5251,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Requerimientos numerados de forma correcta matriz de trazabilidad y lista de requerimientos
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77474B95-24B6-4129-8DC0-1CB4D0CDE535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B730CD4-1278-42D0-AD8B-385D03D29E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -1153,39 +1153,9 @@
     <t>/tesis_aceptar_nota_prorroga_director</t>
   </si>
   <si>
-    <t>21a</t>
-  </si>
-  <si>
-    <t>21b</t>
-  </si>
-  <si>
-    <t>21c</t>
-  </si>
-  <si>
-    <t>21d</t>
-  </si>
-  <si>
-    <t>21e</t>
-  </si>
-  <si>
-    <t>21f</t>
-  </si>
-  <si>
-    <t>21g</t>
-  </si>
-  <si>
-    <t>21h</t>
-  </si>
-  <si>
     <t>Director de Tesis</t>
   </si>
   <si>
-    <t>21i</t>
-  </si>
-  <si>
-    <t>21j</t>
-  </si>
-  <si>
     <t>TesisController.php @index_al_sec</t>
   </si>
   <si>
@@ -1232,6 +1202,36 @@
   </si>
   <si>
     <t>Proyecto</t>
+  </si>
+  <si>
+    <t>19a</t>
+  </si>
+  <si>
+    <t>19b</t>
+  </si>
+  <si>
+    <t>19c</t>
+  </si>
+  <si>
+    <t>19d</t>
+  </si>
+  <si>
+    <t>19e</t>
+  </si>
+  <si>
+    <t>19g</t>
+  </si>
+  <si>
+    <t>19f</t>
+  </si>
+  <si>
+    <t>19h</t>
+  </si>
+  <si>
+    <t>19i</t>
+  </si>
+  <si>
+    <t>19j</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LR93"/>
+  <dimension ref="A1:LR91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GY1" workbookViewId="0">
-      <selection activeCell="HD3" sqref="HD3"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K96" sqref="K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,13 +2355,13 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>334</v>
@@ -2388,10 +2388,10 @@
         <v>331</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -2418,31 +2418,31 @@
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AZ3" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BA3" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BB3" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BC3" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BD3" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
@@ -2458,7 +2458,7 @@
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
       <c r="BS3" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="BT3" s="1" t="s">
         <v>330</v>
@@ -2467,7 +2467,7 @@
         <v>331</v>
       </c>
       <c r="BV3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="BW3" s="1" t="s">
         <v>333</v>
@@ -2500,10 +2500,10 @@
       <c r="DA3" s="1"/>
       <c r="DB3" s="1"/>
       <c r="DC3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="DD3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
@@ -2526,7 +2526,7 @@
         <v>335</v>
       </c>
       <c r="DO3" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="DP3" s="1"/>
       <c r="DQ3" s="1"/>
@@ -2546,13 +2546,13 @@
       <c r="EC3" s="1"/>
       <c r="ED3" s="1"/>
       <c r="EE3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="EF3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="EG3" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
@@ -2565,7 +2565,7 @@
         <v>334</v>
       </c>
       <c r="EP3" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="EQ3" s="1"/>
       <c r="ER3" s="1"/>
@@ -2583,10 +2583,10 @@
       <c r="FB3" s="1"/>
       <c r="FC3" s="1"/>
       <c r="FI3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="FJ3" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="GE3" t="s">
         <v>331</v>
@@ -2595,7 +2595,7 @@
         <v>331</v>
       </c>
       <c r="GW3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="HD3" t="s">
         <v>329</v>
@@ -2634,7 +2634,7 @@
         <v>335</v>
       </c>
       <c r="IC3" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="IE3" t="s">
         <v>330</v>
@@ -2652,10 +2652,10 @@
         <v>331</v>
       </c>
       <c r="IU3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="IW3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="IY3" t="s">
         <v>330</v>
@@ -2664,19 +2664,19 @@
         <v>329</v>
       </c>
       <c r="JK3" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="KB3" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="LB3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="LC3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="LD3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:330" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -2828,7 +2828,7 @@
         <v>50</v>
       </c>
       <c r="AY4" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="AZ4" t="s">
         <v>52</v>
@@ -2864,7 +2864,7 @@
         <v>62</v>
       </c>
       <c r="BK4" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="BL4" t="s">
         <v>63</v>
@@ -2900,7 +2900,7 @@
         <v>73</v>
       </c>
       <c r="BW4" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="BX4" t="s">
         <v>74</v>
@@ -2933,7 +2933,7 @@
         <v>78</v>
       </c>
       <c r="CH4" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="CI4" t="s">
         <v>79</v>
@@ -3056,7 +3056,7 @@
         <v>116</v>
       </c>
       <c r="DW4" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="DX4" t="s">
         <v>117</v>
@@ -3212,7 +3212,7 @@
         <v>167</v>
       </c>
       <c r="FW4" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="FX4" t="s">
         <v>168</v>
@@ -3488,7 +3488,7 @@
         <v>257</v>
       </c>
       <c r="JK4" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="JL4" s="2" t="s">
         <v>258</v>
@@ -3842,11 +3842,29 @@
       <c r="A15">
         <v>11</v>
       </c>
+      <c r="N15" t="s">
+        <v>318</v>
+      </c>
+      <c r="DK15" t="s">
+        <v>318</v>
+      </c>
+      <c r="HP15" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="16" spans="1:330" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
+      <c r="N16" t="s">
+        <v>318</v>
+      </c>
+      <c r="DL16" t="s">
+        <v>318</v>
+      </c>
+      <c r="HQ16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="17" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -3855,10 +3873,10 @@
       <c r="N17" t="s">
         <v>318</v>
       </c>
-      <c r="DK17" t="s">
-        <v>318</v>
-      </c>
-      <c r="HP17" t="s">
+      <c r="DN17" t="s">
+        <v>318</v>
+      </c>
+      <c r="HR17" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3869,10 +3887,10 @@
       <c r="N18" t="s">
         <v>318</v>
       </c>
-      <c r="DL18" t="s">
-        <v>318</v>
-      </c>
-      <c r="HQ18" t="s">
+      <c r="DM18" t="s">
+        <v>318</v>
+      </c>
+      <c r="HS18" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3883,10 +3901,13 @@
       <c r="N19" t="s">
         <v>318</v>
       </c>
-      <c r="DN19" t="s">
-        <v>318</v>
-      </c>
-      <c r="HR19" t="s">
+      <c r="EA19" t="s">
+        <v>318</v>
+      </c>
+      <c r="IE19" t="s">
+        <v>318</v>
+      </c>
+      <c r="IF19" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3897,10 +3918,13 @@
       <c r="N20" t="s">
         <v>318</v>
       </c>
-      <c r="DM20" t="s">
-        <v>318</v>
-      </c>
-      <c r="HS20" t="s">
+      <c r="EB20" t="s">
+        <v>318</v>
+      </c>
+      <c r="IG20" t="s">
+        <v>318</v>
+      </c>
+      <c r="IH20" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3911,13 +3935,22 @@
       <c r="N21" t="s">
         <v>318</v>
       </c>
-      <c r="EA21" t="s">
-        <v>318</v>
-      </c>
-      <c r="IE21" t="s">
-        <v>318</v>
-      </c>
-      <c r="IF21" t="s">
+      <c r="CA21" t="s">
+        <v>318</v>
+      </c>
+      <c r="CB21" t="s">
+        <v>318</v>
+      </c>
+      <c r="KD21" t="s">
+        <v>318</v>
+      </c>
+      <c r="KE21" t="s">
+        <v>318</v>
+      </c>
+      <c r="KF21" t="s">
+        <v>318</v>
+      </c>
+      <c r="KG21" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3928,74 +3961,65 @@
       <c r="N22" t="s">
         <v>318</v>
       </c>
-      <c r="EB22" t="s">
-        <v>318</v>
-      </c>
-      <c r="IG22" t="s">
-        <v>318</v>
-      </c>
-      <c r="IH22" t="s">
+      <c r="CC22" t="s">
+        <v>318</v>
+      </c>
+      <c r="CD22" t="s">
+        <v>318</v>
+      </c>
+      <c r="CT22" t="s">
+        <v>318</v>
+      </c>
+      <c r="KT22" t="s">
+        <v>318</v>
+      </c>
+      <c r="KU22" t="s">
+        <v>318</v>
+      </c>
+      <c r="KV22" t="s">
+        <v>318</v>
+      </c>
+      <c r="KW22" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>19</v>
+      <c r="A23" s="5" t="s">
+        <v>359</v>
       </c>
       <c r="N23" t="s">
         <v>318</v>
       </c>
-      <c r="CA23" t="s">
-        <v>318</v>
-      </c>
-      <c r="CB23" t="s">
-        <v>318</v>
-      </c>
-      <c r="KD23" t="s">
-        <v>318</v>
-      </c>
-      <c r="KE23" t="s">
-        <v>318</v>
-      </c>
-      <c r="KF23" t="s">
-        <v>318</v>
-      </c>
-      <c r="KG23" t="s">
+      <c r="DU23" t="s">
+        <v>318</v>
+      </c>
+      <c r="EE23" t="s">
+        <v>318</v>
+      </c>
+      <c r="JF23" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
+      <c r="A24" t="s">
+        <v>360</v>
       </c>
       <c r="N24" t="s">
         <v>318</v>
       </c>
-      <c r="CC24" t="s">
-        <v>318</v>
-      </c>
-      <c r="CD24" t="s">
-        <v>318</v>
-      </c>
-      <c r="CT24" t="s">
-        <v>318</v>
-      </c>
-      <c r="KT24" t="s">
-        <v>318</v>
-      </c>
-      <c r="KU24" t="s">
-        <v>318</v>
-      </c>
-      <c r="KV24" t="s">
-        <v>318</v>
-      </c>
-      <c r="KW24" t="s">
+      <c r="DU24" t="s">
+        <v>318</v>
+      </c>
+      <c r="EH24" t="s">
+        <v>318</v>
+      </c>
+      <c r="JG24" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>342</v>
+      <c r="A25" t="s">
+        <v>361</v>
       </c>
       <c r="N25" t="s">
         <v>318</v>
@@ -4003,16 +4027,16 @@
       <c r="DU25" t="s">
         <v>318</v>
       </c>
-      <c r="EE25" t="s">
-        <v>318</v>
-      </c>
-      <c r="JF25" t="s">
+      <c r="EG25" t="s">
+        <v>318</v>
+      </c>
+      <c r="JI25" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
       <c r="N26" t="s">
         <v>318</v>
@@ -4020,140 +4044,137 @@
       <c r="DU26" t="s">
         <v>318</v>
       </c>
-      <c r="EH26" t="s">
-        <v>318</v>
-      </c>
-      <c r="JG26" t="s">
+      <c r="EF26" t="s">
+        <v>318</v>
+      </c>
+      <c r="JH26" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
       <c r="N27" t="s">
         <v>318</v>
       </c>
+      <c r="DC27" t="s">
+        <v>318</v>
+      </c>
       <c r="DU27" t="s">
         <v>318</v>
       </c>
-      <c r="EG27" t="s">
-        <v>318</v>
-      </c>
-      <c r="JI27" t="s">
+      <c r="IU27" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="N28" t="s">
         <v>318</v>
       </c>
+      <c r="DD28" t="s">
+        <v>318</v>
+      </c>
       <c r="DU28" t="s">
         <v>318</v>
       </c>
-      <c r="EF28" t="s">
-        <v>318</v>
-      </c>
-      <c r="JH28" t="s">
+      <c r="IW28" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="N29" t="s">
         <v>318</v>
       </c>
-      <c r="DC29" t="s">
+      <c r="DB29" t="s">
         <v>318</v>
       </c>
       <c r="DU29" t="s">
         <v>318</v>
       </c>
-      <c r="IU29" t="s">
+      <c r="IS29" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>347</v>
+        <v>366</v>
       </c>
       <c r="N30" t="s">
         <v>318</v>
       </c>
-      <c r="DD30" t="s">
+      <c r="DF30" t="s">
         <v>318</v>
       </c>
       <c r="DU30" t="s">
         <v>318</v>
       </c>
-      <c r="IW30" t="s">
+      <c r="HT30" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>348</v>
+        <v>367</v>
       </c>
       <c r="N31" t="s">
         <v>318</v>
       </c>
-      <c r="DB31" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU31" t="s">
-        <v>318</v>
-      </c>
-      <c r="IS31" t="s">
+      <c r="ED31" t="s">
+        <v>318</v>
+      </c>
+      <c r="JZ31" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:309" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="N32" t="s">
         <v>318</v>
       </c>
-      <c r="DF32" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU32" t="s">
-        <v>318</v>
-      </c>
-      <c r="HT32" t="s">
+      <c r="EJ32" t="s">
+        <v>318</v>
+      </c>
+      <c r="KA32" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>351</v>
+      <c r="A33">
+        <v>20</v>
       </c>
       <c r="N33" t="s">
         <v>318</v>
       </c>
-      <c r="ED33" t="s">
-        <v>318</v>
-      </c>
-      <c r="JZ33" t="s">
+      <c r="DO33" t="s">
+        <v>318</v>
+      </c>
+      <c r="JK33" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="34" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>352</v>
+      <c r="A34">
+        <v>21</v>
       </c>
       <c r="N34" t="s">
         <v>318</v>
       </c>
-      <c r="EJ34" t="s">
-        <v>318</v>
-      </c>
-      <c r="KA34" t="s">
+      <c r="FB34" t="s">
+        <v>318</v>
+      </c>
+      <c r="JA34" t="s">
+        <v>318</v>
+      </c>
+      <c r="JB34" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4164,10 +4185,13 @@
       <c r="N35" t="s">
         <v>318</v>
       </c>
-      <c r="DO35" t="s">
-        <v>318</v>
-      </c>
-      <c r="JK35" t="s">
+      <c r="CT35" t="s">
+        <v>318</v>
+      </c>
+      <c r="JQ35" t="s">
+        <v>318</v>
+      </c>
+      <c r="JR35" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4178,13 +4202,13 @@
       <c r="N36" t="s">
         <v>318</v>
       </c>
-      <c r="FB36" t="s">
-        <v>318</v>
-      </c>
-      <c r="JA36" t="s">
-        <v>318</v>
-      </c>
-      <c r="JB36" t="s">
+      <c r="CT36" t="s">
+        <v>318</v>
+      </c>
+      <c r="JQ36" t="s">
+        <v>318</v>
+      </c>
+      <c r="JR36" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4195,13 +4219,10 @@
       <c r="N37" t="s">
         <v>318</v>
       </c>
-      <c r="CT37" t="s">
-        <v>318</v>
-      </c>
-      <c r="JQ37" t="s">
-        <v>318</v>
-      </c>
-      <c r="JR37" t="s">
+      <c r="EO37" t="s">
+        <v>318</v>
+      </c>
+      <c r="HN37" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4212,13 +4233,10 @@
       <c r="N38" t="s">
         <v>318</v>
       </c>
-      <c r="CT38" t="s">
-        <v>318</v>
-      </c>
-      <c r="JQ38" t="s">
-        <v>318</v>
-      </c>
-      <c r="JR38" t="s">
+      <c r="DX38" t="s">
+        <v>318</v>
+      </c>
+      <c r="HO38" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4226,13 +4244,13 @@
       <c r="A39">
         <v>26</v>
       </c>
-      <c r="N39" t="s">
-        <v>318</v>
-      </c>
-      <c r="EO39" t="s">
-        <v>318</v>
-      </c>
-      <c r="HN39" t="s">
+      <c r="C39" t="s">
+        <v>318</v>
+      </c>
+      <c r="R39" t="s">
+        <v>318</v>
+      </c>
+      <c r="FC39" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4240,13 +4258,22 @@
       <c r="A40">
         <v>27</v>
       </c>
-      <c r="N40" t="s">
-        <v>318</v>
-      </c>
-      <c r="DX40" t="s">
-        <v>318</v>
-      </c>
-      <c r="HO40" t="s">
+      <c r="C40" t="s">
+        <v>318</v>
+      </c>
+      <c r="P40" t="s">
+        <v>318</v>
+      </c>
+      <c r="R40" t="s">
+        <v>318</v>
+      </c>
+      <c r="FC40" t="s">
+        <v>318</v>
+      </c>
+      <c r="FD40" t="s">
+        <v>318</v>
+      </c>
+      <c r="FH40" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4257,10 +4284,19 @@
       <c r="C41" t="s">
         <v>318</v>
       </c>
+      <c r="Q41" t="s">
+        <v>318</v>
+      </c>
       <c r="R41" t="s">
         <v>318</v>
       </c>
       <c r="FC41" t="s">
+        <v>318</v>
+      </c>
+      <c r="FE41" t="s">
+        <v>318</v>
+      </c>
+      <c r="FF41" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4271,19 +4307,10 @@
       <c r="C42" t="s">
         <v>318</v>
       </c>
-      <c r="P42" t="s">
-        <v>318</v>
-      </c>
       <c r="R42" t="s">
         <v>318</v>
       </c>
-      <c r="FC42" t="s">
-        <v>318</v>
-      </c>
-      <c r="FD42" t="s">
-        <v>318</v>
-      </c>
-      <c r="FH42" t="s">
+      <c r="FG42" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4291,22 +4318,13 @@
       <c r="A43">
         <v>30</v>
       </c>
-      <c r="C43" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>318</v>
-      </c>
-      <c r="R43" t="s">
-        <v>318</v>
-      </c>
-      <c r="FC43" t="s">
-        <v>318</v>
-      </c>
-      <c r="FE43" t="s">
-        <v>318</v>
-      </c>
-      <c r="FF43" t="s">
+      <c r="N43" t="s">
+        <v>318</v>
+      </c>
+      <c r="EW43" t="s">
+        <v>318</v>
+      </c>
+      <c r="KB43" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4314,13 +4332,16 @@
       <c r="A44">
         <v>31</v>
       </c>
-      <c r="C44" t="s">
-        <v>318</v>
-      </c>
-      <c r="R44" t="s">
-        <v>318</v>
-      </c>
-      <c r="FG44" t="s">
+      <c r="N44" t="s">
+        <v>318</v>
+      </c>
+      <c r="BU44" t="s">
+        <v>318</v>
+      </c>
+      <c r="GE44" t="s">
+        <v>318</v>
+      </c>
+      <c r="GF44" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4328,13 +4349,37 @@
       <c r="A45">
         <v>32</v>
       </c>
-      <c r="N45" t="s">
-        <v>318</v>
-      </c>
-      <c r="EW45" t="s">
-        <v>318</v>
-      </c>
-      <c r="KB45" t="s">
+      <c r="O45" t="s">
+        <v>318</v>
+      </c>
+      <c r="S45" t="s">
+        <v>318</v>
+      </c>
+      <c r="T45" t="s">
+        <v>318</v>
+      </c>
+      <c r="U45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LL45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LM45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LN45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LO45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LP45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LQ45" t="s">
+        <v>318</v>
+      </c>
+      <c r="LR45" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4342,16 +4387,16 @@
       <c r="A46">
         <v>33</v>
       </c>
-      <c r="N46" t="s">
-        <v>318</v>
-      </c>
-      <c r="BU46" t="s">
-        <v>318</v>
-      </c>
-      <c r="GE46" t="s">
-        <v>318</v>
-      </c>
-      <c r="GF46" t="s">
+      <c r="M46" t="s">
+        <v>318</v>
+      </c>
+      <c r="BK46" t="s">
+        <v>318</v>
+      </c>
+      <c r="HJ46" t="s">
+        <v>318</v>
+      </c>
+      <c r="HK46" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4359,37 +4404,16 @@
       <c r="A47">
         <v>34</v>
       </c>
-      <c r="O47" t="s">
-        <v>318</v>
-      </c>
-      <c r="S47" t="s">
-        <v>318</v>
-      </c>
-      <c r="T47" t="s">
-        <v>318</v>
-      </c>
-      <c r="U47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LL47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LM47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LN47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LO47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LP47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LQ47" t="s">
-        <v>318</v>
-      </c>
-      <c r="LR47" t="s">
+      <c r="M47" t="s">
+        <v>318</v>
+      </c>
+      <c r="BJ47" t="s">
+        <v>318</v>
+      </c>
+      <c r="HL47" t="s">
+        <v>318</v>
+      </c>
+      <c r="HM47" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4397,16 +4421,13 @@
       <c r="A48">
         <v>35</v>
       </c>
-      <c r="M48" t="s">
-        <v>318</v>
-      </c>
-      <c r="BK48" t="s">
-        <v>318</v>
-      </c>
-      <c r="HJ48" t="s">
-        <v>318</v>
-      </c>
-      <c r="HK48" t="s">
+      <c r="N48" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT48" t="s">
+        <v>318</v>
+      </c>
+      <c r="JL48" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4414,16 +4435,16 @@
       <c r="A49">
         <v>36</v>
       </c>
-      <c r="M49" t="s">
-        <v>318</v>
-      </c>
-      <c r="BJ49" t="s">
-        <v>318</v>
-      </c>
-      <c r="HL49" t="s">
-        <v>318</v>
-      </c>
-      <c r="HM49" t="s">
+      <c r="L49" t="s">
+        <v>318</v>
+      </c>
+      <c r="N49" t="s">
+        <v>318</v>
+      </c>
+      <c r="BE49" t="s">
+        <v>318</v>
+      </c>
+      <c r="CJ49" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4431,13 +4452,22 @@
       <c r="A50">
         <v>37</v>
       </c>
+      <c r="M50" t="s">
+        <v>318</v>
+      </c>
       <c r="N50" t="s">
         <v>318</v>
       </c>
-      <c r="DT50" t="s">
-        <v>318</v>
-      </c>
-      <c r="JL50" t="s">
+      <c r="EL50" t="s">
+        <v>318</v>
+      </c>
+      <c r="EM50" t="s">
+        <v>318</v>
+      </c>
+      <c r="JM50" t="s">
+        <v>318</v>
+      </c>
+      <c r="JN50" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4448,13 +4478,10 @@
       <c r="L51" t="s">
         <v>318</v>
       </c>
-      <c r="N51" t="s">
-        <v>318</v>
-      </c>
-      <c r="BE51" t="s">
-        <v>318</v>
-      </c>
-      <c r="CJ51" t="s">
+      <c r="AY51" t="s">
+        <v>318</v>
+      </c>
+      <c r="GW51" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4462,22 +4489,16 @@
       <c r="A52">
         <v>39</v>
       </c>
-      <c r="M52" t="s">
-        <v>318</v>
-      </c>
-      <c r="N52" t="s">
-        <v>318</v>
-      </c>
-      <c r="EL52" t="s">
-        <v>318</v>
-      </c>
-      <c r="EM52" t="s">
-        <v>318</v>
-      </c>
-      <c r="JM52" t="s">
-        <v>318</v>
-      </c>
-      <c r="JN52" t="s">
+      <c r="L52" t="s">
+        <v>318</v>
+      </c>
+      <c r="AW52" t="s">
+        <v>318</v>
+      </c>
+      <c r="GX52" t="s">
+        <v>318</v>
+      </c>
+      <c r="GY52" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4488,10 +4509,16 @@
       <c r="L53" t="s">
         <v>318</v>
       </c>
-      <c r="AY53" t="s">
-        <v>318</v>
-      </c>
-      <c r="GW53" t="s">
+      <c r="AX53" t="s">
+        <v>318</v>
+      </c>
+      <c r="GZ53" t="s">
+        <v>318</v>
+      </c>
+      <c r="HA53" t="s">
+        <v>318</v>
+      </c>
+      <c r="HB53" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4499,16 +4526,40 @@
       <c r="A54">
         <v>41</v>
       </c>
-      <c r="L54" t="s">
-        <v>318</v>
-      </c>
-      <c r="AW54" t="s">
-        <v>318</v>
-      </c>
-      <c r="GX54" t="s">
-        <v>318</v>
-      </c>
-      <c r="GY54" t="s">
+      <c r="N54" t="s">
+        <v>318</v>
+      </c>
+      <c r="AZ54" t="s">
+        <v>318</v>
+      </c>
+      <c r="BA54" t="s">
+        <v>318</v>
+      </c>
+      <c r="BB54" t="s">
+        <v>318</v>
+      </c>
+      <c r="BC54" t="s">
+        <v>318</v>
+      </c>
+      <c r="BD54" t="s">
+        <v>318</v>
+      </c>
+      <c r="DW54" t="s">
+        <v>318</v>
+      </c>
+      <c r="KJ54" t="s">
+        <v>318</v>
+      </c>
+      <c r="KK54" t="s">
+        <v>318</v>
+      </c>
+      <c r="KL54" t="s">
+        <v>318</v>
+      </c>
+      <c r="KM54" t="s">
+        <v>318</v>
+      </c>
+      <c r="KN54" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4516,19 +4567,16 @@
       <c r="A55">
         <v>42</v>
       </c>
-      <c r="L55" t="s">
-        <v>318</v>
-      </c>
-      <c r="AX55" t="s">
-        <v>318</v>
-      </c>
-      <c r="GZ55" t="s">
-        <v>318</v>
-      </c>
-      <c r="HA55" t="s">
-        <v>318</v>
-      </c>
-      <c r="HB55" t="s">
+      <c r="F55" t="s">
+        <v>318</v>
+      </c>
+      <c r="N55" t="s">
+        <v>318</v>
+      </c>
+      <c r="DJ55" t="s">
+        <v>318</v>
+      </c>
+      <c r="GG55" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4536,40 +4584,22 @@
       <c r="A56">
         <v>43</v>
       </c>
+      <c r="F56" t="s">
+        <v>318</v>
+      </c>
       <c r="N56" t="s">
         <v>318</v>
       </c>
-      <c r="AZ56" t="s">
-        <v>318</v>
-      </c>
-      <c r="BA56" t="s">
-        <v>318</v>
-      </c>
-      <c r="BB56" t="s">
-        <v>318</v>
-      </c>
-      <c r="BC56" t="s">
-        <v>318</v>
-      </c>
-      <c r="BD56" t="s">
-        <v>318</v>
-      </c>
-      <c r="DW56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KJ56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KK56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KL56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KM56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KN56" t="s">
+      <c r="CH56" t="s">
+        <v>318</v>
+      </c>
+      <c r="CL56" t="s">
+        <v>318</v>
+      </c>
+      <c r="CM56" t="s">
+        <v>318</v>
+      </c>
+      <c r="KQ56" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4583,10 +4613,13 @@
       <c r="N57" t="s">
         <v>318</v>
       </c>
-      <c r="DJ57" t="s">
-        <v>318</v>
-      </c>
-      <c r="GG57" t="s">
+      <c r="EI57" t="s">
+        <v>318</v>
+      </c>
+      <c r="IJ57" t="s">
+        <v>318</v>
+      </c>
+      <c r="IK57" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4594,22 +4627,16 @@
       <c r="A58">
         <v>45</v>
       </c>
-      <c r="F58" t="s">
-        <v>318</v>
-      </c>
-      <c r="N58" t="s">
-        <v>318</v>
-      </c>
-      <c r="CH58" t="s">
-        <v>318</v>
-      </c>
-      <c r="CL58" t="s">
-        <v>318</v>
-      </c>
-      <c r="CM58" t="s">
-        <v>318</v>
-      </c>
-      <c r="KQ58" t="s">
+      <c r="O58" t="s">
+        <v>318</v>
+      </c>
+      <c r="BO58" t="s">
+        <v>318</v>
+      </c>
+      <c r="LC58" t="s">
+        <v>318</v>
+      </c>
+      <c r="LD58" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4617,19 +4644,16 @@
       <c r="A59">
         <v>46</v>
       </c>
-      <c r="F59" t="s">
-        <v>318</v>
-      </c>
-      <c r="N59" t="s">
-        <v>318</v>
-      </c>
-      <c r="EI59" t="s">
-        <v>318</v>
-      </c>
-      <c r="IJ59" t="s">
-        <v>318</v>
-      </c>
-      <c r="IK59" t="s">
+      <c r="E59" t="s">
+        <v>318</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>318</v>
+      </c>
+      <c r="DL59" t="s">
+        <v>318</v>
+      </c>
+      <c r="FS59" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4637,16 +4661,16 @@
       <c r="A60">
         <v>47</v>
       </c>
-      <c r="O60" t="s">
-        <v>318</v>
-      </c>
-      <c r="BO60" t="s">
-        <v>318</v>
-      </c>
-      <c r="LC60" t="s">
-        <v>318</v>
-      </c>
-      <c r="LD60" t="s">
+      <c r="E60" t="s">
+        <v>318</v>
+      </c>
+      <c r="AI60" t="s">
+        <v>318</v>
+      </c>
+      <c r="FT60" t="s">
+        <v>318</v>
+      </c>
+      <c r="FV60" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4657,13 +4681,13 @@
       <c r="E61" t="s">
         <v>318</v>
       </c>
-      <c r="AJ61" t="s">
-        <v>318</v>
-      </c>
-      <c r="DL61" t="s">
-        <v>318</v>
-      </c>
-      <c r="FS61" t="s">
+      <c r="AH61" t="s">
+        <v>318</v>
+      </c>
+      <c r="FU61" t="s">
+        <v>318</v>
+      </c>
+      <c r="FW61" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4671,16 +4695,13 @@
       <c r="A62">
         <v>49</v>
       </c>
-      <c r="E62" t="s">
-        <v>318</v>
-      </c>
-      <c r="AI62" t="s">
-        <v>318</v>
-      </c>
-      <c r="FT62" t="s">
-        <v>318</v>
-      </c>
-      <c r="FV62" t="s">
+      <c r="D62" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>318</v>
+      </c>
+      <c r="FJ62" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4688,16 +4709,16 @@
       <c r="A63">
         <v>50</v>
       </c>
-      <c r="E63" t="s">
-        <v>318</v>
-      </c>
-      <c r="AH63" t="s">
-        <v>318</v>
-      </c>
-      <c r="FU63" t="s">
-        <v>318</v>
-      </c>
-      <c r="FW63" t="s">
+      <c r="D63" t="s">
+        <v>318</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>318</v>
+      </c>
+      <c r="FM63" t="s">
+        <v>318</v>
+      </c>
+      <c r="FN63" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4711,202 +4732,199 @@
       <c r="AB64" t="s">
         <v>318</v>
       </c>
-      <c r="FJ64" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="FO64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>52</v>
       </c>
       <c r="D65" t="s">
         <v>318</v>
       </c>
-      <c r="Z65" t="s">
-        <v>318</v>
-      </c>
-      <c r="FM65" t="s">
-        <v>318</v>
-      </c>
-      <c r="FN65" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="66" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="AB65" t="s">
+        <v>318</v>
+      </c>
+      <c r="FJ65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>53</v>
       </c>
+      <c r="C66" t="s">
+        <v>352</v>
+      </c>
       <c r="D66" t="s">
         <v>318</v>
       </c>
       <c r="AB66" t="s">
         <v>318</v>
       </c>
-      <c r="FO66" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="FJ66" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>54</v>
       </c>
       <c r="D67" t="s">
         <v>318</v>
       </c>
-      <c r="AB67" t="s">
-        <v>318</v>
-      </c>
-      <c r="FJ67" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="68" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="AA67" t="s">
+        <v>318</v>
+      </c>
+      <c r="FI67" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="68" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>55</v>
       </c>
-      <c r="C68" t="s">
-        <v>362</v>
-      </c>
       <c r="D68" t="s">
         <v>318</v>
       </c>
-      <c r="AB68" t="s">
-        <v>318</v>
-      </c>
-      <c r="FJ68" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="69" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="AD68" t="s">
+        <v>318</v>
+      </c>
+      <c r="FL68" t="s">
+        <v>318</v>
+      </c>
+      <c r="FP68" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="69" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>56</v>
       </c>
       <c r="D69" t="s">
         <v>318</v>
       </c>
-      <c r="AA69" t="s">
-        <v>318</v>
-      </c>
-      <c r="FI69" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="70" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="Y69" t="s">
+        <v>318</v>
+      </c>
+      <c r="FL69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>57</v>
       </c>
-      <c r="D70" t="s">
-        <v>318</v>
-      </c>
-      <c r="AD70" t="s">
-        <v>318</v>
-      </c>
-      <c r="FL70" t="s">
-        <v>318</v>
-      </c>
-      <c r="FP70" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="O70" t="s">
+        <v>318</v>
+      </c>
+      <c r="BT70" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV70" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>58</v>
       </c>
-      <c r="D71" t="s">
-        <v>318</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>318</v>
-      </c>
-      <c r="FL71" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="O71" t="s">
+        <v>318</v>
+      </c>
+      <c r="BY71" t="s">
+        <v>318</v>
+      </c>
+      <c r="GV71" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="72" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>59</v>
       </c>
       <c r="O72" t="s">
         <v>318</v>
       </c>
-      <c r="BT72" t="s">
+      <c r="BW72" t="s">
         <v>318</v>
       </c>
       <c r="GV72" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="73" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>60</v>
       </c>
       <c r="O73" t="s">
         <v>318</v>
       </c>
-      <c r="BY73" t="s">
+      <c r="BV73" t="s">
         <v>318</v>
       </c>
       <c r="GV73" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="74" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>61</v>
       </c>
       <c r="O74" t="s">
         <v>318</v>
       </c>
-      <c r="BW74" t="s">
+      <c r="BZ74" t="s">
         <v>318</v>
       </c>
       <c r="GV74" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="75" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>62</v>
       </c>
       <c r="O75" t="s">
         <v>318</v>
       </c>
-      <c r="BV75" t="s">
+      <c r="BS75" t="s">
         <v>318</v>
       </c>
       <c r="GV75" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>63</v>
       </c>
-      <c r="O76" t="s">
-        <v>318</v>
-      </c>
-      <c r="BZ76" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV76" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="N76" t="s">
+        <v>318</v>
+      </c>
+      <c r="EP76" t="s">
+        <v>318</v>
+      </c>
+      <c r="IC76" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>64</v>
       </c>
-      <c r="O77" t="s">
-        <v>318</v>
-      </c>
-      <c r="BS77" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV77" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="78" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="N77" t="s">
+        <v>318</v>
+      </c>
+      <c r="EP77" t="s">
+        <v>318</v>
+      </c>
+      <c r="IC77" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="78" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>65</v>
       </c>
@@ -4920,237 +4938,209 @@
         <v>318</v>
       </c>
     </row>
-    <row r="79" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>66</v>
       </c>
-      <c r="N79" t="s">
-        <v>318</v>
-      </c>
-      <c r="EP79" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC79" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="80" spans="1:237" x14ac:dyDescent="0.25">
+      <c r="O79" t="s">
+        <v>318</v>
+      </c>
+      <c r="BR79" t="s">
+        <v>318</v>
+      </c>
+      <c r="LB79" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="80" spans="1:314" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>67</v>
       </c>
-      <c r="N80" t="s">
-        <v>318</v>
-      </c>
-      <c r="EP80" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC80" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="81" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>318</v>
+      </c>
+      <c r="AR80" t="s">
+        <v>318</v>
+      </c>
+      <c r="GH80" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>68</v>
       </c>
-      <c r="O81" t="s">
-        <v>318</v>
-      </c>
-      <c r="BR81" t="s">
-        <v>318</v>
-      </c>
-      <c r="LB81" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="82" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>318</v>
+      </c>
+      <c r="AP81" t="s">
+        <v>318</v>
+      </c>
+      <c r="GI81" t="s">
+        <v>318</v>
+      </c>
+      <c r="GJ81" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="82" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>69</v>
       </c>
       <c r="H82" t="s">
         <v>318</v>
       </c>
-      <c r="AR82" t="s">
-        <v>318</v>
-      </c>
-      <c r="GH82" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="83" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="AQ82" t="s">
+        <v>318</v>
+      </c>
+      <c r="GK82" t="s">
+        <v>318</v>
+      </c>
+      <c r="GL82" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="83" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>70</v>
       </c>
-      <c r="H83" t="s">
-        <v>318</v>
-      </c>
-      <c r="AP83" t="s">
-        <v>318</v>
-      </c>
-      <c r="GI83" t="s">
-        <v>318</v>
-      </c>
-      <c r="GJ83" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="84" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>318</v>
+      </c>
+      <c r="AN83" t="s">
+        <v>318</v>
+      </c>
+      <c r="FX83" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="84" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>71</v>
       </c>
-      <c r="H84" t="s">
-        <v>318</v>
-      </c>
-      <c r="AQ84" t="s">
-        <v>318</v>
-      </c>
-      <c r="GK84" t="s">
-        <v>318</v>
-      </c>
-      <c r="GL84" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="85" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>318</v>
+      </c>
+      <c r="AL84" t="s">
+        <v>318</v>
+      </c>
+      <c r="FY84" t="s">
+        <v>318</v>
+      </c>
+      <c r="FZ84" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="85" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>72</v>
       </c>
       <c r="G85" t="s">
         <v>318</v>
       </c>
-      <c r="AN85" t="s">
-        <v>318</v>
-      </c>
-      <c r="FX85" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="86" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="GB85" t="s">
+        <v>318</v>
+      </c>
+      <c r="GC85" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="86" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>73</v>
       </c>
-      <c r="G86" t="s">
-        <v>318</v>
-      </c>
-      <c r="AL86" t="s">
-        <v>318</v>
-      </c>
-      <c r="FY86" t="s">
-        <v>318</v>
-      </c>
-      <c r="FZ86" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="87" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>318</v>
+      </c>
+      <c r="AM86" t="s">
+        <v>318</v>
+      </c>
+      <c r="AS86" t="s">
+        <v>318</v>
+      </c>
+      <c r="AU86" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="87" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>74</v>
       </c>
-      <c r="G87" t="s">
-        <v>318</v>
-      </c>
-      <c r="GB87" t="s">
-        <v>318</v>
-      </c>
-      <c r="GC87" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="88" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>318</v>
+      </c>
+      <c r="AT87" t="s">
+        <v>318</v>
+      </c>
+      <c r="GO87" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>75</v>
       </c>
       <c r="I88" t="s">
         <v>318</v>
       </c>
-      <c r="AM88" t="s">
-        <v>318</v>
-      </c>
-      <c r="AS88" t="s">
-        <v>318</v>
-      </c>
-      <c r="AU88" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="89" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="GP88" t="s">
+        <v>318</v>
+      </c>
+      <c r="GQ88" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="89" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>76</v>
       </c>
-      <c r="I89" t="s">
-        <v>318</v>
-      </c>
-      <c r="AT89" t="s">
-        <v>318</v>
-      </c>
-      <c r="GO89" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="90" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>318</v>
+      </c>
+      <c r="BI89" t="s">
+        <v>318</v>
+      </c>
+      <c r="GS89" t="s">
+        <v>318</v>
+      </c>
+      <c r="GT89" t="s">
+        <v>318</v>
+      </c>
+      <c r="HC89" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>77</v>
       </c>
-      <c r="I90" t="s">
-        <v>318</v>
-      </c>
-      <c r="GP90" t="s">
-        <v>318</v>
-      </c>
-      <c r="GQ90" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="91" spans="1:314" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>318</v>
+      </c>
+      <c r="BG90" t="s">
+        <v>318</v>
+      </c>
+      <c r="HD90" t="s">
+        <v>318</v>
+      </c>
+      <c r="HE90" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="91" spans="1:216" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>78</v>
       </c>
       <c r="J91" t="s">
         <v>318</v>
       </c>
-      <c r="BI91" t="s">
-        <v>318</v>
-      </c>
-      <c r="GS91" t="s">
-        <v>318</v>
-      </c>
-      <c r="GT91" t="s">
-        <v>318</v>
-      </c>
-      <c r="HC91" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="92" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>79</v>
-      </c>
-      <c r="J92" t="s">
-        <v>318</v>
-      </c>
-      <c r="BG92" t="s">
-        <v>318</v>
-      </c>
-      <c r="HD92" t="s">
-        <v>318</v>
-      </c>
-      <c r="HE92" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="93" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>80</v>
-      </c>
-      <c r="J93" t="s">
-        <v>318</v>
-      </c>
-      <c r="BH93" t="s">
-        <v>318</v>
-      </c>
-      <c r="HG93" t="s">
-        <v>318</v>
-      </c>
-      <c r="HH93" t="s">
+      <c r="BH91" t="s">
+        <v>318</v>
+      </c>
+      <c r="HG91" t="s">
+        <v>318</v>
+      </c>
+      <c r="HH91" t="s">
         <v>318</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Faltaba requerimiento de tesis propias del alumno
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B730CD4-1278-42D0-AD8B-385D03D29E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D082D48-27C0-4142-96C4-A90DC8D2018E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="370">
   <si>
     <t>MVC</t>
   </si>
@@ -506,9 +506,6 @@
     <t>/tesis/recopilacion_inf2</t>
   </si>
   <si>
-    <t>/tesis/recopilacion_inf_alumno2</t>
-  </si>
-  <si>
     <t>/tesis/repositorio_tesis</t>
   </si>
   <si>
@@ -1118,29 +1115,6 @@
     <t>TesisController @pedir_nota_pendiente</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Controlad</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>or:</t>
-    </r>
-  </si>
-  <si>
     <t>/tesis/aceptar_nota_pendiente</t>
   </si>
   <si>
@@ -1232,13 +1206,22 @@
   </si>
   <si>
     <t>19j</t>
+  </si>
+  <si>
+    <t>Profesor guia</t>
+  </si>
+  <si>
+    <t>Todos usuarios logueados</t>
+  </si>
+  <si>
+    <t>Profesor guia/Director Tesis/Alumno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1264,14 +1247,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1330,12 +1305,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1347,16 +1321,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1672,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LR91"/>
+  <dimension ref="A1:LQ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="K96" sqref="K96"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="DJ55" sqref="DJ55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1796,7 @@
     <col min="141" max="141" width="31.85546875" customWidth="1"/>
     <col min="142" max="142" width="25.42578125" customWidth="1"/>
     <col min="143" max="143" width="31" customWidth="1"/>
-    <col min="144" max="144" width="21.42578125" customWidth="1"/>
+    <col min="144" max="144" width="35" customWidth="1"/>
     <col min="145" max="145" width="24" customWidth="1"/>
     <col min="146" max="146" width="35.85546875" customWidth="1"/>
     <col min="147" max="147" width="20.7109375" customWidth="1"/>
@@ -1837,7 +1817,7 @@
     <col min="163" max="163" width="46" customWidth="1"/>
     <col min="164" max="164" width="30" customWidth="1"/>
     <col min="165" max="165" width="47" customWidth="1"/>
-    <col min="166" max="166" width="28.42578125" customWidth="1"/>
+    <col min="166" max="166" width="38" customWidth="1"/>
     <col min="167" max="167" width="31.140625" customWidth="1"/>
     <col min="168" max="168" width="39.42578125" customWidth="1"/>
     <col min="169" max="169" width="39.28515625" customWidth="1"/>
@@ -1859,9 +1839,9 @@
     <col min="185" max="185" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="186" max="186" width="28.7109375" customWidth="1"/>
     <col min="187" max="187" width="53.7109375" customWidth="1"/>
-    <col min="188" max="188" width="27.42578125" customWidth="1"/>
+    <col min="188" max="188" width="56.7109375" customWidth="1"/>
     <col min="189" max="189" width="26.85546875" customWidth="1"/>
-    <col min="190" max="190" width="25.28515625" customWidth="1"/>
+    <col min="190" max="190" width="38.42578125" customWidth="1"/>
     <col min="191" max="191" width="27.7109375" customWidth="1"/>
     <col min="192" max="192" width="29.140625" customWidth="1"/>
     <col min="193" max="193" width="35.42578125" customWidth="1"/>
@@ -1871,16 +1851,15 @@
     <col min="198" max="198" width="35.42578125" customWidth="1"/>
     <col min="199" max="199" width="38.42578125" customWidth="1"/>
     <col min="200" max="200" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="31.42578125" customWidth="1"/>
+    <col min="201" max="201" width="37.5703125" customWidth="1"/>
+    <col min="202" max="203" width="43.5703125" customWidth="1"/>
     <col min="204" max="204" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="30.140625" customWidth="1"/>
+    <col min="205" max="205" width="43.140625" customWidth="1"/>
     <col min="206" max="206" width="32.5703125" customWidth="1"/>
-    <col min="207" max="207" width="28.28515625" customWidth="1"/>
+    <col min="207" max="207" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="208" max="208" width="31" customWidth="1"/>
-    <col min="209" max="209" width="29.85546875" customWidth="1"/>
-    <col min="210" max="210" width="27.7109375" customWidth="1"/>
+    <col min="209" max="209" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="33.5703125" customWidth="1"/>
     <col min="211" max="211" width="26.140625" customWidth="1"/>
     <col min="212" max="212" width="28" customWidth="1"/>
     <col min="213" max="213" width="28.28515625" customWidth="1"/>
@@ -1891,18 +1870,18 @@
     <col min="218" max="218" width="34.7109375" customWidth="1"/>
     <col min="219" max="219" width="37.140625" customWidth="1"/>
     <col min="220" max="220" width="38.5703125" customWidth="1"/>
-    <col min="221" max="221" width="30.28515625" customWidth="1"/>
+    <col min="221" max="221" width="46.85546875" customWidth="1"/>
     <col min="222" max="222" width="38.42578125" customWidth="1"/>
     <col min="223" max="223" width="45.5703125" customWidth="1"/>
     <col min="224" max="224" width="39.85546875" customWidth="1"/>
     <col min="225" max="225" width="40" bestFit="1" customWidth="1"/>
     <col min="226" max="226" width="54.140625" customWidth="1"/>
-    <col min="227" max="227" width="23.85546875" customWidth="1"/>
+    <col min="227" max="227" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="45" customWidth="1"/>
     <col min="229" max="229" width="29.85546875" customWidth="1"/>
     <col min="230" max="230" width="26.85546875" customWidth="1"/>
     <col min="231" max="231" width="33.42578125" customWidth="1"/>
-    <col min="232" max="232" width="22.140625" customWidth="1"/>
+    <col min="232" max="232" width="36.28515625" customWidth="1"/>
     <col min="233" max="233" width="43.5703125" customWidth="1"/>
     <col min="234" max="234" width="39.85546875" customWidth="1"/>
     <col min="235" max="235" width="37.28515625" customWidth="1"/>
@@ -2002,7 +1981,8 @@
     <col min="330" max="330" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:330" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -2013,385 +1993,388 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:330" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="9"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="9"/>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="9"/>
-      <c r="CA2" s="9"/>
-      <c r="CB2" s="9"/>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="9"/>
-      <c r="CE2" s="9"/>
-      <c r="CF2" s="9"/>
-      <c r="CG2" s="9"/>
-      <c r="CH2" s="9"/>
-      <c r="CI2" s="9"/>
-      <c r="CJ2" s="9"/>
-      <c r="CK2" s="9"/>
-      <c r="CL2" s="9"/>
-      <c r="CM2" s="9"/>
-      <c r="CN2" s="9"/>
-      <c r="CO2" s="9"/>
-      <c r="CP2" s="9"/>
-      <c r="CQ2" s="9"/>
-      <c r="CR2" s="9"/>
-      <c r="CS2" s="9"/>
-      <c r="CT2" s="9"/>
-      <c r="CU2" s="9"/>
-      <c r="CV2" s="9"/>
-      <c r="CW2" s="9"/>
-      <c r="CX2" s="9"/>
-      <c r="CY2" s="9"/>
-      <c r="CZ2" s="9"/>
-      <c r="DA2" s="9"/>
-      <c r="DB2" s="9"/>
-      <c r="DC2" s="9"/>
-      <c r="DD2" s="9"/>
-      <c r="DE2" s="9"/>
-      <c r="DF2" s="9"/>
-      <c r="DG2" s="9"/>
-      <c r="DH2" s="9"/>
-      <c r="DI2" s="9"/>
-      <c r="DJ2" s="9"/>
-      <c r="DK2" s="9"/>
-      <c r="DL2" s="9"/>
-      <c r="DM2" s="9"/>
-      <c r="DN2" s="9"/>
-      <c r="DO2" s="9"/>
-      <c r="DP2" s="9"/>
-      <c r="DQ2" s="9"/>
-      <c r="DR2" s="9"/>
-      <c r="DS2" s="9"/>
-      <c r="DT2" s="9"/>
-      <c r="DU2" s="9"/>
-      <c r="DV2" s="9"/>
-      <c r="DW2" s="9"/>
-      <c r="DX2" s="9"/>
-      <c r="DY2" s="9"/>
-      <c r="DZ2" s="9"/>
-      <c r="EA2" s="9"/>
-      <c r="EB2" s="9"/>
-      <c r="EC2" s="9"/>
-      <c r="ED2" s="9"/>
-      <c r="EE2" s="9"/>
-      <c r="EF2" s="9"/>
-      <c r="EG2" s="9"/>
-      <c r="EH2" s="9"/>
-      <c r="EI2" s="9"/>
-      <c r="EJ2" s="9"/>
-      <c r="EK2" s="9"/>
-      <c r="EL2" s="9"/>
-      <c r="EM2" s="9"/>
-      <c r="EN2" s="9"/>
-      <c r="EO2" s="9"/>
-      <c r="EP2" s="9"/>
-      <c r="EQ2" s="9"/>
-      <c r="ER2" s="9"/>
-      <c r="ES2" s="9"/>
-      <c r="ET2" s="9"/>
-      <c r="EU2" s="9"/>
-      <c r="EV2" s="9"/>
-      <c r="EW2" s="9"/>
-      <c r="EX2" s="9"/>
-      <c r="EY2" s="9"/>
-      <c r="EZ2" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="FA2" s="11"/>
-      <c r="FB2" s="11"/>
-      <c r="FC2" s="11"/>
-      <c r="FD2" s="11"/>
-      <c r="FE2" s="11"/>
-      <c r="FF2" s="11"/>
-      <c r="FG2" s="11"/>
-      <c r="FH2" s="11"/>
-      <c r="FI2" s="11"/>
-      <c r="FJ2" s="11"/>
-      <c r="FK2" s="11"/>
-      <c r="FL2" s="11"/>
-      <c r="FM2" s="11"/>
-      <c r="FN2" s="11"/>
-      <c r="FO2" s="11"/>
-      <c r="FP2" s="11"/>
-      <c r="FQ2" s="11"/>
-      <c r="FR2" s="11"/>
-      <c r="FS2" s="11"/>
-      <c r="FT2" s="11"/>
-      <c r="FU2" s="11"/>
-      <c r="FV2" s="11"/>
-      <c r="FW2" s="11"/>
-      <c r="FX2" s="11"/>
-      <c r="FY2" s="11"/>
-      <c r="FZ2" s="11"/>
-      <c r="GA2" s="11"/>
-      <c r="GB2" s="11"/>
-      <c r="GC2" s="11"/>
-      <c r="GD2" s="11"/>
-      <c r="GE2" s="11"/>
-      <c r="GF2" s="11"/>
-      <c r="GG2" s="11"/>
-      <c r="GH2" s="11"/>
-      <c r="GI2" s="11"/>
-      <c r="GJ2" s="11"/>
-      <c r="GK2" s="11"/>
-      <c r="GL2" s="11"/>
-      <c r="GM2" s="11"/>
-      <c r="GN2" s="11"/>
-      <c r="GO2" s="11"/>
-      <c r="GP2" s="11"/>
-      <c r="GQ2" s="11"/>
-      <c r="GR2" s="11"/>
-      <c r="GS2" s="11"/>
-      <c r="GT2" s="11"/>
-      <c r="GU2" s="11"/>
-      <c r="GV2" s="11"/>
-      <c r="GW2" s="11"/>
-      <c r="GX2" s="11"/>
-      <c r="GY2" s="11"/>
-      <c r="GZ2" s="11"/>
-      <c r="HA2" s="11"/>
-      <c r="HB2" s="11"/>
-      <c r="HC2" s="11"/>
-      <c r="HD2" s="11"/>
-      <c r="HE2" s="11"/>
-      <c r="HF2" s="11"/>
-      <c r="HG2" s="11"/>
-      <c r="HH2" s="11"/>
-      <c r="HI2" s="11"/>
-      <c r="HJ2" s="11"/>
-      <c r="HK2" s="11"/>
-      <c r="HL2" s="11"/>
-      <c r="HM2" s="11"/>
-      <c r="HN2" s="11"/>
-      <c r="HO2" s="11"/>
-      <c r="HP2" s="11"/>
-      <c r="HQ2" s="11"/>
-      <c r="HR2" s="11"/>
-      <c r="HS2" s="11"/>
-      <c r="HT2" s="11"/>
-      <c r="HU2" s="11"/>
-      <c r="HV2" s="11"/>
-      <c r="HW2" s="11"/>
-      <c r="HX2" s="11"/>
-      <c r="HY2" s="11"/>
-      <c r="HZ2" s="11"/>
-      <c r="IA2" s="11"/>
-      <c r="IB2" s="11"/>
-      <c r="IC2" s="11"/>
-      <c r="ID2" s="11"/>
-      <c r="IE2" s="11"/>
-      <c r="IF2" s="11"/>
-      <c r="IG2" s="11"/>
-      <c r="IH2" s="11"/>
-      <c r="II2" s="11"/>
-      <c r="IJ2" s="11"/>
-      <c r="IK2" s="11"/>
-      <c r="IL2" s="11"/>
-      <c r="IM2" s="11"/>
-      <c r="IN2" s="11"/>
-      <c r="IO2" s="11"/>
-      <c r="IP2" s="11"/>
-      <c r="IQ2" s="11"/>
-      <c r="IR2" s="11"/>
-      <c r="IS2" s="11"/>
-      <c r="IT2" s="11"/>
-      <c r="IU2" s="11"/>
-      <c r="IV2" s="11"/>
-      <c r="IW2" s="11"/>
-      <c r="IX2" s="11"/>
-      <c r="IY2" s="11"/>
-      <c r="IZ2" s="11"/>
-      <c r="JA2" s="11"/>
-      <c r="JB2" s="11"/>
-      <c r="JC2" s="11"/>
-      <c r="JD2" s="11"/>
-      <c r="JE2" s="11"/>
-      <c r="JF2" s="11"/>
-      <c r="JG2" s="11"/>
-      <c r="JH2" s="11"/>
-      <c r="JI2" s="11"/>
-      <c r="JJ2" s="11"/>
-      <c r="JK2" s="11"/>
-      <c r="JL2" s="11"/>
-      <c r="JM2" s="11"/>
-      <c r="JN2" s="11"/>
-      <c r="JO2" s="11"/>
-      <c r="JP2" s="11"/>
-      <c r="JQ2" s="11"/>
-      <c r="JR2" s="11"/>
-      <c r="JS2" s="11"/>
-      <c r="JT2" s="11"/>
-      <c r="JU2" s="11"/>
-      <c r="JV2" s="11"/>
-      <c r="JW2" s="11"/>
-      <c r="JX2" s="11"/>
-      <c r="JY2" s="11"/>
-      <c r="JZ2" s="11"/>
-      <c r="KA2" s="11"/>
-      <c r="KB2" s="11"/>
-      <c r="KC2" s="11"/>
-      <c r="KD2" s="11"/>
-      <c r="KE2" s="11"/>
-      <c r="KF2" s="11"/>
-      <c r="KG2" s="11"/>
-      <c r="KH2" s="11"/>
-      <c r="KI2" s="11"/>
-      <c r="KJ2" s="11"/>
-      <c r="KK2" s="11"/>
-      <c r="KL2" s="11"/>
-      <c r="KM2" s="11"/>
-      <c r="KN2" s="11"/>
-      <c r="KO2" s="11"/>
-      <c r="KP2" s="11"/>
-      <c r="KQ2" s="11"/>
-      <c r="KR2" s="11"/>
-      <c r="KS2" s="11"/>
-      <c r="KT2" s="11"/>
-      <c r="KU2" s="11"/>
-      <c r="KV2" s="11"/>
-      <c r="KW2" s="11"/>
-      <c r="KX2" s="11"/>
-      <c r="KY2" s="11"/>
-      <c r="KZ2" s="11"/>
-      <c r="LA2" s="11"/>
-      <c r="LB2" s="11"/>
-      <c r="LC2" s="11"/>
-      <c r="LD2" s="11"/>
-      <c r="LE2" s="11"/>
-      <c r="LF2" s="11"/>
-      <c r="LG2" s="11"/>
-      <c r="LH2" s="11"/>
-      <c r="LI2" s="11"/>
-      <c r="LJ2" s="11"/>
-      <c r="LK2" s="11"/>
-      <c r="LL2" s="11"/>
-      <c r="LM2" s="11"/>
-      <c r="LN2" s="4"/>
-      <c r="LO2" s="4"/>
-      <c r="LP2" s="4"/>
-    </row>
-    <row r="3" spans="1:330" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
+      <c r="DA2" s="8"/>
+      <c r="DB2" s="8"/>
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8"/>
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
+      <c r="DS2" s="8"/>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8"/>
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8"/>
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
+      <c r="EP2" s="8"/>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
+      <c r="ET2" s="8"/>
+      <c r="EU2" s="8"/>
+      <c r="EV2" s="8"/>
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
+      <c r="EZ2" s="13"/>
+      <c r="FA2" s="12"/>
+      <c r="FB2" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="FC2" s="10"/>
+      <c r="FD2" s="10"/>
+      <c r="FE2" s="10"/>
+      <c r="FF2" s="10"/>
+      <c r="FG2" s="10"/>
+      <c r="FH2" s="10"/>
+      <c r="FI2" s="10"/>
+      <c r="FJ2" s="10"/>
+      <c r="FK2" s="10"/>
+      <c r="FL2" s="10"/>
+      <c r="FM2" s="10"/>
+      <c r="FN2" s="10"/>
+      <c r="FO2" s="10"/>
+      <c r="FP2" s="10"/>
+      <c r="FQ2" s="10"/>
+      <c r="FR2" s="10"/>
+      <c r="FS2" s="10"/>
+      <c r="FT2" s="10"/>
+      <c r="FU2" s="10"/>
+      <c r="FV2" s="10"/>
+      <c r="FW2" s="10"/>
+      <c r="FX2" s="10"/>
+      <c r="FY2" s="10"/>
+      <c r="FZ2" s="10"/>
+      <c r="GA2" s="10"/>
+      <c r="GB2" s="10"/>
+      <c r="GC2" s="10"/>
+      <c r="GD2" s="10"/>
+      <c r="GE2" s="10"/>
+      <c r="GF2" s="10"/>
+      <c r="GG2" s="10"/>
+      <c r="GH2" s="10"/>
+      <c r="GI2" s="10"/>
+      <c r="GJ2" s="10"/>
+      <c r="GK2" s="10"/>
+      <c r="GL2" s="10"/>
+      <c r="GM2" s="10"/>
+      <c r="GN2" s="10"/>
+      <c r="GO2" s="10"/>
+      <c r="GP2" s="10"/>
+      <c r="GQ2" s="10"/>
+      <c r="GR2" s="10"/>
+      <c r="GS2" s="10"/>
+      <c r="GT2" s="10"/>
+      <c r="GU2" s="10"/>
+      <c r="GV2" s="10"/>
+      <c r="GW2" s="10"/>
+      <c r="GX2" s="10"/>
+      <c r="GY2" s="10"/>
+      <c r="GZ2" s="10"/>
+      <c r="HA2" s="10"/>
+      <c r="HB2" s="10"/>
+      <c r="HC2" s="10"/>
+      <c r="HD2" s="10"/>
+      <c r="HE2" s="10"/>
+      <c r="HF2" s="10"/>
+      <c r="HG2" s="10"/>
+      <c r="HH2" s="10"/>
+      <c r="HI2" s="10"/>
+      <c r="HJ2" s="10"/>
+      <c r="HK2" s="10"/>
+      <c r="HL2" s="10"/>
+      <c r="HM2" s="10"/>
+      <c r="HN2" s="10"/>
+      <c r="HO2" s="10"/>
+      <c r="HP2" s="10"/>
+      <c r="HQ2" s="10"/>
+      <c r="HR2" s="10"/>
+      <c r="HS2" s="10"/>
+      <c r="HT2" s="10"/>
+      <c r="HU2" s="10"/>
+      <c r="HV2" s="10"/>
+      <c r="HW2" s="10"/>
+      <c r="HX2" s="10"/>
+      <c r="HY2" s="10"/>
+      <c r="HZ2" s="10"/>
+      <c r="IA2" s="10"/>
+      <c r="IB2" s="10"/>
+      <c r="IC2" s="10"/>
+      <c r="ID2" s="10"/>
+      <c r="IE2" s="10"/>
+      <c r="IF2" s="10"/>
+      <c r="IG2" s="10"/>
+      <c r="IH2" s="10"/>
+      <c r="II2" s="10"/>
+      <c r="IJ2" s="10"/>
+      <c r="IK2" s="10"/>
+      <c r="IL2" s="10"/>
+      <c r="IM2" s="10"/>
+      <c r="IN2" s="10"/>
+      <c r="IO2" s="10"/>
+      <c r="IP2" s="10"/>
+      <c r="IQ2" s="10"/>
+      <c r="IR2" s="10"/>
+      <c r="IS2" s="10"/>
+      <c r="IT2" s="10"/>
+      <c r="IU2" s="10"/>
+      <c r="IV2" s="10"/>
+      <c r="IW2" s="10"/>
+      <c r="IX2" s="10"/>
+      <c r="IY2" s="10"/>
+      <c r="IZ2" s="10"/>
+      <c r="JA2" s="10"/>
+      <c r="JB2" s="10"/>
+      <c r="JC2" s="10"/>
+      <c r="JD2" s="10"/>
+      <c r="JE2" s="10"/>
+      <c r="JF2" s="10"/>
+      <c r="JG2" s="10"/>
+      <c r="JH2" s="10"/>
+      <c r="JI2" s="10"/>
+      <c r="JJ2" s="10"/>
+      <c r="JK2" s="10"/>
+      <c r="JL2" s="10"/>
+      <c r="JM2" s="10"/>
+      <c r="JN2" s="10"/>
+      <c r="JO2" s="10"/>
+      <c r="JP2" s="10"/>
+      <c r="JQ2" s="10"/>
+      <c r="JR2" s="10"/>
+      <c r="JS2" s="10"/>
+      <c r="JT2" s="10"/>
+      <c r="JU2" s="10"/>
+      <c r="JV2" s="10"/>
+      <c r="JW2" s="10"/>
+      <c r="JX2" s="10"/>
+      <c r="JY2" s="10"/>
+      <c r="JZ2" s="10"/>
+      <c r="KA2" s="10"/>
+      <c r="KB2" s="10"/>
+      <c r="KC2" s="10"/>
+      <c r="KD2" s="10"/>
+      <c r="KE2" s="10"/>
+      <c r="KF2" s="10"/>
+      <c r="KG2" s="10"/>
+      <c r="KH2" s="10"/>
+      <c r="KI2" s="10"/>
+      <c r="KJ2" s="10"/>
+      <c r="KK2" s="10"/>
+      <c r="KL2" s="10"/>
+      <c r="KM2" s="10"/>
+      <c r="KN2" s="10"/>
+      <c r="KO2" s="10"/>
+      <c r="KP2" s="10"/>
+      <c r="KQ2" s="10"/>
+      <c r="KR2" s="10"/>
+      <c r="KS2" s="10"/>
+      <c r="KT2" s="10"/>
+      <c r="KU2" s="10"/>
+      <c r="KV2" s="10"/>
+      <c r="KW2" s="10"/>
+      <c r="KX2" s="10"/>
+      <c r="KY2" s="10"/>
+      <c r="KZ2" s="10"/>
+      <c r="LA2" s="10"/>
+      <c r="LB2" s="10"/>
+      <c r="LC2" s="10"/>
+      <c r="LD2" s="10"/>
+      <c r="LE2" s="10"/>
+      <c r="LF2" s="10"/>
+      <c r="LG2" s="10"/>
+      <c r="LH2" s="10"/>
+      <c r="LI2" s="10"/>
+      <c r="LJ2" s="10"/>
+      <c r="LK2" s="10"/>
+      <c r="LL2" s="10"/>
+      <c r="LM2" s="10"/>
+      <c r="LN2" s="10"/>
+      <c r="LO2" s="10"/>
+      <c r="LP2" s="10"/>
+      <c r="LQ2" s="10"/>
+    </row>
+    <row r="3" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="W3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -2400,10 +2383,10 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -2418,31 +2401,31 @@
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="BA3" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="BB3" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="AZ3" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="BA3" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="BB3" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>344</v>
+      <c r="BC3" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="BD3" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
@@ -2458,19 +2441,19 @@
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
       <c r="BS3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="BT3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="BU3" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="BU3" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="BV3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="BW3" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="BX3" s="1"/>
       <c r="BY3" s="1"/>
@@ -2500,10 +2483,10 @@
       <c r="DA3" s="1"/>
       <c r="DB3" s="1"/>
       <c r="DC3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="DD3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
@@ -2511,22 +2494,22 @@
       <c r="DH3" s="1"/>
       <c r="DI3" s="1"/>
       <c r="DJ3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="DK3" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="DK3" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="DL3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="DM3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="DN3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="DO3" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="DP3" s="1"/>
       <c r="DQ3" s="1"/>
@@ -2540,19 +2523,19 @@
       <c r="DY3" s="1"/>
       <c r="DZ3" s="1"/>
       <c r="EA3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="EB3" s="1"/>
       <c r="EC3" s="1"/>
       <c r="ED3" s="1"/>
       <c r="EE3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="EF3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="EG3" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
@@ -2560,128 +2543,279 @@
       <c r="EK3" s="1"/>
       <c r="EL3" s="1"/>
       <c r="EM3" s="1"/>
-      <c r="EN3" s="1"/>
+      <c r="EN3" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="EO3" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="EP3" s="1" t="s">
-        <v>357</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="EP3" s="1"/>
       <c r="EQ3" s="1"/>
       <c r="ER3" s="1"/>
       <c r="ES3" s="1"/>
       <c r="ET3" s="1"/>
       <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
-      <c r="EW3" s="1" t="s">
-        <v>332</v>
-      </c>
+      <c r="EV3" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="EW3" s="1"/>
       <c r="EX3" s="1"/>
       <c r="EY3" s="1"/>
       <c r="EZ3" s="1"/>
       <c r="FA3" s="1"/>
-      <c r="FB3" s="1"/>
-      <c r="FC3" s="1"/>
+      <c r="FB3" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>348</v>
+      </c>
+      <c r="FD3" t="s">
+        <v>348</v>
+      </c>
+      <c r="FE3" t="s">
+        <v>348</v>
+      </c>
+      <c r="FF3" t="s">
+        <v>348</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>348</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>340</v>
+      </c>
       <c r="FI3" t="s">
+        <v>351</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>328</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>328</v>
+      </c>
+      <c r="FL3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FN3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FP3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>330</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FT3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>367</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>330</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>330</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>329</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GH3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GJ3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GK3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GL3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GN3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GO3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GQ3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GR3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GS3" t="s">
+        <v>367</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>368</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>340</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>340</v>
+      </c>
+      <c r="GX3" t="s">
+        <v>340</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>340</v>
+      </c>
+      <c r="GZ3" t="s">
+        <v>340</v>
+      </c>
+      <c r="HA3" t="s">
+        <v>340</v>
+      </c>
+      <c r="HB3" t="s">
+        <v>340</v>
+      </c>
+      <c r="HC3" t="s">
+        <v>367</v>
+      </c>
+      <c r="HD3" t="s">
+        <v>367</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>367</v>
+      </c>
+      <c r="HF3" t="s">
+        <v>367</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>367</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HJ3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>368</v>
+      </c>
+      <c r="HN3" t="s">
+        <v>369</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>330</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>334</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>334</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>334</v>
+      </c>
+      <c r="HT3" t="s">
+        <v>334</v>
+      </c>
+      <c r="HU3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HW3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IB3" t="s">
+        <v>354</v>
+      </c>
+      <c r="ID3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IJ3" t="s">
+        <v>331</v>
+      </c>
+      <c r="IK3" t="s">
+        <v>333</v>
+      </c>
+      <c r="IL3" t="s">
+        <v>332</v>
+      </c>
+      <c r="IM3" t="s">
+        <v>330</v>
+      </c>
+      <c r="IT3" t="s">
+        <v>340</v>
+      </c>
+      <c r="IV3" t="s">
+        <v>340</v>
+      </c>
+      <c r="IX3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IY3" t="s">
+        <v>328</v>
+      </c>
+      <c r="JJ3" t="s">
         <v>342</v>
       </c>
-      <c r="FJ3" t="s">
-        <v>353</v>
-      </c>
-      <c r="GE3" t="s">
-        <v>331</v>
-      </c>
-      <c r="GF3" t="s">
-        <v>331</v>
-      </c>
-      <c r="GW3" t="s">
-        <v>342</v>
-      </c>
-      <c r="HD3" t="s">
-        <v>329</v>
-      </c>
-      <c r="HE3" t="s">
-        <v>329</v>
-      </c>
-      <c r="HG3" t="s">
-        <v>329</v>
-      </c>
-      <c r="HH3" t="s">
-        <v>329</v>
-      </c>
-      <c r="HJ3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HK3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HL3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HM3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HP3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HQ3" t="s">
-        <v>331</v>
-      </c>
-      <c r="HR3" t="s">
-        <v>335</v>
-      </c>
-      <c r="HS3" t="s">
-        <v>335</v>
-      </c>
-      <c r="IC3" t="s">
-        <v>356</v>
-      </c>
-      <c r="IE3" t="s">
-        <v>330</v>
-      </c>
-      <c r="IK3" t="s">
-        <v>332</v>
-      </c>
-      <c r="IL3" t="s">
-        <v>334</v>
-      </c>
-      <c r="IM3" t="s">
-        <v>333</v>
-      </c>
-      <c r="IN3" t="s">
-        <v>331</v>
-      </c>
-      <c r="IU3" t="s">
-        <v>342</v>
-      </c>
-      <c r="IW3" t="s">
-        <v>342</v>
-      </c>
-      <c r="IY3" t="s">
-        <v>330</v>
-      </c>
-      <c r="IZ3" t="s">
-        <v>329</v>
-      </c>
-      <c r="JK3" t="s">
-        <v>344</v>
-      </c>
-      <c r="KB3" t="s">
-        <v>345</v>
+      <c r="KA3" t="s">
+        <v>343</v>
+      </c>
+      <c r="LA3" t="s">
+        <v>348</v>
       </c>
       <c r="LB3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="LC3" t="s">
-        <v>350</v>
-      </c>
-      <c r="LD3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>320</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>319</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2705,7 +2839,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -2741,13 +2875,13 @@
         <v>25</v>
       </c>
       <c r="V4" t="s">
+        <v>325</v>
+      </c>
+      <c r="W4" t="s">
+        <v>324</v>
+      </c>
+      <c r="X4" t="s">
         <v>326</v>
-      </c>
-      <c r="W4" t="s">
-        <v>325</v>
-      </c>
-      <c r="X4" t="s">
-        <v>327</v>
       </c>
       <c r="Y4" t="s">
         <v>26</v>
@@ -2828,7 +2962,7 @@
         <v>50</v>
       </c>
       <c r="AY4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AZ4" t="s">
         <v>52</v>
@@ -2864,7 +2998,7 @@
         <v>62</v>
       </c>
       <c r="BK4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="BL4" t="s">
         <v>63</v>
@@ -2900,7 +3034,7 @@
         <v>73</v>
       </c>
       <c r="BW4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BX4" t="s">
         <v>74</v>
@@ -2912,19 +3046,19 @@
         <v>76</v>
       </c>
       <c r="CA4" t="s">
+        <v>336</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>337</v>
+      </c>
+      <c r="CC4" t="s">
         <v>338</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CD4" t="s">
         <v>339</v>
       </c>
-      <c r="CC4" t="s">
-        <v>340</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>341</v>
-      </c>
       <c r="CE4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="CF4" t="s">
         <v>77</v>
@@ -2933,7 +3067,7 @@
         <v>78</v>
       </c>
       <c r="CH4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="CI4" t="s">
         <v>79</v>
@@ -3056,7 +3190,7 @@
         <v>116</v>
       </c>
       <c r="DW4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="DX4" t="s">
         <v>117</v>
@@ -3209,10 +3343,10 @@
         <v>166</v>
       </c>
       <c r="FV4" t="s">
+        <v>349</v>
+      </c>
+      <c r="FW4" t="s">
         <v>167</v>
-      </c>
-      <c r="FW4" t="s">
-        <v>351</v>
       </c>
       <c r="FX4" t="s">
         <v>168</v>
@@ -3283,16 +3417,16 @@
       <c r="GT4" t="s">
         <v>190</v>
       </c>
-      <c r="GU4" t="s">
+      <c r="GU4" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="GV4" s="2" t="s">
+      <c r="GV4" t="s">
         <v>192</v>
       </c>
-      <c r="GW4" t="s">
+      <c r="GW4" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="GX4" s="2" t="s">
+      <c r="GX4" t="s">
         <v>194</v>
       </c>
       <c r="GY4" t="s">
@@ -3340,19 +3474,19 @@
       <c r="HM4" t="s">
         <v>209</v>
       </c>
-      <c r="HN4" t="s">
+      <c r="HN4" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="HO4" s="2" t="s">
+      <c r="HO4" t="s">
         <v>211</v>
       </c>
       <c r="HP4" t="s">
         <v>212</v>
       </c>
-      <c r="HQ4" t="s">
+      <c r="HQ4" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="HR4" s="2" t="s">
+      <c r="HR4" t="s">
         <v>214</v>
       </c>
       <c r="HS4" t="s">
@@ -3389,15 +3523,15 @@
         <v>225</v>
       </c>
       <c r="ID4" t="s">
+        <v>335</v>
+      </c>
+      <c r="IE4" t="s">
         <v>226</v>
       </c>
-      <c r="IE4" t="s">
-        <v>336</v>
-      </c>
-      <c r="IF4" t="s">
+      <c r="IF4" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="IG4" s="2" t="s">
+      <c r="IG4" t="s">
         <v>228</v>
       </c>
       <c r="IH4" t="s">
@@ -3409,10 +3543,10 @@
       <c r="IJ4" t="s">
         <v>231</v>
       </c>
-      <c r="IK4" t="s">
+      <c r="IK4" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="IL4" s="2" t="s">
+      <c r="IL4" t="s">
         <v>233</v>
       </c>
       <c r="IM4" t="s">
@@ -3439,10 +3573,10 @@
       <c r="IT4" t="s">
         <v>241</v>
       </c>
-      <c r="IU4" t="s">
+      <c r="IU4" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="IV4" s="2" t="s">
+      <c r="IV4" t="s">
         <v>243</v>
       </c>
       <c r="IW4" t="s">
@@ -3478,19 +3612,19 @@
       <c r="JG4" t="s">
         <v>254</v>
       </c>
-      <c r="JH4" t="s">
+      <c r="JH4" s="2" t="s">
         <v>255</v>
       </c>
       <c r="JI4" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="JJ4" s="2" t="s">
+      <c r="JJ4" t="s">
+        <v>341</v>
+      </c>
+      <c r="JK4" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="JK4" t="s">
-        <v>343</v>
-      </c>
-      <c r="JL4" s="2" t="s">
+      <c r="JL4" t="s">
         <v>258</v>
       </c>
       <c r="JM4" t="s">
@@ -3526,10 +3660,10 @@
       <c r="JW4" t="s">
         <v>269</v>
       </c>
-      <c r="JX4" t="s">
+      <c r="JX4" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="JY4" s="2" t="s">
+      <c r="JY4" t="s">
         <v>271</v>
       </c>
       <c r="JZ4" t="s">
@@ -3541,10 +3675,10 @@
       <c r="KB4" t="s">
         <v>274</v>
       </c>
-      <c r="KC4" t="s">
+      <c r="KC4" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="KD4" s="2" t="s">
+      <c r="KD4" t="s">
         <v>276</v>
       </c>
       <c r="KE4" t="s">
@@ -3553,10 +3687,10 @@
       <c r="KF4" t="s">
         <v>278</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KG4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="KH4" s="2" t="s">
+      <c r="KH4" t="s">
         <v>280</v>
       </c>
       <c r="KI4" t="s">
@@ -3652,1518 +3786,1549 @@
       <c r="LM4" t="s">
         <v>311</v>
       </c>
-      <c r="LN4" t="s">
+      <c r="LN4" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="LO4" s="2" t="s">
+      <c r="LO4" t="s">
+        <v>315</v>
+      </c>
+      <c r="LP4" t="s">
+        <v>314</v>
+      </c>
+      <c r="LQ4" t="s">
         <v>313</v>
       </c>
-      <c r="LP4" t="s">
-        <v>316</v>
-      </c>
-      <c r="LQ4" t="s">
-        <v>315</v>
-      </c>
-      <c r="LR4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="5" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A5">
+    </row>
+    <row r="5" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BL5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BM5" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="KX5" t="s">
+        <v>317</v>
       </c>
       <c r="KY5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KZ5" t="s">
-        <v>318</v>
-      </c>
-      <c r="LA5" t="s">
-        <v>318</v>
-      </c>
-      <c r="LF5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>317</v>
+      </c>
+      <c r="LE5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="8" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CG8" t="s">
-        <v>318</v>
-      </c>
-      <c r="HX8" t="s">
-        <v>318</v>
-      </c>
-      <c r="IB8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>317</v>
+      </c>
+      <c r="HW8" t="s">
+        <v>317</v>
+      </c>
+      <c r="IA8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>5</v>
       </c>
+      <c r="F9" t="s">
+        <v>317</v>
+      </c>
       <c r="N9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CL9" t="s">
-        <v>318</v>
-      </c>
-      <c r="IJ9" t="s">
-        <v>318</v>
-      </c>
-      <c r="IY9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="10" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>317</v>
+      </c>
+      <c r="II9" t="s">
+        <v>317</v>
+      </c>
+      <c r="IX9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
+      <c r="F10" t="s">
+        <v>317</v>
+      </c>
       <c r="N10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CL10" t="s">
-        <v>318</v>
-      </c>
-      <c r="IJ10" t="s">
-        <v>318</v>
-      </c>
-      <c r="IY10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>317</v>
+      </c>
+      <c r="II10" t="s">
+        <v>317</v>
+      </c>
+      <c r="IX10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>7</v>
       </c>
       <c r="N11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CK11" t="s">
-        <v>318</v>
-      </c>
-      <c r="ID11" t="s">
-        <v>318</v>
-      </c>
-      <c r="IX11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="12" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A12">
+        <v>317</v>
+      </c>
+      <c r="IC11" t="s">
+        <v>317</v>
+      </c>
+      <c r="IW11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>8</v>
       </c>
+      <c r="F12" t="s">
+        <v>317</v>
+      </c>
       <c r="N12" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
       <c r="N13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CK13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CL13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CS13" t="s">
-        <v>318</v>
-      </c>
-      <c r="ID13" t="s">
-        <v>318</v>
-      </c>
-      <c r="IJ13" t="s">
-        <v>318</v>
-      </c>
-      <c r="IM13" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>317</v>
+      </c>
+      <c r="IC13" t="s">
+        <v>317</v>
+      </c>
+      <c r="II13" t="s">
+        <v>317</v>
+      </c>
+      <c r="IL13" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CK14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CR14" t="s">
-        <v>318</v>
-      </c>
-      <c r="ID14" t="s">
-        <v>318</v>
-      </c>
-      <c r="IN14" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="15" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A15">
+        <v>317</v>
+      </c>
+      <c r="IC14" t="s">
+        <v>317</v>
+      </c>
+      <c r="IM14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>11</v>
       </c>
       <c r="N15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DK15" t="s">
-        <v>318</v>
-      </c>
-      <c r="HP15" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A16">
+        <v>317</v>
+      </c>
+      <c r="HO15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
       <c r="N16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DL16" t="s">
-        <v>318</v>
-      </c>
-      <c r="HQ16" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A17">
+        <v>317</v>
+      </c>
+      <c r="HP16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>13</v>
       </c>
       <c r="N17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DN17" t="s">
-        <v>318</v>
-      </c>
-      <c r="HR17" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A18">
+        <v>317</v>
+      </c>
+      <c r="HQ17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DM18" t="s">
-        <v>318</v>
-      </c>
-      <c r="HS18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A19">
+        <v>317</v>
+      </c>
+      <c r="HR18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>15</v>
       </c>
       <c r="N19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EA19" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="ID19" t="s">
+        <v>317</v>
       </c>
       <c r="IE19" t="s">
-        <v>318</v>
-      </c>
-      <c r="IF19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A20">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EB20" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="IF20" t="s">
+        <v>317</v>
       </c>
       <c r="IG20" t="s">
-        <v>318</v>
-      </c>
-      <c r="IH20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A21">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CA21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CB21" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="KC21" t="s">
+        <v>317</v>
       </c>
       <c r="KD21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KE21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KF21" t="s">
-        <v>318</v>
-      </c>
-      <c r="KG21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A22">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>18</v>
       </c>
       <c r="N22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CC22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CD22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CT22" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="KS22" t="s">
+        <v>317</v>
       </c>
       <c r="KT22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KU22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KV22" t="s">
-        <v>318</v>
-      </c>
-      <c r="KW22" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="N23" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU23" t="s">
+        <v>317</v>
+      </c>
+      <c r="EE23" t="s">
+        <v>317</v>
+      </c>
+      <c r="JE23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="N24" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU24" t="s">
+        <v>317</v>
+      </c>
+      <c r="EH24" t="s">
+        <v>317</v>
+      </c>
+      <c r="JF24" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="N23" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU23" t="s">
-        <v>318</v>
-      </c>
-      <c r="EE23" t="s">
-        <v>318</v>
-      </c>
-      <c r="JF23" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="24" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="N25" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>317</v>
+      </c>
+      <c r="EG25" t="s">
+        <v>317</v>
+      </c>
+      <c r="JH25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="N24" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU24" t="s">
-        <v>318</v>
-      </c>
-      <c r="EH24" t="s">
-        <v>318</v>
-      </c>
-      <c r="JG24" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="N26" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU26" t="s">
+        <v>317</v>
+      </c>
+      <c r="EF26" t="s">
+        <v>317</v>
+      </c>
+      <c r="JG26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="N25" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU25" t="s">
-        <v>318</v>
-      </c>
-      <c r="EG25" t="s">
-        <v>318</v>
-      </c>
-      <c r="JI25" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="26" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="N27" t="s">
+        <v>317</v>
+      </c>
+      <c r="DC27" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU27" t="s">
+        <v>317</v>
+      </c>
+      <c r="IT27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="N28" t="s">
+        <v>317</v>
+      </c>
+      <c r="DD28" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU28" t="s">
+        <v>317</v>
+      </c>
+      <c r="IV28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="N26" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU26" t="s">
-        <v>318</v>
-      </c>
-      <c r="EF26" t="s">
-        <v>318</v>
-      </c>
-      <c r="JH26" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="27" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>363</v>
-      </c>
-      <c r="N27" t="s">
-        <v>318</v>
-      </c>
-      <c r="DC27" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU27" t="s">
-        <v>318</v>
-      </c>
-      <c r="IU27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="N29" t="s">
+        <v>317</v>
+      </c>
+      <c r="DB29" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU29" t="s">
+        <v>317</v>
+      </c>
+      <c r="IR29" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="N30" t="s">
+        <v>317</v>
+      </c>
+      <c r="DF30" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU30" t="s">
+        <v>317</v>
+      </c>
+      <c r="HS30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="N28" t="s">
-        <v>318</v>
-      </c>
-      <c r="DD28" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU28" t="s">
-        <v>318</v>
-      </c>
-      <c r="IW28" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>364</v>
-      </c>
-      <c r="N29" t="s">
-        <v>318</v>
-      </c>
-      <c r="DB29" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU29" t="s">
-        <v>318</v>
-      </c>
-      <c r="IS29" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="N31" t="s">
+        <v>317</v>
+      </c>
+      <c r="ED31" t="s">
+        <v>317</v>
+      </c>
+      <c r="JY31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:308" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="N30" t="s">
-        <v>318</v>
-      </c>
-      <c r="DF30" t="s">
-        <v>318</v>
-      </c>
-      <c r="DU30" t="s">
-        <v>318</v>
-      </c>
-      <c r="HT30" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="31" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>367</v>
-      </c>
-      <c r="N31" t="s">
-        <v>318</v>
-      </c>
-      <c r="ED31" t="s">
-        <v>318</v>
-      </c>
-      <c r="JZ31" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="32" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>368</v>
-      </c>
       <c r="N32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EJ32" t="s">
-        <v>318</v>
-      </c>
-      <c r="KA32" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="33" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A33">
+        <v>317</v>
+      </c>
+      <c r="JZ32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>20</v>
       </c>
       <c r="N33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DO33" t="s">
-        <v>318</v>
-      </c>
-      <c r="JK33" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="34" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A34">
+        <v>317</v>
+      </c>
+      <c r="JJ33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>21</v>
       </c>
       <c r="N34" t="s">
-        <v>318</v>
-      </c>
-      <c r="FB34" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="FA34" t="s">
+        <v>317</v>
+      </c>
+      <c r="IZ34" t="s">
+        <v>317</v>
       </c>
       <c r="JA34" t="s">
-        <v>318</v>
-      </c>
-      <c r="JB34" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="35" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>22</v>
       </c>
       <c r="N35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CT35" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="JP35" t="s">
+        <v>317</v>
       </c>
       <c r="JQ35" t="s">
-        <v>318</v>
-      </c>
-      <c r="JR35" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="36" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A36">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>23</v>
       </c>
       <c r="N36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CT36" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="JP36" t="s">
+        <v>317</v>
       </c>
       <c r="JQ36" t="s">
-        <v>318</v>
-      </c>
-      <c r="JR36" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="37" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A37">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>24</v>
       </c>
       <c r="N37" t="s">
-        <v>318</v>
-      </c>
-      <c r="EO37" t="s">
-        <v>318</v>
-      </c>
-      <c r="HN37" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="38" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A38">
+        <v>317</v>
+      </c>
+      <c r="EN37" t="s">
+        <v>317</v>
+      </c>
+      <c r="HM37" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DX38" t="s">
-        <v>318</v>
-      </c>
-      <c r="HO38" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="39" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A39">
+        <v>317</v>
+      </c>
+      <c r="HN38" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R39" t="s">
-        <v>318</v>
-      </c>
-      <c r="FC39" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="40" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A40">
+        <v>317</v>
+      </c>
+      <c r="FB39" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="40" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R40" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="FB40" t="s">
+        <v>317</v>
       </c>
       <c r="FC40" t="s">
-        <v>318</v>
-      </c>
-      <c r="FD40" t="s">
-        <v>318</v>
-      </c>
-      <c r="FH40" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="41" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A41">
+        <v>317</v>
+      </c>
+      <c r="FG40" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="41" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R41" t="s">
-        <v>318</v>
-      </c>
-      <c r="FC41" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="FB41" t="s">
+        <v>317</v>
+      </c>
+      <c r="FD41" t="s">
+        <v>317</v>
       </c>
       <c r="FE41" t="s">
-        <v>318</v>
-      </c>
-      <c r="FF41" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="42" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A42">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R42" t="s">
-        <v>318</v>
-      </c>
-      <c r="FG42" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="43" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A43">
+        <v>317</v>
+      </c>
+      <c r="FF42" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
         <v>30</v>
       </c>
       <c r="N43" t="s">
-        <v>318</v>
-      </c>
-      <c r="EW43" t="s">
-        <v>318</v>
-      </c>
-      <c r="KB43" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="44" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A44">
+        <v>317</v>
+      </c>
+      <c r="EV43" t="s">
+        <v>317</v>
+      </c>
+      <c r="KA43" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>31</v>
       </c>
       <c r="N44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BU44" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GD44" t="s">
+        <v>317</v>
       </c>
       <c r="GE44" t="s">
-        <v>318</v>
-      </c>
-      <c r="GF44" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="45" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="45" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
         <v>32</v>
       </c>
       <c r="O45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U45" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="LK45" t="s">
+        <v>317</v>
       </c>
       <c r="LL45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="LM45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="LN45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="LO45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="LP45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="LQ45" t="s">
-        <v>318</v>
-      </c>
-      <c r="LR45" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A46">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="46" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>33</v>
       </c>
       <c r="M46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BK46" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="HI46" t="s">
+        <v>317</v>
       </c>
       <c r="HJ46" t="s">
-        <v>318</v>
-      </c>
-      <c r="HK46" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="47" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A47">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>34</v>
       </c>
       <c r="M47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BJ47" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="HK47" t="s">
+        <v>317</v>
       </c>
       <c r="HL47" t="s">
-        <v>318</v>
-      </c>
-      <c r="HM47" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="48" spans="1:330" x14ac:dyDescent="0.25">
-      <c r="A48">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:329" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>35</v>
       </c>
       <c r="N48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DT48" t="s">
-        <v>318</v>
-      </c>
-      <c r="JL48" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="49" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A49">
+        <v>317</v>
+      </c>
+      <c r="JK48" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="49" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>36</v>
       </c>
       <c r="L49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BE49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CJ49" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="50" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A50">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>37</v>
       </c>
       <c r="M50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EL50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EM50" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="JL50" t="s">
+        <v>317</v>
       </c>
       <c r="JM50" t="s">
-        <v>318</v>
-      </c>
-      <c r="JN50" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="51" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A51">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>38</v>
       </c>
       <c r="L51" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AY51" t="s">
-        <v>318</v>
-      </c>
-      <c r="GW51" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="52" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A52">
+        <v>317</v>
+      </c>
+      <c r="GV51" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>39</v>
       </c>
       <c r="L52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AW52" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GW52" t="s">
+        <v>317</v>
       </c>
       <c r="GX52" t="s">
-        <v>318</v>
-      </c>
-      <c r="GY52" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="53" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A53">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>40</v>
       </c>
       <c r="L53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AX53" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GY53" t="s">
+        <v>317</v>
       </c>
       <c r="GZ53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="HA53" t="s">
-        <v>318</v>
-      </c>
-      <c r="HB53" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="54" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A54">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
         <v>41</v>
       </c>
       <c r="N54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AZ54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BA54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BB54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BC54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BD54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DW54" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="KI54" t="s">
+        <v>317</v>
       </c>
       <c r="KJ54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KK54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KL54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="KM54" t="s">
-        <v>318</v>
-      </c>
-      <c r="KN54" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="55" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A55">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="55" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
         <v>42</v>
       </c>
       <c r="F55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DJ55" t="s">
-        <v>318</v>
-      </c>
-      <c r="GG55" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="56" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A56">
+        <v>317</v>
+      </c>
+      <c r="GF55" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="56" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CH56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CL56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CM56" t="s">
-        <v>318</v>
-      </c>
-      <c r="KQ56" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="57" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A57">
+        <v>317</v>
+      </c>
+      <c r="KP56" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="57" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="EI57" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="II57" t="s">
+        <v>317</v>
       </c>
       <c r="IJ57" t="s">
-        <v>318</v>
-      </c>
-      <c r="IK57" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="58" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A58">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
         <v>45</v>
       </c>
       <c r="O58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BO58" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="LB58" t="s">
+        <v>317</v>
       </c>
       <c r="LC58" t="s">
-        <v>318</v>
-      </c>
-      <c r="LD58" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="59" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A59">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="59" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AJ59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="DL59" t="s">
-        <v>318</v>
-      </c>
-      <c r="FS59" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="60" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A60">
+        <v>317</v>
+      </c>
+      <c r="FR59" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="60" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
         <v>47</v>
       </c>
       <c r="E60" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI60" t="s">
-        <v>318</v>
-      </c>
-      <c r="FT60" t="s">
-        <v>318</v>
-      </c>
-      <c r="FV60" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="61" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A61">
+        <v>317</v>
+      </c>
+      <c r="FS60" t="s">
+        <v>317</v>
+      </c>
+      <c r="FU60" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="61" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
         <v>48</v>
       </c>
       <c r="E61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AH61" t="s">
-        <v>318</v>
-      </c>
-      <c r="FU61" t="s">
-        <v>318</v>
-      </c>
-      <c r="FW61" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="62" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A62">
+        <v>317</v>
+      </c>
+      <c r="FT61" t="s">
+        <v>317</v>
+      </c>
+      <c r="FV61" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="62" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
         <v>49</v>
       </c>
       <c r="D62" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB62" t="s">
-        <v>318</v>
-      </c>
-      <c r="FJ62" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="63" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A63">
+        <v>317</v>
+      </c>
+      <c r="FI62" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="63" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
         <v>50</v>
       </c>
       <c r="D63" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z63" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="FL63" t="s">
+        <v>317</v>
       </c>
       <c r="FM63" t="s">
-        <v>318</v>
-      </c>
-      <c r="FN63" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="64" spans="1:316" x14ac:dyDescent="0.25">
-      <c r="A64">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="64" spans="1:315" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
         <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB64" t="s">
-        <v>318</v>
-      </c>
-      <c r="FO64" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A65">
+        <v>317</v>
+      </c>
+      <c r="FN64" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
         <v>52</v>
       </c>
       <c r="D65" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB65" t="s">
-        <v>318</v>
-      </c>
-      <c r="FJ65" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="66" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A66">
+        <v>317</v>
+      </c>
+      <c r="FI65" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="66" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
         <v>53</v>
       </c>
       <c r="C66" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB66" t="s">
-        <v>318</v>
-      </c>
-      <c r="FJ66" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A67">
+        <v>317</v>
+      </c>
+      <c r="FI66" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="67" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
         <v>54</v>
       </c>
       <c r="D67" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA67" t="s">
-        <v>318</v>
-      </c>
-      <c r="FI67" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="68" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A68">
+        <v>317</v>
+      </c>
+      <c r="FH67" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="68" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
         <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD68" t="s">
-        <v>318</v>
-      </c>
-      <c r="FL68" t="s">
-        <v>318</v>
-      </c>
-      <c r="FP68" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="69" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A69">
+        <v>317</v>
+      </c>
+      <c r="FK68" t="s">
+        <v>317</v>
+      </c>
+      <c r="FO68" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="69" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
         <v>56</v>
       </c>
       <c r="D69" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Y69" t="s">
-        <v>318</v>
-      </c>
-      <c r="FL69" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="70" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A70">
+        <v>317</v>
+      </c>
+      <c r="FK69" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="70" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
         <v>57</v>
       </c>
       <c r="O70" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BT70" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV70" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A71">
+        <v>317</v>
+      </c>
+      <c r="GU70" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
         <v>58</v>
       </c>
       <c r="O71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BY71" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV71" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A72">
+        <v>317</v>
+      </c>
+      <c r="GU71" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="72" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
         <v>59</v>
       </c>
       <c r="O72" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BW72" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV72" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="73" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A73">
+        <v>317</v>
+      </c>
+      <c r="GU72" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="73" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
         <v>60</v>
       </c>
       <c r="O73" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BV73" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV73" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="74" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A74">
+        <v>317</v>
+      </c>
+      <c r="GU73" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="74" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
         <v>61</v>
       </c>
       <c r="O74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BZ74" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV74" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A75">
+        <v>317</v>
+      </c>
+      <c r="GU74" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="75" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
         <v>62</v>
       </c>
       <c r="O75" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BS75" t="s">
-        <v>318</v>
-      </c>
-      <c r="GV75" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="76" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A76">
+        <v>317</v>
+      </c>
+      <c r="GU75" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
         <v>63</v>
       </c>
       <c r="N76" t="s">
-        <v>318</v>
-      </c>
-      <c r="EP76" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC76" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A77">
+        <v>317</v>
+      </c>
+      <c r="EO76" t="s">
+        <v>317</v>
+      </c>
+      <c r="IB76" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
         <v>64</v>
       </c>
       <c r="N77" t="s">
-        <v>318</v>
-      </c>
-      <c r="EP77" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC77" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="78" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A78">
+        <v>317</v>
+      </c>
+      <c r="EO77" t="s">
+        <v>317</v>
+      </c>
+      <c r="IB77" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
         <v>65</v>
       </c>
       <c r="N78" t="s">
-        <v>318</v>
-      </c>
-      <c r="EP78" t="s">
-        <v>318</v>
-      </c>
-      <c r="IC78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="79" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A79">
+        <v>317</v>
+      </c>
+      <c r="EO78" t="s">
+        <v>317</v>
+      </c>
+      <c r="IB78" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="79" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
         <v>66</v>
       </c>
       <c r="O79" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BR79" t="s">
-        <v>318</v>
-      </c>
-      <c r="LB79" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="80" spans="1:314" x14ac:dyDescent="0.25">
-      <c r="A80">
+        <v>317</v>
+      </c>
+      <c r="LA79" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="80" spans="1:313" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
         <v>67</v>
       </c>
       <c r="H80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AR80" t="s">
-        <v>318</v>
-      </c>
-      <c r="GH80" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="81" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A81">
+        <v>317</v>
+      </c>
+      <c r="GG80" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="81" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
         <v>68</v>
       </c>
       <c r="H81" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AP81" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GH81" t="s">
+        <v>317</v>
       </c>
       <c r="GI81" t="s">
-        <v>318</v>
-      </c>
-      <c r="GJ81" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="82" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A82">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="82" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
         <v>69</v>
       </c>
       <c r="H82" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AQ82" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GJ82" t="s">
+        <v>317</v>
       </c>
       <c r="GK82" t="s">
-        <v>318</v>
-      </c>
-      <c r="GL82" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="83" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A83">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="83" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
         <v>70</v>
       </c>
       <c r="G83" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AN83" t="s">
-        <v>318</v>
-      </c>
-      <c r="FX83" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="84" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A84">
+        <v>317</v>
+      </c>
+      <c r="FW83" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
         <v>71</v>
       </c>
       <c r="G84" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AL84" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="FX84" t="s">
+        <v>317</v>
       </c>
       <c r="FY84" t="s">
-        <v>318</v>
-      </c>
-      <c r="FZ84" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="85" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A85">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
         <v>72</v>
       </c>
       <c r="G85" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GA85" t="s">
+        <v>317</v>
       </c>
       <c r="GB85" t="s">
-        <v>318</v>
-      </c>
-      <c r="GC85" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="86" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A86">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
         <v>73</v>
       </c>
       <c r="I86" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AM86" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AS86" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AU86" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="87" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A87">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="87" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
         <v>74</v>
       </c>
       <c r="I87" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AT87" t="s">
-        <v>318</v>
-      </c>
-      <c r="GO87" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="88" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A88">
+        <v>317</v>
+      </c>
+      <c r="GN87" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
         <v>75</v>
       </c>
       <c r="I88" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GO88" t="s">
+        <v>317</v>
       </c>
       <c r="GP88" t="s">
-        <v>318</v>
-      </c>
-      <c r="GQ88" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="89" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A89">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="89" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
         <v>76</v>
       </c>
       <c r="J89" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BI89" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="GR89" t="s">
+        <v>317</v>
       </c>
       <c r="GS89" t="s">
-        <v>318</v>
-      </c>
-      <c r="GT89" t="s">
-        <v>318</v>
-      </c>
-      <c r="HC89" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="90" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A90">
+        <v>317</v>
+      </c>
+      <c r="HB89" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="90" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
         <v>77</v>
       </c>
       <c r="J90" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BG90" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="HC90" t="s">
+        <v>317</v>
       </c>
       <c r="HD90" t="s">
-        <v>318</v>
-      </c>
-      <c r="HE90" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="91" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="A91">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="91" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
         <v>78</v>
       </c>
       <c r="J91" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BH91" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="HF91" t="s">
+        <v>317</v>
       </c>
       <c r="HG91" t="s">
-        <v>318</v>
-      </c>
-      <c r="HH91" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>79</v>
+      </c>
+      <c r="F92" t="s">
+        <v>317</v>
+      </c>
+      <c r="N92" t="s">
+        <v>317</v>
+      </c>
+      <c r="EO92" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:215" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>80</v>
+      </c>
+      <c r="N93" t="s">
+        <v>317</v>
+      </c>
+      <c r="DJ93" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C2:O2"/>
     <mergeCell ref="P2:EY2"/>
-    <mergeCell ref="EZ2:LM2"/>
+    <mergeCell ref="FB2:LQ2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="GX4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
-    <hyperlink ref="HO4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
-    <hyperlink ref="HR4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
-    <hyperlink ref="IG4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
-    <hyperlink ref="IL4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
-    <hyperlink ref="IV4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
-    <hyperlink ref="JI4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
-    <hyperlink ref="JJ4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
-    <hyperlink ref="JL4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
-    <hyperlink ref="JY4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
-    <hyperlink ref="KD4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
-    <hyperlink ref="KH4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
-    <hyperlink ref="LO4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
+    <hyperlink ref="GW4" r:id="rId1" display="MemorandumController@create" xr:uid="{259B2840-58E5-4B68-8412-6C1F5DBA155C}"/>
+    <hyperlink ref="HN4" r:id="rId2" display="TesisController@mostrar_tesis" xr:uid="{9DE7EAE2-6EAB-4C58-A5A0-2D5E3B1B9E54}"/>
+    <hyperlink ref="HQ4" r:id="rId3" display="TesisController@index3" xr:uid="{416C4C72-B6CC-4DC2-91C9-314AFA020695}"/>
+    <hyperlink ref="IF4" r:id="rId4" display="TesisController@peditr_nota_prorroga" xr:uid="{AFA3C804-3E5F-45D6-A9F4-5EA653FE9E2A}"/>
+    <hyperlink ref="IK4" r:id="rId5" display="TesisController@sinpermiso" xr:uid="{3A145C06-A786-4A9D-83E4-3B0E973BB03D}"/>
+    <hyperlink ref="IU4" r:id="rId6" display="TesisController@filtro_nota_prorroga" xr:uid="{05B22BEB-3FE3-4627-866D-E0CDF547128B}"/>
+    <hyperlink ref="JH4" r:id="rId7" display="TesisControllerr@" xr:uid="{BE768AAE-7C3F-4A8B-9090-22809D6A8F42}"/>
+    <hyperlink ref="JI4" r:id="rId8" display="TesisController@acta_examen" xr:uid="{C548118C-EED5-4FFE-B155-C7029F99A7FE}"/>
+    <hyperlink ref="JK4" r:id="rId9" display="TesisController@index_titulados_sec" xr:uid="{9DDD327F-1CA7-4D42-8F5D-D23F30E36A99}"/>
+    <hyperlink ref="JX4" r:id="rId10" display="TesisControllerr@informes_rangos_fechas" xr:uid="{AB3E1A2E-C8C0-4E49-80C4-EDA924CDB04A}"/>
+    <hyperlink ref="KC4" r:id="rId11" display="TesisController@" xr:uid="{99A079A2-237C-4890-A9BA-C5C554FA5767}"/>
+    <hyperlink ref="KG4" r:id="rId12" display="TesisController@create_num_memo" xr:uid="{F2875A30-1153-4062-A325-3D9E67E96F1C}"/>
+    <hyperlink ref="LN4" r:id="rId13" display="UsersController@credentials" xr:uid="{F097848D-0348-45EC-ACEC-69D8B62450B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -5182,20 +5347,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -5205,17 +5370,17 @@
         <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="9"/>
       <c r="H3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -5223,17 +5388,17 @@
         <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="10"/>
       <c r="H5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -5241,13 +5406,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Revisión matriz de trazabilidad y lista de requerimientos, faltaba num memo en memorandum de revision tesis
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717BBD6-6506-4362-A8A2-46EDCD0CB5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2DC775-74E1-4916-B61E-8732F670781F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="383">
   <si>
     <t>MVC</t>
   </si>
@@ -1253,6 +1253,24 @@
   </si>
   <si>
     <t>Profesor Guia/Director Tesis</t>
+  </si>
+  <si>
+    <t>/Auth/ ForgotController</t>
+  </si>
+  <si>
+    <t>/Auth/ LoginController</t>
+  </si>
+  <si>
+    <t>/Auth/ RegisterController</t>
+  </si>
+  <si>
+    <t>/Auth/ ResetPassword</t>
+  </si>
+  <si>
+    <t>VerificationController</t>
+  </si>
+  <si>
+    <t>Todos usuarios</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1399,20 +1417,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1729,10 +1748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LU94"/>
+  <dimension ref="A1:LY94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="LQ1" workbookViewId="0">
-      <selection activeCell="LT94" sqref="LT94"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,9 +1834,9 @@
     <col min="83" max="83" width="34.5703125" customWidth="1"/>
     <col min="84" max="84" width="16.7109375" customWidth="1"/>
     <col min="85" max="85" width="34.5703125" customWidth="1"/>
-    <col min="86" max="86" width="12.140625" customWidth="1"/>
+    <col min="86" max="86" width="47.42578125" customWidth="1"/>
     <col min="87" max="87" width="34.85546875" customWidth="1"/>
-    <col min="88" max="88" width="20.85546875" customWidth="1"/>
+    <col min="88" max="88" width="37.7109375" customWidth="1"/>
     <col min="89" max="89" width="24.42578125" customWidth="1"/>
     <col min="90" max="90" width="15.7109375" customWidth="1"/>
     <col min="91" max="91" width="14.85546875" customWidth="1"/>
@@ -1927,7 +1946,7 @@
     <col min="197" max="197" width="34.85546875" customWidth="1"/>
     <col min="198" max="198" width="35.42578125" customWidth="1"/>
     <col min="199" max="199" width="38.42578125" customWidth="1"/>
-    <col min="200" max="200" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="34.28515625" customWidth="1"/>
     <col min="201" max="201" width="37.5703125" customWidth="1"/>
     <col min="202" max="203" width="43.5703125" customWidth="1"/>
     <col min="204" max="204" width="48.140625" bestFit="1" customWidth="1"/>
@@ -1988,8 +2007,8 @@
     <col min="259" max="259" width="45.85546875" customWidth="1"/>
     <col min="260" max="260" width="39" customWidth="1"/>
     <col min="261" max="261" width="30" customWidth="1"/>
-    <col min="262" max="262" width="32.140625" customWidth="1"/>
-    <col min="263" max="263" width="31.28515625" customWidth="1"/>
+    <col min="262" max="262" width="43.85546875" customWidth="1"/>
+    <col min="263" max="263" width="45.42578125" customWidth="1"/>
     <col min="264" max="264" width="34.85546875" customWidth="1"/>
     <col min="265" max="265" width="32.5703125" customWidth="1"/>
     <col min="266" max="266" width="32.7109375" customWidth="1"/>
@@ -2005,7 +2024,7 @@
     <col min="276" max="276" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="277" max="277" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="278" max="278" width="36.140625" customWidth="1"/>
-    <col min="279" max="279" width="39.42578125" customWidth="1"/>
+    <col min="279" max="279" width="54" customWidth="1"/>
     <col min="280" max="280" width="43.7109375" customWidth="1"/>
     <col min="281" max="281" width="44.140625" customWidth="1"/>
     <col min="282" max="282" width="40.85546875" customWidth="1"/>
@@ -2045,7 +2064,7 @@
     <col min="316" max="316" width="43" customWidth="1"/>
     <col min="317" max="317" width="55.28515625" customWidth="1"/>
     <col min="318" max="318" width="45.5703125" customWidth="1"/>
-    <col min="319" max="319" width="42.5703125" customWidth="1"/>
+    <col min="319" max="319" width="56.42578125" customWidth="1"/>
     <col min="320" max="320" width="40.85546875" customWidth="1"/>
     <col min="321" max="321" width="34" bestFit="1" customWidth="1"/>
     <col min="322" max="322" width="45.85546875" customWidth="1"/>
@@ -2059,9 +2078,14 @@
     <col min="330" max="330" width="42" customWidth="1"/>
     <col min="331" max="331" width="42.85546875" customWidth="1"/>
     <col min="332" max="332" width="36.5703125" customWidth="1"/>
+    <col min="333" max="333" width="25.28515625" customWidth="1"/>
+    <col min="334" max="334" width="22.28515625" customWidth="1"/>
+    <col min="335" max="335" width="29.28515625" customWidth="1"/>
+    <col min="336" max="336" width="24" customWidth="1"/>
+    <col min="337" max="337" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="8" t="s">
         <v>367</v>
@@ -2076,173 +2100,173 @@
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="14" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
-      <c r="BF2" s="15"/>
-      <c r="BG2" s="15"/>
-      <c r="BH2" s="15"/>
-      <c r="BI2" s="15"/>
-      <c r="BJ2" s="15"/>
-      <c r="BK2" s="15"/>
-      <c r="BL2" s="15"/>
-      <c r="BM2" s="15"/>
-      <c r="BN2" s="15"/>
-      <c r="BO2" s="15"/>
-      <c r="BP2" s="15"/>
-      <c r="BQ2" s="15"/>
-      <c r="BR2" s="15"/>
-      <c r="BS2" s="15"/>
-      <c r="BT2" s="15"/>
-      <c r="BU2" s="15"/>
-      <c r="BV2" s="15"/>
-      <c r="BW2" s="15"/>
-      <c r="BX2" s="15"/>
-      <c r="BY2" s="15"/>
-      <c r="BZ2" s="15"/>
-      <c r="CA2" s="15"/>
-      <c r="CB2" s="15"/>
-      <c r="CC2" s="15"/>
-      <c r="CD2" s="15"/>
-      <c r="CE2" s="15"/>
-      <c r="CF2" s="15"/>
-      <c r="CG2" s="15"/>
-      <c r="CH2" s="15"/>
-      <c r="CI2" s="15"/>
-      <c r="CJ2" s="15"/>
-      <c r="CK2" s="15"/>
-      <c r="CL2" s="15"/>
-      <c r="CM2" s="15"/>
-      <c r="CN2" s="15"/>
-      <c r="CO2" s="15"/>
-      <c r="CP2" s="15"/>
-      <c r="CQ2" s="15"/>
-      <c r="CR2" s="15"/>
-      <c r="CS2" s="15"/>
-      <c r="CT2" s="15"/>
-      <c r="CU2" s="15"/>
-      <c r="CV2" s="15"/>
-      <c r="CW2" s="15"/>
-      <c r="CX2" s="15"/>
-      <c r="CY2" s="15"/>
-      <c r="CZ2" s="15"/>
-      <c r="DA2" s="15"/>
-      <c r="DB2" s="15"/>
-      <c r="DC2" s="15"/>
-      <c r="DD2" s="15"/>
-      <c r="DE2" s="15"/>
-      <c r="DF2" s="15"/>
-      <c r="DG2" s="15"/>
-      <c r="DH2" s="15"/>
-      <c r="DI2" s="15"/>
-      <c r="DJ2" s="15"/>
-      <c r="DK2" s="15"/>
-      <c r="DL2" s="15"/>
-      <c r="DM2" s="15"/>
-      <c r="DN2" s="15"/>
-      <c r="DO2" s="15"/>
-      <c r="DP2" s="15"/>
-      <c r="DQ2" s="15"/>
-      <c r="DR2" s="15"/>
-      <c r="DS2" s="15"/>
-      <c r="DT2" s="15"/>
-      <c r="DU2" s="15"/>
-      <c r="DV2" s="15"/>
-      <c r="DW2" s="15"/>
-      <c r="DX2" s="15"/>
-      <c r="DY2" s="15"/>
-      <c r="DZ2" s="15"/>
-      <c r="EA2" s="15"/>
-      <c r="EB2" s="15"/>
-      <c r="EC2" s="15"/>
-      <c r="ED2" s="15"/>
-      <c r="EE2" s="15"/>
-      <c r="EF2" s="15"/>
-      <c r="EG2" s="15"/>
-      <c r="EH2" s="15"/>
-      <c r="EI2" s="15"/>
-      <c r="EJ2" s="15"/>
-      <c r="EK2" s="15"/>
-      <c r="EL2" s="15"/>
-      <c r="EM2" s="15"/>
-      <c r="EN2" s="15"/>
-      <c r="EO2" s="15"/>
-      <c r="EP2" s="15"/>
-      <c r="EQ2" s="15"/>
-      <c r="ER2" s="15"/>
-      <c r="ES2" s="15"/>
-      <c r="ET2" s="15"/>
-      <c r="EU2" s="15"/>
-      <c r="EV2" s="15"/>
-      <c r="EW2" s="15"/>
-      <c r="EX2" s="15"/>
-      <c r="EY2" s="15"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+      <c r="AV2" s="18"/>
+      <c r="AW2" s="18"/>
+      <c r="AX2" s="18"/>
+      <c r="AY2" s="18"/>
+      <c r="AZ2" s="18"/>
+      <c r="BA2" s="18"/>
+      <c r="BB2" s="18"/>
+      <c r="BC2" s="18"/>
+      <c r="BD2" s="18"/>
+      <c r="BE2" s="18"/>
+      <c r="BF2" s="18"/>
+      <c r="BG2" s="18"/>
+      <c r="BH2" s="18"/>
+      <c r="BI2" s="18"/>
+      <c r="BJ2" s="18"/>
+      <c r="BK2" s="18"/>
+      <c r="BL2" s="18"/>
+      <c r="BM2" s="18"/>
+      <c r="BN2" s="18"/>
+      <c r="BO2" s="18"/>
+      <c r="BP2" s="18"/>
+      <c r="BQ2" s="18"/>
+      <c r="BR2" s="18"/>
+      <c r="BS2" s="18"/>
+      <c r="BT2" s="18"/>
+      <c r="BU2" s="18"/>
+      <c r="BV2" s="18"/>
+      <c r="BW2" s="18"/>
+      <c r="BX2" s="18"/>
+      <c r="BY2" s="18"/>
+      <c r="BZ2" s="18"/>
+      <c r="CA2" s="18"/>
+      <c r="CB2" s="18"/>
+      <c r="CC2" s="18"/>
+      <c r="CD2" s="18"/>
+      <c r="CE2" s="18"/>
+      <c r="CF2" s="18"/>
+      <c r="CG2" s="18"/>
+      <c r="CH2" s="18"/>
+      <c r="CI2" s="18"/>
+      <c r="CJ2" s="18"/>
+      <c r="CK2" s="18"/>
+      <c r="CL2" s="18"/>
+      <c r="CM2" s="18"/>
+      <c r="CN2" s="18"/>
+      <c r="CO2" s="18"/>
+      <c r="CP2" s="18"/>
+      <c r="CQ2" s="18"/>
+      <c r="CR2" s="18"/>
+      <c r="CS2" s="18"/>
+      <c r="CT2" s="18"/>
+      <c r="CU2" s="18"/>
+      <c r="CV2" s="18"/>
+      <c r="CW2" s="18"/>
+      <c r="CX2" s="18"/>
+      <c r="CY2" s="18"/>
+      <c r="CZ2" s="18"/>
+      <c r="DA2" s="18"/>
+      <c r="DB2" s="18"/>
+      <c r="DC2" s="18"/>
+      <c r="DD2" s="18"/>
+      <c r="DE2" s="18"/>
+      <c r="DF2" s="18"/>
+      <c r="DG2" s="18"/>
+      <c r="DH2" s="18"/>
+      <c r="DI2" s="18"/>
+      <c r="DJ2" s="18"/>
+      <c r="DK2" s="18"/>
+      <c r="DL2" s="18"/>
+      <c r="DM2" s="18"/>
+      <c r="DN2" s="18"/>
+      <c r="DO2" s="18"/>
+      <c r="DP2" s="18"/>
+      <c r="DQ2" s="18"/>
+      <c r="DR2" s="18"/>
+      <c r="DS2" s="18"/>
+      <c r="DT2" s="18"/>
+      <c r="DU2" s="18"/>
+      <c r="DV2" s="18"/>
+      <c r="DW2" s="18"/>
+      <c r="DX2" s="18"/>
+      <c r="DY2" s="18"/>
+      <c r="DZ2" s="18"/>
+      <c r="EA2" s="18"/>
+      <c r="EB2" s="18"/>
+      <c r="EC2" s="18"/>
+      <c r="ED2" s="18"/>
+      <c r="EE2" s="18"/>
+      <c r="EF2" s="18"/>
+      <c r="EG2" s="18"/>
+      <c r="EH2" s="18"/>
+      <c r="EI2" s="18"/>
+      <c r="EJ2" s="18"/>
+      <c r="EK2" s="18"/>
+      <c r="EL2" s="18"/>
+      <c r="EM2" s="18"/>
+      <c r="EN2" s="18"/>
+      <c r="EO2" s="18"/>
+      <c r="EP2" s="18"/>
+      <c r="EQ2" s="18"/>
+      <c r="ER2" s="18"/>
+      <c r="ES2" s="18"/>
+      <c r="ET2" s="18"/>
+      <c r="EU2" s="18"/>
+      <c r="EV2" s="18"/>
+      <c r="EW2" s="18"/>
+      <c r="EX2" s="18"/>
+      <c r="EY2" s="18"/>
       <c r="EZ2" s="16"/>
       <c r="FA2" s="16"/>
       <c r="FB2" s="16"/>
       <c r="FC2" s="16"/>
-      <c r="FD2" s="19" t="s">
+      <c r="FD2" s="15" t="s">
         <v>312</v>
       </c>
       <c r="FE2" s="16"/>
@@ -2417,9 +2441,9 @@
       <c r="LR2" s="16"/>
       <c r="LS2" s="16"/>
       <c r="LT2" s="16"/>
-      <c r="LU2" s="18"/>
-    </row>
-    <row r="3" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="LU2" s="14"/>
+    </row>
+    <row r="3" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -2660,8 +2684,12 @@
       <c r="EK3" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="EL3" s="1"/>
-      <c r="EM3" s="1"/>
+      <c r="EL3" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EM3" s="13" t="s">
+        <v>325</v>
+      </c>
       <c r="EN3" s="1" t="s">
         <v>329</v>
       </c>
@@ -2809,6 +2837,9 @@
       <c r="GN3" t="s">
         <v>363</v>
       </c>
+      <c r="GO3" t="s">
+        <v>326</v>
+      </c>
       <c r="GP3" t="s">
         <v>363</v>
       </c>
@@ -2822,10 +2853,13 @@
         <v>363</v>
       </c>
       <c r="GT3" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="GU3" t="s">
-        <v>363</v>
+        <v>326</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>326</v>
       </c>
       <c r="GW3" t="s">
         <v>364</v>
@@ -2879,7 +2913,7 @@
         <v>325</v>
       </c>
       <c r="HO3" t="s">
-        <v>364</v>
+        <v>382</v>
       </c>
       <c r="HP3" t="s">
         <v>365</v>
@@ -2965,8 +2999,23 @@
       <c r="LT3" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="4" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="LU3" t="s">
+        <v>329</v>
+      </c>
+      <c r="LV3" t="s">
+        <v>329</v>
+      </c>
+      <c r="LW3" t="s">
+        <v>325</v>
+      </c>
+      <c r="LX3" t="s">
+        <v>329</v>
+      </c>
+      <c r="LY3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>315</v>
       </c>
@@ -3960,8 +4009,23 @@
       <c r="LT4" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="5" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="LU4" t="s">
+        <v>377</v>
+      </c>
+      <c r="LV4" t="s">
+        <v>378</v>
+      </c>
+      <c r="LW4" t="s">
+        <v>379</v>
+      </c>
+      <c r="LX4" t="s">
+        <v>380</v>
+      </c>
+      <c r="LY4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3987,7 +4051,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -3997,25 +4061,31 @@
       <c r="W6" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="7" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="LW6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="O7" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="8" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>313</v>
+      </c>
+      <c r="LV7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="N8" t="s">
         <v>313</v>
       </c>
-      <c r="V8" t="s">
-        <v>313</v>
-      </c>
       <c r="CG8" t="s">
         <v>313</v>
       </c>
@@ -4029,7 +4099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -4049,7 +4119,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -4069,7 +4139,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -4086,7 +4156,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -4096,8 +4166,11 @@
       <c r="N12" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="13" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="CL12" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -4123,7 +4196,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -4143,7 +4216,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -4157,7 +4230,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:333" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -4452,7 +4525,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>20</v>
       </c>
@@ -4466,7 +4539,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="34" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>21</v>
       </c>
@@ -4483,7 +4556,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="35" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>22</v>
       </c>
@@ -4500,24 +4573,24 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>23</v>
       </c>
       <c r="N36" t="s">
         <v>313</v>
       </c>
-      <c r="CT36" t="s">
-        <v>313</v>
-      </c>
-      <c r="JR36" t="s">
-        <v>313</v>
-      </c>
-      <c r="JS36" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="37" spans="1:331" x14ac:dyDescent="0.25">
+      <c r="FA36" t="s">
+        <v>313</v>
+      </c>
+      <c r="JB36" t="s">
+        <v>313</v>
+      </c>
+      <c r="JC36" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="37" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>24</v>
       </c>
@@ -4531,7 +4604,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>25</v>
       </c>
@@ -4545,7 +4618,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>26</v>
       </c>
@@ -4559,7 +4632,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="40" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>27</v>
       </c>
@@ -4582,7 +4655,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>28</v>
       </c>
@@ -4605,7 +4678,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="42" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>29</v>
       </c>
@@ -4619,7 +4692,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="43" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>30</v>
       </c>
@@ -4633,7 +4706,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="44" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>31</v>
       </c>
@@ -4650,7 +4723,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>32</v>
       </c>
@@ -4687,8 +4760,17 @@
       <c r="LS45" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="46" spans="1:331" x14ac:dyDescent="0.25">
+      <c r="LU45" t="s">
+        <v>313</v>
+      </c>
+      <c r="LX45" t="s">
+        <v>313</v>
+      </c>
+      <c r="LY45" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="46" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>33</v>
       </c>
@@ -4705,7 +4787,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="47" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>34</v>
       </c>
@@ -4722,7 +4804,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="48" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>35</v>
       </c>
@@ -4898,12 +4980,6 @@
       <c r="CH56" t="s">
         <v>313</v>
       </c>
-      <c r="CL56" t="s">
-        <v>313</v>
-      </c>
-      <c r="CM56" t="s">
-        <v>313</v>
-      </c>
       <c r="KR56" t="s">
         <v>313</v>
       </c>
@@ -5366,6 +5442,9 @@
       <c r="AU86" t="s">
         <v>313</v>
       </c>
+      <c r="GP86" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="87" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
@@ -5388,10 +5467,10 @@
       <c r="I88" t="s">
         <v>313</v>
       </c>
-      <c r="GQ88" t="s">
-        <v>313</v>
-      </c>
-      <c r="GR88" t="s">
+      <c r="GT88" t="s">
+        <v>313</v>
+      </c>
+      <c r="GU88" t="s">
         <v>313</v>
       </c>
     </row>
@@ -5403,12 +5482,6 @@
         <v>313</v>
       </c>
       <c r="BI89" t="s">
-        <v>313</v>
-      </c>
-      <c r="GT89" t="s">
-        <v>313</v>
-      </c>
-      <c r="GU89" t="s">
         <v>313</v>
       </c>
       <c r="HD89" t="s">
@@ -5542,7 +5615,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -5556,13 +5629,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="20"/>
       <c r="H3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -5580,7 +5653,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="20">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -5588,13 +5661,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Actualizando requerimientos y Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2DC775-74E1-4916-B61E-8732F670781F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1984DAAF-2D54-4EEB-ACE8-0FF989B39367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="384">
   <si>
     <t>MVC</t>
   </si>
@@ -1271,6 +1271,9 @@
   </si>
   <si>
     <t>Todos usuarios</t>
+  </si>
+  <si>
+    <t>Alumno/Profesor Guia</t>
   </si>
 </sst>
 </file>
@@ -1748,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LY94"/>
+  <dimension ref="A1:LY96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="IM76" workbookViewId="0">
+      <selection activeCell="IN96" sqref="IN96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,6 +2102,12 @@
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
+      <c r="CR1" t="s">
+        <v>326</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="2" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -2585,9 +2594,15 @@
       <c r="CH3" s="1"/>
       <c r="CI3" s="1"/>
       <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
+      <c r="CK3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="CM3" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="CN3" s="1"/>
       <c r="CO3" s="1"/>
       <c r="CP3" s="1"/>
@@ -2973,7 +2988,10 @@
         <v>325</v>
       </c>
       <c r="JA3" t="s">
-        <v>324</v>
+        <v>330</v>
+      </c>
+      <c r="JF3" t="s">
+        <v>383</v>
       </c>
       <c r="JL3" t="s">
         <v>338</v>
@@ -4101,7 +4119,7 @@
     </row>
     <row r="9" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
         <v>313</v>
@@ -4121,27 +4139,24 @@
     </row>
     <row r="10" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>313</v>
+        <v>7</v>
       </c>
       <c r="N10" t="s">
         <v>313</v>
       </c>
-      <c r="CL10" t="s">
-        <v>313</v>
-      </c>
-      <c r="IK10" t="s">
-        <v>313</v>
-      </c>
-      <c r="IZ10" t="s">
+      <c r="CK10" t="s">
+        <v>313</v>
+      </c>
+      <c r="IE10" t="s">
+        <v>313</v>
+      </c>
+      <c r="IY10" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N11" t="s">
         <v>313</v>
@@ -4149,221 +4164,224 @@
       <c r="CK11" t="s">
         <v>313</v>
       </c>
+      <c r="CL11" t="s">
+        <v>313</v>
+      </c>
+      <c r="CS11" t="s">
+        <v>313</v>
+      </c>
       <c r="IE11" t="s">
         <v>313</v>
       </c>
-      <c r="IY11" t="s">
+      <c r="IK11" t="s">
+        <v>313</v>
+      </c>
+      <c r="IN11" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>313</v>
+        <v>10</v>
       </c>
       <c r="N12" t="s">
         <v>313</v>
       </c>
-      <c r="CL12" t="s">
+      <c r="CK12" t="s">
+        <v>313</v>
+      </c>
+      <c r="CR12" t="s">
+        <v>313</v>
+      </c>
+      <c r="IE12" t="s">
+        <v>313</v>
+      </c>
+      <c r="IO12" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N13" t="s">
         <v>313</v>
       </c>
-      <c r="CK13" t="s">
-        <v>313</v>
-      </c>
-      <c r="CL13" t="s">
-        <v>313</v>
-      </c>
-      <c r="CS13" t="s">
-        <v>313</v>
-      </c>
-      <c r="IE13" t="s">
-        <v>313</v>
-      </c>
-      <c r="IK13" t="s">
-        <v>313</v>
-      </c>
-      <c r="IN13" t="s">
+      <c r="DK13" t="s">
+        <v>313</v>
+      </c>
+      <c r="HQ13" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N14" t="s">
         <v>313</v>
       </c>
-      <c r="CK14" t="s">
-        <v>313</v>
-      </c>
-      <c r="CR14" t="s">
-        <v>313</v>
-      </c>
-      <c r="IE14" t="s">
-        <v>313</v>
-      </c>
-      <c r="IO14" t="s">
+      <c r="DL14" t="s">
+        <v>313</v>
+      </c>
+      <c r="HR14" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N15" t="s">
         <v>313</v>
       </c>
-      <c r="DK15" t="s">
-        <v>313</v>
-      </c>
-      <c r="HQ15" t="s">
+      <c r="DN15" t="s">
+        <v>313</v>
+      </c>
+      <c r="HS15" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N16" t="s">
         <v>313</v>
       </c>
-      <c r="DL16" t="s">
-        <v>313</v>
-      </c>
-      <c r="HR16" t="s">
+      <c r="DM16" t="s">
+        <v>313</v>
+      </c>
+      <c r="HT16" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N17" t="s">
         <v>313</v>
       </c>
-      <c r="DN17" t="s">
-        <v>313</v>
-      </c>
-      <c r="HS17" t="s">
+      <c r="EA17" t="s">
+        <v>313</v>
+      </c>
+      <c r="IF17" t="s">
+        <v>313</v>
+      </c>
+      <c r="IG17" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N18" t="s">
         <v>313</v>
       </c>
-      <c r="DM18" t="s">
-        <v>313</v>
-      </c>
-      <c r="HT18" t="s">
+      <c r="EB18" t="s">
+        <v>313</v>
+      </c>
+      <c r="IH18" t="s">
+        <v>313</v>
+      </c>
+      <c r="II18" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N19" t="s">
         <v>313</v>
       </c>
-      <c r="EA19" t="s">
-        <v>313</v>
-      </c>
-      <c r="IF19" t="s">
-        <v>313</v>
-      </c>
-      <c r="IG19" t="s">
+      <c r="CA19" t="s">
+        <v>313</v>
+      </c>
+      <c r="CB19" t="s">
+        <v>313</v>
+      </c>
+      <c r="KE19" t="s">
+        <v>313</v>
+      </c>
+      <c r="KF19" t="s">
+        <v>313</v>
+      </c>
+      <c r="KG19" t="s">
+        <v>313</v>
+      </c>
+      <c r="KH19" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N20" t="s">
         <v>313</v>
       </c>
-      <c r="EB20" t="s">
-        <v>313</v>
-      </c>
-      <c r="IH20" t="s">
-        <v>313</v>
-      </c>
-      <c r="II20" t="s">
+      <c r="CC20" t="s">
+        <v>313</v>
+      </c>
+      <c r="CD20" t="s">
+        <v>313</v>
+      </c>
+      <c r="CT20" t="s">
+        <v>313</v>
+      </c>
+      <c r="KU20" t="s">
+        <v>313</v>
+      </c>
+      <c r="KV20" t="s">
+        <v>313</v>
+      </c>
+      <c r="KW20" t="s">
+        <v>313</v>
+      </c>
+      <c r="KX20" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:310" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>17</v>
+      <c r="A21" s="4" t="s">
+        <v>353</v>
       </c>
       <c r="N21" t="s">
         <v>313</v>
       </c>
-      <c r="CA21" t="s">
-        <v>313</v>
-      </c>
-      <c r="CB21" t="s">
-        <v>313</v>
-      </c>
-      <c r="KE21" t="s">
-        <v>313</v>
-      </c>
-      <c r="KF21" t="s">
-        <v>313</v>
-      </c>
-      <c r="KG21" t="s">
-        <v>313</v>
-      </c>
-      <c r="KH21" t="s">
+      <c r="DU21" t="s">
+        <v>313</v>
+      </c>
+      <c r="EE21" t="s">
+        <v>313</v>
+      </c>
+      <c r="JG21" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:310" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>18</v>
+      <c r="A22" s="4" t="s">
+        <v>354</v>
       </c>
       <c r="N22" t="s">
         <v>313</v>
       </c>
-      <c r="CC22" t="s">
-        <v>313</v>
-      </c>
-      <c r="CD22" t="s">
-        <v>313</v>
-      </c>
-      <c r="CT22" t="s">
-        <v>313</v>
-      </c>
-      <c r="KU22" t="s">
-        <v>313</v>
-      </c>
-      <c r="KV22" t="s">
-        <v>313</v>
-      </c>
-      <c r="KW22" t="s">
-        <v>313</v>
-      </c>
-      <c r="KX22" t="s">
+      <c r="DU22" t="s">
+        <v>313</v>
+      </c>
+      <c r="EH22" t="s">
+        <v>313</v>
+      </c>
+      <c r="JH22" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="N23" t="s">
         <v>313</v>
@@ -4371,16 +4389,16 @@
       <c r="DU23" t="s">
         <v>313</v>
       </c>
-      <c r="EE23" t="s">
-        <v>313</v>
-      </c>
-      <c r="JG23" t="s">
+      <c r="EG23" t="s">
+        <v>313</v>
+      </c>
+      <c r="JJ23" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="N24" t="s">
         <v>313</v>
@@ -4388,160 +4406,160 @@
       <c r="DU24" t="s">
         <v>313</v>
       </c>
-      <c r="EH24" t="s">
-        <v>313</v>
-      </c>
-      <c r="JH24" t="s">
+      <c r="EF24" t="s">
+        <v>313</v>
+      </c>
+      <c r="JI24" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="N25" t="s">
         <v>313</v>
       </c>
+      <c r="DC25" t="s">
+        <v>313</v>
+      </c>
       <c r="DU25" t="s">
         <v>313</v>
       </c>
-      <c r="EG25" t="s">
-        <v>313</v>
-      </c>
-      <c r="JJ25" t="s">
+      <c r="IV25" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="N26" t="s">
         <v>313</v>
       </c>
+      <c r="DD26" t="s">
+        <v>313</v>
+      </c>
       <c r="DU26" t="s">
         <v>313</v>
       </c>
-      <c r="EF26" t="s">
-        <v>313</v>
-      </c>
-      <c r="JI26" t="s">
+      <c r="IX26" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N27" t="s">
         <v>313</v>
       </c>
-      <c r="DC27" t="s">
+      <c r="DB27" t="s">
         <v>313</v>
       </c>
       <c r="DU27" t="s">
         <v>313</v>
       </c>
-      <c r="IV27" t="s">
+      <c r="IT27" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="N28" t="s">
         <v>313</v>
       </c>
-      <c r="DD28" t="s">
+      <c r="DF28" t="s">
         <v>313</v>
       </c>
       <c r="DU28" t="s">
         <v>313</v>
       </c>
-      <c r="IX28" t="s">
+      <c r="HU28" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="N29" t="s">
         <v>313</v>
       </c>
-      <c r="DB29" t="s">
-        <v>313</v>
-      </c>
-      <c r="DU29" t="s">
-        <v>313</v>
-      </c>
-      <c r="IT29" t="s">
+      <c r="ED29" t="s">
+        <v>313</v>
+      </c>
+      <c r="KA29" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="N30" t="s">
         <v>313</v>
       </c>
-      <c r="DF30" t="s">
-        <v>313</v>
-      </c>
-      <c r="DU30" t="s">
-        <v>313</v>
-      </c>
-      <c r="HU30" t="s">
+      <c r="EJ30" t="s">
+        <v>313</v>
+      </c>
+      <c r="KB30" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:310" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>361</v>
+      <c r="A31" s="4">
+        <v>20</v>
       </c>
       <c r="N31" t="s">
         <v>313</v>
       </c>
-      <c r="ED31" t="s">
-        <v>313</v>
-      </c>
-      <c r="KA31" t="s">
+      <c r="DO31" t="s">
+        <v>313</v>
+      </c>
+      <c r="JL31" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:310" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>362</v>
+      <c r="A32" s="4">
+        <v>21</v>
       </c>
       <c r="N32" t="s">
         <v>313</v>
       </c>
-      <c r="EJ32" t="s">
-        <v>313</v>
-      </c>
-      <c r="KB32" t="s">
+      <c r="FA32" t="s">
+        <v>313</v>
+      </c>
+      <c r="JB32" t="s">
+        <v>313</v>
+      </c>
+      <c r="JC32" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N33" t="s">
         <v>313</v>
       </c>
-      <c r="DO33" t="s">
-        <v>313</v>
-      </c>
-      <c r="JL33" t="s">
+      <c r="CT33" t="s">
+        <v>313</v>
+      </c>
+      <c r="JR33" t="s">
+        <v>313</v>
+      </c>
+      <c r="JS33" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N34" t="s">
         <v>313</v>
@@ -4558,401 +4576,401 @@
     </row>
     <row r="35" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N35" t="s">
         <v>313</v>
       </c>
-      <c r="CT35" t="s">
-        <v>313</v>
-      </c>
-      <c r="JR35" t="s">
-        <v>313</v>
-      </c>
-      <c r="JS35" t="s">
+      <c r="EN35" t="s">
+        <v>313</v>
+      </c>
+      <c r="HO35" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N36" t="s">
         <v>313</v>
       </c>
-      <c r="FA36" t="s">
-        <v>313</v>
-      </c>
-      <c r="JB36" t="s">
-        <v>313</v>
-      </c>
-      <c r="JC36" t="s">
+      <c r="DX36" t="s">
+        <v>313</v>
+      </c>
+      <c r="HP36" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>24</v>
-      </c>
-      <c r="N37" t="s">
-        <v>313</v>
-      </c>
-      <c r="EN37" t="s">
-        <v>313</v>
-      </c>
-      <c r="HO37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>313</v>
+      </c>
+      <c r="R37" t="s">
+        <v>313</v>
+      </c>
+      <c r="FD37" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>25</v>
-      </c>
-      <c r="N38" t="s">
-        <v>313</v>
-      </c>
-      <c r="DX38" t="s">
-        <v>313</v>
-      </c>
-      <c r="HP38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>313</v>
+      </c>
+      <c r="P38" t="s">
+        <v>313</v>
+      </c>
+      <c r="R38" t="s">
+        <v>313</v>
+      </c>
+      <c r="FD38" t="s">
+        <v>313</v>
+      </c>
+      <c r="FE38" t="s">
+        <v>313</v>
+      </c>
+      <c r="FI38" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>313</v>
       </c>
+      <c r="Q39" t="s">
+        <v>313</v>
+      </c>
       <c r="R39" t="s">
         <v>313</v>
       </c>
       <c r="FD39" t="s">
+        <v>313</v>
+      </c>
+      <c r="FF39" t="s">
+        <v>313</v>
+      </c>
+      <c r="FG39" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
         <v>313</v>
       </c>
-      <c r="P40" t="s">
-        <v>313</v>
-      </c>
       <c r="R40" t="s">
         <v>313</v>
       </c>
-      <c r="FD40" t="s">
-        <v>313</v>
-      </c>
-      <c r="FE40" t="s">
-        <v>313</v>
-      </c>
-      <c r="FI40" t="s">
+      <c r="FH40" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>28</v>
-      </c>
-      <c r="C41" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>313</v>
-      </c>
-      <c r="R41" t="s">
-        <v>313</v>
-      </c>
-      <c r="FD41" t="s">
-        <v>313</v>
-      </c>
-      <c r="FF41" t="s">
-        <v>313</v>
-      </c>
-      <c r="FG41" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" t="s">
+        <v>313</v>
+      </c>
+      <c r="EV41" t="s">
+        <v>313</v>
+      </c>
+      <c r="KC41" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>313</v>
-      </c>
-      <c r="R42" t="s">
-        <v>313</v>
-      </c>
-      <c r="FH42" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" t="s">
+        <v>313</v>
+      </c>
+      <c r="BU42" t="s">
+        <v>313</v>
+      </c>
+      <c r="GF42" t="s">
+        <v>313</v>
+      </c>
+      <c r="GG42" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>30</v>
-      </c>
-      <c r="N43" t="s">
-        <v>313</v>
-      </c>
-      <c r="EV43" t="s">
-        <v>313</v>
-      </c>
-      <c r="KC43" t="s">
+        <v>32</v>
+      </c>
+      <c r="O43" t="s">
+        <v>313</v>
+      </c>
+      <c r="S43" t="s">
+        <v>313</v>
+      </c>
+      <c r="T43" t="s">
+        <v>313</v>
+      </c>
+      <c r="U43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LM43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LN43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LO43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LP43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LQ43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LR43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LS43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LU43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LX43" t="s">
+        <v>313</v>
+      </c>
+      <c r="LY43" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>31</v>
-      </c>
-      <c r="N44" t="s">
-        <v>313</v>
-      </c>
-      <c r="BU44" t="s">
-        <v>313</v>
-      </c>
-      <c r="GF44" t="s">
-        <v>313</v>
-      </c>
-      <c r="GG44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M44" t="s">
+        <v>313</v>
+      </c>
+      <c r="BK44" t="s">
+        <v>313</v>
+      </c>
+      <c r="HK44" t="s">
+        <v>313</v>
+      </c>
+      <c r="HL44" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>32</v>
-      </c>
-      <c r="O45" t="s">
-        <v>313</v>
-      </c>
-      <c r="S45" t="s">
-        <v>313</v>
-      </c>
-      <c r="T45" t="s">
-        <v>313</v>
-      </c>
-      <c r="U45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LM45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LN45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LO45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LP45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LQ45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LR45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LS45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LU45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LX45" t="s">
-        <v>313</v>
-      </c>
-      <c r="LY45" t="s">
+        <v>34</v>
+      </c>
+      <c r="M45" t="s">
+        <v>313</v>
+      </c>
+      <c r="BJ45" t="s">
+        <v>313</v>
+      </c>
+      <c r="HM45" t="s">
+        <v>313</v>
+      </c>
+      <c r="HN45" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>33</v>
-      </c>
-      <c r="M46" t="s">
-        <v>313</v>
-      </c>
-      <c r="BK46" t="s">
-        <v>313</v>
-      </c>
-      <c r="HK46" t="s">
-        <v>313</v>
-      </c>
-      <c r="HL46" t="s">
+        <v>35</v>
+      </c>
+      <c r="N46" t="s">
+        <v>313</v>
+      </c>
+      <c r="DT46" t="s">
+        <v>313</v>
+      </c>
+      <c r="JM46" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>34</v>
-      </c>
-      <c r="M47" t="s">
-        <v>313</v>
-      </c>
-      <c r="BJ47" t="s">
-        <v>313</v>
-      </c>
-      <c r="HM47" t="s">
-        <v>313</v>
-      </c>
-      <c r="HN47" t="s">
+        <v>36</v>
+      </c>
+      <c r="L47" t="s">
+        <v>313</v>
+      </c>
+      <c r="N47" t="s">
+        <v>313</v>
+      </c>
+      <c r="BE47" t="s">
+        <v>313</v>
+      </c>
+      <c r="CJ47" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="M48" t="s">
+        <v>313</v>
       </c>
       <c r="N48" t="s">
         <v>313</v>
       </c>
-      <c r="DT48" t="s">
-        <v>313</v>
-      </c>
-      <c r="JM48" t="s">
+      <c r="EL48" t="s">
+        <v>313</v>
+      </c>
+      <c r="EM48" t="s">
+        <v>313</v>
+      </c>
+      <c r="JN48" t="s">
+        <v>313</v>
+      </c>
+      <c r="JO48" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L49" t="s">
         <v>313</v>
       </c>
-      <c r="N49" t="s">
-        <v>313</v>
-      </c>
-      <c r="BE49" t="s">
-        <v>313</v>
-      </c>
-      <c r="CJ49" t="s">
+      <c r="AY49" t="s">
+        <v>313</v>
+      </c>
+      <c r="GX49" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>37</v>
-      </c>
-      <c r="M50" t="s">
-        <v>313</v>
-      </c>
-      <c r="N50" t="s">
-        <v>313</v>
-      </c>
-      <c r="EL50" t="s">
-        <v>313</v>
-      </c>
-      <c r="EM50" t="s">
-        <v>313</v>
-      </c>
-      <c r="JN50" t="s">
-        <v>313</v>
-      </c>
-      <c r="JO50" t="s">
+        <v>39</v>
+      </c>
+      <c r="L50" t="s">
+        <v>313</v>
+      </c>
+      <c r="AW50" t="s">
+        <v>313</v>
+      </c>
+      <c r="GY50" t="s">
+        <v>313</v>
+      </c>
+      <c r="GZ50" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L51" t="s">
         <v>313</v>
       </c>
-      <c r="AY51" t="s">
-        <v>313</v>
-      </c>
-      <c r="GX51" t="s">
+      <c r="AX51" t="s">
+        <v>313</v>
+      </c>
+      <c r="HA51" t="s">
+        <v>313</v>
+      </c>
+      <c r="HB51" t="s">
+        <v>313</v>
+      </c>
+      <c r="HC51" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="52" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>39</v>
-      </c>
-      <c r="L52" t="s">
-        <v>313</v>
-      </c>
-      <c r="AW52" t="s">
-        <v>313</v>
-      </c>
-      <c r="GY52" t="s">
-        <v>313</v>
-      </c>
-      <c r="GZ52" t="s">
+        <v>41</v>
+      </c>
+      <c r="N52" t="s">
+        <v>313</v>
+      </c>
+      <c r="AZ52" t="s">
+        <v>313</v>
+      </c>
+      <c r="BA52" t="s">
+        <v>313</v>
+      </c>
+      <c r="BB52" t="s">
+        <v>313</v>
+      </c>
+      <c r="BC52" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD52" t="s">
+        <v>313</v>
+      </c>
+      <c r="DW52" t="s">
+        <v>313</v>
+      </c>
+      <c r="KK52" t="s">
+        <v>313</v>
+      </c>
+      <c r="KL52" t="s">
+        <v>313</v>
+      </c>
+      <c r="KM52" t="s">
+        <v>313</v>
+      </c>
+      <c r="KN52" t="s">
+        <v>313</v>
+      </c>
+      <c r="KO52" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>40</v>
-      </c>
-      <c r="L53" t="s">
-        <v>313</v>
-      </c>
-      <c r="AX53" t="s">
-        <v>313</v>
-      </c>
-      <c r="HA53" t="s">
-        <v>313</v>
-      </c>
-      <c r="HB53" t="s">
-        <v>313</v>
-      </c>
-      <c r="HC53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" t="s">
+        <v>313</v>
+      </c>
+      <c r="N53" t="s">
+        <v>313</v>
+      </c>
+      <c r="DJ53" t="s">
+        <v>313</v>
+      </c>
+      <c r="GH53" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="F54" t="s">
+        <v>313</v>
       </c>
       <c r="N54" t="s">
         <v>313</v>
       </c>
-      <c r="AZ54" t="s">
-        <v>313</v>
-      </c>
-      <c r="BA54" t="s">
-        <v>313</v>
-      </c>
-      <c r="BB54" t="s">
-        <v>313</v>
-      </c>
-      <c r="BC54" t="s">
-        <v>313</v>
-      </c>
-      <c r="BD54" t="s">
-        <v>313</v>
-      </c>
-      <c r="DW54" t="s">
-        <v>313</v>
-      </c>
-      <c r="KK54" t="s">
-        <v>313</v>
-      </c>
-      <c r="KL54" t="s">
-        <v>313</v>
-      </c>
-      <c r="KM54" t="s">
-        <v>313</v>
-      </c>
-      <c r="KN54" t="s">
-        <v>313</v>
-      </c>
-      <c r="KO54" t="s">
+      <c r="CH54" t="s">
+        <v>313</v>
+      </c>
+      <c r="KR54" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F55" t="s">
         <v>313</v>
@@ -4960,121 +4978,118 @@
       <c r="N55" t="s">
         <v>313</v>
       </c>
-      <c r="DJ55" t="s">
-        <v>313</v>
-      </c>
-      <c r="GH55" t="s">
+      <c r="EI55" t="s">
+        <v>313</v>
+      </c>
+      <c r="IK55" t="s">
+        <v>313</v>
+      </c>
+      <c r="IL55" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>43</v>
-      </c>
-      <c r="F56" t="s">
-        <v>313</v>
-      </c>
-      <c r="N56" t="s">
-        <v>313</v>
-      </c>
-      <c r="CH56" t="s">
-        <v>313</v>
-      </c>
-      <c r="KR56" t="s">
+        <v>45</v>
+      </c>
+      <c r="O56" t="s">
+        <v>313</v>
+      </c>
+      <c r="BO56" t="s">
+        <v>313</v>
+      </c>
+      <c r="LD56" t="s">
+        <v>313</v>
+      </c>
+      <c r="LE56" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>44</v>
-      </c>
-      <c r="F57" t="s">
-        <v>313</v>
-      </c>
-      <c r="N57" t="s">
-        <v>313</v>
-      </c>
-      <c r="EI57" t="s">
-        <v>313</v>
-      </c>
-      <c r="IK57" t="s">
-        <v>313</v>
-      </c>
-      <c r="IL57" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" t="s">
+        <v>313</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>313</v>
+      </c>
+      <c r="DL57" t="s">
+        <v>313</v>
+      </c>
+      <c r="FT57" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>45</v>
-      </c>
-      <c r="O58" t="s">
-        <v>313</v>
-      </c>
-      <c r="BO58" t="s">
-        <v>313</v>
-      </c>
-      <c r="LD58" t="s">
-        <v>313</v>
-      </c>
-      <c r="LE58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI58" t="s">
+        <v>313</v>
+      </c>
+      <c r="FU58" t="s">
+        <v>313</v>
+      </c>
+      <c r="FW58" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E59" t="s">
         <v>313</v>
       </c>
-      <c r="AJ59" t="s">
-        <v>313</v>
-      </c>
-      <c r="DL59" t="s">
-        <v>313</v>
-      </c>
-      <c r="FT59" t="s">
+      <c r="AH59" t="s">
+        <v>313</v>
+      </c>
+      <c r="FV59" t="s">
+        <v>313</v>
+      </c>
+      <c r="FX59" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>47</v>
-      </c>
-      <c r="E60" t="s">
-        <v>313</v>
-      </c>
-      <c r="AI60" t="s">
-        <v>313</v>
-      </c>
-      <c r="FU60" t="s">
-        <v>313</v>
-      </c>
-      <c r="FW60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" t="s">
+        <v>313</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>313</v>
+      </c>
+      <c r="FK60" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="61" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>48</v>
-      </c>
-      <c r="E61" t="s">
-        <v>313</v>
-      </c>
-      <c r="AH61" t="s">
-        <v>313</v>
-      </c>
-      <c r="FV61" t="s">
-        <v>313</v>
-      </c>
-      <c r="FX61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D61" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>313</v>
+      </c>
+      <c r="FN61" t="s">
+        <v>313</v>
+      </c>
+      <c r="FO61" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="62" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
         <v>313</v>
@@ -5082,30 +5097,30 @@
       <c r="AB62" t="s">
         <v>313</v>
       </c>
-      <c r="FK62" t="s">
+      <c r="FP62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="63" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D63" t="s">
         <v>313</v>
       </c>
-      <c r="Z63" t="s">
-        <v>313</v>
-      </c>
-      <c r="FN63" t="s">
-        <v>313</v>
-      </c>
-      <c r="FO63" t="s">
+      <c r="AB63" t="s">
+        <v>313</v>
+      </c>
+      <c r="FK63" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:317" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C64" t="s">
+        <v>346</v>
       </c>
       <c r="D64" t="s">
         <v>313</v>
@@ -5113,94 +5128,91 @@
       <c r="AB64" t="s">
         <v>313</v>
       </c>
-      <c r="FP64" t="s">
+      <c r="FK64" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="65" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D65" t="s">
         <v>313</v>
       </c>
-      <c r="AB65" t="s">
-        <v>313</v>
-      </c>
-      <c r="FK65" t="s">
+      <c r="AA65" t="s">
+        <v>313</v>
+      </c>
+      <c r="FJ65" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>53</v>
-      </c>
-      <c r="C66" t="s">
-        <v>346</v>
+        <v>55</v>
       </c>
       <c r="D66" t="s">
         <v>313</v>
       </c>
-      <c r="AB66" t="s">
-        <v>313</v>
-      </c>
-      <c r="FK66" t="s">
+      <c r="AD66" t="s">
+        <v>313</v>
+      </c>
+      <c r="FM66" t="s">
+        <v>313</v>
+      </c>
+      <c r="FQ66" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D67" t="s">
         <v>313</v>
       </c>
-      <c r="AA67" t="s">
-        <v>313</v>
-      </c>
-      <c r="FJ67" t="s">
+      <c r="Y67" t="s">
+        <v>313</v>
+      </c>
+      <c r="FM67" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="68" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>55</v>
-      </c>
-      <c r="D68" t="s">
-        <v>313</v>
-      </c>
-      <c r="AD68" t="s">
-        <v>313</v>
-      </c>
-      <c r="FM68" t="s">
-        <v>313</v>
-      </c>
-      <c r="FQ68" t="s">
+        <v>57</v>
+      </c>
+      <c r="O68" t="s">
+        <v>313</v>
+      </c>
+      <c r="BT68" t="s">
+        <v>313</v>
+      </c>
+      <c r="GW68" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="69" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>56</v>
-      </c>
-      <c r="D69" t="s">
-        <v>313</v>
-      </c>
-      <c r="Y69" t="s">
-        <v>313</v>
-      </c>
-      <c r="FM69" t="s">
+        <v>58</v>
+      </c>
+      <c r="O69" t="s">
+        <v>313</v>
+      </c>
+      <c r="BY69" t="s">
+        <v>313</v>
+      </c>
+      <c r="GW69" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O70" t="s">
         <v>313</v>
       </c>
-      <c r="BT70" t="s">
+      <c r="BW70" t="s">
         <v>313</v>
       </c>
       <c r="GW70" t="s">
@@ -5209,12 +5221,12 @@
     </row>
     <row r="71" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O71" t="s">
         <v>313</v>
       </c>
-      <c r="BY71" t="s">
+      <c r="BV71" t="s">
         <v>313</v>
       </c>
       <c r="GW71" t="s">
@@ -5223,12 +5235,12 @@
     </row>
     <row r="72" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O72" t="s">
         <v>313</v>
       </c>
-      <c r="BW72" t="s">
+      <c r="BZ72" t="s">
         <v>313</v>
       </c>
       <c r="GW72" t="s">
@@ -5237,12 +5249,12 @@
     </row>
     <row r="73" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O73" t="s">
         <v>313</v>
       </c>
-      <c r="BV73" t="s">
+      <c r="BS73" t="s">
         <v>313</v>
       </c>
       <c r="GW73" t="s">
@@ -5251,35 +5263,35 @@
     </row>
     <row r="74" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>61</v>
-      </c>
-      <c r="O74" t="s">
-        <v>313</v>
-      </c>
-      <c r="BZ74" t="s">
-        <v>313</v>
-      </c>
-      <c r="GW74" t="s">
+        <v>63</v>
+      </c>
+      <c r="N74" t="s">
+        <v>313</v>
+      </c>
+      <c r="EO74" t="s">
+        <v>313</v>
+      </c>
+      <c r="ID74" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="75" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>62</v>
-      </c>
-      <c r="O75" t="s">
-        <v>313</v>
-      </c>
-      <c r="BS75" t="s">
-        <v>313</v>
-      </c>
-      <c r="GW75" t="s">
+        <v>64</v>
+      </c>
+      <c r="N75" t="s">
+        <v>313</v>
+      </c>
+      <c r="EO75" t="s">
+        <v>313</v>
+      </c>
+      <c r="ID75" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="76" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N76" t="s">
         <v>313</v>
@@ -5293,274 +5305,308 @@
     </row>
     <row r="77" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>64</v>
-      </c>
-      <c r="N77" t="s">
-        <v>313</v>
-      </c>
-      <c r="EO77" t="s">
-        <v>313</v>
-      </c>
-      <c r="ID77" t="s">
+        <v>66</v>
+      </c>
+      <c r="O77" t="s">
+        <v>313</v>
+      </c>
+      <c r="BR77" t="s">
+        <v>313</v>
+      </c>
+      <c r="LC77" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
-        <v>65</v>
-      </c>
-      <c r="N78" t="s">
-        <v>313</v>
-      </c>
-      <c r="EO78" t="s">
-        <v>313</v>
-      </c>
-      <c r="ID78" t="s">
+        <v>67</v>
+      </c>
+      <c r="H78" t="s">
+        <v>313</v>
+      </c>
+      <c r="AR78" t="s">
+        <v>313</v>
+      </c>
+      <c r="GI78" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="79" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
-        <v>66</v>
-      </c>
-      <c r="O79" t="s">
-        <v>313</v>
-      </c>
-      <c r="BR79" t="s">
-        <v>313</v>
-      </c>
-      <c r="LC79" t="s">
+        <v>68</v>
+      </c>
+      <c r="H79" t="s">
+        <v>313</v>
+      </c>
+      <c r="AP79" t="s">
+        <v>313</v>
+      </c>
+      <c r="GJ79" t="s">
+        <v>313</v>
+      </c>
+      <c r="GK79" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="80" spans="1:315" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H80" t="s">
         <v>313</v>
       </c>
-      <c r="AR80" t="s">
-        <v>313</v>
-      </c>
-      <c r="GI80" t="s">
+      <c r="AQ80" t="s">
+        <v>313</v>
+      </c>
+      <c r="GL80" t="s">
+        <v>313</v>
+      </c>
+      <c r="GM80" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="81" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>68</v>
-      </c>
-      <c r="H81" t="s">
-        <v>313</v>
-      </c>
-      <c r="AP81" t="s">
-        <v>313</v>
-      </c>
-      <c r="GJ81" t="s">
-        <v>313</v>
-      </c>
-      <c r="GK81" t="s">
+        <v>70</v>
+      </c>
+      <c r="G81" t="s">
+        <v>313</v>
+      </c>
+      <c r="AN81" t="s">
+        <v>313</v>
+      </c>
+      <c r="FY81" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="82" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>69</v>
-      </c>
-      <c r="H82" t="s">
-        <v>313</v>
-      </c>
-      <c r="AQ82" t="s">
-        <v>313</v>
-      </c>
-      <c r="GL82" t="s">
-        <v>313</v>
-      </c>
-      <c r="GM82" t="s">
+        <v>71</v>
+      </c>
+      <c r="G82" t="s">
+        <v>313</v>
+      </c>
+      <c r="AL82" t="s">
+        <v>313</v>
+      </c>
+      <c r="FZ82" t="s">
+        <v>313</v>
+      </c>
+      <c r="GA82" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G83" t="s">
         <v>313</v>
       </c>
-      <c r="AN83" t="s">
-        <v>313</v>
-      </c>
-      <c r="FY83" t="s">
+      <c r="GC83" t="s">
+        <v>313</v>
+      </c>
+      <c r="GD83" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="84" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
-        <v>71</v>
-      </c>
-      <c r="G84" t="s">
-        <v>313</v>
-      </c>
-      <c r="AL84" t="s">
-        <v>313</v>
-      </c>
-      <c r="FZ84" t="s">
-        <v>313</v>
-      </c>
-      <c r="GA84" t="s">
+        <v>73</v>
+      </c>
+      <c r="I84" t="s">
+        <v>313</v>
+      </c>
+      <c r="AM84" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS84" t="s">
+        <v>313</v>
+      </c>
+      <c r="AU84" t="s">
+        <v>313</v>
+      </c>
+      <c r="GP84" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="85" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
-        <v>72</v>
-      </c>
-      <c r="G85" t="s">
-        <v>313</v>
-      </c>
-      <c r="GC85" t="s">
-        <v>313</v>
-      </c>
-      <c r="GD85" t="s">
+        <v>74</v>
+      </c>
+      <c r="I85" t="s">
+        <v>313</v>
+      </c>
+      <c r="AT85" t="s">
+        <v>313</v>
+      </c>
+      <c r="GP85" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="86" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I86" t="s">
         <v>313</v>
       </c>
-      <c r="AM86" t="s">
-        <v>313</v>
-      </c>
-      <c r="AS86" t="s">
-        <v>313</v>
-      </c>
-      <c r="AU86" t="s">
-        <v>313</v>
-      </c>
-      <c r="GP86" t="s">
+      <c r="GT86" t="s">
+        <v>313</v>
+      </c>
+      <c r="GU86" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>74</v>
-      </c>
-      <c r="I87" t="s">
-        <v>313</v>
-      </c>
-      <c r="AT87" t="s">
-        <v>313</v>
-      </c>
-      <c r="GP87" t="s">
+        <v>76</v>
+      </c>
+      <c r="J87" t="s">
+        <v>313</v>
+      </c>
+      <c r="BI87" t="s">
+        <v>313</v>
+      </c>
+      <c r="HD87" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="88" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>75</v>
-      </c>
-      <c r="I88" t="s">
-        <v>313</v>
-      </c>
-      <c r="GT88" t="s">
-        <v>313</v>
-      </c>
-      <c r="GU88" t="s">
+        <v>77</v>
+      </c>
+      <c r="J88" t="s">
+        <v>313</v>
+      </c>
+      <c r="BG88" t="s">
+        <v>313</v>
+      </c>
+      <c r="HE88" t="s">
+        <v>313</v>
+      </c>
+      <c r="HF88" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="89" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J89" t="s">
         <v>313</v>
       </c>
-      <c r="BI89" t="s">
-        <v>313</v>
-      </c>
-      <c r="HD89" t="s">
+      <c r="BH89" t="s">
+        <v>313</v>
+      </c>
+      <c r="HH89" t="s">
+        <v>313</v>
+      </c>
+      <c r="HI89" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="90" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
-        <v>77</v>
-      </c>
-      <c r="J90" t="s">
-        <v>313</v>
-      </c>
-      <c r="BG90" t="s">
-        <v>313</v>
-      </c>
-      <c r="HE90" t="s">
-        <v>313</v>
-      </c>
-      <c r="HF90" t="s">
+        <v>79</v>
+      </c>
+      <c r="F90" t="s">
+        <v>313</v>
+      </c>
+      <c r="N90" t="s">
+        <v>313</v>
+      </c>
+      <c r="EO90" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
-        <v>78</v>
-      </c>
-      <c r="J91" t="s">
-        <v>313</v>
-      </c>
-      <c r="BH91" t="s">
-        <v>313</v>
-      </c>
-      <c r="HH91" t="s">
-        <v>313</v>
-      </c>
-      <c r="HI91" t="s">
+        <v>80</v>
+      </c>
+      <c r="N91" t="s">
+        <v>313</v>
+      </c>
+      <c r="DJ91" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="92" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
-        <v>79</v>
-      </c>
-      <c r="F92" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" t="s">
         <v>313</v>
       </c>
       <c r="N92" t="s">
         <v>313</v>
       </c>
-      <c r="EO92" t="s">
+      <c r="FC92" t="s">
+        <v>313</v>
+      </c>
+      <c r="LT92" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="93" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N93" t="s">
         <v>313</v>
       </c>
       <c r="DJ93" t="s">
+        <v>313</v>
+      </c>
+      <c r="JF93" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="94" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
-        <v>81</v>
-      </c>
-      <c r="D94" t="s">
-        <v>313</v>
+        <v>83</v>
       </c>
       <c r="N94" t="s">
         <v>313</v>
       </c>
-      <c r="FC94" t="s">
-        <v>313</v>
-      </c>
-      <c r="LT94" t="s">
+      <c r="CM94" t="s">
+        <v>313</v>
+      </c>
+      <c r="IL94" t="s">
+        <v>313</v>
+      </c>
+      <c r="JA94" t="s">
+        <v>313</v>
+      </c>
+      <c r="JF94" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="95" spans="1:332" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>84</v>
+      </c>
+      <c r="N95" t="s">
+        <v>313</v>
+      </c>
+      <c r="CR95" t="s">
+        <v>313</v>
+      </c>
+      <c r="IO95" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="96" spans="1:332" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>85</v>
+      </c>
+      <c r="N96" t="s">
+        <v>313</v>
+      </c>
+      <c r="CS96" t="s">
+        <v>313</v>
+      </c>
+      <c r="IN96" t="s">
         <v>313</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Colocando Tipos de usuarios  vistas y controladores
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1984DAAF-2D54-4EEB-ACE8-0FF989B39367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE51559A-D7D3-4D35-AD1E-11491C560CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="388">
   <si>
     <t>MVC</t>
   </si>
@@ -738,9 +738,6 @@
   </si>
   <si>
     <t>TesisController.php @evaluar</t>
-  </si>
-  <si>
-    <t>TesisController.php @llamar_filtro_pendient_vencida</t>
   </si>
   <si>
     <t>TesisController.php @llamar_filtro_prorroga_vencida</t>
@@ -1274,6 +1271,21 @@
   </si>
   <si>
     <t>Alumno/Profesor Guia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos </t>
+  </si>
+  <si>
+    <t>Secretaria/Alumno</t>
+  </si>
+  <si>
+    <t>Titulados</t>
+  </si>
+  <si>
+    <t>/tesis/error_cantidad_espacios</t>
+  </si>
+  <si>
+    <t>TesisController.php @llamar_filtro_pendiente_vencida</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +1414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1421,7 +1433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1436,6 +1448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1753,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
   <dimension ref="A1:LY96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="IM76" workbookViewId="0">
-      <selection activeCell="IN96" sqref="IN96"/>
+    <sheetView tabSelected="1" topLeftCell="LT71" workbookViewId="0">
+      <selection activeCell="LT92" sqref="LT92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,8 +1797,8 @@
     <col min="28" max="28" width="32.42578125" customWidth="1"/>
     <col min="29" max="29" width="36.5703125" customWidth="1"/>
     <col min="30" max="30" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.85546875" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" customWidth="1"/>
+    <col min="31" max="31" width="39.28515625" customWidth="1"/>
+    <col min="32" max="32" width="26.7109375" customWidth="1"/>
     <col min="33" max="33" width="18.28515625" customWidth="1"/>
     <col min="34" max="34" width="23.7109375" customWidth="1"/>
     <col min="35" max="35" width="25.140625" customWidth="1"/>
@@ -1794,7 +1807,7 @@
     <col min="38" max="38" width="19.85546875" customWidth="1"/>
     <col min="39" max="39" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="18.28515625" customWidth="1"/>
-    <col min="41" max="41" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.42578125" customWidth="1"/>
     <col min="42" max="42" width="18" customWidth="1"/>
     <col min="43" max="43" width="16.7109375" customWidth="1"/>
     <col min="44" max="44" width="18" customWidth="1"/>
@@ -1819,7 +1832,7 @@
     <col min="64" max="64" width="14.7109375" customWidth="1"/>
     <col min="65" max="65" width="30.28515625" customWidth="1"/>
     <col min="66" max="66" width="29.85546875" customWidth="1"/>
-    <col min="67" max="67" width="12.28515625" customWidth="1"/>
+    <col min="67" max="67" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="30.42578125" customWidth="1"/>
     <col min="69" max="69" width="16.7109375" customWidth="1"/>
     <col min="70" max="71" width="15.5703125" customWidth="1"/>
@@ -1830,12 +1843,12 @@
     <col min="76" max="76" width="30.140625" customWidth="1"/>
     <col min="77" max="77" width="17.42578125" customWidth="1"/>
     <col min="78" max="78" width="31.5703125" customWidth="1"/>
-    <col min="79" max="79" width="28.7109375" customWidth="1"/>
+    <col min="79" max="79" width="34.42578125" customWidth="1"/>
     <col min="80" max="80" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="42.5703125" customWidth="1"/>
     <col min="82" max="82" width="41.5703125" customWidth="1"/>
     <col min="83" max="83" width="34.5703125" customWidth="1"/>
-    <col min="84" max="84" width="16.7109375" customWidth="1"/>
+    <col min="84" max="84" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="34.5703125" customWidth="1"/>
     <col min="86" max="86" width="47.42578125" customWidth="1"/>
     <col min="87" max="87" width="34.85546875" customWidth="1"/>
@@ -1844,7 +1857,7 @@
     <col min="90" max="90" width="15.7109375" customWidth="1"/>
     <col min="91" max="91" width="14.85546875" customWidth="1"/>
     <col min="92" max="92" width="25.85546875" customWidth="1"/>
-    <col min="93" max="93" width="22.7109375" customWidth="1"/>
+    <col min="93" max="93" width="43.140625" customWidth="1"/>
     <col min="94" max="94" width="25" customWidth="1"/>
     <col min="95" max="95" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="30.5703125" customWidth="1"/>
@@ -1860,10 +1873,9 @@
     <col min="106" max="106" width="32.7109375" customWidth="1"/>
     <col min="107" max="107" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="38.28515625" customWidth="1"/>
-    <col min="109" max="109" width="49.28515625" customWidth="1"/>
-    <col min="110" max="110" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="20.85546875" customWidth="1"/>
-    <col min="112" max="112" width="20.140625" customWidth="1"/>
+    <col min="109" max="109" width="24" customWidth="1"/>
+    <col min="110" max="110" width="34.5703125" customWidth="1"/>
+    <col min="111" max="112" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="17.28515625" customWidth="1"/>
     <col min="114" max="114" width="19.140625" customWidth="1"/>
     <col min="115" max="115" width="20.140625" customWidth="1"/>
@@ -1878,12 +1890,12 @@
     <col min="124" max="124" width="35.85546875" customWidth="1"/>
     <col min="125" max="125" width="39" customWidth="1"/>
     <col min="126" max="126" width="38.5703125" customWidth="1"/>
-    <col min="127" max="127" width="32.140625" customWidth="1"/>
+    <col min="127" max="127" width="50.5703125" customWidth="1"/>
     <col min="128" max="128" width="29" customWidth="1"/>
     <col min="129" max="129" width="26.28515625" customWidth="1"/>
     <col min="130" max="130" width="25.140625" customWidth="1"/>
     <col min="131" max="131" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="21.28515625" customWidth="1"/>
+    <col min="132" max="132" width="31.85546875" customWidth="1"/>
     <col min="133" max="133" width="26.7109375" customWidth="1"/>
     <col min="134" max="134" width="28.42578125" customWidth="1"/>
     <col min="135" max="135" width="19.42578125" customWidth="1"/>
@@ -1901,7 +1913,7 @@
     <col min="147" max="147" width="25.85546875" customWidth="1"/>
     <col min="148" max="148" width="34.5703125" customWidth="1"/>
     <col min="149" max="149" width="28.5703125" customWidth="1"/>
-    <col min="150" max="150" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="39.7109375" customWidth="1"/>
     <col min="151" max="151" width="32.140625" customWidth="1"/>
     <col min="152" max="152" width="32.5703125" customWidth="1"/>
     <col min="153" max="154" width="24.85546875" customWidth="1"/>
@@ -1917,7 +1929,7 @@
     <col min="164" max="164" width="30" customWidth="1"/>
     <col min="165" max="165" width="47" customWidth="1"/>
     <col min="166" max="166" width="38" customWidth="1"/>
-    <col min="167" max="167" width="31.140625" customWidth="1"/>
+    <col min="167" max="167" width="50.5703125" customWidth="1"/>
     <col min="168" max="168" width="39.42578125" customWidth="1"/>
     <col min="169" max="169" width="39.28515625" customWidth="1"/>
     <col min="170" max="170" width="36.42578125" customWidth="1"/>
@@ -2002,7 +2014,7 @@
     <col min="251" max="251" width="53.5703125" customWidth="1"/>
     <col min="252" max="252" width="39.42578125" customWidth="1"/>
     <col min="253" max="253" width="51.42578125" customWidth="1"/>
-    <col min="254" max="254" width="27.85546875" customWidth="1"/>
+    <col min="254" max="254" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="255" max="255" width="47.7109375" customWidth="1"/>
     <col min="256" max="256" width="33.7109375" customWidth="1"/>
     <col min="257" max="257" width="38.7109375" bestFit="1" customWidth="1"/>
@@ -2091,22 +2103,22 @@
     <row r="1" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C1" s="8"/>
       <c r="E1" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>368</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>369</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="CR1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="CS1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:337" x14ac:dyDescent="0.25">
@@ -2276,7 +2288,7 @@
       <c r="FB2" s="16"/>
       <c r="FC2" s="16"/>
       <c r="FD2" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="FE2" s="16"/>
       <c r="FF2" s="16"/>
@@ -2450,7 +2462,11 @@
       <c r="LR2" s="16"/>
       <c r="LS2" s="16"/>
       <c r="LT2" s="16"/>
-      <c r="LU2" s="14"/>
+      <c r="LU2" s="21"/>
+      <c r="LV2" s="21"/>
+      <c r="LW2" s="21"/>
+      <c r="LX2" s="21"/>
+      <c r="LY2" s="21"/>
     </row>
     <row r="3" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2458,584 +2474,742 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE3" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="AF3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AL3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AM3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AN3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AO3" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="AP3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AQ3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AR3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AS3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AU3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="AV3" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="BB3" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="BD3" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BF3" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="BG3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="BH3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="BI3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="BJ3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BL3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BM3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BN3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BO3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BP3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BQ3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BR3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="BS3" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="BU3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="BX3" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="BY3" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="BZ3" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="CA3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="CB3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="CC3" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="CD3" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="CE3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="CF3" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="CG3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="CH3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="CI3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="CJ3" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="CK3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="CM3" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="CN3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="CO3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="CP3" s="1"/>
+      <c r="CQ3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="CR3" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="CS3" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="CT3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="CU3" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="CV3" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="AC3" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="AD3" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="BA3" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="BB3" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="BC3" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="BD3" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="BE3" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="BU3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="BV3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="BW3" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="BX3" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="BY3" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="BZ3" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="CM3" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
-      <c r="CU3" s="1"/>
-      <c r="CV3" s="1"/>
-      <c r="CW3" s="1"/>
-      <c r="CX3" s="1"/>
-      <c r="CY3" s="1"/>
-      <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
+      <c r="CW3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="CX3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="CY3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="CZ3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="DA3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="DB3" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="DC3" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="DD3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
-      <c r="DG3" s="1"/>
-      <c r="DH3" s="1"/>
+        <v>335</v>
+      </c>
+      <c r="DE3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="DF3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="DG3" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="DH3" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="DI3" s="1"/>
       <c r="DJ3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="DK3" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="DK3" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="DL3" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="DM3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="DN3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="DO3" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="DP3" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="DQ3" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="DR3" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="DS3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="DT3" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="DU3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="DV3" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
+        <v>337</v>
+      </c>
+      <c r="DW3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="DX3" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="DY3" s="14" t="s">
+        <v>324</v>
+      </c>
       <c r="DZ3" s="1"/>
       <c r="EA3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="EB3" s="1"/>
-      <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
+        <v>324</v>
+      </c>
+      <c r="EB3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="EC3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="ED3" s="14" t="s">
+        <v>337</v>
+      </c>
       <c r="EE3" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="EF3" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="EG3" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="EH3" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="EI3" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="EJ3" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="EK3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="EL3" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="EM3" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="EN3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="EO3" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="EP3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="EQ3" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="ER3" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="EO3" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="EP3" s="1" t="s">
+      <c r="ES3" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="EQ3" s="1"/>
-      <c r="ER3" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="ES3" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="ET3" s="1"/>
+      <c r="ET3" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="EU3" s="6" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
       <c r="EV3" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="EW3" s="6" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
       <c r="EX3" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="EY3" s="1"/>
       <c r="EZ3" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="FA3" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="FB3" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="FC3" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="FD3" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="FE3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FF3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>335</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>346</v>
+      </c>
+      <c r="FL3" t="s">
+        <v>323</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>323</v>
+      </c>
+      <c r="FN3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>325</v>
+      </c>
+      <c r="FT3" t="s">
+        <v>329</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>362</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GC3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GH3" t="s">
+        <v>324</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GJ3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GK3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GL3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GM3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GN3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GO3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GQ3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GR3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GS3" t="s">
+        <v>362</v>
+      </c>
+      <c r="GT3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>325</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>363</v>
+      </c>
+      <c r="GX3" t="s">
+        <v>335</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>335</v>
+      </c>
+      <c r="GZ3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HA3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HB3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HC3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HD3" t="s">
+        <v>335</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>362</v>
+      </c>
+      <c r="HF3" t="s">
+        <v>362</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>362</v>
+      </c>
+      <c r="HH3" t="s">
+        <v>362</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>362</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>324</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>324</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>324</v>
+      </c>
+      <c r="HN3" t="s">
+        <v>324</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>381</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>364</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>325</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>325</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HT3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HU3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HV3" t="s">
+        <v>329</v>
+      </c>
+      <c r="HW3" t="s">
+        <v>324</v>
+      </c>
+      <c r="HY3" t="s">
+        <v>324</v>
+      </c>
+      <c r="IC3" t="s">
+        <v>324</v>
+      </c>
+      <c r="ID3" t="s">
+        <v>349</v>
+      </c>
+      <c r="IF3" t="s">
+        <v>324</v>
+      </c>
+      <c r="IL3" t="s">
+        <v>326</v>
+      </c>
+      <c r="IM3" t="s">
+        <v>328</v>
+      </c>
+      <c r="IN3" t="s">
+        <v>327</v>
+      </c>
+      <c r="IO3" t="s">
+        <v>325</v>
+      </c>
+      <c r="IP3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IQ3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IR3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IS3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IT3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IU3" t="s">
+        <v>329</v>
+      </c>
+      <c r="IV3" t="s">
+        <v>335</v>
+      </c>
+      <c r="IX3" t="s">
+        <v>335</v>
+      </c>
+      <c r="IY3" t="s">
+        <v>324</v>
+      </c>
+      <c r="IZ3" t="s">
+        <v>324</v>
+      </c>
+      <c r="JA3" t="s">
+        <v>329</v>
+      </c>
+      <c r="JF3" t="s">
+        <v>382</v>
+      </c>
+      <c r="JL3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KC3" t="s">
         <v>338</v>
       </c>
-      <c r="FA3" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="FB3" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="FC3" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="FD3" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="FE3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FF3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FG3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FH3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FI3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FJ3" t="s">
-        <v>336</v>
-      </c>
-      <c r="FK3" t="s">
-        <v>347</v>
-      </c>
-      <c r="FL3" t="s">
+      <c r="KU3" t="s">
+        <v>335</v>
+      </c>
+      <c r="KV3" t="s">
+        <v>335</v>
+      </c>
+      <c r="LC3" t="s">
+        <v>343</v>
+      </c>
+      <c r="LD3" t="s">
+        <v>343</v>
+      </c>
+      <c r="LE3" t="s">
+        <v>343</v>
+      </c>
+      <c r="LT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LU3" t="s">
+        <v>328</v>
+      </c>
+      <c r="LV3" t="s">
+        <v>328</v>
+      </c>
+      <c r="LW3" t="s">
         <v>324</v>
       </c>
-      <c r="FM3" t="s">
-        <v>324</v>
-      </c>
-      <c r="FN3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FO3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FP3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FQ3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FR3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FS3" t="s">
-        <v>326</v>
-      </c>
-      <c r="FU3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FW3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FX3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FY3" t="s">
-        <v>363</v>
-      </c>
-      <c r="FZ3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GA3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GB3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GC3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GD3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GF3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GG3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GH3" t="s">
-        <v>325</v>
-      </c>
-      <c r="GI3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GJ3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GK3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GL3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GM3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GN3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GO3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GP3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GQ3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GR3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GS3" t="s">
-        <v>363</v>
-      </c>
-      <c r="GT3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GU3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GV3" t="s">
-        <v>326</v>
-      </c>
-      <c r="GW3" t="s">
-        <v>364</v>
-      </c>
-      <c r="GX3" t="s">
-        <v>336</v>
-      </c>
-      <c r="GY3" t="s">
-        <v>336</v>
-      </c>
-      <c r="GZ3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HA3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HB3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HC3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HD3" t="s">
-        <v>336</v>
-      </c>
-      <c r="HE3" t="s">
-        <v>363</v>
-      </c>
-      <c r="HF3" t="s">
-        <v>363</v>
-      </c>
-      <c r="HG3" t="s">
-        <v>363</v>
-      </c>
-      <c r="HH3" t="s">
-        <v>363</v>
-      </c>
-      <c r="HI3" t="s">
-        <v>363</v>
-      </c>
-      <c r="HK3" t="s">
-        <v>325</v>
-      </c>
-      <c r="HL3" t="s">
-        <v>325</v>
-      </c>
-      <c r="HM3" t="s">
-        <v>325</v>
-      </c>
-      <c r="HN3" t="s">
-        <v>325</v>
-      </c>
-      <c r="HO3" t="s">
-        <v>382</v>
-      </c>
-      <c r="HP3" t="s">
-        <v>365</v>
-      </c>
-      <c r="HQ3" t="s">
-        <v>326</v>
-      </c>
-      <c r="HR3" t="s">
-        <v>326</v>
-      </c>
-      <c r="HS3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HT3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HU3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HV3" t="s">
-        <v>330</v>
-      </c>
-      <c r="HW3" t="s">
-        <v>325</v>
-      </c>
-      <c r="HY3" t="s">
-        <v>325</v>
-      </c>
-      <c r="IC3" t="s">
-        <v>325</v>
-      </c>
-      <c r="ID3" t="s">
-        <v>350</v>
-      </c>
-      <c r="IF3" t="s">
-        <v>325</v>
-      </c>
-      <c r="IL3" t="s">
-        <v>327</v>
-      </c>
-      <c r="IM3" t="s">
-        <v>329</v>
-      </c>
-      <c r="IN3" t="s">
+      <c r="LX3" t="s">
         <v>328</v>
       </c>
-      <c r="IO3" t="s">
-        <v>326</v>
-      </c>
-      <c r="IV3" t="s">
-        <v>336</v>
-      </c>
-      <c r="IX3" t="s">
-        <v>336</v>
-      </c>
-      <c r="IZ3" t="s">
-        <v>325</v>
-      </c>
-      <c r="JA3" t="s">
-        <v>330</v>
-      </c>
-      <c r="JF3" t="s">
-        <v>383</v>
-      </c>
-      <c r="JL3" t="s">
-        <v>338</v>
-      </c>
-      <c r="KC3" t="s">
-        <v>339</v>
-      </c>
-      <c r="KU3" t="s">
-        <v>336</v>
-      </c>
-      <c r="KV3" t="s">
-        <v>336</v>
-      </c>
-      <c r="LC3" t="s">
-        <v>344</v>
-      </c>
-      <c r="LD3" t="s">
-        <v>344</v>
-      </c>
-      <c r="LE3" t="s">
-        <v>344</v>
-      </c>
-      <c r="LT3" t="s">
-        <v>376</v>
-      </c>
-      <c r="LU3" t="s">
-        <v>329</v>
-      </c>
-      <c r="LV3" t="s">
-        <v>329</v>
-      </c>
-      <c r="LW3" t="s">
-        <v>325</v>
-      </c>
-      <c r="LX3" t="s">
-        <v>329</v>
-      </c>
       <c r="LY3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3059,7 +3233,7 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
@@ -3095,13 +3269,13 @@
         <v>22</v>
       </c>
       <c r="V4" t="s">
+        <v>320</v>
+      </c>
+      <c r="W4" t="s">
+        <v>319</v>
+      </c>
+      <c r="X4" t="s">
         <v>321</v>
-      </c>
-      <c r="W4" t="s">
-        <v>320</v>
-      </c>
-      <c r="X4" t="s">
-        <v>322</v>
       </c>
       <c r="Y4" t="s">
         <v>23</v>
@@ -3182,7 +3356,7 @@
         <v>47</v>
       </c>
       <c r="AY4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AZ4" t="s">
         <v>49</v>
@@ -3218,7 +3392,7 @@
         <v>59</v>
       </c>
       <c r="BK4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BL4" t="s">
         <v>60</v>
@@ -3254,7 +3428,7 @@
         <v>70</v>
       </c>
       <c r="BW4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BX4" t="s">
         <v>71</v>
@@ -3266,19 +3440,19 @@
         <v>73</v>
       </c>
       <c r="CA4" t="s">
+        <v>331</v>
+      </c>
+      <c r="CB4" t="s">
         <v>332</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CC4" t="s">
         <v>333</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>334</v>
       </c>
-      <c r="CD4" t="s">
-        <v>335</v>
-      </c>
       <c r="CE4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="CF4" t="s">
         <v>74</v>
@@ -3287,7 +3461,7 @@
         <v>75</v>
       </c>
       <c r="CH4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="CI4" t="s">
         <v>76</v>
@@ -3308,7 +3482,7 @@
         <v>81</v>
       </c>
       <c r="CO4" t="s">
-        <v>81</v>
+        <v>386</v>
       </c>
       <c r="CP4" t="s">
         <v>82</v>
@@ -3410,7 +3584,7 @@
         <v>113</v>
       </c>
       <c r="DW4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="DX4" t="s">
         <v>114</v>
@@ -3500,13 +3674,13 @@
         <v>142</v>
       </c>
       <c r="FA4" t="s">
+        <v>370</v>
+      </c>
+      <c r="FB4" t="s">
         <v>371</v>
       </c>
-      <c r="FB4" t="s">
-        <v>372</v>
-      </c>
       <c r="FC4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="FD4" t="s">
         <v>143</v>
@@ -3569,7 +3743,7 @@
         <v>162</v>
       </c>
       <c r="FX4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="FY4" t="s">
         <v>163</v>
@@ -3749,7 +3923,7 @@
         <v>221</v>
       </c>
       <c r="IF4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="IG4" t="s">
         <v>222</v>
@@ -3779,268 +3953,268 @@
         <v>230</v>
       </c>
       <c r="IP4" t="s">
+        <v>387</v>
+      </c>
+      <c r="IQ4" t="s">
         <v>231</v>
       </c>
-      <c r="IQ4" t="s">
+      <c r="IR4" t="s">
         <v>232</v>
       </c>
-      <c r="IR4" t="s">
+      <c r="IS4" t="s">
         <v>233</v>
       </c>
-      <c r="IS4" t="s">
+      <c r="IT4" t="s">
         <v>234</v>
       </c>
-      <c r="IT4" t="s">
+      <c r="IU4" t="s">
         <v>235</v>
       </c>
-      <c r="IU4" t="s">
+      <c r="IV4" t="s">
         <v>236</v>
       </c>
-      <c r="IV4" t="s">
+      <c r="IW4" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="IW4" s="2" t="s">
+      <c r="IX4" t="s">
         <v>238</v>
       </c>
-      <c r="IX4" t="s">
+      <c r="IY4" t="s">
         <v>239</v>
       </c>
-      <c r="IY4" t="s">
+      <c r="IZ4" t="s">
         <v>240</v>
       </c>
-      <c r="IZ4" t="s">
+      <c r="JA4" t="s">
         <v>241</v>
       </c>
-      <c r="JA4" t="s">
+      <c r="JB4" t="s">
         <v>242</v>
       </c>
-      <c r="JB4" t="s">
+      <c r="JC4" t="s">
         <v>243</v>
       </c>
-      <c r="JC4" t="s">
+      <c r="JD4" t="s">
         <v>244</v>
       </c>
-      <c r="JD4" t="s">
+      <c r="JE4" t="s">
         <v>245</v>
       </c>
-      <c r="JE4" t="s">
+      <c r="JF4" t="s">
         <v>246</v>
       </c>
-      <c r="JF4" t="s">
+      <c r="JG4" t="s">
         <v>247</v>
       </c>
-      <c r="JG4" t="s">
+      <c r="JH4" t="s">
         <v>248</v>
       </c>
-      <c r="JH4" t="s">
+      <c r="JI4" t="s">
         <v>249</v>
       </c>
-      <c r="JI4" t="s">
+      <c r="JJ4" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="JJ4" s="2" t="s">
+      <c r="JK4" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="JK4" s="2" t="s">
+      <c r="JL4" t="s">
+        <v>336</v>
+      </c>
+      <c r="JM4" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="JL4" t="s">
-        <v>337</v>
-      </c>
-      <c r="JM4" s="2" t="s">
+      <c r="JN4" t="s">
         <v>253</v>
       </c>
-      <c r="JN4" t="s">
+      <c r="JO4" t="s">
         <v>254</v>
       </c>
-      <c r="JO4" t="s">
+      <c r="JP4" t="s">
         <v>255</v>
       </c>
-      <c r="JP4" t="s">
+      <c r="JQ4" t="s">
         <v>256</v>
       </c>
-      <c r="JQ4" t="s">
+      <c r="JR4" t="s">
         <v>257</v>
       </c>
-      <c r="JR4" t="s">
+      <c r="JS4" t="s">
         <v>258</v>
       </c>
-      <c r="JS4" t="s">
+      <c r="JT4" t="s">
         <v>259</v>
       </c>
-      <c r="JT4" t="s">
+      <c r="JU4" t="s">
         <v>260</v>
       </c>
-      <c r="JU4" t="s">
+      <c r="JV4" t="s">
         <v>261</v>
       </c>
-      <c r="JV4" t="s">
+      <c r="JW4" t="s">
         <v>262</v>
       </c>
-      <c r="JW4" t="s">
+      <c r="JX4" t="s">
         <v>263</v>
       </c>
-      <c r="JX4" t="s">
+      <c r="JY4" t="s">
         <v>264</v>
       </c>
-      <c r="JY4" t="s">
+      <c r="JZ4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="JZ4" s="2" t="s">
+      <c r="KA4" t="s">
         <v>266</v>
       </c>
-      <c r="KA4" t="s">
+      <c r="KB4" t="s">
         <v>267</v>
       </c>
-      <c r="KB4" t="s">
+      <c r="KC4" t="s">
         <v>268</v>
       </c>
-      <c r="KC4" t="s">
+      <c r="KD4" t="s">
         <v>269</v>
       </c>
-      <c r="KD4" t="s">
+      <c r="KE4" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="KE4" s="2" t="s">
+      <c r="KF4" t="s">
         <v>271</v>
       </c>
-      <c r="KF4" t="s">
+      <c r="KG4" t="s">
         <v>272</v>
       </c>
-      <c r="KG4" t="s">
+      <c r="KH4" t="s">
         <v>273</v>
       </c>
-      <c r="KH4" t="s">
+      <c r="KI4" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="KI4" s="2" t="s">
+      <c r="KJ4" t="s">
         <v>275</v>
       </c>
-      <c r="KJ4" t="s">
+      <c r="KK4" t="s">
         <v>276</v>
       </c>
-      <c r="KK4" t="s">
+      <c r="KL4" t="s">
         <v>277</v>
       </c>
-      <c r="KL4" t="s">
+      <c r="KM4" t="s">
         <v>278</v>
       </c>
-      <c r="KM4" t="s">
+      <c r="KN4" t="s">
         <v>279</v>
       </c>
-      <c r="KN4" t="s">
+      <c r="KO4" t="s">
         <v>280</v>
       </c>
-      <c r="KO4" t="s">
+      <c r="KP4" t="s">
         <v>281</v>
       </c>
-      <c r="KP4" t="s">
+      <c r="KQ4" t="s">
         <v>282</v>
       </c>
-      <c r="KQ4" t="s">
+      <c r="KR4" t="s">
         <v>283</v>
       </c>
-      <c r="KR4" t="s">
+      <c r="KS4" t="s">
         <v>284</v>
       </c>
-      <c r="KS4" t="s">
+      <c r="KT4" t="s">
         <v>285</v>
       </c>
-      <c r="KT4" t="s">
+      <c r="KU4" t="s">
         <v>286</v>
       </c>
-      <c r="KU4" t="s">
+      <c r="KV4" t="s">
         <v>287</v>
       </c>
-      <c r="KV4" t="s">
+      <c r="KW4" t="s">
         <v>288</v>
       </c>
-      <c r="KW4" t="s">
+      <c r="KX4" t="s">
         <v>289</v>
       </c>
-      <c r="KX4" t="s">
+      <c r="KY4" t="s">
         <v>290</v>
       </c>
-      <c r="KY4" t="s">
+      <c r="KZ4" t="s">
         <v>291</v>
       </c>
-      <c r="KZ4" t="s">
+      <c r="LA4" t="s">
         <v>292</v>
       </c>
-      <c r="LA4" t="s">
+      <c r="LB4" t="s">
         <v>293</v>
       </c>
-      <c r="LB4" t="s">
+      <c r="LC4" t="s">
         <v>294</v>
       </c>
-      <c r="LC4" t="s">
+      <c r="LD4" t="s">
         <v>295</v>
       </c>
-      <c r="LD4" t="s">
+      <c r="LE4" t="s">
         <v>296</v>
       </c>
-      <c r="LE4" t="s">
+      <c r="LF4" t="s">
         <v>297</v>
       </c>
-      <c r="LF4" t="s">
+      <c r="LG4" t="s">
         <v>298</v>
       </c>
-      <c r="LG4" t="s">
+      <c r="LH4" t="s">
         <v>299</v>
       </c>
-      <c r="LH4" t="s">
+      <c r="LI4" t="s">
         <v>300</v>
       </c>
-      <c r="LI4" t="s">
+      <c r="LJ4" t="s">
         <v>301</v>
       </c>
-      <c r="LJ4" t="s">
+      <c r="LK4" t="s">
         <v>302</v>
       </c>
-      <c r="LK4" t="s">
+      <c r="LL4" t="s">
         <v>303</v>
       </c>
-      <c r="LL4" t="s">
+      <c r="LM4" t="s">
         <v>304</v>
       </c>
-      <c r="LM4" t="s">
+      <c r="LN4" t="s">
         <v>305</v>
       </c>
-      <c r="LN4" t="s">
+      <c r="LO4" t="s">
         <v>306</v>
       </c>
-      <c r="LO4" t="s">
+      <c r="LP4" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="LP4" s="2" t="s">
+      <c r="LQ4" t="s">
+        <v>310</v>
+      </c>
+      <c r="LR4" t="s">
+        <v>309</v>
+      </c>
+      <c r="LS4" t="s">
         <v>308</v>
       </c>
-      <c r="LQ4" t="s">
-        <v>311</v>
-      </c>
-      <c r="LR4" t="s">
-        <v>310</v>
-      </c>
-      <c r="LS4" t="s">
-        <v>309</v>
-      </c>
       <c r="LT4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="LU4" t="s">
+        <v>376</v>
+      </c>
+      <c r="LV4" t="s">
         <v>377</v>
       </c>
-      <c r="LV4" t="s">
+      <c r="LW4" t="s">
         <v>378</v>
       </c>
-      <c r="LW4" t="s">
+      <c r="LX4" t="s">
         <v>379</v>
       </c>
-      <c r="LX4" t="s">
+      <c r="LY4" t="s">
         <v>380</v>
-      </c>
-      <c r="LY4" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:337" x14ac:dyDescent="0.25">
@@ -4048,25 +4222,25 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BL5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BM5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KZ5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LA5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LB5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LG5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:337" x14ac:dyDescent="0.25">
@@ -4074,13 +4248,13 @@
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="W6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LW6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:337" x14ac:dyDescent="0.25">
@@ -4088,13 +4262,13 @@
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="V7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LV7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:337" x14ac:dyDescent="0.25">
@@ -4102,19 +4276,43 @@
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CG8" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="CN8" t="s">
+        <v>312</v>
+      </c>
+      <c r="CO8" t="s">
+        <v>312</v>
+      </c>
+      <c r="CQ8" t="s">
+        <v>312</v>
+      </c>
+      <c r="EQ8" t="s">
+        <v>312</v>
+      </c>
+      <c r="EY8" t="s">
+        <v>312</v>
       </c>
       <c r="FB8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HY8" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="HZ8" t="s">
+        <v>312</v>
+      </c>
+      <c r="IA8" t="s">
+        <v>312</v>
+      </c>
+      <c r="IB8" t="s">
+        <v>312</v>
       </c>
       <c r="IC8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:337" x14ac:dyDescent="0.25">
@@ -4122,19 +4320,19 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CL9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IK9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IZ9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:337" x14ac:dyDescent="0.25">
@@ -4142,16 +4340,22 @@
         <v>7</v>
       </c>
       <c r="N10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CK10" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="DY10" t="s">
+        <v>312</v>
+      </c>
+      <c r="IA10" t="s">
+        <v>312</v>
       </c>
       <c r="IE10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IY10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:337" x14ac:dyDescent="0.25">
@@ -4159,25 +4363,25 @@
         <v>9</v>
       </c>
       <c r="N11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CK11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CL11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CS11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IE11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IK11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IN11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:337" x14ac:dyDescent="0.25">
@@ -4185,19 +4389,19 @@
         <v>10</v>
       </c>
       <c r="N12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CK12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CR12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IE12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IO12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:337" x14ac:dyDescent="0.25">
@@ -4205,13 +4409,13 @@
         <v>11</v>
       </c>
       <c r="N13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DK13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HQ13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:337" x14ac:dyDescent="0.25">
@@ -4219,13 +4423,13 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DL14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HR14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:337" x14ac:dyDescent="0.25">
@@ -4233,13 +4437,13 @@
         <v>13</v>
       </c>
       <c r="N15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DN15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HS15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:337" x14ac:dyDescent="0.25">
@@ -4247,13 +4451,13 @@
         <v>14</v>
       </c>
       <c r="N16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DM16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HT16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:310" x14ac:dyDescent="0.25">
@@ -4261,16 +4465,16 @@
         <v>15</v>
       </c>
       <c r="N17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EA17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IF17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IG17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:310" x14ac:dyDescent="0.25">
@@ -4278,16 +4482,16 @@
         <v>16</v>
       </c>
       <c r="N18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EB18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IH18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="II18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:310" x14ac:dyDescent="0.25">
@@ -4295,25 +4499,25 @@
         <v>17</v>
       </c>
       <c r="N19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CA19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CB19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KE19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KF19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KG19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KH19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:310" x14ac:dyDescent="0.25">
@@ -4321,192 +4525,192 @@
         <v>18</v>
       </c>
       <c r="N20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CC20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CD20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CT20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KU20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KV20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KW20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KX20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EE21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JG21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EH22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JH22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EG23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JJ23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EF24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JI24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DC25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IV25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DD26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IX26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DB27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IT27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DF28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DU28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HU28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="ED29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KA29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:310" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EJ30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KB30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:310" x14ac:dyDescent="0.25">
@@ -4514,13 +4718,13 @@
         <v>20</v>
       </c>
       <c r="N31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DO31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JL31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:310" x14ac:dyDescent="0.25">
@@ -4528,16 +4732,16 @@
         <v>21</v>
       </c>
       <c r="N32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FA32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JB32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JC32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:337" x14ac:dyDescent="0.25">
@@ -4545,16 +4749,16 @@
         <v>22</v>
       </c>
       <c r="N33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CT33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JR33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JS33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:337" x14ac:dyDescent="0.25">
@@ -4562,16 +4766,16 @@
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FA34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JB34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JC34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:337" x14ac:dyDescent="0.25">
@@ -4579,13 +4783,13 @@
         <v>24</v>
       </c>
       <c r="N35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EN35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HO35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:337" x14ac:dyDescent="0.25">
@@ -4593,13 +4797,13 @@
         <v>25</v>
       </c>
       <c r="N36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DX36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HP36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:337" x14ac:dyDescent="0.25">
@@ -4607,13 +4811,13 @@
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FD37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:337" x14ac:dyDescent="0.25">
@@ -4621,22 +4825,22 @@
         <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FD38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FE38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FI38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:337" x14ac:dyDescent="0.25">
@@ -4644,22 +4848,22 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FD39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FF39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FG39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:337" x14ac:dyDescent="0.25">
@@ -4667,13 +4871,13 @@
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FH40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:337" x14ac:dyDescent="0.25">
@@ -4681,13 +4885,13 @@
         <v>30</v>
       </c>
       <c r="N41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EV41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KC41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:337" x14ac:dyDescent="0.25">
@@ -4695,16 +4899,16 @@
         <v>31</v>
       </c>
       <c r="N42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BU42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GF42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GG42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:337" x14ac:dyDescent="0.25">
@@ -4712,46 +4916,46 @@
         <v>32</v>
       </c>
       <c r="O43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LM43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LN43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LO43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LP43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LQ43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LR43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LS43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LU43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LX43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LY43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:337" x14ac:dyDescent="0.25">
@@ -4759,16 +4963,16 @@
         <v>33</v>
       </c>
       <c r="M44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BK44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HK44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HL44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:337" x14ac:dyDescent="0.25">
@@ -4776,16 +4980,16 @@
         <v>34</v>
       </c>
       <c r="M45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BJ45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HM45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HN45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:337" x14ac:dyDescent="0.25">
@@ -4793,13 +4997,13 @@
         <v>35</v>
       </c>
       <c r="N46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DT46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JM46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:337" x14ac:dyDescent="0.25">
@@ -4807,16 +5011,16 @@
         <v>36</v>
       </c>
       <c r="L47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BE47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CJ47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:337" x14ac:dyDescent="0.25">
@@ -4824,22 +5028,22 @@
         <v>37</v>
       </c>
       <c r="M48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EL48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EM48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JN48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JO48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:317" x14ac:dyDescent="0.25">
@@ -4847,13 +5051,13 @@
         <v>38</v>
       </c>
       <c r="L49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AY49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GX49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:317" x14ac:dyDescent="0.25">
@@ -4861,16 +5065,16 @@
         <v>39</v>
       </c>
       <c r="L50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AW50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GY50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GZ50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:317" x14ac:dyDescent="0.25">
@@ -4878,19 +5082,19 @@
         <v>40</v>
       </c>
       <c r="L51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AX51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HA51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HB51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HC51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:317" x14ac:dyDescent="0.25">
@@ -4898,40 +5102,40 @@
         <v>41</v>
       </c>
       <c r="N52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AZ52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BA52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BB52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BC52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BD52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DW52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KK52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KL52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KM52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KN52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KO52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:317" x14ac:dyDescent="0.25">
@@ -4939,16 +5143,16 @@
         <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DJ53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GH53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:317" x14ac:dyDescent="0.25">
@@ -4956,16 +5160,16 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CH54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="KR54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:317" x14ac:dyDescent="0.25">
@@ -4973,19 +5177,19 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EI55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IK55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IL55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:317" x14ac:dyDescent="0.25">
@@ -4993,16 +5197,16 @@
         <v>45</v>
       </c>
       <c r="O56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BO56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LD56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LE56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:317" x14ac:dyDescent="0.25">
@@ -5010,16 +5214,16 @@
         <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AJ57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DL57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FT57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:317" x14ac:dyDescent="0.25">
@@ -5027,16 +5231,16 @@
         <v>47</v>
       </c>
       <c r="E58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FU58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FW58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:317" x14ac:dyDescent="0.25">
@@ -5044,16 +5248,16 @@
         <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AH59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FV59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FX59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:317" x14ac:dyDescent="0.25">
@@ -5061,13 +5265,13 @@
         <v>49</v>
       </c>
       <c r="D60" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AB60" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FK60" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:317" x14ac:dyDescent="0.25">
@@ -5075,16 +5279,16 @@
         <v>50</v>
       </c>
       <c r="D61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Z61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FN61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FO61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:317" x14ac:dyDescent="0.25">
@@ -5092,13 +5296,13 @@
         <v>51</v>
       </c>
       <c r="D62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AB62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FP62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:317" x14ac:dyDescent="0.25">
@@ -5106,13 +5310,13 @@
         <v>52</v>
       </c>
       <c r="D63" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AB63" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FK63" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:317" x14ac:dyDescent="0.25">
@@ -5120,16 +5324,16 @@
         <v>53</v>
       </c>
       <c r="C64" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AB64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FK64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:315" x14ac:dyDescent="0.25">
@@ -5137,13 +5341,13 @@
         <v>54</v>
       </c>
       <c r="D65" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AA65" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FJ65" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:315" x14ac:dyDescent="0.25">
@@ -5151,16 +5355,16 @@
         <v>55</v>
       </c>
       <c r="D66" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AD66" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FM66" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FQ66" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:315" x14ac:dyDescent="0.25">
@@ -5168,13 +5372,13 @@
         <v>56</v>
       </c>
       <c r="D67" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y67" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FM67" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:315" x14ac:dyDescent="0.25">
@@ -5182,13 +5386,13 @@
         <v>57</v>
       </c>
       <c r="O68" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BT68" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW68" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="69" spans="1:315" x14ac:dyDescent="0.25">
@@ -5196,13 +5400,13 @@
         <v>58</v>
       </c>
       <c r="O69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BY69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:315" x14ac:dyDescent="0.25">
@@ -5210,13 +5414,13 @@
         <v>59</v>
       </c>
       <c r="O70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BW70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="71" spans="1:315" x14ac:dyDescent="0.25">
@@ -5224,13 +5428,13 @@
         <v>60</v>
       </c>
       <c r="O71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BV71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="1:315" x14ac:dyDescent="0.25">
@@ -5238,13 +5442,13 @@
         <v>61</v>
       </c>
       <c r="O72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BZ72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:315" x14ac:dyDescent="0.25">
@@ -5252,13 +5456,13 @@
         <v>62</v>
       </c>
       <c r="O73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BS73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GW73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="74" spans="1:315" x14ac:dyDescent="0.25">
@@ -5266,13 +5470,13 @@
         <v>63</v>
       </c>
       <c r="N74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EO74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="ID74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="1:315" x14ac:dyDescent="0.25">
@@ -5280,13 +5484,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EO75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="ID75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:315" x14ac:dyDescent="0.25">
@@ -5294,13 +5498,13 @@
         <v>65</v>
       </c>
       <c r="N76" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EO76" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="ID76" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:315" x14ac:dyDescent="0.25">
@@ -5308,13 +5512,13 @@
         <v>66</v>
       </c>
       <c r="O77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BR77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LC77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:315" x14ac:dyDescent="0.25">
@@ -5322,13 +5526,13 @@
         <v>67</v>
       </c>
       <c r="H78" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AR78" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GI78" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:315" x14ac:dyDescent="0.25">
@@ -5336,16 +5540,16 @@
         <v>68</v>
       </c>
       <c r="H79" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AP79" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GJ79" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GK79" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:315" x14ac:dyDescent="0.25">
@@ -5353,16 +5557,16 @@
         <v>69</v>
       </c>
       <c r="H80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AQ80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GL80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GM80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:332" x14ac:dyDescent="0.25">
@@ -5370,13 +5574,13 @@
         <v>70</v>
       </c>
       <c r="G81" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AN81" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FY81" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:332" x14ac:dyDescent="0.25">
@@ -5384,16 +5588,16 @@
         <v>71</v>
       </c>
       <c r="G82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AL82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FZ82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GA82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="1:332" x14ac:dyDescent="0.25">
@@ -5401,13 +5605,13 @@
         <v>72</v>
       </c>
       <c r="G83" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GC83" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GD83" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="84" spans="1:332" x14ac:dyDescent="0.25">
@@ -5415,19 +5619,19 @@
         <v>73</v>
       </c>
       <c r="I84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AM84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AS84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AU84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GP84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:332" x14ac:dyDescent="0.25">
@@ -5435,13 +5639,13 @@
         <v>74</v>
       </c>
       <c r="I85" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AT85" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GP85" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:332" x14ac:dyDescent="0.25">
@@ -5449,13 +5653,13 @@
         <v>75</v>
       </c>
       <c r="I86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GT86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="GU86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" spans="1:332" x14ac:dyDescent="0.25">
@@ -5463,13 +5667,13 @@
         <v>76</v>
       </c>
       <c r="J87" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BI87" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HD87" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:332" x14ac:dyDescent="0.25">
@@ -5477,16 +5681,16 @@
         <v>77</v>
       </c>
       <c r="J88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BG88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HE88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HF88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" spans="1:332" x14ac:dyDescent="0.25">
@@ -5494,16 +5698,16 @@
         <v>78</v>
       </c>
       <c r="J89" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BH89" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HH89" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="HI89" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="90" spans="1:332" x14ac:dyDescent="0.25">
@@ -5511,13 +5715,13 @@
         <v>79</v>
       </c>
       <c r="F90" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N90" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="EO90" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="1:332" x14ac:dyDescent="0.25">
@@ -5525,10 +5729,10 @@
         <v>80</v>
       </c>
       <c r="N91" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DJ91" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="92" spans="1:332" x14ac:dyDescent="0.25">
@@ -5536,16 +5740,16 @@
         <v>81</v>
       </c>
       <c r="D92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="FC92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="LT92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="93" spans="1:332" x14ac:dyDescent="0.25">
@@ -5553,13 +5757,13 @@
         <v>82</v>
       </c>
       <c r="N93" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="DJ93" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JF93" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="1:332" x14ac:dyDescent="0.25">
@@ -5567,19 +5771,19 @@
         <v>83</v>
       </c>
       <c r="N94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CM94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IL94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JA94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="JF94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:332" x14ac:dyDescent="0.25">
@@ -5587,13 +5791,13 @@
         <v>84</v>
       </c>
       <c r="N95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CR95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IO95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" spans="1:332" x14ac:dyDescent="0.25">
@@ -5601,13 +5805,13 @@
         <v>85</v>
       </c>
       <c r="N96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CS96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="IN96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -5648,16 +5852,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5671,13 +5875,13 @@
         <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="H3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5689,13 +5893,13 @@
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion final de matriz de trazabilidad y lista de requerimientos
</commit_message>
<xml_diff>
--- a/Matrizdetrazabilidad.xlsx
+++ b/Matrizdetrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LI\Documents\GitHub\Proyectosw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE51559A-D7D3-4D35-AD1E-11491C560CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F2EEA-0948-4F96-8299-BF66A6B362B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{666A54C7-0CBB-48E4-ADFF-9708C8504249}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="387">
   <si>
     <t>MVC</t>
   </si>
@@ -1137,9 +1137,6 @@
   </si>
   <si>
     <t>Todos usuarios logueados</t>
-  </si>
-  <si>
-    <t>Profesor guia/Director Tesis/Alumno</t>
   </si>
   <si>
     <t>profesor guia</t>
@@ -1279,13 +1276,13 @@
     <t>Secretaria/Alumno</t>
   </si>
   <si>
-    <t>Titulados</t>
-  </si>
-  <si>
     <t>/tesis/error_cantidad_espacios</t>
   </si>
   <si>
     <t>TesisController.php @llamar_filtro_pendiente_vencida</t>
+  </si>
+  <si>
+    <t>Profesor Guia/Director Escuela</t>
   </si>
 </sst>
 </file>
@@ -1434,6 +1431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1448,7 +1446,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1764,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA74E8E-0163-4D78-BE60-1042DE1A5478}">
-  <dimension ref="A1:LY96"/>
+  <dimension ref="A1:LY100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="LT71" workbookViewId="0">
-      <selection activeCell="LT92" sqref="LT92"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1801,7 @@
     <col min="35" max="35" width="25.140625" customWidth="1"/>
     <col min="36" max="36" width="28.7109375" customWidth="1"/>
     <col min="37" max="37" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.85546875" customWidth="1"/>
+    <col min="38" max="38" width="34.5703125" customWidth="1"/>
     <col min="39" max="39" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="18.28515625" customWidth="1"/>
     <col min="41" max="41" width="29.42578125" customWidth="1"/>
@@ -1871,7 +1868,7 @@
     <col min="104" max="104" width="30" customWidth="1"/>
     <col min="105" max="105" width="37.42578125" customWidth="1"/>
     <col min="106" max="106" width="32.7109375" customWidth="1"/>
-    <col min="107" max="107" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="43.7109375" customWidth="1"/>
     <col min="108" max="108" width="38.28515625" customWidth="1"/>
     <col min="109" max="109" width="24" customWidth="1"/>
     <col min="110" max="110" width="34.5703125" customWidth="1"/>
@@ -1926,7 +1923,7 @@
     <col min="161" max="161" width="31.140625" customWidth="1"/>
     <col min="162" max="162" width="40.7109375" customWidth="1"/>
     <col min="163" max="163" width="46" customWidth="1"/>
-    <col min="164" max="164" width="30" customWidth="1"/>
+    <col min="164" max="164" width="45.5703125" customWidth="1"/>
     <col min="165" max="165" width="47" customWidth="1"/>
     <col min="166" max="166" width="38" customWidth="1"/>
     <col min="167" max="167" width="50.5703125" customWidth="1"/>
@@ -1941,7 +1938,7 @@
     <col min="176" max="176" width="38.7109375" customWidth="1"/>
     <col min="177" max="177" width="45.5703125" customWidth="1"/>
     <col min="178" max="178" width="57.28515625" customWidth="1"/>
-    <col min="179" max="179" width="30" customWidth="1"/>
+    <col min="179" max="179" width="44.85546875" customWidth="1"/>
     <col min="180" max="180" width="29.85546875" customWidth="1"/>
     <col min="181" max="181" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="182" max="182" width="29.85546875" customWidth="1"/>
@@ -1952,7 +1949,7 @@
     <col min="187" max="187" width="53.7109375" customWidth="1"/>
     <col min="188" max="188" width="56.7109375" customWidth="1"/>
     <col min="189" max="189" width="26.85546875" customWidth="1"/>
-    <col min="190" max="190" width="38.42578125" customWidth="1"/>
+    <col min="190" max="190" width="51" customWidth="1"/>
     <col min="191" max="191" width="27.7109375" customWidth="1"/>
     <col min="192" max="192" width="29.140625" customWidth="1"/>
     <col min="193" max="193" width="35.42578125" customWidth="1"/>
@@ -1971,7 +1968,7 @@
     <col min="208" max="208" width="31" customWidth="1"/>
     <col min="209" max="209" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="210" max="210" width="33.5703125" customWidth="1"/>
-    <col min="211" max="211" width="26.140625" customWidth="1"/>
+    <col min="211" max="211" width="43.7109375" customWidth="1"/>
     <col min="212" max="212" width="28" customWidth="1"/>
     <col min="213" max="213" width="28.28515625" customWidth="1"/>
     <col min="214" max="214" width="34.42578125" customWidth="1"/>
@@ -1989,7 +1986,7 @@
     <col min="226" max="226" width="54.140625" customWidth="1"/>
     <col min="227" max="227" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="45" customWidth="1"/>
-    <col min="229" max="229" width="29.85546875" customWidth="1"/>
+    <col min="229" max="229" width="44.140625" customWidth="1"/>
     <col min="230" max="230" width="26.85546875" customWidth="1"/>
     <col min="231" max="231" width="33.42578125" customWidth="1"/>
     <col min="232" max="232" width="36.28515625" customWidth="1"/>
@@ -2000,7 +1997,7 @@
     <col min="237" max="237" width="38.140625" customWidth="1"/>
     <col min="238" max="238" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="239" max="239" width="30.42578125" customWidth="1"/>
-    <col min="240" max="240" width="26.28515625" customWidth="1"/>
+    <col min="240" max="240" width="41.42578125" customWidth="1"/>
     <col min="241" max="241" width="39" customWidth="1"/>
     <col min="242" max="242" width="38.28515625" customWidth="1"/>
     <col min="243" max="243" width="36.140625" bestFit="1" customWidth="1"/>
@@ -2016,8 +2013,8 @@
     <col min="253" max="253" width="51.42578125" customWidth="1"/>
     <col min="254" max="254" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="255" max="255" width="47.7109375" customWidth="1"/>
-    <col min="256" max="256" width="33.7109375" customWidth="1"/>
-    <col min="257" max="257" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="57.5703125" customWidth="1"/>
+    <col min="257" max="257" width="54.42578125" customWidth="1"/>
     <col min="258" max="258" width="38.28515625" customWidth="1"/>
     <col min="259" max="259" width="45.85546875" customWidth="1"/>
     <col min="260" max="260" width="39" customWidth="1"/>
@@ -2037,8 +2034,8 @@
     <col min="274" max="274" width="37" customWidth="1"/>
     <col min="275" max="275" width="45.42578125" customWidth="1"/>
     <col min="276" max="276" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="36.140625" customWidth="1"/>
+    <col min="277" max="277" width="43.140625" customWidth="1"/>
+    <col min="278" max="278" width="55" customWidth="1"/>
     <col min="279" max="279" width="54" customWidth="1"/>
     <col min="280" max="280" width="43.7109375" customWidth="1"/>
     <col min="281" max="281" width="44.140625" customWidth="1"/>
@@ -2047,15 +2044,15 @@
     <col min="284" max="284" width="50.140625" customWidth="1"/>
     <col min="285" max="285" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="286" max="286" width="41.140625" customWidth="1"/>
-    <col min="287" max="287" width="38.140625" customWidth="1"/>
+    <col min="287" max="287" width="47.140625" customWidth="1"/>
     <col min="288" max="288" width="40.140625" customWidth="1"/>
     <col min="289" max="289" width="37.7109375" customWidth="1"/>
     <col min="290" max="290" width="54.140625" customWidth="1"/>
     <col min="291" max="291" width="37.42578125" customWidth="1"/>
     <col min="292" max="292" width="36.140625" customWidth="1"/>
-    <col min="293" max="293" width="36" customWidth="1"/>
+    <col min="293" max="293" width="51.7109375" customWidth="1"/>
     <col min="294" max="294" width="41.42578125" customWidth="1"/>
-    <col min="295" max="295" width="36.42578125" customWidth="1"/>
+    <col min="295" max="295" width="39" bestFit="1" customWidth="1"/>
     <col min="296" max="296" width="50.5703125" customWidth="1"/>
     <col min="297" max="297" width="44.42578125" customWidth="1"/>
     <col min="298" max="298" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -2074,7 +2071,7 @@
     <col min="311" max="311" width="33.140625" customWidth="1"/>
     <col min="312" max="312" width="32.85546875" customWidth="1"/>
     <col min="313" max="313" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="48" customWidth="1"/>
+    <col min="314" max="314" width="68" customWidth="1"/>
     <col min="315" max="315" width="35.85546875" customWidth="1"/>
     <col min="316" max="316" width="43" customWidth="1"/>
     <col min="317" max="317" width="55.28515625" customWidth="1"/>
@@ -2103,14 +2100,14 @@
     <row r="1" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C1" s="8"/>
       <c r="E1" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -2126,347 +2123,347 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="17" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
-      <c r="AN2" s="18"/>
-      <c r="AO2" s="18"/>
-      <c r="AP2" s="18"/>
-      <c r="AQ2" s="18"/>
-      <c r="AR2" s="18"/>
-      <c r="AS2" s="18"/>
-      <c r="AT2" s="18"/>
-      <c r="AU2" s="18"/>
-      <c r="AV2" s="18"/>
-      <c r="AW2" s="18"/>
-      <c r="AX2" s="18"/>
-      <c r="AY2" s="18"/>
-      <c r="AZ2" s="18"/>
-      <c r="BA2" s="18"/>
-      <c r="BB2" s="18"/>
-      <c r="BC2" s="18"/>
-      <c r="BD2" s="18"/>
-      <c r="BE2" s="18"/>
-      <c r="BF2" s="18"/>
-      <c r="BG2" s="18"/>
-      <c r="BH2" s="18"/>
-      <c r="BI2" s="18"/>
-      <c r="BJ2" s="18"/>
-      <c r="BK2" s="18"/>
-      <c r="BL2" s="18"/>
-      <c r="BM2" s="18"/>
-      <c r="BN2" s="18"/>
-      <c r="BO2" s="18"/>
-      <c r="BP2" s="18"/>
-      <c r="BQ2" s="18"/>
-      <c r="BR2" s="18"/>
-      <c r="BS2" s="18"/>
-      <c r="BT2" s="18"/>
-      <c r="BU2" s="18"/>
-      <c r="BV2" s="18"/>
-      <c r="BW2" s="18"/>
-      <c r="BX2" s="18"/>
-      <c r="BY2" s="18"/>
-      <c r="BZ2" s="18"/>
-      <c r="CA2" s="18"/>
-      <c r="CB2" s="18"/>
-      <c r="CC2" s="18"/>
-      <c r="CD2" s="18"/>
-      <c r="CE2" s="18"/>
-      <c r="CF2" s="18"/>
-      <c r="CG2" s="18"/>
-      <c r="CH2" s="18"/>
-      <c r="CI2" s="18"/>
-      <c r="CJ2" s="18"/>
-      <c r="CK2" s="18"/>
-      <c r="CL2" s="18"/>
-      <c r="CM2" s="18"/>
-      <c r="CN2" s="18"/>
-      <c r="CO2" s="18"/>
-      <c r="CP2" s="18"/>
-      <c r="CQ2" s="18"/>
-      <c r="CR2" s="18"/>
-      <c r="CS2" s="18"/>
-      <c r="CT2" s="18"/>
-      <c r="CU2" s="18"/>
-      <c r="CV2" s="18"/>
-      <c r="CW2" s="18"/>
-      <c r="CX2" s="18"/>
-      <c r="CY2" s="18"/>
-      <c r="CZ2" s="18"/>
-      <c r="DA2" s="18"/>
-      <c r="DB2" s="18"/>
-      <c r="DC2" s="18"/>
-      <c r="DD2" s="18"/>
-      <c r="DE2" s="18"/>
-      <c r="DF2" s="18"/>
-      <c r="DG2" s="18"/>
-      <c r="DH2" s="18"/>
-      <c r="DI2" s="18"/>
-      <c r="DJ2" s="18"/>
-      <c r="DK2" s="18"/>
-      <c r="DL2" s="18"/>
-      <c r="DM2" s="18"/>
-      <c r="DN2" s="18"/>
-      <c r="DO2" s="18"/>
-      <c r="DP2" s="18"/>
-      <c r="DQ2" s="18"/>
-      <c r="DR2" s="18"/>
-      <c r="DS2" s="18"/>
-      <c r="DT2" s="18"/>
-      <c r="DU2" s="18"/>
-      <c r="DV2" s="18"/>
-      <c r="DW2" s="18"/>
-      <c r="DX2" s="18"/>
-      <c r="DY2" s="18"/>
-      <c r="DZ2" s="18"/>
-      <c r="EA2" s="18"/>
-      <c r="EB2" s="18"/>
-      <c r="EC2" s="18"/>
-      <c r="ED2" s="18"/>
-      <c r="EE2" s="18"/>
-      <c r="EF2" s="18"/>
-      <c r="EG2" s="18"/>
-      <c r="EH2" s="18"/>
-      <c r="EI2" s="18"/>
-      <c r="EJ2" s="18"/>
-      <c r="EK2" s="18"/>
-      <c r="EL2" s="18"/>
-      <c r="EM2" s="18"/>
-      <c r="EN2" s="18"/>
-      <c r="EO2" s="18"/>
-      <c r="EP2" s="18"/>
-      <c r="EQ2" s="18"/>
-      <c r="ER2" s="18"/>
-      <c r="ES2" s="18"/>
-      <c r="ET2" s="18"/>
-      <c r="EU2" s="18"/>
-      <c r="EV2" s="18"/>
-      <c r="EW2" s="18"/>
-      <c r="EX2" s="18"/>
-      <c r="EY2" s="18"/>
-      <c r="EZ2" s="16"/>
-      <c r="FA2" s="16"/>
-      <c r="FB2" s="16"/>
-      <c r="FC2" s="16"/>
-      <c r="FD2" s="15" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+      <c r="AQ2" s="19"/>
+      <c r="AR2" s="19"/>
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="19"/>
+      <c r="BH2" s="19"/>
+      <c r="BI2" s="19"/>
+      <c r="BJ2" s="19"/>
+      <c r="BK2" s="19"/>
+      <c r="BL2" s="19"/>
+      <c r="BM2" s="19"/>
+      <c r="BN2" s="19"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
+      <c r="BQ2" s="19"/>
+      <c r="BR2" s="19"/>
+      <c r="BS2" s="19"/>
+      <c r="BT2" s="19"/>
+      <c r="BU2" s="19"/>
+      <c r="BV2" s="19"/>
+      <c r="BW2" s="19"/>
+      <c r="BX2" s="19"/>
+      <c r="BY2" s="19"/>
+      <c r="BZ2" s="19"/>
+      <c r="CA2" s="19"/>
+      <c r="CB2" s="19"/>
+      <c r="CC2" s="19"/>
+      <c r="CD2" s="19"/>
+      <c r="CE2" s="19"/>
+      <c r="CF2" s="19"/>
+      <c r="CG2" s="19"/>
+      <c r="CH2" s="19"/>
+      <c r="CI2" s="19"/>
+      <c r="CJ2" s="19"/>
+      <c r="CK2" s="19"/>
+      <c r="CL2" s="19"/>
+      <c r="CM2" s="19"/>
+      <c r="CN2" s="19"/>
+      <c r="CO2" s="19"/>
+      <c r="CP2" s="19"/>
+      <c r="CQ2" s="19"/>
+      <c r="CR2" s="19"/>
+      <c r="CS2" s="19"/>
+      <c r="CT2" s="19"/>
+      <c r="CU2" s="19"/>
+      <c r="CV2" s="19"/>
+      <c r="CW2" s="19"/>
+      <c r="CX2" s="19"/>
+      <c r="CY2" s="19"/>
+      <c r="CZ2" s="19"/>
+      <c r="DA2" s="19"/>
+      <c r="DB2" s="19"/>
+      <c r="DC2" s="19"/>
+      <c r="DD2" s="19"/>
+      <c r="DE2" s="19"/>
+      <c r="DF2" s="19"/>
+      <c r="DG2" s="19"/>
+      <c r="DH2" s="19"/>
+      <c r="DI2" s="19"/>
+      <c r="DJ2" s="19"/>
+      <c r="DK2" s="19"/>
+      <c r="DL2" s="19"/>
+      <c r="DM2" s="19"/>
+      <c r="DN2" s="19"/>
+      <c r="DO2" s="19"/>
+      <c r="DP2" s="19"/>
+      <c r="DQ2" s="19"/>
+      <c r="DR2" s="19"/>
+      <c r="DS2" s="19"/>
+      <c r="DT2" s="19"/>
+      <c r="DU2" s="19"/>
+      <c r="DV2" s="19"/>
+      <c r="DW2" s="19"/>
+      <c r="DX2" s="19"/>
+      <c r="DY2" s="19"/>
+      <c r="DZ2" s="19"/>
+      <c r="EA2" s="19"/>
+      <c r="EB2" s="19"/>
+      <c r="EC2" s="19"/>
+      <c r="ED2" s="19"/>
+      <c r="EE2" s="19"/>
+      <c r="EF2" s="19"/>
+      <c r="EG2" s="19"/>
+      <c r="EH2" s="19"/>
+      <c r="EI2" s="19"/>
+      <c r="EJ2" s="19"/>
+      <c r="EK2" s="19"/>
+      <c r="EL2" s="19"/>
+      <c r="EM2" s="19"/>
+      <c r="EN2" s="19"/>
+      <c r="EO2" s="19"/>
+      <c r="EP2" s="19"/>
+      <c r="EQ2" s="19"/>
+      <c r="ER2" s="19"/>
+      <c r="ES2" s="19"/>
+      <c r="ET2" s="19"/>
+      <c r="EU2" s="19"/>
+      <c r="EV2" s="19"/>
+      <c r="EW2" s="19"/>
+      <c r="EX2" s="19"/>
+      <c r="EY2" s="19"/>
+      <c r="EZ2" s="17"/>
+      <c r="FA2" s="17"/>
+      <c r="FB2" s="17"/>
+      <c r="FC2" s="17"/>
+      <c r="FD2" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="FE2" s="16"/>
-      <c r="FF2" s="16"/>
-      <c r="FG2" s="16"/>
-      <c r="FH2" s="16"/>
-      <c r="FI2" s="16"/>
-      <c r="FJ2" s="16"/>
-      <c r="FK2" s="16"/>
-      <c r="FL2" s="16"/>
-      <c r="FM2" s="16"/>
-      <c r="FN2" s="16"/>
-      <c r="FO2" s="16"/>
-      <c r="FP2" s="16"/>
-      <c r="FQ2" s="16"/>
-      <c r="FR2" s="16"/>
-      <c r="FS2" s="16"/>
-      <c r="FT2" s="16"/>
-      <c r="FU2" s="16"/>
-      <c r="FV2" s="16"/>
-      <c r="FW2" s="16"/>
-      <c r="FX2" s="16"/>
-      <c r="FY2" s="16"/>
-      <c r="FZ2" s="16"/>
-      <c r="GA2" s="16"/>
-      <c r="GB2" s="16"/>
-      <c r="GC2" s="16"/>
-      <c r="GD2" s="16"/>
-      <c r="GE2" s="16"/>
-      <c r="GF2" s="16"/>
-      <c r="GG2" s="16"/>
-      <c r="GH2" s="16"/>
-      <c r="GI2" s="16"/>
-      <c r="GJ2" s="16"/>
-      <c r="GK2" s="16"/>
-      <c r="GL2" s="16"/>
-      <c r="GM2" s="16"/>
-      <c r="GN2" s="16"/>
-      <c r="GO2" s="16"/>
-      <c r="GP2" s="16"/>
-      <c r="GQ2" s="16"/>
-      <c r="GR2" s="16"/>
-      <c r="GS2" s="16"/>
-      <c r="GT2" s="16"/>
-      <c r="GU2" s="16"/>
-      <c r="GV2" s="16"/>
-      <c r="GW2" s="16"/>
-      <c r="GX2" s="16"/>
-      <c r="GY2" s="16"/>
-      <c r="GZ2" s="16"/>
-      <c r="HA2" s="16"/>
-      <c r="HB2" s="16"/>
-      <c r="HC2" s="16"/>
-      <c r="HD2" s="16"/>
-      <c r="HE2" s="16"/>
-      <c r="HF2" s="16"/>
-      <c r="HG2" s="16"/>
-      <c r="HH2" s="16"/>
-      <c r="HI2" s="16"/>
-      <c r="HJ2" s="16"/>
-      <c r="HK2" s="16"/>
-      <c r="HL2" s="16"/>
-      <c r="HM2" s="16"/>
-      <c r="HN2" s="16"/>
-      <c r="HO2" s="16"/>
-      <c r="HP2" s="16"/>
-      <c r="HQ2" s="16"/>
-      <c r="HR2" s="16"/>
-      <c r="HS2" s="16"/>
-      <c r="HT2" s="16"/>
-      <c r="HU2" s="16"/>
-      <c r="HV2" s="16"/>
-      <c r="HW2" s="16"/>
-      <c r="HX2" s="16"/>
-      <c r="HY2" s="16"/>
-      <c r="HZ2" s="16"/>
-      <c r="IA2" s="16"/>
-      <c r="IB2" s="16"/>
-      <c r="IC2" s="16"/>
-      <c r="ID2" s="16"/>
-      <c r="IE2" s="16"/>
-      <c r="IF2" s="16"/>
-      <c r="IG2" s="16"/>
-      <c r="IH2" s="16"/>
-      <c r="II2" s="16"/>
-      <c r="IJ2" s="16"/>
-      <c r="IK2" s="16"/>
-      <c r="IL2" s="16"/>
-      <c r="IM2" s="16"/>
-      <c r="IN2" s="16"/>
-      <c r="IO2" s="16"/>
-      <c r="IP2" s="16"/>
-      <c r="IQ2" s="16"/>
-      <c r="IR2" s="16"/>
-      <c r="IS2" s="16"/>
-      <c r="IT2" s="16"/>
-      <c r="IU2" s="16"/>
-      <c r="IV2" s="16"/>
-      <c r="IW2" s="16"/>
-      <c r="IX2" s="16"/>
-      <c r="IY2" s="16"/>
-      <c r="IZ2" s="16"/>
-      <c r="JA2" s="16"/>
-      <c r="JB2" s="16"/>
-      <c r="JC2" s="16"/>
-      <c r="JD2" s="16"/>
-      <c r="JE2" s="16"/>
-      <c r="JF2" s="16"/>
-      <c r="JG2" s="16"/>
-      <c r="JH2" s="16"/>
-      <c r="JI2" s="16"/>
-      <c r="JJ2" s="16"/>
-      <c r="JK2" s="16"/>
-      <c r="JL2" s="16"/>
-      <c r="JM2" s="16"/>
-      <c r="JN2" s="16"/>
-      <c r="JO2" s="16"/>
-      <c r="JP2" s="16"/>
-      <c r="JQ2" s="16"/>
-      <c r="JR2" s="16"/>
-      <c r="JS2" s="16"/>
-      <c r="JT2" s="16"/>
-      <c r="JU2" s="16"/>
-      <c r="JV2" s="16"/>
-      <c r="JW2" s="16"/>
-      <c r="JX2" s="16"/>
-      <c r="JY2" s="16"/>
-      <c r="JZ2" s="16"/>
-      <c r="KA2" s="16"/>
-      <c r="KB2" s="16"/>
-      <c r="KC2" s="16"/>
-      <c r="KD2" s="16"/>
-      <c r="KE2" s="16"/>
-      <c r="KF2" s="16"/>
-      <c r="KG2" s="16"/>
-      <c r="KH2" s="16"/>
-      <c r="KI2" s="16"/>
-      <c r="KJ2" s="16"/>
-      <c r="KK2" s="16"/>
-      <c r="KL2" s="16"/>
-      <c r="KM2" s="16"/>
-      <c r="KN2" s="16"/>
-      <c r="KO2" s="16"/>
-      <c r="KP2" s="16"/>
-      <c r="KQ2" s="16"/>
-      <c r="KR2" s="16"/>
-      <c r="KS2" s="16"/>
-      <c r="KT2" s="16"/>
-      <c r="KU2" s="16"/>
-      <c r="KV2" s="16"/>
-      <c r="KW2" s="16"/>
-      <c r="KX2" s="16"/>
-      <c r="KY2" s="16"/>
-      <c r="KZ2" s="16"/>
-      <c r="LA2" s="16"/>
-      <c r="LB2" s="16"/>
-      <c r="LC2" s="16"/>
-      <c r="LD2" s="16"/>
-      <c r="LE2" s="16"/>
-      <c r="LF2" s="16"/>
-      <c r="LG2" s="16"/>
-      <c r="LH2" s="16"/>
-      <c r="LI2" s="16"/>
-      <c r="LJ2" s="16"/>
-      <c r="LK2" s="16"/>
-      <c r="LL2" s="16"/>
-      <c r="LM2" s="16"/>
-      <c r="LN2" s="16"/>
-      <c r="LO2" s="16"/>
-      <c r="LP2" s="16"/>
-      <c r="LQ2" s="16"/>
-      <c r="LR2" s="16"/>
-      <c r="LS2" s="16"/>
-      <c r="LT2" s="16"/>
-      <c r="LU2" s="21"/>
-      <c r="LV2" s="21"/>
-      <c r="LW2" s="21"/>
-      <c r="LX2" s="21"/>
-      <c r="LY2" s="21"/>
+      <c r="FE2" s="17"/>
+      <c r="FF2" s="17"/>
+      <c r="FG2" s="17"/>
+      <c r="FH2" s="17"/>
+      <c r="FI2" s="17"/>
+      <c r="FJ2" s="17"/>
+      <c r="FK2" s="17"/>
+      <c r="FL2" s="17"/>
+      <c r="FM2" s="17"/>
+      <c r="FN2" s="17"/>
+      <c r="FO2" s="17"/>
+      <c r="FP2" s="17"/>
+      <c r="FQ2" s="17"/>
+      <c r="FR2" s="17"/>
+      <c r="FS2" s="17"/>
+      <c r="FT2" s="17"/>
+      <c r="FU2" s="17"/>
+      <c r="FV2" s="17"/>
+      <c r="FW2" s="17"/>
+      <c r="FX2" s="17"/>
+      <c r="FY2" s="17"/>
+      <c r="FZ2" s="17"/>
+      <c r="GA2" s="17"/>
+      <c r="GB2" s="17"/>
+      <c r="GC2" s="17"/>
+      <c r="GD2" s="17"/>
+      <c r="GE2" s="17"/>
+      <c r="GF2" s="17"/>
+      <c r="GG2" s="17"/>
+      <c r="GH2" s="17"/>
+      <c r="GI2" s="17"/>
+      <c r="GJ2" s="17"/>
+      <c r="GK2" s="17"/>
+      <c r="GL2" s="17"/>
+      <c r="GM2" s="17"/>
+      <c r="GN2" s="17"/>
+      <c r="GO2" s="17"/>
+      <c r="GP2" s="17"/>
+      <c r="GQ2" s="17"/>
+      <c r="GR2" s="17"/>
+      <c r="GS2" s="17"/>
+      <c r="GT2" s="17"/>
+      <c r="GU2" s="17"/>
+      <c r="GV2" s="17"/>
+      <c r="GW2" s="17"/>
+      <c r="GX2" s="17"/>
+      <c r="GY2" s="17"/>
+      <c r="GZ2" s="17"/>
+      <c r="HA2" s="17"/>
+      <c r="HB2" s="17"/>
+      <c r="HC2" s="17"/>
+      <c r="HD2" s="17"/>
+      <c r="HE2" s="17"/>
+      <c r="HF2" s="17"/>
+      <c r="HG2" s="17"/>
+      <c r="HH2" s="17"/>
+      <c r="HI2" s="17"/>
+      <c r="HJ2" s="17"/>
+      <c r="HK2" s="17"/>
+      <c r="HL2" s="17"/>
+      <c r="HM2" s="17"/>
+      <c r="HN2" s="17"/>
+      <c r="HO2" s="17"/>
+      <c r="HP2" s="17"/>
+      <c r="HQ2" s="17"/>
+      <c r="HR2" s="17"/>
+      <c r="HS2" s="17"/>
+      <c r="HT2" s="17"/>
+      <c r="HU2" s="17"/>
+      <c r="HV2" s="17"/>
+      <c r="HW2" s="17"/>
+      <c r="HX2" s="17"/>
+      <c r="HY2" s="17"/>
+      <c r="HZ2" s="17"/>
+      <c r="IA2" s="17"/>
+      <c r="IB2" s="17"/>
+      <c r="IC2" s="17"/>
+      <c r="ID2" s="17"/>
+      <c r="IE2" s="17"/>
+      <c r="IF2" s="17"/>
+      <c r="IG2" s="17"/>
+      <c r="IH2" s="17"/>
+      <c r="II2" s="17"/>
+      <c r="IJ2" s="17"/>
+      <c r="IK2" s="17"/>
+      <c r="IL2" s="17"/>
+      <c r="IM2" s="17"/>
+      <c r="IN2" s="17"/>
+      <c r="IO2" s="17"/>
+      <c r="IP2" s="17"/>
+      <c r="IQ2" s="17"/>
+      <c r="IR2" s="17"/>
+      <c r="IS2" s="17"/>
+      <c r="IT2" s="17"/>
+      <c r="IU2" s="17"/>
+      <c r="IV2" s="17"/>
+      <c r="IW2" s="17"/>
+      <c r="IX2" s="17"/>
+      <c r="IY2" s="17"/>
+      <c r="IZ2" s="17"/>
+      <c r="JA2" s="17"/>
+      <c r="JB2" s="17"/>
+      <c r="JC2" s="17"/>
+      <c r="JD2" s="17"/>
+      <c r="JE2" s="17"/>
+      <c r="JF2" s="17"/>
+      <c r="JG2" s="17"/>
+      <c r="JH2" s="17"/>
+      <c r="JI2" s="17"/>
+      <c r="JJ2" s="17"/>
+      <c r="JK2" s="17"/>
+      <c r="JL2" s="17"/>
+      <c r="JM2" s="17"/>
+      <c r="JN2" s="17"/>
+      <c r="JO2" s="17"/>
+      <c r="JP2" s="17"/>
+      <c r="JQ2" s="17"/>
+      <c r="JR2" s="17"/>
+      <c r="JS2" s="17"/>
+      <c r="JT2" s="17"/>
+      <c r="JU2" s="17"/>
+      <c r="JV2" s="17"/>
+      <c r="JW2" s="17"/>
+      <c r="JX2" s="17"/>
+      <c r="JY2" s="17"/>
+      <c r="JZ2" s="17"/>
+      <c r="KA2" s="17"/>
+      <c r="KB2" s="17"/>
+      <c r="KC2" s="17"/>
+      <c r="KD2" s="17"/>
+      <c r="KE2" s="17"/>
+      <c r="KF2" s="17"/>
+      <c r="KG2" s="17"/>
+      <c r="KH2" s="17"/>
+      <c r="KI2" s="17"/>
+      <c r="KJ2" s="17"/>
+      <c r="KK2" s="17"/>
+      <c r="KL2" s="17"/>
+      <c r="KM2" s="17"/>
+      <c r="KN2" s="17"/>
+      <c r="KO2" s="17"/>
+      <c r="KP2" s="17"/>
+      <c r="KQ2" s="17"/>
+      <c r="KR2" s="17"/>
+      <c r="KS2" s="17"/>
+      <c r="KT2" s="17"/>
+      <c r="KU2" s="17"/>
+      <c r="KV2" s="17"/>
+      <c r="KW2" s="17"/>
+      <c r="KX2" s="17"/>
+      <c r="KY2" s="17"/>
+      <c r="KZ2" s="17"/>
+      <c r="LA2" s="17"/>
+      <c r="LB2" s="17"/>
+      <c r="LC2" s="17"/>
+      <c r="LD2" s="17"/>
+      <c r="LE2" s="17"/>
+      <c r="LF2" s="17"/>
+      <c r="LG2" s="17"/>
+      <c r="LH2" s="17"/>
+      <c r="LI2" s="17"/>
+      <c r="LJ2" s="17"/>
+      <c r="LK2" s="17"/>
+      <c r="LL2" s="17"/>
+      <c r="LM2" s="17"/>
+      <c r="LN2" s="17"/>
+      <c r="LO2" s="17"/>
+      <c r="LP2" s="17"/>
+      <c r="LQ2" s="17"/>
+      <c r="LR2" s="17"/>
+      <c r="LS2" s="17"/>
+      <c r="LT2" s="17"/>
+      <c r="LU2" s="15"/>
+      <c r="LV2" s="15"/>
+      <c r="LW2" s="15"/>
+      <c r="LX2" s="15"/>
+      <c r="LY2" s="15"/>
     </row>
     <row r="3" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2513,7 +2510,7 @@
         <v>347</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AD3" s="11" t="s">
         <v>323</v>
@@ -2540,7 +2537,7 @@
         <v>325</v>
       </c>
       <c r="AL3" s="14" t="s">
-        <v>325</v>
+        <v>386</v>
       </c>
       <c r="AM3" s="14" t="s">
         <v>325</v>
@@ -2549,7 +2546,7 @@
         <v>325</v>
       </c>
       <c r="AO3" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AP3" s="14" t="s">
         <v>325</v>
@@ -2678,7 +2675,7 @@
         <v>337</v>
       </c>
       <c r="CF3" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="CG3" s="14" t="s">
         <v>324</v>
@@ -2690,7 +2687,7 @@
         <v>337</v>
       </c>
       <c r="CJ3" s="14" t="s">
-        <v>385</v>
+        <v>337</v>
       </c>
       <c r="CK3" s="1" t="s">
         <v>324</v>
@@ -2788,7 +2785,7 @@
         <v>329</v>
       </c>
       <c r="DR3" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="DS3" s="1" t="s">
         <v>329</v>
@@ -2895,7 +2892,7 @@
         <v>324</v>
       </c>
       <c r="FC3" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="FD3" s="1" t="s">
         <v>343</v>
@@ -3081,10 +3078,10 @@
         <v>324</v>
       </c>
       <c r="HO3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="HP3" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
       <c r="HQ3" t="s">
         <v>325</v>
@@ -3116,6 +3113,9 @@
       <c r="ID3" t="s">
         <v>349</v>
       </c>
+      <c r="IE3" t="s">
+        <v>324</v>
+      </c>
       <c r="IF3" t="s">
         <v>324</v>
       </c>
@@ -3164,15 +3164,66 @@
       <c r="JA3" t="s">
         <v>329</v>
       </c>
+      <c r="JB3" t="s">
+        <v>324</v>
+      </c>
+      <c r="JC3" t="s">
+        <v>324</v>
+      </c>
+      <c r="JD3" t="s">
+        <v>325</v>
+      </c>
+      <c r="JE3" t="s">
+        <v>329</v>
+      </c>
       <c r="JF3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="JL3" t="s">
         <v>337</v>
       </c>
+      <c r="JM3" t="s">
+        <v>337</v>
+      </c>
+      <c r="JN3" t="s">
+        <v>337</v>
+      </c>
+      <c r="JO3" t="s">
+        <v>337</v>
+      </c>
+      <c r="JP3" t="s">
+        <v>337</v>
+      </c>
       <c r="KC3" t="s">
         <v>338</v>
       </c>
+      <c r="KI3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KJ3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KK3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KL3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KM3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KN3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KO3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KP3" t="s">
+        <v>337</v>
+      </c>
+      <c r="KQ3" t="s">
+        <v>337</v>
+      </c>
       <c r="KU3" t="s">
         <v>335</v>
       </c>
@@ -3189,7 +3240,7 @@
         <v>343</v>
       </c>
       <c r="LT3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="LU3" t="s">
         <v>328</v>
@@ -3482,7 +3533,7 @@
         <v>81</v>
       </c>
       <c r="CO4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="CP4" t="s">
         <v>82</v>
@@ -3674,13 +3725,13 @@
         <v>142</v>
       </c>
       <c r="FA4" t="s">
+        <v>369</v>
+      </c>
+      <c r="FB4" t="s">
         <v>370</v>
       </c>
-      <c r="FB4" t="s">
-        <v>371</v>
-      </c>
       <c r="FC4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="FD4" t="s">
         <v>143</v>
@@ -3953,7 +4004,7 @@
         <v>230</v>
       </c>
       <c r="IP4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="IQ4" t="s">
         <v>231</v>
@@ -4199,22 +4250,22 @@
         <v>308</v>
       </c>
       <c r="LT4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="LU4" t="s">
+        <v>375</v>
+      </c>
+      <c r="LV4" t="s">
         <v>376</v>
       </c>
-      <c r="LV4" t="s">
+      <c r="LW4" t="s">
         <v>377</v>
       </c>
-      <c r="LW4" t="s">
+      <c r="LX4" t="s">
         <v>378</v>
       </c>
-      <c r="LX4" t="s">
+      <c r="LY4" t="s">
         <v>379</v>
-      </c>
-      <c r="LY4" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:337" x14ac:dyDescent="0.25">
@@ -4533,9 +4584,6 @@
       <c r="CD20" t="s">
         <v>312</v>
       </c>
-      <c r="CT20" t="s">
-        <v>312</v>
-      </c>
       <c r="KU20" t="s">
         <v>312</v>
       </c>
@@ -4720,10 +4768,22 @@
       <c r="N31" t="s">
         <v>312</v>
       </c>
+      <c r="CE31" t="s">
+        <v>312</v>
+      </c>
+      <c r="CT31" t="s">
+        <v>312</v>
+      </c>
       <c r="DO31" t="s">
         <v>312</v>
       </c>
       <c r="JL31" t="s">
+        <v>312</v>
+      </c>
+      <c r="JP31" t="s">
+        <v>312</v>
+      </c>
+      <c r="JQ31" t="s">
         <v>312</v>
       </c>
     </row>
@@ -4876,6 +4936,9 @@
       <c r="R40" t="s">
         <v>312</v>
       </c>
+      <c r="FD40" t="s">
+        <v>312</v>
+      </c>
       <c r="FH40" t="s">
         <v>312</v>
       </c>
@@ -5022,6 +5085,12 @@
       <c r="CJ47" t="s">
         <v>312</v>
       </c>
+      <c r="KP47" t="s">
+        <v>312</v>
+      </c>
+      <c r="KQ47" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="48" spans="1:337" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
@@ -5267,10 +5336,16 @@
       <c r="D60" t="s">
         <v>312</v>
       </c>
+      <c r="Y60" t="s">
+        <v>312</v>
+      </c>
       <c r="AB60" t="s">
         <v>312</v>
       </c>
-      <c r="FK60" t="s">
+      <c r="FL60" t="s">
+        <v>312</v>
+      </c>
+      <c r="FM60" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5357,6 +5432,9 @@
       <c r="D66" t="s">
         <v>312</v>
       </c>
+      <c r="AB66" t="s">
+        <v>312</v>
+      </c>
       <c r="AD66" t="s">
         <v>312</v>
       </c>
@@ -5562,9 +5640,6 @@
       <c r="AQ80" t="s">
         <v>312</v>
       </c>
-      <c r="GL80" t="s">
-        <v>312</v>
-      </c>
       <c r="GM80" t="s">
         <v>312</v>
       </c>
@@ -5641,10 +5716,16 @@
       <c r="I85" t="s">
         <v>312</v>
       </c>
-      <c r="AT85" t="s">
+      <c r="AS85" t="s">
         <v>312</v>
       </c>
       <c r="GP85" t="s">
+        <v>312</v>
+      </c>
+      <c r="GQ85" t="s">
+        <v>312</v>
+      </c>
+      <c r="GR85" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5655,6 +5736,9 @@
       <c r="I86" t="s">
         <v>312</v>
       </c>
+      <c r="AT86" t="s">
+        <v>312</v>
+      </c>
       <c r="GT86" t="s">
         <v>312</v>
       </c>
@@ -5723,6 +5807,9 @@
       <c r="EO90" t="s">
         <v>312</v>
       </c>
+      <c r="ID90" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="91" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
@@ -5734,6 +5821,9 @@
       <c r="DJ91" t="s">
         <v>312</v>
       </c>
+      <c r="HW91" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="92" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
@@ -5773,10 +5863,7 @@
       <c r="N94" t="s">
         <v>312</v>
       </c>
-      <c r="CM94" t="s">
-        <v>312</v>
-      </c>
-      <c r="IL94" t="s">
+      <c r="DK94" t="s">
         <v>312</v>
       </c>
       <c r="JA94" t="s">
@@ -5799,6 +5886,9 @@
       <c r="IO95" t="s">
         <v>312</v>
       </c>
+      <c r="JD95" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="96" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
@@ -5811,6 +5901,74 @@
         <v>312</v>
       </c>
       <c r="IN96" t="s">
+        <v>312</v>
+      </c>
+      <c r="JE96" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:218" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>86</v>
+      </c>
+      <c r="H97" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR97" t="s">
+        <v>312</v>
+      </c>
+      <c r="GI97" t="s">
+        <v>312</v>
+      </c>
+      <c r="GO97" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="98" spans="1:218" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>87</v>
+      </c>
+      <c r="J98" t="s">
+        <v>312</v>
+      </c>
+      <c r="BI98" t="s">
+        <v>312</v>
+      </c>
+      <c r="HJ98" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="99" spans="1:218" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>88</v>
+      </c>
+      <c r="I99" t="s">
+        <v>312</v>
+      </c>
+      <c r="AU99" t="s">
+        <v>312</v>
+      </c>
+      <c r="GP99" t="s">
+        <v>312</v>
+      </c>
+      <c r="GV99" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:218" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>89</v>
+      </c>
+      <c r="G100" t="s">
+        <v>312</v>
+      </c>
+      <c r="AN100" t="s">
+        <v>312</v>
+      </c>
+      <c r="FY100" t="s">
+        <v>312</v>
+      </c>
+      <c r="GE100" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5865,7 +6023,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -5879,13 +6037,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="H3" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -5897,13 +6055,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="H5" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="21">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -5911,13 +6069,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>